<commit_message>
Reordenando los archivos para que queden en la carpeta correcta ```
</commit_message>
<xml_diff>
--- a/email-branding/excel/minified_html_output.xlsx
+++ b/email-branding/excel/minified_html_output.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\w\iconstruye-temp\email-branding\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A28789-FFD4-4160-9DB0-68CED6BB1B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFC56DD-D4A2-4753-8619-39D57DE01CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="862">
   <si>
     <t>IDMAIL</t>
   </si>
@@ -6096,6 +6097,9 @@
   <si>
     <t>INSERT_R</t>
   </si>
+  <si>
+    <t>PASO QA</t>
+  </si>
 </sst>
 </file>
 
@@ -6113,6 +6117,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -6313,40 +6318,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -6757,13 +6728,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -6777,6 +6741,47 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -6793,32 +6798,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61FA007A-AA43-4E1A-83D1-64EBEDF43D0B}" name="Table1" displayName="Table1" ref="A1:T124" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="21">
-  <autoFilter ref="A1:T124" xr:uid="{61FA007A-AA43-4E1A-83D1-64EBEDF43D0B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61FA007A-AA43-4E1A-83D1-64EBEDF43D0B}" name="Table1" displayName="Table1" ref="A1:T124" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="A1:T124" xr:uid="{61FA007A-AA43-4E1A-83D1-64EBEDF43D0B}">
+    <filterColumn colId="13">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{519630D5-32E9-43AD-901E-330444893321}" name="IDMAIL" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{28E8B7EE-155F-4153-B74A-2C6DEC729EE7}" name="SUFIJO_A" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{32B475BF-227B-4B06-90BD-2398AA863C5C}" name="SUFIJO_R" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{84A2A707-CBA0-4678-884E-389C8DB405B3}" name="MREMITENTE" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{9D4919C7-5EBD-4CA0-91C3-42EFDAB1B9A0}" name="MREMITENTEMAIL" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{C4ACF937-7FF3-4F6B-9708-71CCE96F0A4F}" name="MASUNTO" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{C15EF5EF-072F-4264-9AC8-01F669E1881B}" name="MASUNTO_A" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{1FCE37FF-5DE6-4FCD-B981-FD60452321DC}" name="MASUNTO_R" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{16B8A6D6-FBEC-4080-BC85-8F03E6D0F6F2}" name="MCUERPO1" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{7298CDE6-1232-4E2A-A84B-3C57F1DB1BC5}" name="DESCRIPCION" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{A4D64EB4-1B4E-4823-96E2-C02B4E45E7A9}" name="TANDA" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{386BD175-89F7-4E88-885D-BDC58C687AE7}" name="MCUERPO1_AGILICE" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{3219CBFA-CF31-464D-8778-A4BC64BB65C0}" name="MCUERPO1_REDMAT" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{2B663266-14EC-4D79-A756-4B34801E5DA1}" name="DONE_A" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{8F60D44D-4D06-468E-B810-9918ACC050D0}" name="DONE_R" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{7E1E2F16-80A1-42AD-BBDC-25831719E72B}" name="OBS" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{86DDD47D-ADED-4264-8D03-262A9E416357}" name="A_minified" dataDxfId="4" dataCellStyle="Neutral"/>
-    <tableColumn id="19" xr3:uid="{86DC3FA1-E4F6-433D-BAC1-248EBF5F0195}" name="R_minified" dataDxfId="3" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{519630D5-32E9-43AD-901E-330444893321}" name="IDMAIL" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{28E8B7EE-155F-4153-B74A-2C6DEC729EE7}" name="SUFIJO_A" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{32B475BF-227B-4B06-90BD-2398AA863C5C}" name="SUFIJO_R" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{84A2A707-CBA0-4678-884E-389C8DB405B3}" name="MREMITENTE" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{9D4919C7-5EBD-4CA0-91C3-42EFDAB1B9A0}" name="MREMITENTEMAIL" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{C4ACF937-7FF3-4F6B-9708-71CCE96F0A4F}" name="MASUNTO" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{C15EF5EF-072F-4264-9AC8-01F669E1881B}" name="MASUNTO_A" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{1FCE37FF-5DE6-4FCD-B981-FD60452321DC}" name="MASUNTO_R" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{16B8A6D6-FBEC-4080-BC85-8F03E6D0F6F2}" name="MCUERPO1" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{7298CDE6-1232-4E2A-A84B-3C57F1DB1BC5}" name="DESCRIPCION" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{A4D64EB4-1B4E-4823-96E2-C02B4E45E7A9}" name="TANDA" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{386BD175-89F7-4E88-885D-BDC58C687AE7}" name="MCUERPO1_AGILICE" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{3219CBFA-CF31-464D-8778-A4BC64BB65C0}" name="MCUERPO1_REDMAT" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{2B663266-14EC-4D79-A756-4B34801E5DA1}" name="DONE_A" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{8F60D44D-4D06-468E-B810-9918ACC050D0}" name="DONE_R" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{7E1E2F16-80A1-42AD-BBDC-25831719E72B}" name="OBS" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{86DDD47D-ADED-4264-8D03-262A9E416357}" name="A_minified" dataDxfId="3" dataCellStyle="Neutral"/>
+    <tableColumn id="19" xr3:uid="{86DC3FA1-E4F6-433D-BAC1-248EBF5F0195}" name="R_minified" dataDxfId="2" dataCellStyle="Neutral"/>
     <tableColumn id="20" xr3:uid="{C4F06B56-9ADE-4CDD-829D-8B4E98E633A3}" name="INSERT_A" dataDxfId="1">
-      <calculatedColumnFormula>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</calculatedColumnFormula>
+      <calculatedColumnFormula>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="21" xr3:uid="{89DEE760-DF0C-4A51-B7C4-A982EBC41AEE}" name="INSERT_R" dataDxfId="0">
-      <calculatedColumnFormula>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</calculatedColumnFormula>
+      <calculatedColumnFormula>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7110,36 +7121,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:T124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.90625" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" customWidth="1"/>
-    <col min="10" max="10" width="14.08984375" customWidth="1"/>
-    <col min="12" max="12" width="19.90625" customWidth="1"/>
-    <col min="13" max="13" width="20.7265625" customWidth="1"/>
-    <col min="14" max="14" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="69.1796875" customWidth="1"/>
-    <col min="17" max="17" width="11.81640625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="11.7265625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="97.1796875" customWidth="1"/>
-    <col min="20" max="20" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="69.21875" customWidth="1"/>
+    <col min="17" max="18" width="11.77734375" style="4" customWidth="1"/>
+    <col min="19" max="19" width="97.21875" customWidth="1"/>
+    <col min="20" max="20" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7201,7 +7212,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>202</v>
       </c>
@@ -7257,8 +7268,8 @@
         <v>28</v>
       </c>
       <c r="S2" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20202, 'Agilice','iconstruye@iconstruye.com', '¡Gracias por actualizar tu información! Ya puedes acceder con tu correo a AGILICE', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;AGILICE&lt;/title&gt;&lt;style type=text/css&gt;* {margin: 0;font-family: "Helvetica Neue", Helvetica, Arial, sans-serif;box-sizing: border-box;font-size: 14px;}img {max-width: 100%;}body {-webkit-font-smoothing: antialiased;-webkit-text-size-adjust: none;width: 100% !important;height: 100%;line-height: 1.6em;}table td {vertical-align: top;}body {background-color: #f6f6f6;}.body-wrap {background-color: #f6f6f6;width: 100%;}.container {display: block !important;max-width: 600px !important;margin: 0 auto !important;clear: both !important;}.content {max-width: 600px;margin: 0 auto;display: block;padding: 20px;}.main {background-color: #fff;border-bottom: 2px solid #EAEAEA;border-radius: 3px;}.content-wrap {padding: 15px 20px;}.content-block {padding: 0 0 20px;}.header {width: 100%;margin-bottom: 20px;}.pre-footer {width: 100%;clear: both;color: #333;padding: 20px 0px;}.footer {width: 100%;clear: both;color: #999;padding: 15px;}.footer p, .footer a, .footer td {color: #999;font-size: 11px;}.resume-box {background: #FFF0E5;}h1, h2, h3 {color: #000;margin: 20px 0 0;line-height: 1.2em;font-weight: 400;}h1 {font-size: 20px;font-weight: 500;}h2 {font-size: 24px;}h3 {font-size: 18px;}h4 {font-size: 14px;font-weight: 600;}p, ul, ol {margin-bottom: 10px;font-weight: normal;}p li, ul li, ol li {margin-left: 5px;list-style-position: inside;line-height: 1.3em;}a {color: #348eda;text-decoration: underline;}.btn-primary {background:#00A7E1; color:#fff !important; padding:10px 20px; text-decoration: none; border-radius:8px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight:bold;line-height: 23px;}.aligncenter {text-align: center;}.alignright {text-align: right;}.alignleft {text-align: left;}.clear {clear: both;}@media only screen and (max-width: 480px) {body {  padding: 0 !important;}h1, h2, h3, h4 { margin: 20px 0 5px !important;}h1 {  font-size: 22px !important;}h2 {  font-size: 18px !important;}h3 {  font-size: 16px !important;}.container {  padding: 0 !important;  width: 100% !important;}.content {  padding: 0 !important;}.content-wrap {  padding: 15px !important;}.mcnImage {max-width:100% !important;width:100% !important;} .img-app{margin-bottom: 10px;} table#banner td.w50{width: 50%;}a.button{width: 70px; margin-bottom: 10px;}span.sub-text{font-size: 16px;}}.sub-text{font-size: 18px;}a.button {
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20202, 'Agilice','iconstruye@iconstruye.com', '¡Gracias por actualizar tu información! Ya puedes acceder con tu correo a AGILICE', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;AGILICE&lt;/title&gt;&lt;style type=text/css&gt;* {margin: 0;font-family: "Helvetica Neue", Helvetica, Arial, sans-serif;box-sizing: border-box;font-size: 14px;}img {max-width: 100%;}body {-webkit-font-smoothing: antialiased;-webkit-text-size-adjust: none;width: 100% !important;height: 100%;line-height: 1.6em;}table td {vertical-align: top;}body {background-color: #f6f6f6;}.body-wrap {background-color: #f6f6f6;width: 100%;}.container {display: block !important;max-width: 600px !important;margin: 0 auto !important;clear: both !important;}.content {max-width: 600px;margin: 0 auto;display: block;padding: 20px;}.main {background-color: #fff;border-bottom: 2px solid #EAEAEA;border-radius: 3px;}.content-wrap {padding: 15px 20px;}.content-block {padding: 0 0 20px;}.header {width: 100%;margin-bottom: 20px;}.pre-footer {width: 100%;clear: both;color: #333;padding: 20px 0px;}.footer {width: 100%;clear: both;color: #999;padding: 15px;}.footer p, .footer a, .footer td {color: #999;font-size: 11px;}.resume-box {background: #FFF0E5;}h1, h2, h3 {color: #000;margin: 20px 0 0;line-height: 1.2em;font-weight: 400;}h1 {font-size: 20px;font-weight: 500;}h2 {font-size: 24px;}h3 {font-size: 18px;}h4 {font-size: 14px;font-weight: 600;}p, ul, ol {margin-bottom: 10px;font-weight: normal;}p li, ul li, ol li {margin-left: 5px;list-style-position: inside;line-height: 1.3em;}a {color: #348eda;text-decoration: underline;}.btn-primary {background:#00A7E1; color:#fff !important; padding:10px 20px; text-decoration: none; border-radius:8px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight:bold;line-height: 23px;}.aligncenter {text-align: center;}.alignright {text-align: right;}.alignleft {text-align: left;}.clear {clear: both;}@media only screen and (max-width: 480px) {body {  padding: 0 !important;}h1, h2, h3, h4 { margin: 20px 0 5px !important;}h1 {  font-size: 22px !important;}h2 {  font-size: 18px !important;}h3 {  font-size: 16px !important;}.container {  padding: 0 !important;  width: 100% !important;}.content {  padding: 0 !important;}.content-wrap {  padding: 15px !important;}.mcnImage {max-width:100% !important;width:100% !important;} .img-app{margin-bottom: 10px;} table#banner td.w50{width: 50%;}a.button{width: 70px; margin-bottom: 10px;}span.sub-text{font-size: 16px;}}.sub-text{font-size: 18px;}a.button {
     text-decoration: none;
 }.img-app{border: 1px solid #00A7E1;
     border-radius:8px;
@@ -7266,11 +7277,11 @@
   	width:140px;
   	height: auto;
   	margin-right: 10px;
-  	cursor: pointer;}&lt;/style&gt;&lt;/head&gt; &lt;body itemscope itemtype=http://schema.org/EmailMessage&gt; &lt;table class=body-wrap&gt; &lt;tr&gt; &lt;td&gt;&lt;/td&gt; &lt;td class=container width=600&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td valign=top&gt; &lt;img align=center alt src=https://i.ibb.co/TcBfKbx/header-placeholder.png width=600 style="max-width: 600px;padding-bottom: 0;display: inline !important;vertical-align: bottom;border: 0;height: auto;outline: none;text-decoration: none;-ms-interpolation-mode: bicubic;" class=mcnImage&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td class=content-block colspan=2&gt; &lt;h4&gt;&lt;b&gt;¡Datos actualizados correctamente!&lt;/b&gt;&lt;/h4&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td class=content-block&gt; &lt;hr style="border-top: 1px solid #00A7E1;border-bottom: none;"&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td colspan=2&gt; &lt;p style=color:#000&gt;Hola &lt;b&gt;&lt;nombre_usuario&gt;&lt;/b&gt;,&lt;br&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;h5&gt;¡Gracias por actualizar tus datos!&lt;/h5&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;p&gt;Ya puedes acceder a AGILICE con tu cuenta de correo electrónico &lt;correo_usuario&gt; y contraseña&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;Si olvidaste tu contraseña puedes recuperarla &lt;a href=http://apps.agilice.com/loginsso.aspx&gt;aqui&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr class=aligncenter&gt; &lt;td&gt; &lt;a href=https://apps.agilice.com class=btn-primary&gt;Ingresa a AGILICE&lt;/a&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;p&gt;Si tienes alguna duda comunícate con nosotros por correo electrónico a mesadeayuda@agilice.com&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellspacing=0 cellpadding=0&gt; &lt;tr&gt; &lt;td class=content-block&gt;&lt;p style=color:#000&gt;Saluda atentamente&lt;br&gt;&lt;b style=color:#000&gt;Equipo AGILICE &lt;br&gt;&lt;span style="color: #00A7E1;"&gt;AGILICE®&lt;/span&gt;&lt;/b&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=footer&gt; &lt;table width=100%&gt; &lt;tr&gt; &lt;td class="aligncenter content-block"&gt; &lt;em style="font-size: 12px !important;"&gt;Correo enviado a través de &lt;a href=https://apps.agilice.com style="color: #00A7E1;"&gt;AGILICE&lt;/a&gt;®&amp;nbsp;· Copyright ©&amp;nbsp; Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;td&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/body&gt; &lt;/html&gt;','Se envia cuando se actualizan los datos en el formulario');</v>
+  	cursor: pointer;}&lt;/style&gt;&lt;/head&gt; &lt;body itemscope itemtype=http://schema.org/EmailMessage&gt; &lt;table class=body-wrap&gt; &lt;tr&gt; &lt;td&gt;&lt;/td&gt; &lt;td class=container width=600&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td valign=top&gt; &lt;img align=center alt src=https://i.ibb.co/TcBfKbx/header-placeholder.png width=600 style="max-width: 600px;padding-bottom: 0;display: inline !important;vertical-align: bottom;border: 0;height: auto;outline: none;text-decoration: none;-ms-interpolation-mode: bicubic;" class=mcnImage&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td class=content-block colspan=2&gt; &lt;h4&gt;&lt;b&gt;¡Datos actualizados correctamente!&lt;/b&gt;&lt;/h4&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td class=content-block&gt; &lt;hr style="border-top: 1px solid #00A7E1;border-bottom: none;"&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td colspan=2&gt; &lt;p style=color:#000&gt;Hola &lt;b&gt;&lt;nombre_usuario&gt;&lt;/b&gt;,&lt;br&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;h5&gt;¡Gracias por actualizar tus datos!&lt;/h5&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;p&gt;Ya puedes acceder a AGILICE con tu cuenta de correo electrónico &lt;correo_usuario&gt; y contraseña&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;Si olvidaste tu contraseña puedes recuperarla &lt;a href=http://apps.agilice.com/loginsso.aspx&gt;aqui&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr class=aligncenter&gt; &lt;td&gt; &lt;a href=https://apps.agilice.com class=btn-primary&gt;Ingresa a AGILICE&lt;/a&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;p&gt;Si tienes alguna duda comunícate con nosotros por correo electrónico a mesadeayuda@agilice.com&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellspacing=0 cellpadding=0&gt; &lt;tr&gt; &lt;td class=content-block&gt;&lt;p style=color:#000&gt;Saluda atentamente&lt;br&gt;&lt;b style=color:#000&gt;Equipo AGILICE &lt;br&gt;&lt;span style="color: #00A7E1;"&gt;AGILICE®&lt;/span&gt;&lt;/b&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=footer&gt; &lt;table width=100%&gt; &lt;tr&gt; &lt;td class="aligncenter content-block"&gt; &lt;em style="font-size: 12px !important;"&gt;Correo enviado a través de &lt;a href=https://apps.agilice.com style="color: #00A7E1;"&gt;AGILICE&lt;/a&gt;®&amp;nbsp;· Copyright ©&amp;nbsp; Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;td&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/body&gt; &lt;/html&gt;','Se envia cuando se actualizan los datos en el formulario',202,2);</v>
       </c>
       <c r="T2" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20202, 'Redmat','iconstruye@iconstruye.com', '¡Gracias por actualizar tu información! Ya puedes acceder con tu correo a REDMAT', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;REDMAT&lt;/title&gt;&lt;style type=text/css&gt;* {margin: 0;font-family: "Helvetica Neue", Helvetica, Arial, sans-serif;box-sizing: border-box;font-size: 14px;}img {max-width: 100%;}body {-webkit-font-smoothing: antialiased;-webkit-text-size-adjust: none;width: 100% !important;height: 100%;line-height: 1.6em;}table td {vertical-align: top;}body {background-color: #f6f6f6;}.body-wrap {background-color: #f6f6f6;width: 100%;}.container {display: block !important;max-width: 600px !important;margin: 0 auto !important;clear: both !important;}.content {max-width: 600px;margin: 0 auto;display: block;padding: 20px;}.main {background-color: #fff;border-bottom: 2px solid #EAEAEA;border-radius: 3px;}.content-wrap {padding: 15px 20px;}.content-block {padding: 0 0 20px;}.header {width: 100%;margin-bottom: 20px;}.pre-footer {width: 100%;clear: both;color: #333;padding: 20px 0px;}.footer {width: 100%;clear: both;color: #999;padding: 15px;}.footer p, .footer a, .footer td {color: #999;font-size: 11px;}.resume-box {background: #FFF0E5;}h1, h2, h3 {color: #000;margin: 20px 0 0;line-height: 1.2em;font-weight: 400;}h1 {font-size: 20px;font-weight: 500;}h2 {font-size: 24px;}h3 {font-size: 18px;}h4 {font-size: 14px;font-weight: 600;}p, ul, ol {margin-bottom: 10px;font-weight: normal;}p li, ul li, ol li {margin-left: 5px;list-style-position: inside;line-height: 1.3em;}a {color: #F78E28;text-decoration: underline;}.btn-primary {background:#083F75; color:#fff !important; padding:10px 20px; text-decoration: none; border-radius:8px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight:bold;line-height: 23px;}.aligncenter {text-align: center;}.alignright {text-align: right;}.alignleft {text-align: left;}.clear {clear: both;}@media only screen and (max-width: 480px) {body {  padding: 0 !important;}h1, h2, h3, h4 { margin: 20px 0 5px !important;}h1 {  font-size: 22px !important;}h2 {  font-size: 18px !important;}h3 {  font-size: 16px !important;}.container {  padding: 0 !important;  width: 100% !important;}.content {  padding: 0 !important;}.content-wrap {  padding: 15px !important;}.mcnImage {max-width:100% !important;width:100% !important;} .img-app{margin-bottom: 10px;} table#banner td.w50{width: 50%;}a.button{width: 70px; margin-bottom: 10px;}span.sub-text{font-size: 16px;}}.sub-text{font-size: 18px;}a.button {
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30202, 'Redmat','iconstruye@iconstruye.com', '¡Gracias por actualizar tu información! Ya puedes acceder con tu correo a REDMAT', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;REDMAT&lt;/title&gt;&lt;style type=text/css&gt;* {margin: 0;font-family: "Helvetica Neue", Helvetica, Arial, sans-serif;box-sizing: border-box;font-size: 14px;}img {max-width: 100%;}body {-webkit-font-smoothing: antialiased;-webkit-text-size-adjust: none;width: 100% !important;height: 100%;line-height: 1.6em;}table td {vertical-align: top;}body {background-color: #f6f6f6;}.body-wrap {background-color: #f6f6f6;width: 100%;}.container {display: block !important;max-width: 600px !important;margin: 0 auto !important;clear: both !important;}.content {max-width: 600px;margin: 0 auto;display: block;padding: 20px;}.main {background-color: #fff;border-bottom: 2px solid #EAEAEA;border-radius: 3px;}.content-wrap {padding: 15px 20px;}.content-block {padding: 0 0 20px;}.header {width: 100%;margin-bottom: 20px;}.pre-footer {width: 100%;clear: both;color: #333;padding: 20px 0px;}.footer {width: 100%;clear: both;color: #999;padding: 15px;}.footer p, .footer a, .footer td {color: #999;font-size: 11px;}.resume-box {background: #FFF0E5;}h1, h2, h3 {color: #000;margin: 20px 0 0;line-height: 1.2em;font-weight: 400;}h1 {font-size: 20px;font-weight: 500;}h2 {font-size: 24px;}h3 {font-size: 18px;}h4 {font-size: 14px;font-weight: 600;}p, ul, ol {margin-bottom: 10px;font-weight: normal;}p li, ul li, ol li {margin-left: 5px;list-style-position: inside;line-height: 1.3em;}a {color: #F78E28;text-decoration: underline;}.btn-primary {background:#083F75; color:#fff !important; padding:10px 20px; text-decoration: none; border-radius:8px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight:bold;line-height: 23px;}.aligncenter {text-align: center;}.alignright {text-align: right;}.alignleft {text-align: left;}.clear {clear: both;}@media only screen and (max-width: 480px) {body {  padding: 0 !important;}h1, h2, h3, h4 { margin: 20px 0 5px !important;}h1 {  font-size: 22px !important;}h2 {  font-size: 18px !important;}h3 {  font-size: 16px !important;}.container {  padding: 0 !important;  width: 100% !important;}.content {  padding: 0 !important;}.content-wrap {  padding: 15px !important;}.mcnImage {max-width:100% !important;width:100% !important;} .img-app{margin-bottom: 10px;} table#banner td.w50{width: 50%;}a.button{width: 70px; margin-bottom: 10px;}span.sub-text{font-size: 16px;}}.sub-text{font-size: 18px;}a.button {
     text-decoration: none;
 }.img-app{border: 1px solid #083F75;
     border-radius:8px;
@@ -7278,10 +7289,10 @@
   	width:140px;
   	height: auto;
   	margin-right: 10px;
-  	cursor: pointer;}&lt;/style&gt;&lt;/head&gt; &lt;body itemscope itemtype=http://schema.org/EmailMessage&gt; &lt;table class=body-wrap&gt; &lt;tr&gt; &lt;td&gt;&lt;/td&gt; &lt;td class=container width=600&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td valign=top&gt; &lt;img align=center alt src=https://i.ibb.co/TcBfKbx/header-placeholder.png width=600 style="max-width: 600px;padding-bottom: 0;display: inline !important;vertical-align: bottom;border: 0;height: auto;outline: none;text-decoration: none;-ms-interpolation-mode: bicubic;" class=mcnImage&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td class=content-block colspan=2&gt; &lt;h4&gt;&lt;b&gt;¡Datos actualizados correctamente!&lt;/b&gt;&lt;/h4&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td class=content-block&gt; &lt;hr style="border-top: 1px solid #083F75;border-bottom: none;"&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td colspan=2&gt; &lt;p style=color:#000&gt;Hola &lt;b&gt;&lt;nombre_usuario&gt;&lt;/b&gt;,&lt;br&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;h5&gt;¡Gracias por actualizar tus datos!&lt;/h5&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;p&gt;Ya puedes acceder a REDMAT con tu cuenta de correo electrónico &lt;correo_usuario&gt; y contraseña&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;Si olvidaste tu contraseña puedes recuperarla &lt;a href=https://redmat.iconstruye.com/loginsso.aspx&gt;aqui&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr class=aligncenter&gt; &lt;td&gt; &lt;a href=https://redmat.iconstruye.com class=btn-primary&gt;Ingresa a REDMAT&lt;/a&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;p&gt;Si tienes alguna duda comunícate con nosotros por correo electrónico a mesadeayuda@iconstruye.com&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellspacing=0 cellpadding=0&gt; &lt;tr&gt; &lt;td class=content-block&gt;&lt;p style=color:#000&gt;Saluda atentamente&lt;br&gt;&lt;b style=color:#000&gt;Equipo REDMAT &lt;br&gt;&lt;span style="color: #083F75;"&gt;REDMAT®&lt;/span&gt;&lt;/b&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=footer&gt; &lt;table width=100%&gt; &lt;tr&gt; &lt;td class="aligncenter content-block"&gt; &lt;em style="font-size: 12px !important;"&gt;Correo enviado a través de &lt;a href=https://redmat.iconstruye.com style="color: #083F75;"&gt;REDMAT&lt;/a&gt;®&amp;nbsp;· Copyright ©&amp;nbsp; Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;td&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/body&gt; &lt;/html&gt;','Se envia cuando se actualizan los datos en el formulario');</v>
+  	cursor: pointer;}&lt;/style&gt;&lt;/head&gt; &lt;body itemscope itemtype=http://schema.org/EmailMessage&gt; &lt;table class=body-wrap&gt; &lt;tr&gt; &lt;td&gt;&lt;/td&gt; &lt;td class=container width=600&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td valign=top&gt; &lt;img align=center alt src=https://i.ibb.co/TcBfKbx/header-placeholder.png width=600 style="max-width: 600px;padding-bottom: 0;display: inline !important;vertical-align: bottom;border: 0;height: auto;outline: none;text-decoration: none;-ms-interpolation-mode: bicubic;" class=mcnImage&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td class=content-block colspan=2&gt; &lt;h4&gt;&lt;b&gt;¡Datos actualizados correctamente!&lt;/b&gt;&lt;/h4&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td class=content-block&gt; &lt;hr style="border-top: 1px solid #083F75;border-bottom: none;"&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td colspan=2&gt; &lt;p style=color:#000&gt;Hola &lt;b&gt;&lt;nombre_usuario&gt;&lt;/b&gt;,&lt;br&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;h5&gt;¡Gracias por actualizar tus datos!&lt;/h5&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;p&gt;Ya puedes acceder a REDMAT con tu cuenta de correo electrónico &lt;correo_usuario&gt; y contraseña&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;Si olvidaste tu contraseña puedes recuperarla &lt;a href=https://redmat.iconstruye.com/loginsso.aspx&gt;aqui&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr class=aligncenter&gt; &lt;td&gt; &lt;a href=https://redmat.iconstruye.com class=btn-primary&gt;Ingresa a REDMAT&lt;/a&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;p&gt;Si tienes alguna duda comunícate con nosotros por correo electrónico a mesadeayuda@iconstruye.com&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellspacing=0 cellpadding=0&gt; &lt;tr&gt; &lt;td class=content-block&gt;&lt;p style=color:#000&gt;Saluda atentamente&lt;br&gt;&lt;b style=color:#000&gt;Equipo REDMAT &lt;br&gt;&lt;span style="color: #083F75;"&gt;REDMAT®&lt;/span&gt;&lt;/b&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=footer&gt; &lt;table width=100%&gt; &lt;tr&gt; &lt;td class="aligncenter content-block"&gt; &lt;em style="font-size: 12px !important;"&gt;Correo enviado a través de &lt;a href=https://redmat.iconstruye.com style="color: #083F75;"&gt;REDMAT&lt;/a&gt;®&amp;nbsp;· Copyright ©&amp;nbsp; Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;td&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/body&gt; &lt;/html&gt;','Se envia cuando se actualizan los datos en el formulario',202,3);</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>200</v>
       </c>
@@ -7335,19 +7346,19 @@
         <v>36</v>
       </c>
       <c r="S3" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20200, 'Agilice','presupuesto_ic@iconstruye.com', '&lt;TipoDocumento&gt; N° &lt;NumeroDocumento&gt; pendiente de aprobación por Presupuesto Anualizado', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt; &lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;style type=text/css&gt;
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20200, 'Agilice','presupuesto_ic@iconstruye.com', '&lt;TipoDocumento&gt; N° &lt;NumeroDocumento&gt; pendiente de aprobación por Presupuesto Anualizado', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt; &lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;style type=text/css&gt;
 body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}
-&lt;/style&gt;&lt;/head&gt; &lt;body style="margin:0; padding:0; background-color:#fff;"&gt; &lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt; &lt;center&gt; &lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#ffffff&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFF&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt; &lt;tr&gt; &lt;td height=20 style="font-size:10px; line-height:20px;"&gt;&amp;nbsp;&lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td class=mobile align=center valign=middle style="padding:10px; text-align:center;"&gt; &lt;img class=logo src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt; &lt;tr&gt; &lt;td align=center valign=top style="padding: 0;"&gt; &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt; &lt;tr&gt; &lt;td align=left valign=middle height=90&gt; &lt;h3 style="font-size: 2em; font-weight: 300; color: #333333; -webkit-margin-before: 1em; -webkit-margin-after: 0.5em; text-align:center;"&gt;Documento pendiente de aprobación por Presupuesto Anualizado&lt;/h3&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt; &lt;tr&gt; &lt;td align=center valign=top style="padding: 0;"&gt; &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt; &lt;tr&gt; &lt;td class=mobile align=left valign=top&gt; &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: left;"&gt;&lt;strong&gt;&lt;nombreusuarioaprobador&gt;&lt;/strong&gt;, te informamos que el documento N° &lt;strong&gt;&lt;numerodocumento&gt;&lt;/strong&gt; se encuentra creado con fecha &lt;strong&gt;&lt;fechamovimiento&gt;&lt;/strong&gt; y está en espera de tu aprobación en el Centro de Gestión &lt;strong&gt;&lt;centrogestion&gt;&lt;/strong&gt;.&lt;/p&gt; &lt;ul style=margin:0;padding:0;list-style-type:none;line-height:30px; class=data-list&gt; &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Tipo de Documento:&lt;/span&gt; &lt;strong&gt;&lt;tipodocumento&gt;&lt;/strong&gt;&lt;/li&gt; &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Nombre de Documento:&lt;/span&gt; &lt;strong&gt;&lt;nombredocumento&gt;&lt;/strong&gt;&lt;/li&gt; &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Solicitante:&lt;/span&gt; &lt;strong&gt;&lt;nombreusuariosolicitante&gt;&lt;/strong&gt;&lt;/li&gt; &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Monto:&lt;/span&gt; &lt;strong&gt;&lt;monto&gt;&lt;/strong&gt;&lt;/li&gt; &lt;/ul&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt; &lt;tr&gt; &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td align=center valign=top style="padding: 10px 0;"&gt; &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt; &lt;tr&gt; &lt;td class=mobile align=left valign=top&gt; &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: left; margin-bottom: 30px;"&gt;Consulta el estado de todos tus documentos en la sección "Presupuesto / Presupuesto Anualizado / Aprobar Documentos".&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td class=mobile align=center valign=top&gt; &lt;a href=https://apps.agilice.com style="background:#00A7E1; color:#fff; padding:10px 20px; text-decoration: none; border-radius:2px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight: 400;line-height: 23px;"&gt;Ir a Agilice.com&lt;/a&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td height=20 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt; &lt;tr&gt; &lt;td class="mobile footer" align=center valign=middle style="padding:5px 10px;"&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt; &lt;tr&gt; &lt;td class="mobile footer" align=center valign=top&gt; &lt;p style="line-height: 1.5em; font-size: 11px; text-align: center; color: #999999;"&gt;Correo enviado a trav&amp;eacute;s de Agilice | Todos los Derechos Reservados&lt;br&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/center&gt; &lt;/body&gt; &lt;/html&gt; ','Se envía correo al generar documento con flujo de aprobación por presupuesto anualizado');</v>
+&lt;/style&gt;&lt;/head&gt; &lt;body style="margin:0; padding:0; background-color:#fff;"&gt; &lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt; &lt;center&gt; &lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#ffffff&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFF&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt; &lt;tr&gt; &lt;td height=20 style="font-size:10px; line-height:20px;"&gt;&amp;nbsp;&lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td class=mobile align=center valign=middle style="padding:10px; text-align:center;"&gt; &lt;img class=logo src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt; &lt;tr&gt; &lt;td align=center valign=top style="padding: 0;"&gt; &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt; &lt;tr&gt; &lt;td align=left valign=middle height=90&gt; &lt;h3 style="font-size: 2em; font-weight: 300; color: #333333; -webkit-margin-before: 1em; -webkit-margin-after: 0.5em; text-align:center;"&gt;Documento pendiente de aprobación por Presupuesto Anualizado&lt;/h3&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt; &lt;tr&gt; &lt;td align=center valign=top style="padding: 0;"&gt; &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt; &lt;tr&gt; &lt;td class=mobile align=left valign=top&gt; &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: left;"&gt;&lt;strong&gt;&lt;nombreusuarioaprobador&gt;&lt;/strong&gt;, te informamos que el documento N° &lt;strong&gt;&lt;numerodocumento&gt;&lt;/strong&gt; se encuentra creado con fecha &lt;strong&gt;&lt;fechamovimiento&gt;&lt;/strong&gt; y está en espera de tu aprobación en el Centro de Gestión &lt;strong&gt;&lt;centrogestion&gt;&lt;/strong&gt;.&lt;/p&gt; &lt;ul style=margin:0;padding:0;list-style-type:none;line-height:30px; class=data-list&gt; &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Tipo de Documento:&lt;/span&gt; &lt;strong&gt;&lt;tipodocumento&gt;&lt;/strong&gt;&lt;/li&gt; &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Nombre de Documento:&lt;/span&gt; &lt;strong&gt;&lt;nombredocumento&gt;&lt;/strong&gt;&lt;/li&gt; &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Solicitante:&lt;/span&gt; &lt;strong&gt;&lt;nombreusuariosolicitante&gt;&lt;/strong&gt;&lt;/li&gt; &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Monto:&lt;/span&gt; &lt;strong&gt;&lt;monto&gt;&lt;/strong&gt;&lt;/li&gt; &lt;/ul&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt; &lt;tr&gt; &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td align=center valign=top style="padding: 10px 0;"&gt; &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt; &lt;tr&gt; &lt;td class=mobile align=left valign=top&gt; &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: left; margin-bottom: 30px;"&gt;Consulta el estado de todos tus documentos en la sección "Presupuesto / Presupuesto Anualizado / Aprobar Documentos".&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td class=mobile align=center valign=top&gt; &lt;a href=https://apps.agilice.com style="background:#00A7E1; color:#fff; padding:10px 20px; text-decoration: none; border-radius:2px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight: 400;line-height: 23px;"&gt;Ir a Agilice.com&lt;/a&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td height=20 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt; &lt;tr&gt; &lt;td class="mobile footer" align=center valign=middle style="padding:5px 10px;"&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt; &lt;tr&gt; &lt;td class="mobile footer" align=center valign=top&gt; &lt;p style="line-height: 1.5em; font-size: 11px; text-align: center; color: #999999;"&gt;Correo enviado a trav&amp;eacute;s de Agilice | Todos los Derechos Reservados&lt;br&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/center&gt; &lt;/body&gt; &lt;/html&gt; ','Se envía correo al generar documento con flujo de aprobación por presupuesto anualizado',200,2);</v>
       </c>
       <c r="T3" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20200, 'Redmat','presupuesto_ic@iconstruye.com', '&lt;TipoDocumento&gt; N° &lt;NumeroDocumento&gt; pendiente de aprobación por Presupuesto Anualizado', '_x000D_ &lt;!DOCTYPE html&gt;_x000D_ &lt;html lang=en&gt;_x000D_ &lt;head&gt;_x000D_ &lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;_x000D_ &lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;_x000D_ &lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;_x000D_ &lt;style type=text/css&gt;_x000D_
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30200, 'Redmat','presupuesto_ic@iconstruye.com', '&lt;TipoDocumento&gt; N° &lt;NumeroDocumento&gt; pendiente de aprobación por Presupuesto Anualizado', '_x000D_ &lt;!DOCTYPE html&gt;_x000D_ &lt;html lang=en&gt;_x000D_ &lt;head&gt;_x000D_ &lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;_x000D_ &lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;_x000D_ &lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;_x000D_ &lt;style type=text/css&gt;_x000D_
 body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}_x000D_
-&lt;/style&gt;_x000D_ &lt;/head&gt;_x000D_ &lt;body style="margin:0; padding:0; background-color:#fff;"&gt;_x000D_ &lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;_x000D_ &lt;center&gt;_x000D_ &lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#ffffff&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=20 style="font-size:10px; line-height:20px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=middle style="padding:10px; text-align:center;"&gt;_x000D_ &lt;img class=logo src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=left valign=middle height=90&gt;_x000D_ &lt;h3 style="font-size: 2em; font-weight: 300; color: #333333; -webkit-margin-before: 1em; -webkit-margin-after: 0.5em; text-align:center;"&gt;Documento pendiente de aprobación por Presupuesto Anualizado&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: left;"&gt;&lt;strong&gt;&lt;nombreusuarioaprobador&gt;&lt;/strong&gt;, te informamos que el documento N° &lt;strong&gt;&lt;numerodocumento&gt;&lt;/strong&gt; se encuentra creado con fecha &lt;strong&gt;&lt;fechamovimiento&gt;&lt;/strong&gt; y está en espera de tu aprobación en el Centro de Gestión &lt;strong&gt;&lt;centrogestion&gt;&lt;/strong&gt;.&lt;/p&gt;_x000D_ &lt;ul style=margin:0;padding:0;list-style-type:none;line-height:30px; class=data-list&gt;_x000D_ &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Tipo de Documento:&lt;/span&gt; &lt;strong&gt;&lt;tipodocumento&gt;&lt;/strong&gt;&lt;/li&gt;_x000D_ &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Nombre de Documento:&lt;/span&gt; &lt;strong&gt;&lt;nombredocumento&gt;&lt;/strong&gt;&lt;/li&gt;_x000D_ &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Solicitante:&lt;/span&gt; &lt;strong&gt;&lt;nombreusuariosolicitante&gt;&lt;/strong&gt;&lt;/li&gt;_x000D_ &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Monto:&lt;/span&gt; &lt;strong&gt;&lt;monto&gt;&lt;/strong&gt;&lt;/li&gt;_x000D_ &lt;/ul&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 10px 0;"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: left; margin-bottom: 30px;"&gt;Consulta el estado de todos tus documentos en la sección "Presupuesto / Presupuesto Anualizado / Aprobar Documentos".&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=top&gt;_x000D_ &lt;a href=https://redmat.iconstruye.com style="background:#F78E28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:2px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight: 400;line-height: 23px;"&gt;Ir a Redmat.com&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=20 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=middle style="padding:5px 10px;"&gt;_x000D_ &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=top&gt;_x000D_ &lt;p style="line-height: 1.5em; font-size: 11px; text-align: center; color: #999999;"&gt;Correo enviado a trav&amp;eacute;s de Redmat | Todos los Derechos Reservados&lt;br&gt;&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt; _x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/center&gt;_x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;_x000D_ ','Se envía correo al generar documento con flujo de aprobación por presupuesto anualizado');</v>
+&lt;/style&gt;_x000D_ &lt;/head&gt;_x000D_ &lt;body style="margin:0; padding:0; background-color:#fff;"&gt;_x000D_ &lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;_x000D_ &lt;center&gt;_x000D_ &lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#ffffff&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=20 style="font-size:10px; line-height:20px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=middle style="padding:10px; text-align:center;"&gt;_x000D_ &lt;img class=logo src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=left valign=middle height=90&gt;_x000D_ &lt;h3 style="font-size: 2em; font-weight: 300; color: #333333; -webkit-margin-before: 1em; -webkit-margin-after: 0.5em; text-align:center;"&gt;Documento pendiente de aprobación por Presupuesto Anualizado&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: left;"&gt;&lt;strong&gt;&lt;nombreusuarioaprobador&gt;&lt;/strong&gt;, te informamos que el documento N° &lt;strong&gt;&lt;numerodocumento&gt;&lt;/strong&gt; se encuentra creado con fecha &lt;strong&gt;&lt;fechamovimiento&gt;&lt;/strong&gt; y está en espera de tu aprobación en el Centro de Gestión &lt;strong&gt;&lt;centrogestion&gt;&lt;/strong&gt;.&lt;/p&gt;_x000D_ &lt;ul style=margin:0;padding:0;list-style-type:none;line-height:30px; class=data-list&gt;_x000D_ &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Tipo de Documento:&lt;/span&gt; &lt;strong&gt;&lt;tipodocumento&gt;&lt;/strong&gt;&lt;/li&gt;_x000D_ &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Nombre de Documento:&lt;/span&gt; &lt;strong&gt;&lt;nombredocumento&gt;&lt;/strong&gt;&lt;/li&gt;_x000D_ &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Solicitante:&lt;/span&gt; &lt;strong&gt;&lt;nombreusuariosolicitante&gt;&lt;/strong&gt;&lt;/li&gt;_x000D_ &lt;li style="border-bottom:1px solid #eee;"&gt;&lt;span style=width:30%;display:inline-block;&gt;Monto:&lt;/span&gt; &lt;strong&gt;&lt;monto&gt;&lt;/strong&gt;&lt;/li&gt;_x000D_ &lt;/ul&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 10px 0;"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: left; margin-bottom: 30px;"&gt;Consulta el estado de todos tus documentos en la sección "Presupuesto / Presupuesto Anualizado / Aprobar Documentos".&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=top&gt;_x000D_ &lt;a href=https://redmat.iconstruye.com style="background:#F78E28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:2px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight: 400;line-height: 23px;"&gt;Ir a Redmat.com&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=20 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=middle style="padding:5px 10px;"&gt;_x000D_ &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=top&gt;_x000D_ &lt;p style="line-height: 1.5em; font-size: 11px; text-align: center; color: #999999;"&gt;Correo enviado a trav&amp;eacute;s de Redmat | Todos los Derechos Reservados&lt;br&gt;&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt; _x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/center&gt;_x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;_x000D_ ','Se envía correo al generar documento con flujo de aprobación por presupuesto anualizado',200,3);</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>201</v>
       </c>
@@ -7401,19 +7412,19 @@
         <v>43</v>
       </c>
       <c r="S4" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20201, 'Agilice','presupuesto_ic@iconstruye.com', 'Cuenta de costo excedida en Presupuesto Anualizado al &lt;FechaEjecucion&gt;', '_x000D_ &lt;!DOCTYPE html&gt;_x000D_ &lt;html lang=en&gt;_x000D_ &lt;head&gt;_x000D_ &lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;_x000D_ &lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;_x000D_ &lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;_x000D_ &lt;style type=text/css&gt;_x000D_
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20201, 'Agilice','presupuesto_ic@iconstruye.com', 'Cuenta de costo excedida en Presupuesto Anualizado al &lt;FechaEjecucion&gt;', '_x000D_ &lt;!DOCTYPE html&gt;_x000D_ &lt;html lang=en&gt;_x000D_ &lt;head&gt;_x000D_ &lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;_x000D_ &lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;_x000D_ &lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;_x000D_ &lt;style type=text/css&gt;_x000D_
 body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}_x000D_
-&lt;/style&gt; _x000D_ &lt;/head&gt;_x000D_ &lt;body style="margin:0; padding:0; background-color:#fff;"&gt;_x000D_ &lt;span style="display: block; width: 840px !important; max-width: 840px; height: 1px" class=mobileOff&gt;&lt;/span&gt;_x000D_ &lt;center&gt;_x000D_ &lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#ffffff&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=middle style="padding:10px; text-align:center;"&gt;_x000D_ &lt;img class=logo src=https://apps.agilice.com/img/logo-agilice.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=left valign=middle height=90&gt;_x000D_ &lt;h3 style="font-size: 2em; font-weight: 300; color: #333333; -webkit-margin-before: 1em; -webkit-margin-after: 0.5em; text-align:center;"&gt;Cuenta de costo &lt;strong&gt;excedida en presupuesto&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: justify;"&gt;Estimado(a) Usuario, te informamos que las siguientes Cuentas de Costos han excedido el monto presupuestado en el Centro de Gestión &lt;strong&gt;&lt;centrogestion&gt;&lt;/strong&gt;:&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#fff style="border-top: 1px solid #fff;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="border-bottom: 1px solid #fff;"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=adaptative bgcolor=#fff&gt;_x000D_ &lt;thead&gt;_x000D_ &lt;tr bgcolor=#fff&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px; vertical-align: middle;" width=22%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Cuenta de Costo&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto presupuestado del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto comprometido del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Diferencia del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto presupuestado acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto comprometido acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Diferencia acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/thead&gt;_x000D_ &lt;tbody&gt;_x000D_ &lt;idtrcuentas&gt;_x000D_ &lt;/tbody&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px; background-color: #fff;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 10px 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: justify; margin-bottom: 30px;"&gt;Consulta el detalle del Presupuesto en el reporte "Presupuesto / Presupuesto Anualizado / Bandeja de Presupuesto".&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=top&gt;_x000D_ &lt;a href=https://apps.agilice.com style="background:#00A7E1; color:#fff; padding:10px 20px; text-decoration: none; border-radius:2px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight: 400;line-height: 23px;"&gt;Ir a Agilice.com&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=20 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=middle style="padding:5px 10px;"&gt;_x000D_ &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=top&gt;_x000D_ &lt;p style="line-height: 1.5em; font-size: 11px; text-align: center; color: #999999;"&gt;Correo enviado a trav&amp;eacute;s de Agilice | Todos los Derechos Reservados&lt;br&gt;&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt; _x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/center&gt;_x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;_x000D_ ','Se envía correo al detectar cuentas de costo con Presupuesto Anualizado excedido, de acuerdo a configuración de tabla PA_FrecuenciaNotificacion');</v>
+&lt;/style&gt; _x000D_ &lt;/head&gt;_x000D_ &lt;body style="margin:0; padding:0; background-color:#fff;"&gt;_x000D_ &lt;span style="display: block; width: 840px !important; max-width: 840px; height: 1px" class=mobileOff&gt;&lt;/span&gt;_x000D_ &lt;center&gt;_x000D_ &lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#ffffff&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=middle style="padding:10px; text-align:center;"&gt;_x000D_ &lt;img class=logo src=https://apps.agilice.com/img/logo-agilice.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=left valign=middle height=90&gt;_x000D_ &lt;h3 style="font-size: 2em; font-weight: 300; color: #333333; -webkit-margin-before: 1em; -webkit-margin-after: 0.5em; text-align:center;"&gt;Cuenta de costo &lt;strong&gt;excedida en presupuesto&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: justify;"&gt;Estimado(a) Usuario, te informamos que las siguientes Cuentas de Costos han excedido el monto presupuestado en el Centro de Gestión &lt;strong&gt;&lt;centrogestion&gt;&lt;/strong&gt;:&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#fff style="border-top: 1px solid #fff;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="border-bottom: 1px solid #fff;"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=adaptative bgcolor=#fff&gt;_x000D_ &lt;thead&gt;_x000D_ &lt;tr bgcolor=#fff&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px; vertical-align: middle;" width=22%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Cuenta de Costo&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto presupuestado del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto comprometido del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Diferencia del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto presupuestado acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto comprometido acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Diferencia acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/thead&gt;_x000D_ &lt;tbody&gt;_x000D_ &lt;idtrcuentas&gt;_x000D_ &lt;/tbody&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px; background-color: #fff;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 10px 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: justify; margin-bottom: 30px;"&gt;Consulta el detalle del Presupuesto en el reporte "Presupuesto / Presupuesto Anualizado / Bandeja de Presupuesto".&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=top&gt;_x000D_ &lt;a href=https://apps.agilice.com style="background:#00A7E1; color:#fff; padding:10px 20px; text-decoration: none; border-radius:2px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight: 400;line-height: 23px;"&gt;Ir a Agilice.com&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=20 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=middle style="padding:5px 10px;"&gt;_x000D_ &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=top&gt;_x000D_ &lt;p style="line-height: 1.5em; font-size: 11px; text-align: center; color: #999999;"&gt;Correo enviado a trav&amp;eacute;s de Agilice | Todos los Derechos Reservados&lt;br&gt;&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt; _x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/center&gt;_x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;_x000D_ ','Se envía correo al detectar cuentas de costo con Presupuesto Anualizado excedido, de acuerdo a configuración de tabla PA_FrecuenciaNotificacion',201,2);</v>
       </c>
       <c r="T4" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20201, 'Redmat','presupuesto_ic@iconstruye.com', 'Cuenta de costo excedida en Presupuesto Anualizado al &lt;FechaEjecucion&gt;', '_x000D_ &lt;!DOCTYPE html&gt;_x000D_ &lt;html lang=en&gt;_x000D_ &lt;head&gt;_x000D_ &lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;_x000D_ &lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;_x000D_ &lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;_x000D_ &lt;style type=text/css&gt;_x000D_
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30201, 'Redmat','presupuesto_ic@iconstruye.com', 'Cuenta de costo excedida en Presupuesto Anualizado al &lt;FechaEjecucion&gt;', '_x000D_ &lt;!DOCTYPE html&gt;_x000D_ &lt;html lang=en&gt;_x000D_ &lt;head&gt;_x000D_ &lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;_x000D_ &lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;_x000D_ &lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;_x000D_ &lt;style type=text/css&gt;_x000D_
 body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}_x000D_
-&lt;/style&gt; _x000D_ &lt;/head&gt;_x000D_ &lt;body style="margin:0; padding:0; background-color:#fff;"&gt;_x000D_ &lt;span style="display: block; width: 840px !important; max-width: 840px; height: 1px" class=mobileOff&gt;&lt;/span&gt;_x000D_ &lt;center&gt;_x000D_ &lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#ffffff&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=middle style="padding:10px; text-align:center;"&gt;_x000D_ &lt;img class=logo src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=left valign=middle height=90&gt;_x000D_ &lt;h3 style="font-size: 2em; font-weight: 300; color: #333333; -webkit-margin-before: 1em; -webkit-margin-after: 0.5em; text-align:center;"&gt;Cuenta de costo &lt;strong&gt;excedida en presupuesto&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: justify;"&gt;Estimado(a) Usuario, te informamos que las siguientes Cuentas de Costos han excedido el monto presupuestado en el Centro de Gestión &lt;strong&gt;&lt;centrogestion&gt;&lt;/strong&gt;:&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#fff style="border-top: 1px solid #fff;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="border-bottom: 1px solid #fff;"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=adaptative bgcolor=#fff&gt;_x000D_ &lt;thead&gt;_x000D_ &lt;tr bgcolor=#fff&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px; vertical-align: middle;" width=22%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Cuenta de Costo&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto presupuestado del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto comprometido del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Diferencia del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto presupuestado acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto comprometido acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Diferencia acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/thead&gt;_x000D_ &lt;tbody&gt;_x000D_ &lt;idtrcuentas&gt;_x000D_ &lt;/tbody&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px; background-color: #fff;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 10px 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: justify; margin-bottom: 30px;"&gt;Consulta el detalle del Presupuesto en el reporte "Presupuesto / Presupuesto Anualizado / Bandeja de Presupuesto".&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=top&gt;_x000D_ &lt;a href=https://redmat.iconstruye.com style="background:#F78E28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:2px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight: 400;line-height: 23px;"&gt;Ir a Redmat.com&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=20 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=middle style="padding:5px 10px;"&gt;_x000D_ &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=top&gt;_x000D_ &lt;p style="line-height: 1.5em; font-size: 11px; text-align: center; color: #999999;"&gt;Correo enviado a trav&amp;eacute;s de Redmat | Todos los Derechos Reservados&lt;br&gt;&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt; _x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/center&gt;_x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;_x000D_ ','Se envía correo al detectar cuentas de costo con Presupuesto Anualizado excedido, de acuerdo a configuración de tabla PA_FrecuenciaNotificacion');</v>
+&lt;/style&gt; _x000D_ &lt;/head&gt;_x000D_ &lt;body style="margin:0; padding:0; background-color:#fff;"&gt;_x000D_ &lt;span style="display: block; width: 840px !important; max-width: 840px; height: 1px" class=mobileOff&gt;&lt;/span&gt;_x000D_ &lt;center&gt;_x000D_ &lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#ffffff&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=middle style="padding:10px; text-align:center;"&gt;_x000D_ &lt;img class=logo src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=left valign=middle height=90&gt;_x000D_ &lt;h3 style="font-size: 2em; font-weight: 300; color: #333333; -webkit-margin-before: 1em; -webkit-margin-after: 0.5em; text-align:center;"&gt;Cuenta de costo &lt;strong&gt;excedida en presupuesto&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: justify;"&gt;Estimado(a) Usuario, te informamos que las siguientes Cuentas de Costos han excedido el monto presupuestado en el Centro de Gestión &lt;strong&gt;&lt;centrogestion&gt;&lt;/strong&gt;:&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#fff style="border-top: 1px solid #fff;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="border-bottom: 1px solid #fff;"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=adaptative bgcolor=#fff&gt;_x000D_ &lt;thead&gt;_x000D_ &lt;tr bgcolor=#fff&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px; vertical-align: middle;" width=22%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Cuenta de Costo&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto presupuestado del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto comprometido del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Diferencia del mes&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto presupuestado acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Monto comprometido acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td align=left valign=top style=" border-bottom:1px solid #eee; padding:0 10px;" width=13%&gt;_x000D_ &lt;h3 class=cabecera style="font-size: 0.8em; font-weight: 500; line-height: 1.4em; margin: 10px 0px;"&gt;&lt;strong&gt;Diferencia acumulado&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/thead&gt;_x000D_ &lt;tbody&gt;_x000D_ &lt;idtrcuentas&gt;_x000D_ &lt;/tbody&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px; background-color: #fff;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=10 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top style="padding: 10px 0;"&gt;_x000D_ &lt;table width=800 cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=left valign=top&gt;_x000D_ &lt;p style=" font-size: 1.1em; line-height: 1.7em; text-align: justify; margin-bottom: 30px;"&gt;Consulta el detalle del Presupuesto en el reporte "Presupuesto / Presupuesto Anualizado / Bandeja de Presupuesto".&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=mobile align=center valign=top&gt;_x000D_ &lt;a href=https://redmat.iconstruye.com style="background:#F78E28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:2px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight: 400;line-height: 23px;"&gt;Ir a Redmat.com&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td height=20 style="font-size:10px; line-height:10px;"&gt;&amp;nbsp;&lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;table width=840 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=middle style="padding:5px 10px;"&gt;_x000D_ &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td align=center valign=top&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0 border=0 class=container&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="mobile footer" align=center valign=top&gt;_x000D_ &lt;p style="line-height: 1.5em; font-size: 11px; text-align: center; color: #999999;"&gt;Correo enviado a trav&amp;eacute;s de Redmat | Todos los Derechos Reservados&lt;br&gt;&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt; _x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/center&gt;_x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;_x000D_ ','Se envía correo al detectar cuentas de costo con Presupuesto Anualizado excedido, de acuerdo a configuración de tabla PA_FrecuenciaNotificacion',201,3);</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>118</v>
       </c>
@@ -7467,15 +7478,15 @@
         <v>50</v>
       </c>
       <c r="S5" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20118, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Traspaso &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Traspaso Pendiente de Aprobar.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá Aprobar este traspaso ingresando al módulo Bodega, opción Salida, Aprobar Traspasos. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Traspaso, Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20118, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Traspaso &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Traspaso Pendiente de Aprobar.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá Aprobar este traspaso ingresando al módulo Bodega, opción Salida, Aprobar Traspasos. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Traspaso, Envío a Aprobación',118,2);</v>
       </c>
       <c r="T5" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20118, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Traspaso &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Traspaso Pendiente de Aprobar.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá Aprobar este traspaso ingresando al módulo Bodega, opción Salida, Aprobar Traspasos. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Traspaso, Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30118, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Traspaso &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Traspaso Pendiente de Aprobar.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá Aprobar este traspaso ingresando al módulo Bodega, opción Salida, Aprobar Traspasos. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Traspaso, Envío a Aprobación',118,3);</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>119</v>
       </c>
@@ -7529,15 +7540,15 @@
         <v>57</v>
       </c>
       <c r="S6" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20119, 'Agilice','iconstruye@iconstruye.com', 'Rechazo de Traspaso &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Traspaso ha sido Rechazado.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Bodega, opción Salida, Consultar Traspasos, para ver el motivo del rechazo. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Traspaso, Rechazado Aprobador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20119, 'Agilice','iconstruye@iconstruye.com', 'Rechazo de Traspaso &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Traspaso ha sido Rechazado.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Bodega, opción Salida, Consultar Traspasos, para ver el motivo del rechazo. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Traspaso, Rechazado Aprobador',119,2);</v>
       </c>
       <c r="T6" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20119, 'Redmat','iconstruye@iconstruye.com', 'Rechazo de Traspaso &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Traspaso ha sido Rechazado.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Bodega, opción Salida, Consultar Traspasos, para ver el motivo del rechazo. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Traspaso, Rechazado Aprobador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30119, 'Redmat','iconstruye@iconstruye.com', 'Rechazo de Traspaso &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Traspaso ha sido Rechazado.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Bodega, opción Salida, Consultar Traspasos, para ver el motivo del rechazo. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Traspaso, Rechazado Aprobador',119,3);</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>126</v>
       </c>
@@ -7591,15 +7602,15 @@
         <v>64</v>
       </c>
       <c r="S7" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20126, 'Agilice','iconstruye@iconstruye.com', 'Orden de Compra, Rechazo de Adjudicacion', 'Estimado Sr(a). &lt;nombusuario&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Orden de Compra generada por usted ha sido Rechazada su Adjudicación. &lt;br&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt; &lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha envío OC: &lt;fechaenvio&gt; &lt;br&gt;Rechazado por: &lt;nombaprobador&gt; &lt;br&gt;Comentario: Rechazo en proceso de Adjudicación &lt;br&gt;&lt;br&gt;Para revisar mayores antecedentes, ingrese al módulo Compras de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Rechazo de Adjudicacion');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20126, 'Agilice','iconstruye@iconstruye.com', 'Orden de Compra, Rechazo de Adjudicacion', 'Estimado Sr(a). &lt;nombusuario&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Orden de Compra generada por usted ha sido Rechazada su Adjudicación. &lt;br&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt; &lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha envío OC: &lt;fechaenvio&gt; &lt;br&gt;Rechazado por: &lt;nombaprobador&gt; &lt;br&gt;Comentario: Rechazo en proceso de Adjudicación &lt;br&gt;&lt;br&gt;Para revisar mayores antecedentes, ingrese al módulo Compras de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Rechazo de Adjudicacion',126,2);</v>
       </c>
       <c r="T7" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20126, 'Redmat','iconstruye@iconstruye.com', 'Orden de Compra, Rechazo de Adjudicacion', 'Estimado Sr(a). &lt;nombusuario&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Orden de Compra generada por usted ha sido Rechazada su Adjudicación. &lt;br&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt; &lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha envío OC: &lt;fechaenvio&gt; &lt;br&gt;Rechazado por: &lt;nombaprobador&gt; &lt;br&gt;Comentario: Rechazo en proceso de Adjudicación &lt;br&gt;&lt;br&gt;Para revisar mayores antecedentes, ingrese al módulo Compras de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Rechazo de Adjudicacion');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30126, 'Redmat','iconstruye@iconstruye.com', 'Orden de Compra, Rechazo de Adjudicacion', 'Estimado Sr(a). &lt;nombusuario&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Orden de Compra generada por usted ha sido Rechazada su Adjudicación. &lt;br&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt; &lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha envío OC: &lt;fechaenvio&gt; &lt;br&gt;Rechazado por: &lt;nombaprobador&gt; &lt;br&gt;Comentario: Rechazo en proceso de Adjudicación &lt;br&gt;&lt;br&gt;Para revisar mayores antecedentes, ingrese al módulo Compras de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Rechazo de Adjudicacion',126,3);</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>130</v>
       </c>
@@ -7640,10 +7651,10 @@
         <v>71</v>
       </c>
       <c r="N8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>72</v>
@@ -7655,8 +7666,8 @@
         <v>74</v>
       </c>
       <c r="S8" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20130, 'Agilice','b2becheverriaizquierdo@iconstruye.com', 'Nueva(s) Órden(es) de Compra de {EmpresaCompradora}', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20130, 'Agilice','b2becheverriaizquierdo@iconstruye.com', 'Nueva(s) Órden(es) de Compra de {EmpresaCompradora}', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;
 		body {
 			font-family: Arial, Helvetica, sans-serif;
 			font-size: small;
@@ -7668,11 +7679,11 @@
 		p.parrafo {
 			text-indent: 24px;
 		}
-	&lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;&lt;strong&gt;Estimado Señor {NombreDestinatario}&lt;/strong&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Por Encargo de &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; le informamos que se ha(n) generado la(s) siguiente(s) Órden(es) de Compra:&lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;strong&gt;Órdenes de Compra:&lt;/strong&gt;&lt;/p&gt; {ListaOC} &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Para Aceptar o Rechazar esta(s) Órden(es) de Compra, debe responder a este Correo, &lt;strong&gt;como Plazo Máximo dentro de 8 horas hábiles&lt;/strong&gt;, señalando claramente su desición. En caso de Rechazar la(s) OC debe explicar claramente las razones del rechazo.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;strong&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra,responda este correo indicado el nombre y correo electrónico del contacto&lt;/strong&gt;.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;a href=https://apps.agilice.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://apps.agilice.com/ clicktracking=off&gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Agilice y realizar enlínea la gestión completa de sus negocios con &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;&lt;strong&gt;NOTAS:&lt;/strong&gt; {Mensaje}&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;p&gt;Agilice S.A.&lt;/p&gt; &lt;p&gt;Servicio de Activación de Órdenes de Compra.&lt;/p&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)');</v>
+	&lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;&lt;strong&gt;Estimado Señor {NombreDestinatario}&lt;/strong&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Por Encargo de &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; le informamos que se ha(n) generado la(s) siguiente(s) Órden(es) de Compra:&lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;strong&gt;Órdenes de Compra:&lt;/strong&gt;&lt;/p&gt; {ListaOC} &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Para Aceptar o Rechazar esta(s) Órden(es) de Compra, debe responder a este Correo, &lt;strong&gt;como Plazo Máximo dentro de 8 horas hábiles&lt;/strong&gt;, señalando claramente su desición. En caso de Rechazar la(s) OC debe explicar claramente las razones del rechazo.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;strong&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra,responda este correo indicado el nombre y correo electrónico del contacto&lt;/strong&gt;.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;a href=https://apps.agilice.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://apps.agilice.com/ clicktracking=off&gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Agilice y realizar enlínea la gestión completa de sus negocios con &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;&lt;strong&gt;NOTAS:&lt;/strong&gt; {Mensaje}&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;p&gt;Agilice S.A.&lt;/p&gt; &lt;p&gt;Servicio de Activación de Órdenes de Compra.&lt;/p&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)',130,2);</v>
       </c>
       <c r="T8" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20130, 'Redmat','b2becheverriaizquierdo@iconstruye.com', 'Nueva(s) Órden(es) de Compra de {EmpresaCompradora}', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30130, 'Redmat','b2becheverriaizquierdo@iconstruye.com', 'Nueva(s) Órden(es) de Compra de {EmpresaCompradora}', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;
 		body {
 			font-family: Arial, Helvetica, sans-serif;
 			font-size: small;
@@ -7684,10 +7695,10 @@
 		p.parrafo {
 			text-indent: 24px;
 		}
-	&lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;&lt;strong&gt;Estimado Señor {NombreDestinatario}&lt;/strong&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Por Encargo de &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; le informamos que se ha(n) generado la(s) siguiente(s) Órden(es) de Compra:&lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;strong&gt;Órdenes de Compra:&lt;/strong&gt;&lt;/p&gt; {ListaOC} &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Para Aceptar o Rechazar esta(s) Órden(es) de Compra, debe responder a este Correo, &lt;strong&gt;como Plazo Máximo dentro de 8 horas hábiles&lt;/strong&gt;, señalando claramente su desición. En caso de Rechazar la(s) OC debe explicar claramente las razones del rechazo.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;strong&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra,responda este correo indicado el nombre y correo electrónico del contacto&lt;/strong&gt;.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Redmat y realizar enlínea la gestión completa de sus negocios con &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt;. &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;&lt;strong&gt;NOTAS:&lt;/strong&gt; {Mensaje}&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;p&gt;Redmat S.A.&lt;/p&gt; &lt;p&gt;Servicio de Activación de Órdenes de Compra.&lt;/p&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)');</v>
+	&lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;&lt;strong&gt;Estimado Señor {NombreDestinatario}&lt;/strong&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Por Encargo de &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; le informamos que se ha(n) generado la(s) siguiente(s) Órden(es) de Compra:&lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;strong&gt;Órdenes de Compra:&lt;/strong&gt;&lt;/p&gt; {ListaOC} &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Para Aceptar o Rechazar esta(s) Órden(es) de Compra, debe responder a este Correo, &lt;strong&gt;como Plazo Máximo dentro de 8 horas hábiles&lt;/strong&gt;, señalando claramente su desición. En caso de Rechazar la(s) OC debe explicar claramente las razones del rechazo.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;strong&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra,responda este correo indicado el nombre y correo electrónico del contacto&lt;/strong&gt;.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Redmat y realizar enlínea la gestión completa de sus negocios con &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt;. &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;&lt;strong&gt;NOTAS:&lt;/strong&gt; {Mensaje}&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;p&gt;Redmat S.A.&lt;/p&gt; &lt;p&gt;Servicio de Activación de Órdenes de Compra.&lt;/p&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)',130,3);</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>6501</v>
       </c>
@@ -7741,15 +7752,15 @@
         <v>82</v>
       </c>
       <c r="S9" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26501, 'Agilice','iconstruye@iconstruye.com', 'Alerta de envío de documento con  parte relacionada. &lt;tipodoc&gt; N°&lt;numdoc&gt;', 'Estimado Sr. &lt;nombrecontralor&gt;:&lt;br&gt;&lt;br&gt;_x000D_ Junto con saludarle, informamos a usted que el &lt;fechenviodoc&gt;, se ha generado un documento &lt;tipodoc&gt; N° &lt;numdoc&gt; el cual es una operación con parte relacionada._x000D_ &lt;br&gt;&lt;br&gt;Tipo: &lt;rolparterelacionada&gt; &lt;br&gt; RUT: &lt;rutparterelacionada&gt; &lt;br&gt;&lt;br&gt;_x000D_ Puede revisar más detalles ingresando a “Consulta Operaciones” en el módulo de Contraloría._x000D_ &lt;br&gt;&lt;br&gt;&lt;br&gt;_x000D_ Atentamente,&lt;br&gt;&lt;br&gt;_x000D_ Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;_x000D_ Mesa de Ayuda&lt;br&gt;_x000D_ 2486 11 11&lt;br&gt;_x000D_ &lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Notificación operacion con parterelacionada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (206501, 'Agilice','iconstruye@iconstruye.com', 'Alerta de envío de documento con  parte relacionada. &lt;tipodoc&gt; N°&lt;numdoc&gt;', 'Estimado Sr. &lt;nombrecontralor&gt;:&lt;br&gt;&lt;br&gt;_x000D_ Junto con saludarle, informamos a usted que el &lt;fechenviodoc&gt;, se ha generado un documento &lt;tipodoc&gt; N° &lt;numdoc&gt; el cual es una operación con parte relacionada._x000D_ &lt;br&gt;&lt;br&gt;Tipo: &lt;rolparterelacionada&gt; &lt;br&gt; RUT: &lt;rutparterelacionada&gt; &lt;br&gt;&lt;br&gt;_x000D_ Puede revisar más detalles ingresando a “Consulta Operaciones” en el módulo de Contraloría._x000D_ &lt;br&gt;&lt;br&gt;&lt;br&gt;_x000D_ Atentamente,&lt;br&gt;&lt;br&gt;_x000D_ Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;_x000D_ Mesa de Ayuda&lt;br&gt;_x000D_ 2486 11 11&lt;br&gt;_x000D_ &lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Notificación operacion con parterelacionada',6501,2);</v>
       </c>
       <c r="T9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26501, 'Redmat','iconstruye@iconstruye.com', 'Alerta de envío de documento con  parte relacionada. &lt;tipodoc&gt; N°&lt;numdoc&gt;', 'Estimado Sr. &lt;nombrecontralor&gt;:&lt;br&gt;&lt;br&gt;_x000D_ Junto con saludarle, informamos a usted que el &lt;fechenviodoc&gt;, se ha generado un documento &lt;tipodoc&gt; N° &lt;numdoc&gt; el cual es una operación con parte relacionada._x000D_ &lt;br&gt;&lt;br&gt;Tipo: &lt;rolparterelacionada&gt; &lt;br&gt; RUT: &lt;rutparterelacionada&gt; &lt;br&gt;&lt;br&gt;_x000D_ Puede revisar más detalles ingresando a “Consulta Operaciones” en el módulo de Contraloría._x000D_ &lt;br&gt;&lt;br&gt;&lt;br&gt;_x000D_ Atentamente,&lt;br&gt;&lt;br&gt;_x000D_ Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;_x000D_ Mesa de Ayuda&lt;br&gt;_x000D_ 2486 11 11&lt;br&gt;_x000D_ &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Notificación operacion con parterelacionada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (306501, 'Redmat','iconstruye@iconstruye.com', 'Alerta de envío de documento con  parte relacionada. &lt;tipodoc&gt; N°&lt;numdoc&gt;', 'Estimado Sr. &lt;nombrecontralor&gt;:&lt;br&gt;&lt;br&gt;_x000D_ Junto con saludarle, informamos a usted que el &lt;fechenviodoc&gt;, se ha generado un documento &lt;tipodoc&gt; N° &lt;numdoc&gt; el cual es una operación con parte relacionada._x000D_ &lt;br&gt;&lt;br&gt;Tipo: &lt;rolparterelacionada&gt; &lt;br&gt; RUT: &lt;rutparterelacionada&gt; &lt;br&gt;&lt;br&gt;_x000D_ Puede revisar más detalles ingresando a “Consulta Operaciones” en el módulo de Contraloría._x000D_ &lt;br&gt;&lt;br&gt;&lt;br&gt;_x000D_ Atentamente,&lt;br&gt;&lt;br&gt;_x000D_ Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;_x000D_ Mesa de Ayuda&lt;br&gt;_x000D_ 2486 11 11&lt;br&gt;_x000D_ &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Notificación operacion con parterelacionada',6501,3);</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>6502</v>
       </c>
@@ -7803,15 +7814,15 @@
         <v>89</v>
       </c>
       <c r="S10" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26502, 'Agilice','iconstruye@iconstruye.com', 'Alerta de envío de documento con  parte relacionada. [No justificado] &lt;tipodoc&gt; N°&lt;numdoc&gt;', 'Estimado Sr. &lt;nombrecontralor&gt;:&lt;br&gt;&lt;br&gt;_x000D_ Junto con saludarle, informamos a usted que el &lt;fechenviodoc&gt;, se ha generado un documento &lt;tipodoc&gt; N° &lt;numdoc&gt; el cual es una operación con parte relacionada y no fué justificada con adjunto DPR._x000D_ &lt;br&gt;&lt;br&gt;Tipo: &lt;rolparterelacionada&gt; &lt;br&gt; RUT: &lt;rutparterelacionada&gt; &lt;br&gt;&lt;br&gt;_x000D_ Puede revisar más detalles ingresando a “Consulta Operaciones” en el módulo de Contraloría._x000D_ &lt;br&gt;&lt;br&gt;&lt;br&gt;_x000D_ Atentamente,&lt;br&gt;&lt;br&gt;_x000D_ Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;_x000D_ Mesa de Ayuda&lt;br&gt;_x000D_ 2486 11 11&lt;br&gt;_x000D_ &lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Notificación operacion con parterelacionada no justificada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (206502, 'Agilice','iconstruye@iconstruye.com', 'Alerta de envío de documento con  parte relacionada. [No justificado] &lt;tipodoc&gt; N°&lt;numdoc&gt;', 'Estimado Sr. &lt;nombrecontralor&gt;:&lt;br&gt;&lt;br&gt;_x000D_ Junto con saludarle, informamos a usted que el &lt;fechenviodoc&gt;, se ha generado un documento &lt;tipodoc&gt; N° &lt;numdoc&gt; el cual es una operación con parte relacionada y no fué justificada con adjunto DPR._x000D_ &lt;br&gt;&lt;br&gt;Tipo: &lt;rolparterelacionada&gt; &lt;br&gt; RUT: &lt;rutparterelacionada&gt; &lt;br&gt;&lt;br&gt;_x000D_ Puede revisar más detalles ingresando a “Consulta Operaciones” en el módulo de Contraloría._x000D_ &lt;br&gt;&lt;br&gt;&lt;br&gt;_x000D_ Atentamente,&lt;br&gt;&lt;br&gt;_x000D_ Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;_x000D_ Mesa de Ayuda&lt;br&gt;_x000D_ 2486 11 11&lt;br&gt;_x000D_ &lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Notificación operacion con parterelacionada no justificada',6502,2);</v>
       </c>
       <c r="T10" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26502, 'Redmat','iconstruye@iconstruye.com', 'Alerta de envío de documento con  parte relacionada. [No justificado] &lt;tipodoc&gt; N°&lt;numdoc&gt;', 'Estimado Sr. &lt;nombrecontralor&gt;:&lt;br&gt;&lt;br&gt;_x000D_ Junto con saludarle, informamos a usted que el &lt;fechenviodoc&gt;, se ha generado un documento &lt;tipodoc&gt; N° &lt;numdoc&gt; el cual es una operación con parte relacionada y no fué justificada con adjunto DPR._x000D_ &lt;br&gt;&lt;br&gt;Tipo: &lt;rolparterelacionada&gt; &lt;br&gt; RUT: &lt;rutparterelacionada&gt; &lt;br&gt;&lt;br&gt;_x000D_ Puede revisar más detalles ingresando a “Consulta Operaciones” en el módulo de Contraloría._x000D_ &lt;br&gt;&lt;br&gt;&lt;br&gt;_x000D_ Atentamente,&lt;br&gt;&lt;br&gt;_x000D_ Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;_x000D_ Mesa de Ayuda&lt;br&gt;_x000D_ 2486 11 11&lt;br&gt;_x000D_ &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Notificación operacion con parterelacionada no justificada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (306502, 'Redmat','iconstruye@iconstruye.com', 'Alerta de envío de documento con  parte relacionada. [No justificado] &lt;tipodoc&gt; N°&lt;numdoc&gt;', 'Estimado Sr. &lt;nombrecontralor&gt;:&lt;br&gt;&lt;br&gt;_x000D_ Junto con saludarle, informamos a usted que el &lt;fechenviodoc&gt;, se ha generado un documento &lt;tipodoc&gt; N° &lt;numdoc&gt; el cual es una operación con parte relacionada y no fué justificada con adjunto DPR._x000D_ &lt;br&gt;&lt;br&gt;Tipo: &lt;rolparterelacionada&gt; &lt;br&gt; RUT: &lt;rutparterelacionada&gt; &lt;br&gt;&lt;br&gt;_x000D_ Puede revisar más detalles ingresando a “Consulta Operaciones” en el módulo de Contraloría._x000D_ &lt;br&gt;&lt;br&gt;&lt;br&gt;_x000D_ Atentamente,&lt;br&gt;&lt;br&gt;_x000D_ Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;_x000D_ Mesa de Ayuda&lt;br&gt;_x000D_ 2486 11 11&lt;br&gt;_x000D_ &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Notificación operacion con parterelacionada no justificada',6502,3);</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>133</v>
       </c>
@@ -7865,15 +7876,15 @@
         <v>93</v>
       </c>
       <c r="S11" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20133, 'Agilice','&lt;DireccionRemitente&gt;', 'Solicitud de Contacto Portal &lt;NombrePortal&gt;', 'Template en Proyecto Web','Correo que envían los usuarios que se quieren registrar en el Portal de Proveedores (Portal de Pagos).');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20133, 'Agilice','&lt;DireccionRemitente&gt;', 'Solicitud de Contacto Portal &lt;NombrePortal&gt;', 'Template en Proyecto Web','Correo que envían los usuarios que se quieren registrar en el Portal de Proveedores (Portal de Pagos).',133,2);</v>
       </c>
       <c r="T11" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20133, 'Redmat','&lt;DireccionRemitente&gt;', 'Solicitud de Contacto Portal &lt;NombrePortal&gt;', 'Template en Proyecto Web','Correo que envían los usuarios que se quieren registrar en el Portal de Proveedores (Portal de Pagos).');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30133, 'Redmat','&lt;DireccionRemitente&gt;', 'Solicitud de Contacto Portal &lt;NombrePortal&gt;', 'Template en Proyecto Web','Correo que envían los usuarios que se quieren registrar en el Portal de Proveedores (Portal de Pagos).',133,3);</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>27</v>
       </c>
@@ -7927,15 +7938,15 @@
         <v>101</v>
       </c>
       <c r="S12" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20027, 'Agilice','iconstruye@iconstruye.com', 'Cierre de Cotización ', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Cotización ha finalizado su tiempo para recibir ofertas:&lt;br&gt;&lt;br&gt;Nº de Cotización: &lt;numcz&gt;&lt;br&gt;Nombre Cotización: &lt;nomcz&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Centro de Gestión: &lt;orgc&gt;&lt;br&gt;&lt;br&gt;Tiempo Duración: &lt;tiempocz&gt;&lt;br&gt; &lt;br&gt;Revise más antecedentes en el Módulo Cotizaciones.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt; + 56 22 486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cotizaciones, Cierre');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2027, 'Agilice','iconstruye@iconstruye.com', 'Cierre de Cotización ', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Cotización ha finalizado su tiempo para recibir ofertas:&lt;br&gt;&lt;br&gt;Nº de Cotización: &lt;numcz&gt;&lt;br&gt;Nombre Cotización: &lt;nomcz&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Centro de Gestión: &lt;orgc&gt;&lt;br&gt;&lt;br&gt;Tiempo Duración: &lt;tiempocz&gt;&lt;br&gt; &lt;br&gt;Revise más antecedentes en el Módulo Cotizaciones.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt; + 56 22 486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cotizaciones, Cierre',27,2);</v>
       </c>
       <c r="T12" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20027, 'Redmat','iconstruye@iconstruye.com', 'Cierre de Cotización ', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Cotización ha finalizado su tiempo para recibir ofertas:&lt;br&gt;&lt;br&gt;Nº de Cotización: &lt;numcz&gt;&lt;br&gt;Nombre Cotización: &lt;nomcz&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Centro de Gestión: &lt;orgc&gt;&lt;br&gt;&lt;br&gt;Tiempo Duración: &lt;tiempocz&gt;&lt;br&gt; &lt;br&gt;Revise más antecedentes en el Módulo Cotizaciones.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt; + 56 22 486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cotizaciones, Cierre');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3027, 'Redmat','iconstruye@iconstruye.com', 'Cierre de Cotización ', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Cotización ha finalizado su tiempo para recibir ofertas:&lt;br&gt;&lt;br&gt;Nº de Cotización: &lt;numcz&gt;&lt;br&gt;Nombre Cotización: &lt;nomcz&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Centro de Gestión: &lt;orgc&gt;&lt;br&gt;&lt;br&gt;Tiempo Duración: &lt;tiempocz&gt;&lt;br&gt; &lt;br&gt;Revise más antecedentes en el Módulo Cotizaciones.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt; + 56 22 486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cotizaciones, Cierre',27,3);</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>28</v>
       </c>
@@ -7989,15 +8000,15 @@
         <v>108</v>
       </c>
       <c r="S13" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20028, 'Agilice','iconstruye@iconstruye.com', 'Adjudicación Cotización', 'Estimados Sres. Empresa &lt;nombproveedor&gt;: &lt;br&gt; &lt;br&gt; Le informamos que su empresa ha sido ganadora del proceso de cotización de &lt;nombempresa&gt; con su oferta &lt;nomof&gt;.&lt;br&gt; &lt;br&gt; No. Cotización : &lt;numcz&gt;&lt;br&gt; Nombre : &lt;nomcz&gt; &lt;br&gt; &lt;br&gt; Felicitaciones,&lt;br&gt; &lt;br&gt; Agilice&lt;br&gt; Mi brazo derecho&lt;br&gt; &lt;link&gt;','Cotizaciones, Adjudicación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2028, 'Agilice','iconstruye@iconstruye.com', 'Adjudicación Cotización', 'Estimados Sres. Empresa &lt;nombproveedor&gt;: &lt;br&gt; &lt;br&gt; Le informamos que su empresa ha sido ganadora del proceso de cotización de &lt;nombempresa&gt; con su oferta &lt;nomof&gt;.&lt;br&gt; &lt;br&gt; No. Cotización : &lt;numcz&gt;&lt;br&gt; Nombre : &lt;nomcz&gt; &lt;br&gt; &lt;br&gt; Felicitaciones,&lt;br&gt; &lt;br&gt; Agilice&lt;br&gt; Mi brazo derecho&lt;br&gt; &lt;link&gt;','Cotizaciones, Adjudicación',28,2);</v>
       </c>
       <c r="T13" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20028, 'Redmat','iconstruye@iconstruye.com', 'Adjudicación Cotización', 'Estimados Sres. Empresa &lt;nombproveedor&gt;: &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Le informamos que su empresa ha sido ganadora del proceso de cotización de _x000D_ &lt;nombempresa&gt; con su oferta &lt;nomof&gt;.&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ No. Cotización : &lt;numcz&gt;&lt;br&gt;_x000D_ Nombre : &lt;nomcz&gt; &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Felicitaciones,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Redmat&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, Adjudicación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3028, 'Redmat','iconstruye@iconstruye.com', 'Adjudicación Cotización', 'Estimados Sres. Empresa &lt;nombproveedor&gt;: &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Le informamos que su empresa ha sido ganadora del proceso de cotización de _x000D_ &lt;nombempresa&gt; con su oferta &lt;nomof&gt;.&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ No. Cotización : &lt;numcz&gt;&lt;br&gt;_x000D_ Nombre : &lt;nomcz&gt; &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Felicitaciones,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Redmat&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, Adjudicación',28,3);</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>29</v>
       </c>
@@ -8051,15 +8062,15 @@
         <v>115</v>
       </c>
       <c r="S14" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20029, 'Agilice','iconstruye@iconstruye.com', 'Cotización No Aceptada', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Le informamos que &lt;nombempresa&gt; ha seleccionado otra alternativa de cotización .&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Agilice&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, No Aceptada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2029, 'Agilice','iconstruye@iconstruye.com', 'Cotización No Aceptada', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Le informamos que &lt;nombempresa&gt; ha seleccionado otra alternativa de cotización .&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Agilice&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, No Aceptada',29,2);</v>
       </c>
       <c r="T14" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20029, 'Redmat','iconstruye@iconstruye.com', 'Cotización No Aceptada', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Le informamos que &lt;nombempresa&gt; ha seleccionado otra alternativa de cotización .&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Redmat&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, No Aceptada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3029, 'Redmat','iconstruye@iconstruye.com', 'Cotización No Aceptada', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Le informamos que &lt;nombempresa&gt; ha seleccionado otra alternativa de cotización .&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Redmat&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, No Aceptada',29,3);</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>30</v>
       </c>
@@ -8113,15 +8124,15 @@
         <v>122</v>
       </c>
       <c r="S15" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20030, 'Agilice','iconstruye@iconstruye.com', 'Cotización Desierta', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Le informamos que la empresa &lt;nombempresa&gt; ha declarado desierta la cotización de &lt;numcz&gt;/&lt;nomcz&gt;.&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Agilice&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, Desierta');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2030, 'Agilice','iconstruye@iconstruye.com', 'Cotización Desierta', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Le informamos que la empresa &lt;nombempresa&gt; ha declarado desierta la cotización de &lt;numcz&gt;/&lt;nomcz&gt;.&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Agilice&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, Desierta',30,2);</v>
       </c>
       <c r="T15" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20030, 'Redmat','iconstruye@iconstruye.com', 'Cotización Desierta', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Le informamos que la empresa &lt;nombempresa&gt; ha declarado desierta la cotización de &lt;numcz&gt;/&lt;nomcz&gt;.&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Redmat&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, Desierta');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3030, 'Redmat','iconstruye@iconstruye.com', 'Cotización Desierta', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Le informamos que la empresa &lt;nombempresa&gt; ha declarado desierta la cotización de &lt;numcz&gt;/&lt;nomcz&gt;.&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Redmat&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, Desierta',30,3);</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>31</v>
       </c>
@@ -8175,15 +8186,15 @@
         <v>129</v>
       </c>
       <c r="S16" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20031, 'Agilice','iconstruye@iconstruye.com', 'Adelanto de adjudicación', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ La empresa&lt;nombempresa&gt; adelantó la adjudicación de &lt;numcz&gt;/&lt;nomcz&gt; para el &lt;fehaadjudicacion&gt; y seleccionó otra alternativa de cotización.&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Agilice&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, Adelanto de Adjudicación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2031, 'Agilice','iconstruye@iconstruye.com', 'Adelanto de adjudicación', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ La empresa&lt;nombempresa&gt; adelantó la adjudicación de &lt;numcz&gt;/&lt;nomcz&gt; para el &lt;fehaadjudicacion&gt; y seleccionó otra alternativa de cotización.&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Agilice&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, Adelanto de Adjudicación',31,2);</v>
       </c>
       <c r="T16" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20031, 'Redmat','iconstruye@iconstruye.com', 'Adelanto de adjudicación', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ La empresa&lt;nombempresa&gt; adelantó la adjudicación de &lt;numcz&gt;/&lt;nomcz&gt; para el &lt;fehaadjudicacion&gt; y seleccionó otra alternativa de cotización.&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Redmat&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, Adelanto de Adjudicación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3031, 'Redmat','iconstruye@iconstruye.com', 'Adelanto de adjudicación', 'Estimados Sres. Empresa &lt;nombproveedor&gt;:&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ La empresa&lt;nombempresa&gt; adelantó la adjudicación de &lt;numcz&gt;/&lt;nomcz&gt; para el &lt;fehaadjudicacion&gt; y seleccionó otra alternativa de cotización.&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente,&lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Redmat&lt;br&gt;_x000D_ Mi brazo derecho&lt;br&gt;_x000D_ &lt;link&gt;','Cotizaciones, Adelanto de Adjudicación',31,3);</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>32</v>
       </c>
@@ -8237,15 +8248,15 @@
         <v>136</v>
       </c>
       <c r="S17" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20032, 'Agilice','iconstruye@iconstruye.com', 'Confirmación de Recepción de Orden de Compra', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha recibido conforme la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Recepción Proveedor');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2032, 'Agilice','iconstruye@iconstruye.com', 'Confirmación de Recepción de Orden de Compra', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha recibido conforme la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Recepción Proveedor',32,2);</v>
       </c>
       <c r="T17" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20032, 'Redmat','iconstruye@iconstruye.com', 'Confirmación de Recepción de Orden de Compra', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha recibido conforme la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Recepción Proveedor');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3032, 'Redmat','iconstruye@iconstruye.com', 'Confirmación de Recepción de Orden de Compra', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha recibido conforme la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Recepción Proveedor',32,3);</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>33</v>
       </c>
@@ -8299,15 +8310,15 @@
         <v>143</v>
       </c>
       <c r="S18" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20033, 'Agilice','iconstruye@iconstruye.com', 'Rechazo de solicitud de cancelación ', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; No Aceptó su Solicitud de Cancelación para la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Rechazo Solicitud Cancelación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2033, 'Agilice','iconstruye@iconstruye.com', 'Rechazo de solicitud de cancelación ', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; No Aceptó su Solicitud de Cancelación para la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Rechazo Solicitud Cancelación',33,2);</v>
       </c>
       <c r="T18" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20033, 'Redmat','iconstruye@iconstruye.com', 'Rechazo de solicitud de cancelación ', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; No Aceptó su Solicitud de Cancelación para la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Rechazo Solicitud Cancelación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3033, 'Redmat','iconstruye@iconstruye.com', 'Rechazo de solicitud de cancelación ', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; No Aceptó su Solicitud de Cancelación para la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Rechazo Solicitud Cancelación',33,3);</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>117</v>
       </c>
@@ -8361,15 +8372,15 @@
         <v>150</v>
       </c>
       <c r="S19" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20117, 'Agilice','iconstruye@iconstruye.com', 'Factura en Espera de Aprobación (Tiempo Excedido)', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo Aprobación: Supera el monto del comprador &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Factura, Envío a Aprobación por Tiempo Excedido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20117, 'Agilice','iconstruye@iconstruye.com', 'Factura en Espera de Aprobación (Tiempo Excedido)', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo Aprobación: Supera el monto del comprador &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Factura, Envío a Aprobación por Tiempo Excedido',117,2);</v>
       </c>
       <c r="T19" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20117, 'Redmat','iconstruye@iconstruye.com', 'Factura en Espera de Aprobación (Tiempo Excedido)', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo Aprobación: Supera el monto del comprador &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Factura, Envío a Aprobación por Tiempo Excedido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30117, 'Redmat','iconstruye@iconstruye.com', 'Factura en Espera de Aprobación (Tiempo Excedido)', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo Aprobación: Supera el monto del comprador &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Factura, Envío a Aprobación por Tiempo Excedido',117,3);</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>6503</v>
       </c>
@@ -8423,8 +8434,8 @@
         <v>157</v>
       </c>
       <c r="S20" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26503, 'Agilice','iconstruye@iconstruye.com', ' &lt;nombsitio&gt; solicitud para recuperación de contraseña', '&lt;!DOCTYPE html
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (206503, 'Agilice','iconstruye@iconstruye.com', ' &lt;nombsitio&gt; solicitud para recuperación de contraseña', '&lt;!DOCTYPE html
 PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html&gt;&lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=utf-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1.0"&gt;&lt;title&gt;SOLICITUD DE CLAVE AGILICE&lt;/title&gt;&lt;style type=text/css&gt;body{
 margin: 10px 0;
 padding: 0 10px;
@@ -8452,11 +8463,11 @@
 width: 80% !important;} .cierre{
 padding: 30px 0 !important;} .cierre p{
 line-height: 0.7em !important;}}
-&lt;/style&gt;&lt;/head&gt;&lt;body style="background:#f2f5f9; color: #666666; padding:20px 0;"&gt;&lt;table border=0 cellpadding=0 cellspacing=0 width=100%&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center bgcolor=#FFFFFF border=0 cellpadding=0 cellspacing=0 width=640&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center bgcolor=#FFFFFF class=responsive-image style="font-size: 0; line-height: 0; padding:10px 0; border-bottom: 1px solid #dcdfe1; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3; border-top: 2px solid #00A7E1;"&gt;&lt;span class=sg-image&gt;&lt;img height=49 src=https://apps.agilice.com/img/logo-agilice.png style=float:left;padding-left:5px&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: left; line-height: 1.7em; vertical-align: top; padding:20px 20px 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1em; margin:0 0 15px; line-height: 1.6em;"&gt;Estimado(a) &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style="font-size: 1.4em; margin:0 0 15px; line-height: 1.7em;" class=contenido&gt;Se ha solicitado la recuperación de la contraseña para la empresa &lt;strong&gt;&lt;nombrefantasia&gt;. &lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="text-align: center; color:#0d5369; font-family:Helvetica; font-size:14px; line-height: 1.4em; overflow:hidden; letter-spacing:normal; padding-top: 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;table width=96% style="border-spacing: 0; border-collapse: collapse; margin: 0 auto 20px;"&gt;&lt;tr&gt;&lt;td style="padding: 0;"&gt;&lt;table style="width: 100%; border-spacing: 0; background: #FFF; border: none;"&gt;&lt;tr&gt;&lt;td colspan=3 style="border-bottom: 1px solid #cccccc;"&gt;&lt;h3 style="font-size: 1.4em; color: #00A7E1; font-weight: 500; text-transform: uppercase;"&gt;Datos del usuario&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr style="background: #FFFFFF; border-bottom: 1px solid #cccccc;"&gt;&lt;td style="padding: 0 10px;" width=50%&gt;&lt;p style="font-size: 1.3em; font-weight: 400; text-align: center; color: #666; -webkit-margin-before: 0.6em; -webkit-margin-after: 0.6em; -webkit-margin-start: 0px; -webkit-margin-end: 0px; border-right: 1px solid #cccccc;"&gt;&lt;strong&gt;usuario&lt;/strong&gt;&lt;br&gt;&lt;idusuario&gt;&lt;/p&gt;&lt;/td&gt;&lt;td style="padding: 0 10px; background: #FFFFFF;" width=50%&gt;&lt;p style="font-size: 1.3em; font-weight: 400; text-align: center; color: #666; -webkit-margin-before: 0.6em; -webkit-margin-after: 0.6em; -webkit-margin-start: 0px; -webkit-margin-end: 0px;"&gt;&lt;strong&gt;empresa&lt;/strong&gt;&lt;br&gt;&lt;nombempresa&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding: 20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1.4em; margin:0 0 10px; line-height: 1.7em;" class=contenido&gt;Para cambiar tu contraseña dirígete al siguiente link&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="color:#555; font-family:Helvetica; font-size:14px; text-align:center; padding-top:10px; overflow:hidden; letter-spacing:normal; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" valign=top&gt;&lt;a href="&lt;urlrecuperar&gt;" style="background:#00A7E1; color:#fff; padding:10px 15px 10px 15px; text-decoration:none; border-radius:4px; margin: 0 0 10px 0;display:inline-block; font-size: 17px; font-weight: 400; line-height: 26px;" class=boton&gt;Recuperar clave&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding:20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" class=cierre&gt;&lt;p style="font-size: 14px; margin:0; line-height: 1.7em;"&gt;Mesa de Ayuda: &lt;strong&gt;22 486 1111&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center border=0 cellpadding=0 cellspacing=0 class=deviceWidth style="margin:0 auto; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td style="border-top:1px solid #dcdfe3; font-size:11px; padding:20px; background: #e9ecf0; border-bottom:1px solid #dcdfe3;"&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;Correo enviado a trav&amp;eacute;s de Agilice | Todos los Derechos Reservados &lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña');</v>
+&lt;/style&gt;&lt;/head&gt;&lt;body style="background:#f2f5f9; color: #666666; padding:20px 0;"&gt;&lt;table border=0 cellpadding=0 cellspacing=0 width=100%&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center bgcolor=#FFFFFF border=0 cellpadding=0 cellspacing=0 width=640&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center bgcolor=#FFFFFF class=responsive-image style="font-size: 0; line-height: 0; padding:10px 0; border-bottom: 1px solid #dcdfe1; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3; border-top: 2px solid #00A7E1;"&gt;&lt;span class=sg-image&gt;&lt;img height=49 src=https://apps.agilice.com/img/logo-agilice.png style=float:left;padding-left:5px&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: left; line-height: 1.7em; vertical-align: top; padding:20px 20px 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1em; margin:0 0 15px; line-height: 1.6em;"&gt;Estimado(a) &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style="font-size: 1.4em; margin:0 0 15px; line-height: 1.7em;" class=contenido&gt;Se ha solicitado la recuperación de la contraseña para la empresa &lt;strong&gt;&lt;nombrefantasia&gt;. &lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="text-align: center; color:#0d5369; font-family:Helvetica; font-size:14px; line-height: 1.4em; overflow:hidden; letter-spacing:normal; padding-top: 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;table width=96% style="border-spacing: 0; border-collapse: collapse; margin: 0 auto 20px;"&gt;&lt;tr&gt;&lt;td style="padding: 0;"&gt;&lt;table style="width: 100%; border-spacing: 0; background: #FFF; border: none;"&gt;&lt;tr&gt;&lt;td colspan=3 style="border-bottom: 1px solid #cccccc;"&gt;&lt;h3 style="font-size: 1.4em; color: #00A7E1; font-weight: 500; text-transform: uppercase;"&gt;Datos del usuario&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr style="background: #FFFFFF; border-bottom: 1px solid #cccccc;"&gt;&lt;td style="padding: 0 10px;" width=50%&gt;&lt;p style="font-size: 1.3em; font-weight: 400; text-align: center; color: #666; -webkit-margin-before: 0.6em; -webkit-margin-after: 0.6em; -webkit-margin-start: 0px; -webkit-margin-end: 0px; border-right: 1px solid #cccccc;"&gt;&lt;strong&gt;usuario&lt;/strong&gt;&lt;br&gt;&lt;idusuario&gt;&lt;/p&gt;&lt;/td&gt;&lt;td style="padding: 0 10px; background: #FFFFFF;" width=50%&gt;&lt;p style="font-size: 1.3em; font-weight: 400; text-align: center; color: #666; -webkit-margin-before: 0.6em; -webkit-margin-after: 0.6em; -webkit-margin-start: 0px; -webkit-margin-end: 0px;"&gt;&lt;strong&gt;empresa&lt;/strong&gt;&lt;br&gt;&lt;nombempresa&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding: 20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1.4em; margin:0 0 10px; line-height: 1.7em;" class=contenido&gt;Para cambiar tu contraseña dirígete al siguiente link&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="color:#555; font-family:Helvetica; font-size:14px; text-align:center; padding-top:10px; overflow:hidden; letter-spacing:normal; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" valign=top&gt;&lt;a href="&lt;urlrecuperar&gt;" style="background:#00A7E1; color:#fff; padding:10px 15px 10px 15px; text-decoration:none; border-radius:4px; margin: 0 0 10px 0;display:inline-block; font-size: 17px; font-weight: 400; line-height: 26px;" class=boton&gt;Recuperar clave&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding:20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" class=cierre&gt;&lt;p style="font-size: 14px; margin:0; line-height: 1.7em;"&gt;Mesa de Ayuda: &lt;strong&gt;22 486 1111&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center border=0 cellpadding=0 cellspacing=0 class=deviceWidth style="margin:0 auto; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td style="border-top:1px solid #dcdfe3; font-size:11px; padding:20px; background: #e9ecf0; border-bottom:1px solid #dcdfe3;"&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;Correo enviado a trav&amp;eacute;s de Agilice | Todos los Derechos Reservados &lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña',6503,2);</v>
       </c>
       <c r="T20" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26503, 'Redmat','iconstruye@iconstruye.com', ' &lt;nombsitio&gt; solicitud para recuperación de contraseña', '&lt;!DOCTYPE html
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (306503, 'Redmat','iconstruye@iconstruye.com', ' &lt;nombsitio&gt; solicitud para recuperación de contraseña', '&lt;!DOCTYPE html
 PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html&gt;&lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=utf-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1.0"&gt;&lt;title&gt;SOLICITUD DE CLAVE REDMAT&lt;/title&gt;&lt;style type=text/css&gt;body{
 margin: 10px 0;
 padding: 0 10px;
@@ -8484,10 +8495,10 @@
 width: 80% !important;} .cierre{
 padding: 30px 0 !important;} .cierre p{
 line-height: 0.7em !important;}}
-&lt;/style&gt;&lt;/head&gt;&lt;body style="background:#f2f5f9; color: #666666; padding:20px 0;"&gt;&lt;table border=0 cellpadding=0 cellspacing=0 width=100%&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center bgcolor=#FFFFFF border=0 cellpadding=0 cellspacing=0 width=640&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center bgcolor=#FFFFFF class=responsive-image style="font-size: 0; line-height: 0; padding:10px 0; border-bottom: 1px solid #dcdfe3; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3; border-top: 2px solid #083F75;"&gt;&lt;span class=sg-image&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: left; line-height: 1.7em; vertical-align: top; padding:20px 20px 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1em; margin:0 0 15px; line-height: 1.6em;"&gt;Estimado(a) &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style="font-size: 1.4em; margin:0 0 15px; line-height: 1.7em;" class=contenido&gt;Se ha solicitado la recuperación de la contraseña para la empresa &lt;strong&gt;&lt;nombrefantasia&gt;. &lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="text-align: center; color:#0d5369; font-family:Helvetica; font-size:14px; line-height: 1.4em; overflow:hidden; letter-spacing:normal; padding-top: 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;table width=96% style="border-spacing: 0; border-collapse: collapse; margin: 0 auto 20px;"&gt;&lt;tr&gt;&lt;td style="padding: 0;"&gt;&lt;table style="width: 100%; border-spacing: 0; background: #FFF; border: none;"&gt;&lt;tr&gt;&lt;td colspan=3 style="border-bottom: 1px solid #cccccc;"&gt;&lt;h3 style="font-size: 1.4em; color: #083F75; font-weight: 500; text-transform: uppercase;"&gt;Datos del usuario&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr style="background: #FFFFFF; border-bottom: 1px solid #cccccc;"&gt;&lt;td style="padding: 0 10px;" width=50%&gt;&lt;p style="font-size: 1.3em; font-weight: 400; text-align: center; color: #666; -webkit-margin-before: 0.6em; -webkit-margin-after: 0.6em; -webkit-margin-start: 0px; -webkit-margin-end: 0px; border-right: 1px solid #cccccc;"&gt;&lt;strong&gt;usuario&lt;/strong&gt;&lt;br&gt;&lt;idusuario&gt;&lt;/p&gt;&lt;/td&gt;&lt;td style="padding: 0 10px; background: #FFFFFF;" width=50%&gt;&lt;p style="font-size: 1.3em; font-weight: 400; text-align: center; color: #666; -webkit-margin-before: 0.6em; -webkit-margin-after: 0.6em; -webkit-margin-start: 0px; -webkit-margin-end: 0px;"&gt;&lt;strong&gt;empresa&lt;/strong&gt;&lt;br&gt;&lt;nombempresa&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding: 20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1.4em; margin:0 0 10px; line-height: 1.7em;" class=contenido&gt;Para cambiar tu contraseña dirígete al siguiente link&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="color:#555; font-family:Helvetica; font-size:14px; text-align:center; padding-top:10px; overflow:hidden; letter-spacing:normal; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" valign=top&gt;&lt;a href="&lt;urlrecuperar&gt;" style="background:#083F75; color:#fff; padding:10px 15px 10px 15px; text-decoration:none; border-radius:4px; margin: 0 0 10px 0;display:inline-block; font-size: 17px; font-weight: 400; line-height: 26px;" class=boton&gt;Recuperar clave&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding:20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" class=cierre&gt;&lt;p style="font-size: 14px; margin:0; line-height: 1.7em;"&gt;Mesa de Ayuda: &lt;strong&gt;22 486 1111&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center border=0 cellpadding=0 cellspacing=0 class=deviceWidth style="margin:0 auto; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td style="border-top:1px solid #dcdfe3; font-size:11px; padding:20px; background: #e9ecf0; border-bottom:1px solid #dcdfe3;"&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;Correo enviado a trav&amp;eacute;s de Redmat | Todos los Derechos Reservados &lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña');</v>
+&lt;/style&gt;&lt;/head&gt;&lt;body style="background:#f2f5f9; color: #666666; padding:20px 0;"&gt;&lt;table border=0 cellpadding=0 cellspacing=0 width=100%&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center bgcolor=#FFFFFF border=0 cellpadding=0 cellspacing=0 width=640&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center bgcolor=#FFFFFF class=responsive-image style="font-size: 0; line-height: 0; padding:10px 0; border-bottom: 1px solid #dcdfe3; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3; border-top: 2px solid #083F75;"&gt;&lt;span class=sg-image&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: left; line-height: 1.7em; vertical-align: top; padding:20px 20px 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1em; margin:0 0 15px; line-height: 1.6em;"&gt;Estimado(a) &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style="font-size: 1.4em; margin:0 0 15px; line-height: 1.7em;" class=contenido&gt;Se ha solicitado la recuperación de la contraseña para la empresa &lt;strong&gt;&lt;nombrefantasia&gt;. &lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="text-align: center; color:#0d5369; font-family:Helvetica; font-size:14px; line-height: 1.4em; overflow:hidden; letter-spacing:normal; padding-top: 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;table width=96% style="border-spacing: 0; border-collapse: collapse; margin: 0 auto 20px;"&gt;&lt;tr&gt;&lt;td style="padding: 0;"&gt;&lt;table style="width: 100%; border-spacing: 0; background: #FFF; border: none;"&gt;&lt;tr&gt;&lt;td colspan=3 style="border-bottom: 1px solid #cccccc;"&gt;&lt;h3 style="font-size: 1.4em; color: #083F75; font-weight: 500; text-transform: uppercase;"&gt;Datos del usuario&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr style="background: #FFFFFF; border-bottom: 1px solid #cccccc;"&gt;&lt;td style="padding: 0 10px;" width=50%&gt;&lt;p style="font-size: 1.3em; font-weight: 400; text-align: center; color: #666; -webkit-margin-before: 0.6em; -webkit-margin-after: 0.6em; -webkit-margin-start: 0px; -webkit-margin-end: 0px; border-right: 1px solid #cccccc;"&gt;&lt;strong&gt;usuario&lt;/strong&gt;&lt;br&gt;&lt;idusuario&gt;&lt;/p&gt;&lt;/td&gt;&lt;td style="padding: 0 10px; background: #FFFFFF;" width=50%&gt;&lt;p style="font-size: 1.3em; font-weight: 400; text-align: center; color: #666; -webkit-margin-before: 0.6em; -webkit-margin-after: 0.6em; -webkit-margin-start: 0px; -webkit-margin-end: 0px;"&gt;&lt;strong&gt;empresa&lt;/strong&gt;&lt;br&gt;&lt;nombempresa&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding: 20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1.4em; margin:0 0 10px; line-height: 1.7em;" class=contenido&gt;Para cambiar tu contraseña dirígete al siguiente link&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="color:#555; font-family:Helvetica; font-size:14px; text-align:center; padding-top:10px; overflow:hidden; letter-spacing:normal; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" valign=top&gt;&lt;a href="&lt;urlrecuperar&gt;" style="background:#083F75; color:#fff; padding:10px 15px 10px 15px; text-decoration:none; border-radius:4px; margin: 0 0 10px 0;display:inline-block; font-size: 17px; font-weight: 400; line-height: 26px;" class=boton&gt;Recuperar clave&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding:20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" class=cierre&gt;&lt;p style="font-size: 14px; margin:0; line-height: 1.7em;"&gt;Mesa de Ayuda: &lt;strong&gt;22 486 1111&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center border=0 cellpadding=0 cellspacing=0 class=deviceWidth style="margin:0 auto; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td style="border-top:1px solid #dcdfe3; font-size:11px; padding:20px; background: #e9ecf0; border-bottom:1px solid #dcdfe3;"&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;Correo enviado a trav&amp;eacute;s de Redmat | Todos los Derechos Reservados &lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña',6503,3);</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>6504</v>
       </c>
@@ -8541,15 +8552,15 @@
         <v>164</v>
       </c>
       <c r="S21" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26504, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a &lt;nombsitio&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html&gt;&lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=utf-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1.0"&gt;&lt;title&gt;CAMBIO DE CLAVE AGILICE&lt;/title&gt;&lt;style type=text/css&gt;body{margin: 10px 0; padding: 0 10px; background: #f2f5f9; font-size: 14px; -webkit-font-smoothing: antialiased;font-family: Helvetica, sans-serif;}table{border-collapse: collapse;}td{font-family: Helvetica, sans-serif; color: #666666;}@media only screen and (max-width: 480px){body,table,td,p,a,li,blockquote{-webkit-text-size-adjust:none !important;}table{width: 100% !important;}.responsive-image img{height: auto !important; max-width: 100% !important; width: 100% !important;}.contenido{font-size: 1.1em !important; line-height: 1.4em !important;}p{text-align: center !important;}.boton{width: 80% !important;}.cierre{padding: 30px 0 !important;}.cierre p{line-height: 0.7em !important;}}&lt;/style&gt;&lt;/head&gt;&lt;body style="background:#f2f5f9; color: #666666; padding:20px 0;"&gt;&lt;table border=0 cellpadding=0 cellspacing=0 width=100%&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center bgcolor=#FFFFFF border=0 cellpadding=0 cellspacing=0 width=640&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center bgcolor=#FFFFFF class=responsive-image style="font-size: 0; line-height: 0; padding:10px 0; border-bottom: 1px solid #dcdfe3; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3; border-top: 2px solid #00A7E1;"&gt;&lt;span class=sg-image&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: left; line-height: 1.7em; vertical-align: top; padding:20px 20px 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1em; margin:0 0 15px; line-height: 1.6em;"&gt;Estimado(a) &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style="font-size: 1.4em; margin:0 0 15px; line-height: 1.7em;" class=contenido&gt;Ha modificado satisfactoriamente la clave para la empresa &lt;strong&gt;&lt;nombrefantasia&gt;&lt;/strong&gt;. Puedes volver a tu cuenta en el siguiente link.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="color:#555; font-family:Helvetica; font-size:14px; text-align:center; padding-top:10px; overflow:hidden; letter-spacing:normal; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" valign=top&gt;&lt;a href="&lt;urlrecuperar&gt;" style="background:#00A7E1; color:#fff; padding:10px 15px 10px 15px; text-decoration:none; border-radius:4px; margin: 0 0 10px 0;display:inline-block; font-size: 17px; font-weight: 400; line-height: 26px;" class=boton&gt;Ingresa a tu cuenta&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding:20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" class=cierre&gt;&lt;p style="font-size: 14px; margin:0; line-height: 1.7em;"&gt;Mesa de Ayuda: &lt;strong&gt;22 486 1111&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center border=0 cellpadding=0 cellspacing=0 class=deviceWidth style="margin:0 auto; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td style="border-top:1px solid #dcdfe3; font-size:11px; padding:20px; background: #e9ecf0; border-bottom:1px solid #dcdfe3;"&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;Correo enviado a trav&amp;eacute;s de Agilice | Todos los Derechos Reservados &lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Exitoso');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (206504, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a &lt;nombsitio&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html&gt;&lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=utf-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1.0"&gt;&lt;title&gt;CAMBIO DE CLAVE AGILICE&lt;/title&gt;&lt;style type=text/css&gt;body{margin: 10px 0; padding: 0 10px; background: #f2f5f9; font-size: 14px; -webkit-font-smoothing: antialiased;font-family: Helvetica, sans-serif;}table{border-collapse: collapse;}td{font-family: Helvetica, sans-serif; color: #666666;}@media only screen and (max-width: 480px){body,table,td,p,a,li,blockquote{-webkit-text-size-adjust:none !important;}table{width: 100% !important;}.responsive-image img{height: auto !important; max-width: 100% !important; width: 100% !important;}.contenido{font-size: 1.1em !important; line-height: 1.4em !important;}p{text-align: center !important;}.boton{width: 80% !important;}.cierre{padding: 30px 0 !important;}.cierre p{line-height: 0.7em !important;}}&lt;/style&gt;&lt;/head&gt;&lt;body style="background:#f2f5f9; color: #666666; padding:20px 0;"&gt;&lt;table border=0 cellpadding=0 cellspacing=0 width=100%&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center bgcolor=#FFFFFF border=0 cellpadding=0 cellspacing=0 width=640&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center bgcolor=#FFFFFF class=responsive-image style="font-size: 0; line-height: 0; padding:10px 0; border-bottom: 1px solid #dcdfe3; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3; border-top: 2px solid #00A7E1;"&gt;&lt;span class=sg-image&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: left; line-height: 1.7em; vertical-align: top; padding:20px 20px 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1em; margin:0 0 15px; line-height: 1.6em;"&gt;Estimado(a) &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style="font-size: 1.4em; margin:0 0 15px; line-height: 1.7em;" class=contenido&gt;Ha modificado satisfactoriamente la clave para la empresa &lt;strong&gt;&lt;nombrefantasia&gt;&lt;/strong&gt;. Puedes volver a tu cuenta en el siguiente link.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="color:#555; font-family:Helvetica; font-size:14px; text-align:center; padding-top:10px; overflow:hidden; letter-spacing:normal; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" valign=top&gt;&lt;a href="&lt;urlrecuperar&gt;" style="background:#00A7E1; color:#fff; padding:10px 15px 10px 15px; text-decoration:none; border-radius:4px; margin: 0 0 10px 0;display:inline-block; font-size: 17px; font-weight: 400; line-height: 26px;" class=boton&gt;Ingresa a tu cuenta&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding:20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" class=cierre&gt;&lt;p style="font-size: 14px; margin:0; line-height: 1.7em;"&gt;Mesa de Ayuda: &lt;strong&gt;22 486 1111&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center border=0 cellpadding=0 cellspacing=0 class=deviceWidth style="margin:0 auto; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td style="border-top:1px solid #dcdfe3; font-size:11px; padding:20px; background: #e9ecf0; border-bottom:1px solid #dcdfe3;"&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;Correo enviado a trav&amp;eacute;s de Agilice | Todos los Derechos Reservados &lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Exitoso',6504,2);</v>
       </c>
       <c r="T21" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26504, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a &lt;nombsitio&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html&gt;&lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=utf-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1.0"&gt;&lt;title&gt;CAMBIO DE CLAVE REDMAT&lt;/title&gt;&lt;style type=text/css&gt;body{margin: 10px 0; padding: 0 10px; background: #f2f5f9; font-size: 14px; -webkit-font-smoothing: antialiased;font-family: Helvetica, sans-serif;}table{border-collapse: collapse;}td{font-family: Helvetica, sans-serif; color: #666666;}@media only screen and (max-width: 480px){body,table,td,p,a,li,blockquote{-webkit-text-size-adjust:none !important;}table{width: 100% !important;}.responsive-image img{height: auto !important; max-width: 100% !important; width: 100% !important;}.contenido{font-size: 1.1em !important; line-height: 1.4em !important;}p{text-align: center !important;}.boton{width: 80% !important;}.cierre{padding: 30px 0 !important;}.cierre p{line-height: 0.7em !important;}}&lt;/style&gt;&lt;/head&gt;&lt;body style="background:#f2f5f9; color: #666666; padding:20px 0;"&gt;&lt;table border=0 cellpadding=0 cellspacing=0 width=100%&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center bgcolor=#FFFFFF border=0 cellpadding=0 cellspacing=0 width=640&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center bgcolor=#FFFFFF class=responsive-image style="font-size: 0; line-height: 0; padding:10px 0; border-bottom: 1px solid #dcdfe3; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3; border-top: 2px solid #083F75;"&gt;&lt;span class=sg-image&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: left; line-height: 1.7em; vertical-align: top; padding:20px 20px 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1em; margin:0 0 15px; line-height: 1.6em;"&gt;Estimado(a) &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style="font-size: 1.4em; margin:0 0 15px; line-height: 1.7em;" class=contenido&gt;Ha modificado satisfactoriamente la clave para la empresa &lt;strong&gt;&lt;nombrefantasia&gt;&lt;/strong&gt;. Puedes volver a tu cuenta en el siguiente link.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="color:#555; font-family:Helvetica; font-size:14px; text-align:center; padding-top:10px; overflow:hidden; letter-spacing:normal; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" valign=top&gt;&lt;a href="&lt;urlrecuperar&gt;" style="background:#F78E28; color:#fff; padding:10px 15px 10px 15px; text-decoration:none; border-radius:4px; margin: 0 0 10px 0;display:inline-block; font-size: 17px; font-weight: 400; line-height: 26px;" class=boton&gt;Ingresa a tu cuenta&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding:20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" class=cierre&gt;&lt;p style="font-size: 14px; margin:0; line-height: 1.7em;"&gt;Mesa de Ayuda: &lt;strong&gt;22 486 1111&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center border=0 cellpadding=0 cellspacing=0 class=deviceWidth style="margin:0 auto; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td style="border-top:1px solid #dcdfe3; font-size:11px; padding:20px; background: #e9ecf0; border-bottom:1px solid #dcdfe3;"&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;Correo enviado a trav&amp;eacute;s de Redmat | Todos los Derechos Reservados &lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Exitoso');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (306504, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a &lt;nombsitio&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html&gt;&lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=utf-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1.0"&gt;&lt;title&gt;CAMBIO DE CLAVE REDMAT&lt;/title&gt;&lt;style type=text/css&gt;body{margin: 10px 0; padding: 0 10px; background: #f2f5f9; font-size: 14px; -webkit-font-smoothing: antialiased;font-family: Helvetica, sans-serif;}table{border-collapse: collapse;}td{font-family: Helvetica, sans-serif; color: #666666;}@media only screen and (max-width: 480px){body,table,td,p,a,li,blockquote{-webkit-text-size-adjust:none !important;}table{width: 100% !important;}.responsive-image img{height: auto !important; max-width: 100% !important; width: 100% !important;}.contenido{font-size: 1.1em !important; line-height: 1.4em !important;}p{text-align: center !important;}.boton{width: 80% !important;}.cierre{padding: 30px 0 !important;}.cierre p{line-height: 0.7em !important;}}&lt;/style&gt;&lt;/head&gt;&lt;body style="background:#f2f5f9; color: #666666; padding:20px 0;"&gt;&lt;table border=0 cellpadding=0 cellspacing=0 width=100%&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center bgcolor=#FFFFFF border=0 cellpadding=0 cellspacing=0 width=640&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center bgcolor=#FFFFFF class=responsive-image style="font-size: 0; line-height: 0; padding:10px 0; border-bottom: 1px solid #dcdfe3; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3; border-top: 2px solid #083F75;"&gt;&lt;span class=sg-image&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: left; line-height: 1.7em; vertical-align: top; padding:20px 20px 0; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;p style="font-size: 1em; margin:0 0 15px; line-height: 1.6em;"&gt;Estimado(a) &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style="font-size: 1.4em; margin:0 0 15px; line-height: 1.7em;" class=contenido&gt;Ha modificado satisfactoriamente la clave para la empresa &lt;strong&gt;&lt;nombrefantasia&gt;&lt;/strong&gt;. Puedes volver a tu cuenta en el siguiente link.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td style="color:#555; font-family:Helvetica; font-size:14px; text-align:center; padding-top:10px; overflow:hidden; letter-spacing:normal; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" valign=top&gt;&lt;a href="&lt;urlrecuperar&gt;" style="background:#F78E28; color:#fff; padding:10px 15px 10px 15px; text-decoration:none; border-radius:4px; margin: 0 0 10px 0;display:inline-block; font-size: 17px; font-weight: 400; line-height: 26px;" class=boton&gt;Ingresa a tu cuenta&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor=#FFF style="font-weight: 400; text-align: center; line-height: 1.7em; vertical-align: top; padding:20px 20px 5px; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;" class=cierre&gt;&lt;p style="font-size: 14px; margin:0; line-height: 1.7em;"&gt;Mesa de Ayuda: &lt;strong&gt;22 486 1111&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;table align=center border=0 cellpadding=0 cellspacing=0 class=deviceWidth style="margin:0 auto; border-left:1px solid #dcdfe3; border-right:1px solid #dcdfe3;"&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td style="border-top:1px solid #dcdfe3; font-size:11px; padding:20px; background: #e9ecf0; border-bottom:1px solid #dcdfe3;"&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;Correo enviado a trav&amp;eacute;s de Redmat | Todos los Derechos Reservados &lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Exitoso',6504,3);</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>122</v>
       </c>
@@ -8605,15 +8616,15 @@
         <v>171</v>
       </c>
       <c r="S22" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20122, 'Agilice','iconstruye@iconstruye.com', 'Servicio Configuración Masiva', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt; &lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;Confirmación de cambios en Configuración&lt;/title&gt;&lt;/head&gt; &lt;body style="margin:0; padding:0;background:#fff;" leftmargin=0 marginwidth=0 topmargin=0 marginheight=0 offset=0&gt; &lt;center&gt; &lt;table align=center border=0 cellpadding=0 cellspacing=0 height=100% width=700px&gt; &lt;tr&gt; &lt;td align=center valign=top style="height:100% !important; margin:0; width:100% !important; padding:20px 15px;"&gt; &lt;table border=0 cellpadding=0 cellspacing=0 style="width:100%; max-width: 780px; border-left:1px solid #e5e5e5; border-right:1px solid #e5e5e5; border-bottom:1px solid #e5e5e5;"&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table border=0 cellpadding=0 cellspacing=0 width=100% style="background-color:#FFFFFF; border-top: 2px solid #00A7E1;border-bottom:1px solid #e5e5e5; padding: 10px 20px;"&gt; &lt;tr&gt; &lt;td valign=top style="padding:10px; background: rgb(255, 255, 255) none repeat scroll 0% 0%; "&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png style="max-width:200px; "&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table border=0 cellpadding=0 cellspacing=0 width=100% style="background-color:#FFFFFF; border-top:1px solid #FFFFFF;"&gt; &lt;tr&gt; &lt;td valign=top style="color:#555; font-family:Helvetica; font-size:14px; line-height: 1.4em; padding:20px 40px 30px 40px; overflow:hidden; letter-spacing:normal;"&gt; &lt;h3 style="margin:0 0 10px 0;"&gt;Estimado &lt;usuario&gt;:&lt;/h3&gt; &lt;p style="margin:0 0 10px 0;"&gt;&lt;accion&gt;:&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr valign=top style="color:#808080;line-height:40px; font-family:Helvetica; font-size:13px; line-height:150%; padding-top:20px; padding-right:20px; padding-bottom:20px; padding-left:20px; width:50%; text-align:center;"&gt;&lt;td&gt;El detalle del proceso de configuración lo puedes consultar en el modulo configuraciones sección Informacion General/Historial Configuración&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt; &lt;td valign=top style="color:#808080; font-family:Helvetica; font-size:12px; line-height:150%; padding-top:20px; padding-right:20px; padding-bottom:20px; padding-left:20px; width:50%; text-align:center;"&gt; Si necesita comunicarse con nosotros escríbanos a &lt;a href=mailto:contactenos@iconstruye.com style="color:#00A7E1; font-weight:normal; text-decoration:none;"&gt;contactenos@iconstruye.com&lt;/a&gt; o llámenos al 2 4861192&lt;br&gt; Al operar en la Plataforma Agilice, los usuarios y la empresa a la que pertenecen aceptan cumplir con los &lt;a href=# style="color:#00A7E1; font-weight:normal; text-decoration:none;"&gt;Términos y Condiciones&lt;/a&gt; de uso. &lt;/td&gt; &lt;/tr&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td style="border-top:1px solid #ddd; font-size:9px; padding:20px; font-family:Helvetica; color:#666;"&gt; © Agilice · Todos los Derechos Reservados. &lt;/td&gt; &lt;tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/center&gt; &lt;/body&gt; &lt;/html&gt;','Servicio Configuración Masiva');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20122, 'Agilice','iconstruye@iconstruye.com', 'Servicio Configuración Masiva', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt; &lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;Confirmación de cambios en Configuración&lt;/title&gt;&lt;/head&gt; &lt;body style="margin:0; padding:0;background:#fff;" leftmargin=0 marginwidth=0 topmargin=0 marginheight=0 offset=0&gt; &lt;center&gt; &lt;table align=center border=0 cellpadding=0 cellspacing=0 height=100% width=700px&gt; &lt;tr&gt; &lt;td align=center valign=top style="height:100% !important; margin:0; width:100% !important; padding:20px 15px;"&gt; &lt;table border=0 cellpadding=0 cellspacing=0 style="width:100%; max-width: 780px; border-left:1px solid #e5e5e5; border-right:1px solid #e5e5e5; border-bottom:1px solid #e5e5e5;"&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table border=0 cellpadding=0 cellspacing=0 width=100% style="background-color:#FFFFFF; border-top: 2px solid #00A7E1;border-bottom:1px solid #e5e5e5; padding: 10px 20px;"&gt; &lt;tr&gt; &lt;td valign=top style="padding:10px; background: rgb(255, 255, 255) none repeat scroll 0% 0%; "&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png style="max-width:200px; "&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table border=0 cellpadding=0 cellspacing=0 width=100% style="background-color:#FFFFFF; border-top:1px solid #FFFFFF;"&gt; &lt;tr&gt; &lt;td valign=top style="color:#555; font-family:Helvetica; font-size:14px; line-height: 1.4em; padding:20px 40px 30px 40px; overflow:hidden; letter-spacing:normal;"&gt; &lt;h3 style="margin:0 0 10px 0;"&gt;Estimado &lt;usuario&gt;:&lt;/h3&gt; &lt;p style="margin:0 0 10px 0;"&gt;&lt;accion&gt;:&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr valign=top style="color:#808080;line-height:40px; font-family:Helvetica; font-size:13px; line-height:150%; padding-top:20px; padding-right:20px; padding-bottom:20px; padding-left:20px; width:50%; text-align:center;"&gt;&lt;td&gt;El detalle del proceso de configuración lo puedes consultar en el modulo configuraciones sección Informacion General/Historial Configuración&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt; &lt;td valign=top style="color:#808080; font-family:Helvetica; font-size:12px; line-height:150%; padding-top:20px; padding-right:20px; padding-bottom:20px; padding-left:20px; width:50%; text-align:center;"&gt; Si necesita comunicarse con nosotros escríbanos a &lt;a href=mailto:contactenos@iconstruye.com style="color:#00A7E1; font-weight:normal; text-decoration:none;"&gt;contactenos@iconstruye.com&lt;/a&gt; o llámenos al 2 4861192&lt;br&gt; Al operar en la Plataforma Agilice, los usuarios y la empresa a la que pertenecen aceptan cumplir con los &lt;a href=# style="color:#00A7E1; font-weight:normal; text-decoration:none;"&gt;Términos y Condiciones&lt;/a&gt; de uso. &lt;/td&gt; &lt;/tr&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td style="border-top:1px solid #ddd; font-size:9px; padding:20px; font-family:Helvetica; color:#666;"&gt; © Agilice · Todos los Derechos Reservados. &lt;/td&gt; &lt;tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/center&gt; &lt;/body&gt; &lt;/html&gt;','Servicio Configuración Masiva',122,2);</v>
       </c>
       <c r="T22" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20122, 'Redmat','iconstruye@iconstruye.com', 'Servicio Configuración Masiva', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt; &lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;Confirmación de cambios en Configuración&lt;/title&gt;&lt;/head&gt; &lt;body style="margin:0; padding:0;background:#fff;" leftmargin=0 marginwidth=0 topmargin=0 marginheight=0 offset=0&gt; &lt;center&gt; &lt;table align=center border=0 cellpadding=0 cellspacing=0 height=100% width=700px&gt; &lt;tr&gt; &lt;td align=center valign=top style="height:100% !important; margin:0; width:100% !important; padding:20px 15px;"&gt; &lt;table border=0 cellpadding=0 cellspacing=0 style="width:100%; max-width: 780px; border-left:1px solid #e5e5e5; border-right:1px solid #e5e5e5; border-bottom:1px solid #e5e5e5;"&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table border=0 cellpadding=0 cellspacing=0 width=100% style="background-color:#FFFFFF; border-top: 2px solid #083F75;border-bottom:1px solid #e5e5e5; padding: 10px 20px;"&gt; &lt;tr&gt; &lt;td valign=top style="padding:10px; background: rgb(255, 255, 255) none repeat scroll 0% 0%; "&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png style="max-width:200px; "&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table border=0 cellpadding=0 cellspacing=0 width=100% style="background-color:#FFFFFF; border-top:1px solid #FFFFFF;"&gt; &lt;tr&gt; &lt;td valign=top style="color:#555; font-family:Helvetica; font-size:14px; line-height: 1.4em; padding:20px 40px 30px 40px; overflow:hidden; letter-spacing:normal;"&gt; &lt;h3 style="margin:0 0 10px 0;"&gt;Estimado &lt;usuario&gt;:&lt;/h3&gt; &lt;p style="margin:0 0 10px 0;"&gt;&lt;accion&gt;:&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr valign=top style="color:#808080;line-height:40px; font-family:Helvetica; font-size:13px; line-height:150%; padding-top:20px; padding-right:20px; padding-bottom:20px; padding-left:20px; width:50%; text-align:center;"&gt;&lt;td&gt;El detalle del proceso de configuración lo puedes consultar en el modulo configuraciones sección Informacion General/Historial Configuración&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt; &lt;td valign=top style="color:#808080; font-family:Helvetica; font-size:12px; line-height:150%; padding-top:20px; padding-right:20px; padding-bottom:20px; padding-left:20px; width:50%; text-align:center;"&gt; Si necesita comunicarse con nosotros escríbanos a &lt;a href=mailto:contactenos@iconstruye.com style="color:#083F75; font-weight:normal; text-decoration:none;"&gt;contactenos@iconstruye.com&lt;/a&gt; o llámenos al 2 4861192&lt;br&gt; Al operar en la Plataforma Redmat, los usuarios y la empresa a la que pertenecen aceptan cumplir con los &lt;a href=# style="color:#083F75; font-weight:normal; text-decoration:none;"&gt;Términos y Condiciones&lt;/a&gt; de uso. &lt;/td&gt; &lt;/tr&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td style="border-top:1px solid #ddd; font-size:9px; padding:20px; font-family:Helvetica; color:#666;"&gt; © Redmat · Todos los Derechos Reservados. &lt;/td&gt; &lt;tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/center&gt; &lt;/body&gt; &lt;/html&gt;','Servicio Configuración Masiva');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30122, 'Redmat','iconstruye@iconstruye.com', 'Servicio Configuración Masiva', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt; &lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;Confirmación de cambios en Configuración&lt;/title&gt;&lt;/head&gt; &lt;body style="margin:0; padding:0;background:#fff;" leftmargin=0 marginwidth=0 topmargin=0 marginheight=0 offset=0&gt; &lt;center&gt; &lt;table align=center border=0 cellpadding=0 cellspacing=0 height=100% width=700px&gt; &lt;tr&gt; &lt;td align=center valign=top style="height:100% !important; margin:0; width:100% !important; padding:20px 15px;"&gt; &lt;table border=0 cellpadding=0 cellspacing=0 style="width:100%; max-width: 780px; border-left:1px solid #e5e5e5; border-right:1px solid #e5e5e5; border-bottom:1px solid #e5e5e5;"&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table border=0 cellpadding=0 cellspacing=0 width=100% style="background-color:#FFFFFF; border-top: 2px solid #083F75;border-bottom:1px solid #e5e5e5; padding: 10px 20px;"&gt; &lt;tr&gt; &lt;td valign=top style="padding:10px; background: rgb(255, 255, 255) none repeat scroll 0% 0%; "&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png style="max-width:200px; "&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td align=center valign=top&gt; &lt;table border=0 cellpadding=0 cellspacing=0 width=100% style="background-color:#FFFFFF; border-top:1px solid #FFFFFF;"&gt; &lt;tr&gt; &lt;td valign=top style="color:#555; font-family:Helvetica; font-size:14px; line-height: 1.4em; padding:20px 40px 30px 40px; overflow:hidden; letter-spacing:normal;"&gt; &lt;h3 style="margin:0 0 10px 0;"&gt;Estimado &lt;usuario&gt;:&lt;/h3&gt; &lt;p style="margin:0 0 10px 0;"&gt;&lt;accion&gt;:&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr valign=top style="color:#808080;line-height:40px; font-family:Helvetica; font-size:13px; line-height:150%; padding-top:20px; padding-right:20px; padding-bottom:20px; padding-left:20px; width:50%; text-align:center;"&gt;&lt;td&gt;El detalle del proceso de configuración lo puedes consultar en el modulo configuraciones sección Informacion General/Historial Configuración&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt; &lt;td valign=top style="color:#808080; font-family:Helvetica; font-size:12px; line-height:150%; padding-top:20px; padding-right:20px; padding-bottom:20px; padding-left:20px; width:50%; text-align:center;"&gt; Si necesita comunicarse con nosotros escríbanos a &lt;a href=mailto:contactenos@iconstruye.com style="color:#083F75; font-weight:normal; text-decoration:none;"&gt;contactenos@iconstruye.com&lt;/a&gt; o llámenos al 2 4861192&lt;br&gt; Al operar en la Plataforma Redmat, los usuarios y la empresa a la que pertenecen aceptan cumplir con los &lt;a href=# style="color:#083F75; font-weight:normal; text-decoration:none;"&gt;Términos y Condiciones&lt;/a&gt; de uso. &lt;/td&gt; &lt;/tr&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td style="border-top:1px solid #ddd; font-size:9px; padding:20px; font-family:Helvetica; color:#666;"&gt; © Redmat · Todos los Derechos Reservados. &lt;/td&gt; &lt;tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/center&gt; &lt;/body&gt; &lt;/html&gt;','Servicio Configuración Masiva',122,3);</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>160</v>
       </c>
@@ -8667,8 +8678,8 @@
         <v>177</v>
       </c>
       <c r="S23" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20160, 'Agilice','iconstruye@iconstruye.com', 'Nueva Orden de compra N° {NumeroOC} de {EmpresaCompradora}.', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20160, 'Agilice','iconstruye@iconstruye.com', 'Nueva Orden de compra N° {NumeroOC} de {EmpresaCompradora}.', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;
 		body {
 			font-family: Arial, Helvetica, sans-serif;
 			font-size: small;
@@ -8677,11 +8688,11 @@
 		p {
 			text-align: justify;
 		}
-	&lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;Estimado Proveedor &lt;p&gt;La empresa &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt;, le ha generado una Órden de Compra N° {NumeroOC} a través de &lt;a clicktracking=off href=https://apps.agilice.com&gt;https://apps.agilice.com&lt;/a&gt;&lt;/p&gt; &lt;p&gt;Para descargar el PDF debe hacer clic en el Número del documento en el siguiente enlace {Link}.&lt;/p&gt; &lt;p&gt;Para Aceptar o Rechazar esta orden de compra, debe &lt;strong&gt;responder a este correo con copia a todos los contactos&lt;/strong&gt;, señalando claramente su decisión. &lt;br&gt; &lt;p&gt;Si deseas mayor información puedes contactarnos en el siguiente link &lt;a href=https://apps.agilice.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; &lt;/p&gt; &lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)');</v>
+	&lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;Estimado Proveedor &lt;p&gt;La empresa &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt;, le ha generado una Órden de Compra N° {NumeroOC} a través de &lt;a clicktracking=off href=https://apps.agilice.com&gt;https://apps.agilice.com&lt;/a&gt;&lt;/p&gt; &lt;p&gt;Para descargar el PDF debe hacer clic en el Número del documento en el siguiente enlace {Link}.&lt;/p&gt; &lt;p&gt;Para Aceptar o Rechazar esta orden de compra, debe &lt;strong&gt;responder a este correo con copia a todos los contactos&lt;/strong&gt;, señalando claramente su decisión. &lt;br&gt; &lt;p&gt;Si deseas mayor información puedes contactarnos en el siguiente link &lt;a href=https://apps.agilice.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; &lt;/p&gt; &lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)',160,2);</v>
       </c>
       <c r="T23" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20160, 'Redmat','iconstruye@iconstruye.com', 'Nueva Orden de compra N° {NumeroOC} de {EmpresaCompradora}.', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30160, 'Redmat','iconstruye@iconstruye.com', 'Nueva Orden de compra N° {NumeroOC} de {EmpresaCompradora}.', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;
 		body {
 			font-family: Arial, Helvetica, sans-serif;
 			font-size: small;
@@ -8690,10 +8701,10 @@
 		p {
 			text-align: justify;
 		}
-	&lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;Estimado Proveedor &lt;p&gt;La empresa &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt;, le ha generado una Órden de Compra N° {NumeroOC} a través de &lt;a clicktracking=off href=https://redmat.iconstruye.com&gt;https://redmat.iconstruye.com&lt;/a&gt;&lt;/p&gt; &lt;p&gt;Para descargar el PDF debe hacer clic en el Número del documento en el siguiente enlace {Link}.&lt;/p&gt; &lt;p&gt;Para Aceptar o Rechazar esta orden de compra, debe &lt;strong&gt;responder a este correo con copia a todos los contactos&lt;/strong&gt;, señalando claramente su decisión. &lt;br&gt; &lt;p&gt;Si deseas mayor información puedes contactarnos en el siguiente link &lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; &lt;/p&gt; &lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)');</v>
+	&lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;Estimado Proveedor &lt;p&gt;La empresa &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt;, le ha generado una Órden de Compra N° {NumeroOC} a través de &lt;a clicktracking=off href=https://redmat.iconstruye.com&gt;https://redmat.iconstruye.com&lt;/a&gt;&lt;/p&gt; &lt;p&gt;Para descargar el PDF debe hacer clic en el Número del documento en el siguiente enlace {Link}.&lt;/p&gt; &lt;p&gt;Para Aceptar o Rechazar esta orden de compra, debe &lt;strong&gt;responder a este correo con copia a todos los contactos&lt;/strong&gt;, señalando claramente su decisión. &lt;br&gt; &lt;p&gt;Si deseas mayor información puedes contactarnos en el siguiente link &lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; &lt;/p&gt; &lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)',160,3);</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>6505</v>
       </c>
@@ -8747,15 +8758,15 @@
         <v>184</v>
       </c>
       <c r="S24" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26505, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de Código Rechazada', '&lt;div style=width:600px&gt;&lt;p style=font-family:Arial;font-size:12px;text-align:left&gt;&lt;b&gt;Estimado Sr(a). &lt;usuario&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de código enviada el día &lt;fechaenvio&gt; del Centro de Gestión &lt;nomorgc&gt;, ha sido rechazada por el usuario &lt;nomusuarioatiende&gt;.&lt;br &amp;lt;br&gt;&lt;br&gt;&lt;b&gt;MATERIAL SOLICITADO&lt;/b&gt;&lt;br &amp;lt;br&gt;&lt;br&gt;&lt;b&gt;Descripcion: &lt;/b&gt;&lt;descripcion1&gt;&lt;br&gt;&lt;b&gt;Unidad: &lt;/b&gt;&lt;unidad1&gt;&lt;br&gt;&lt;b&gt;Motivo de rechazo: &lt;/b&gt;&lt;motivo&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Agilice S.A.&lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se rechaza (eliminación física) los materiales solicitados que estan pendientes');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (206505, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de Código Rechazada', '&lt;div style=width:600px&gt;&lt;p style=font-family:Arial;font-size:12px;text-align:left&gt;&lt;b&gt;Estimado Sr(a). &lt;usuario&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de código enviada el día &lt;fechaenvio&gt; del Centro de Gestión &lt;nomorgc&gt;, ha sido rechazada por el usuario &lt;nomusuarioatiende&gt;.&lt;br &amp;lt;br&gt;&lt;br&gt;&lt;b&gt;MATERIAL SOLICITADO&lt;/b&gt;&lt;br &amp;lt;br&gt;&lt;br&gt;&lt;b&gt;Descripcion: &lt;/b&gt;&lt;descripcion1&gt;&lt;br&gt;&lt;b&gt;Unidad: &lt;/b&gt;&lt;unidad1&gt;&lt;br&gt;&lt;b&gt;Motivo de rechazo: &lt;/b&gt;&lt;motivo&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Agilice S.A.&lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se rechaza (eliminación física) los materiales solicitados que estan pendientes',6505,2);</v>
       </c>
       <c r="T24" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26505, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de Código Rechazada', '&lt;div style=width:600px&gt;&lt;p style=font-family:Arial;font-size:12px;text-align:left&gt;&lt;b&gt;Estimado Sr(a). &lt;usuario&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de código enviada el día &lt;fechaenvio&gt; del Centro de Gestión &lt;nomorgc&gt;, ha sido rechazada por el usuario &lt;nomusuarioatiende&gt;.&lt;br &amp;lt;br&gt;&lt;br&gt;&lt;b&gt;MATERIAL SOLICITADO&lt;/b&gt;&lt;br &amp;lt;br&gt;&lt;br&gt;&lt;b&gt;Descripcion: &lt;/b&gt;&lt;descripcion1&gt;&lt;br&gt;&lt;b&gt;Unidad: &lt;/b&gt;&lt;unidad1&gt;&lt;br&gt;&lt;b&gt;Motivo de rechazo: &lt;/b&gt;&lt;motivo&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Redmat S.A.&lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se rechaza (eliminación física) los materiales solicitados que estan pendientes');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (306505, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de Código Rechazada', '&lt;div style=width:600px&gt;&lt;p style=font-family:Arial;font-size:12px;text-align:left&gt;&lt;b&gt;Estimado Sr(a). &lt;usuario&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de código enviada el día &lt;fechaenvio&gt; del Centro de Gestión &lt;nomorgc&gt;, ha sido rechazada por el usuario &lt;nomusuarioatiende&gt;.&lt;br &amp;lt;br&gt;&lt;br&gt;&lt;b&gt;MATERIAL SOLICITADO&lt;/b&gt;&lt;br &amp;lt;br&gt;&lt;br&gt;&lt;b&gt;Descripcion: &lt;/b&gt;&lt;descripcion1&gt;&lt;br&gt;&lt;b&gt;Unidad: &lt;/b&gt;&lt;unidad1&gt;&lt;br&gt;&lt;b&gt;Motivo de rechazo: &lt;/b&gt;&lt;motivo&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Redmat S.A.&lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se rechaza (eliminación física) los materiales solicitados que estan pendientes',6505,3);</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>6506</v>
       </c>
@@ -8809,15 +8820,15 @@
         <v>191</v>
       </c>
       <c r="S25" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26506, 'Agilice','iconstruye@iconstruye.com', 'Aviso de Creación de Material en Estado Inactivo', '&lt;div style=width:600px;&gt;&lt;p style="font-family:Arial; font-size:12px; text-align:left;"&gt;&lt;b&gt;Estimado Sr(a). &lt;usuariosolicitante&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de creación de código enviada el día &lt;fechaenvio&gt;, del centro de gestión &lt;nomorgc&gt; a sido aprobada por el usuario &lt;nomusuarioatiende&gt;.&lt;b&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;MATERIAL SOLICITADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Descripción:&lt;/td&gt;&lt;td&gt;&lt;descripcion1&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;b&gt; MATERIAL CREADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Código: &lt;/td&gt;&lt;td&gt;&lt;codigo2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Descripción: &lt;/td&gt;&lt;td&gt;&lt;descripcion2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad2&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Estado: &lt;/td&gt;&lt;td&gt;&lt;estadomaterial&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Motivo: &lt;/td&gt;&lt;td&gt;&lt;motivo&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Agilice S.A. &lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se crean desactivados los materiales solicitados que estan pendientes en la administaracion de maestro');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (206506, 'Agilice','iconstruye@iconstruye.com', 'Aviso de Creación de Material en Estado Inactivo', '&lt;div style=width:600px;&gt;&lt;p style="font-family:Arial; font-size:12px; text-align:left;"&gt;&lt;b&gt;Estimado Sr(a). &lt;usuariosolicitante&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de creación de código enviada el día &lt;fechaenvio&gt;, del centro de gestión &lt;nomorgc&gt; a sido aprobada por el usuario &lt;nomusuarioatiende&gt;.&lt;b&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;MATERIAL SOLICITADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Descripción:&lt;/td&gt;&lt;td&gt;&lt;descripcion1&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;b&gt; MATERIAL CREADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Código: &lt;/td&gt;&lt;td&gt;&lt;codigo2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Descripción: &lt;/td&gt;&lt;td&gt;&lt;descripcion2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad2&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Estado: &lt;/td&gt;&lt;td&gt;&lt;estadomaterial&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Motivo: &lt;/td&gt;&lt;td&gt;&lt;motivo&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Agilice S.A. &lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se crean desactivados los materiales solicitados que estan pendientes en la administaracion de maestro',6506,2);</v>
       </c>
       <c r="T25" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26506, 'Redmat','iconstruye@iconstruye.com', 'Aviso de Creación de Material en Estado Inactivo', '&lt;div style=width:600px;&gt;&lt;p style="font-family:Arial; font-size:12px; text-align:left;"&gt;&lt;b&gt;Estimado Sr(a). &lt;usuariosolicitante&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de creación de código enviada el día &lt;fechaenvio&gt;, del centro de gestión &lt;nomorgc&gt; a sido aprobada por el usuario &lt;nomusuarioatiende&gt;.&lt;b&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;MATERIAL SOLICITADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Descripción:&lt;/td&gt;&lt;td&gt;&lt;descripcion1&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;b&gt; MATERIAL CREADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Código: &lt;/td&gt;&lt;td&gt;&lt;codigo2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Descripción: &lt;/td&gt;&lt;td&gt;&lt;descripcion2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad2&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Estado: &lt;/td&gt;&lt;td&gt;&lt;estadomaterial&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Motivo: &lt;/td&gt;&lt;td&gt;&lt;motivo&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Redmat S.A. &lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se crean desactivados los materiales solicitados que estan pendientes en la administaracion de maestro');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (306506, 'Redmat','iconstruye@iconstruye.com', 'Aviso de Creación de Material en Estado Inactivo', '&lt;div style=width:600px;&gt;&lt;p style="font-family:Arial; font-size:12px; text-align:left;"&gt;&lt;b&gt;Estimado Sr(a). &lt;usuariosolicitante&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de creación de código enviada el día &lt;fechaenvio&gt;, del centro de gestión &lt;nomorgc&gt; a sido aprobada por el usuario &lt;nomusuarioatiende&gt;.&lt;b&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;MATERIAL SOLICITADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Descripción:&lt;/td&gt;&lt;td&gt;&lt;descripcion1&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;b&gt; MATERIAL CREADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Código: &lt;/td&gt;&lt;td&gt;&lt;codigo2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Descripción: &lt;/td&gt;&lt;td&gt;&lt;descripcion2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad2&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Estado: &lt;/td&gt;&lt;td&gt;&lt;estadomaterial&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Motivo: &lt;/td&gt;&lt;td&gt;&lt;motivo&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Redmat S.A. &lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se crean desactivados los materiales solicitados que estan pendientes en la administaracion de maestro',6506,3);</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>6509</v>
       </c>
@@ -8871,8 +8882,8 @@
         <v>198</v>
       </c>
       <c r="S26" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26509, 'Agilice','iconstruye@iconstruye.com', 'Archivo de Pago [&lt;Estado&gt;]', '&lt;!DOCTYPE html&gt;_x000D_ &lt;html lang=es&gt;_x000D_ &lt;head&gt;_x000D_ &lt;meta charset=UTF-8&gt;_x000D_ &lt;style type=text/css&gt;_x000D_
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (206509, 'Agilice','iconstruye@iconstruye.com', 'Archivo de Pago [&lt;Estado&gt;]', '&lt;!DOCTYPE html&gt;_x000D_ &lt;html lang=es&gt;_x000D_ &lt;head&gt;_x000D_ &lt;meta charset=UTF-8&gt;_x000D_ &lt;style type=text/css&gt;_x000D_
 		body {_x000D_
 			font-family: Arial, Helvetica, sans-serif;_x000D_
 			font-size: small;_x000D_
@@ -8883,11 +8894,11 @@
 			text-align: justify;_x000D_
 		}_x000D_
 		_x000D_
-	&lt;/style&gt;_x000D_ &lt;/head&gt;_x000D_ &lt;body&gt;_x000D_ &lt;h3&gt;Estimado &lt;strong&gt;&lt;nombreusuario&gt;&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;br&gt;_x000D_ &lt;p&gt;El archivo de pago &lt;strong&gt;&lt;nombrearchivo&gt;&lt;/strong&gt; se encuentra &lt;strong&gt;&lt;estado&gt;&lt;/strong&gt;.&lt;/p&gt;_x000D_ &lt;p&gt;Consulta el estado de todas sus Solicitudes en la sección "&lt;strong&gt;Consulta Archivos de Pago&lt;/strong&gt;".&lt;/p&gt;_x000D_ &lt;br&gt;_x000D_ &lt;p&gt;Ingrese al portal proveedores de &lt;strong&gt;Agilice.com&lt;strong&gt;&lt;/p&gt;_x000D_ &lt;br&gt;_x000D_ &lt;p&gt;Atentamente,&lt;/p&gt;_x000D_ &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt;_x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;','Aviso de Aprobación o Rechazo de un Archivo de Pago en Revisión.');</v>
+	&lt;/style&gt;_x000D_ &lt;/head&gt;_x000D_ &lt;body&gt;_x000D_ &lt;h3&gt;Estimado &lt;strong&gt;&lt;nombreusuario&gt;&lt;/strong&gt;&lt;/h3&gt;_x000D_ &lt;br&gt;_x000D_ &lt;p&gt;El archivo de pago &lt;strong&gt;&lt;nombrearchivo&gt;&lt;/strong&gt; se encuentra &lt;strong&gt;&lt;estado&gt;&lt;/strong&gt;.&lt;/p&gt;_x000D_ &lt;p&gt;Consulta el estado de todas sus Solicitudes en la sección "&lt;strong&gt;Consulta Archivos de Pago&lt;/strong&gt;".&lt;/p&gt;_x000D_ &lt;br&gt;_x000D_ &lt;p&gt;Ingrese al portal proveedores de &lt;strong&gt;Agilice.com&lt;strong&gt;&lt;/p&gt;_x000D_ &lt;br&gt;_x000D_ &lt;p&gt;Atentamente,&lt;/p&gt;_x000D_ &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt;_x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;','Aviso de Aprobación o Rechazo de un Archivo de Pago en Revisión.',6509,2);</v>
       </c>
       <c r="T26" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26509, 'Redmat','iconstruye@iconstruye.com', 'Archivo de Pago [&lt;Estado&gt;]', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (306509, 'Redmat','iconstruye@iconstruye.com', 'Archivo de Pago [&lt;Estado&gt;]', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;
 		body {
 			font-family: Arial, Helvetica, sans-serif;
 			font-size: small;
@@ -8896,10 +8907,10 @@
 		p {
 			text-align: justify;
 		}
-	&lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;h3&gt;Estimado &lt;strong&gt;&lt;nombreusuario&gt;&lt;/strong&gt;&lt;/h3&gt; &lt;br&gt; &lt;p&gt;El archivo de pago &lt;strong&gt;&lt;nombrearchivo&gt;&lt;/strong&gt; se encuentra &lt;strong&gt;&lt;estado&gt;&lt;/strong&gt;.&lt;/p&gt; &lt;p&gt;Consulta el estado de todas sus Solicitudes en la sección "&lt;strong&gt;Consulta Archivos de Pago&lt;/strong&gt;".&lt;/p&gt; &lt;br&gt; &lt;p&gt;Ingrese al portal proveedores de &lt;strong&gt;&lt;a href=https://redmat.iconstruye.com&gt;https://redmat.iconstruye.com&lt;/a&gt;&lt;strong&gt;&lt;/p&gt; &lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Aprobación o Rechazo de un Archivo de Pago en Revisión.');</v>
+	&lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;h3&gt;Estimado &lt;strong&gt;&lt;nombreusuario&gt;&lt;/strong&gt;&lt;/h3&gt; &lt;br&gt; &lt;p&gt;El archivo de pago &lt;strong&gt;&lt;nombrearchivo&gt;&lt;/strong&gt; se encuentra &lt;strong&gt;&lt;estado&gt;&lt;/strong&gt;.&lt;/p&gt; &lt;p&gt;Consulta el estado de todas sus Solicitudes en la sección "&lt;strong&gt;Consulta Archivos de Pago&lt;/strong&gt;".&lt;/p&gt; &lt;br&gt; &lt;p&gt;Ingrese al portal proveedores de &lt;strong&gt;&lt;a href=https://redmat.iconstruye.com&gt;https://redmat.iconstruye.com&lt;/a&gt;&lt;strong&gt;&lt;/p&gt; &lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Aprobación o Rechazo de un Archivo de Pago en Revisión.',6509,3);</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>131</v>
       </c>
@@ -8953,15 +8964,15 @@
         <v>205</v>
       </c>
       <c r="S27" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20131, 'Agilice','iconstruye@iconstruye.com', '{NombreEmpresaCompradora} te invita a participar de la cotización N° {NumeroCotizacion}', '&lt;!DOCTYPE html&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt; &lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;INVITACIÓN A COTIZAR EN AGILICE&lt;/title&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1.0"&gt;&lt;/head&gt; &lt;body leftmargin=0 topmargin=0 marginwidth=0 marginheight=0 yahoo=fix style="font-family: Helvetica, sans-serif; color: #666666; width: 100%; -webkit-font-smoothing: antialiased; background-color: #f2f5f9; margin: 0; padding: 0;" bgcolor=#f2f5f9&gt; &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center style="border-collapse: collapse;"&gt; &lt;tr&gt; &lt;td width=100% valign=top bgcolor=#f2f5f9 style="padding: 20px 0;"&gt; &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center style="border-bottom-style: solid; border-bottom-color: #dcdfe3; border-bottom-width: 1px; border-left-width: 1px; border-left-color: #dcdfe3; border-left-style: solid; border-right-width: 1px; border-right-color: #dcdfe3; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt; &lt;tr&gt; &lt;td width=100% bgcolor=#ffffff style="border-top-width: 2px; border-top-color: #00A7E1; border-top-style: solid; padding: 10px 0;"&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png style&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center bgcolor=#FFF style="border-left-style: solid; border-left-color: #dcdfe3; border-left-width: 1px; border-right-color: #dcdfe3; border-right-width: 1px; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt; &lt;tr&gt; &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 10px 20px 5px;" bgcolor=#FFF align=left valign=top&gt; &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;Estimado (a): {NombreProveedor}&lt;/p&gt; &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;La empresa &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; lo ha invitado a participar de la siguiente cotización:&lt;/p&gt; &lt;ul&gt; &lt;li style="font-size: 0.9em; font-weight: 400; color: #3A5F84;"&gt; &lt;strong&gt;N° de Cotización:&lt;/strong&gt; {NumeroCotizacion}&lt;/li&gt; &lt;li style="font-size: 0.9em; font-weight: 400; color: #3A5F84;"&gt; &lt;strong&gt;Nombre de la cotización:&lt;/strong&gt; {NombreCotizacion}&lt;/li&gt; &lt;li style="font-size: 1em; font-weight: 600; color: #3A5F84;"&gt; &lt;strong&gt;Fecha de Cierre:&lt;/strong&gt; {FechaDeCierre}&lt;/li&gt; &lt;/ul&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 10px 20px 5px;" bgcolor=#FFF align=left valign=top&gt; &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;El detalle de los materiales a cotizar se encuentra en la siguiente tabla:&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td style="text-align: center; color: #0d5369; font-family: Helvetica; font-size: 14px; line-height: 1.4em; overflow: hidden; letter-spacing: normal; padding-top: 0;" align=center&gt; &lt;table width=96% style="border-spacing: 0; border-collapse: collapse; margin: 0 auto;"&gt; &lt;tr&gt; &lt;td style="padding: 0;"&gt; {TablaMateriales} &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td valign=top style="color: #555; font-family: Helvetica; font-size: 14px; text-align: center; padding-top: 30px; overflow: hidden; letter-spacing: normal;" align=center&gt; &lt;a clicktracking=off href=https://apps.agilice.com/ style="background-color: #00A7E1; color: #fff; text-decoration: none; border-radius: 4px; font-size: 17px; font-weight: 400; line-height: 26px; display: inline-block; margin: 0 0 20px; padding: 16px 25px 15px;"&gt;Ingresa a ofertar&lt;/a&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 20px 20px 5px;" bgcolor=#FFF align=left valign=top&gt; &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;No deje pasar esta Oportunidad de hacer Negocios. Para mayor información, ingrese al módulo de Cotizaciones de nuestro sistema.&lt;/p&gt; &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;Atentamente&lt;br&gt; &lt;strong&gt;Equipo Agilice&lt;/strong&gt;&lt;br&gt; &lt;a clicktracking=off href=https://apps.agilice.com&gt;https://apps.agilice.com&lt;/a&gt; &lt;br&gt; Mesa de Ayuda: +56 2 24861111&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center bgcolor=#fff style="border-left-style: solid; border-left-color: #dcdfe3; border-left-width: 1px; border-right-color: #dcdfe3; border-right-width: 1px; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt; &lt;tr&gt; &lt;td style="padding: 20px; border-top-width: 1px; border-top-color: #dcdfe3; border-top-style: solid; font-size: 11px; font-family: Helvetica; color: #666; background-color: #e9ecf0; border-bottom-width: 1px; border-bottom-style: solid; border-bottom-color: #dcdfe3;" bgcolor=#e9ecf0&gt; &lt;p&gt;Correo enviado a través de Agilice · Todos los Derechos Reservados&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/body&gt; &lt;/html&gt;','Invitación a los Proveedores para Participar en una Cotización Publicada.');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20131, 'Agilice','iconstruye@iconstruye.com', '{NombreEmpresaCompradora} te invita a participar de la cotización N° {NumeroCotizacion}', '&lt;!DOCTYPE html&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt; &lt;head&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;INVITACIÓN A COTIZAR EN AGILICE&lt;/title&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1.0"&gt;&lt;/head&gt; &lt;body leftmargin=0 topmargin=0 marginwidth=0 marginheight=0 yahoo=fix style="font-family: Helvetica, sans-serif; color: #666666; width: 100%; -webkit-font-smoothing: antialiased; background-color: #f2f5f9; margin: 0; padding: 0;" bgcolor=#f2f5f9&gt; &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center style="border-collapse: collapse;"&gt; &lt;tr&gt; &lt;td width=100% valign=top bgcolor=#f2f5f9 style="padding: 20px 0;"&gt; &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center style="border-bottom-style: solid; border-bottom-color: #dcdfe3; border-bottom-width: 1px; border-left-width: 1px; border-left-color: #dcdfe3; border-left-style: solid; border-right-width: 1px; border-right-color: #dcdfe3; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt; &lt;tr&gt; &lt;td width=100% bgcolor=#ffffff style="border-top-width: 2px; border-top-color: #00A7E1; border-top-style: solid; padding: 10px 0;"&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png style&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center bgcolor=#FFF style="border-left-style: solid; border-left-color: #dcdfe3; border-left-width: 1px; border-right-color: #dcdfe3; border-right-width: 1px; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt; &lt;tr&gt; &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 10px 20px 5px;" bgcolor=#FFF align=left valign=top&gt; &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;Estimado (a): {NombreProveedor}&lt;/p&gt; &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;La empresa &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; lo ha invitado a participar de la siguiente cotización:&lt;/p&gt; &lt;ul&gt; &lt;li style="font-size: 0.9em; font-weight: 400; color: #3A5F84;"&gt; &lt;strong&gt;N° de Cotización:&lt;/strong&gt; {NumeroCotizacion}&lt;/li&gt; &lt;li style="font-size: 0.9em; font-weight: 400; color: #3A5F84;"&gt; &lt;strong&gt;Nombre de la cotización:&lt;/strong&gt; {NombreCotizacion}&lt;/li&gt; &lt;li style="font-size: 1em; font-weight: 600; color: #3A5F84;"&gt; &lt;strong&gt;Fecha de Cierre:&lt;/strong&gt; {FechaDeCierre}&lt;/li&gt; &lt;/ul&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 10px 20px 5px;" bgcolor=#FFF align=left valign=top&gt; &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;El detalle de los materiales a cotizar se encuentra en la siguiente tabla:&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td style="text-align: center; color: #0d5369; font-family: Helvetica; font-size: 14px; line-height: 1.4em; overflow: hidden; letter-spacing: normal; padding-top: 0;" align=center&gt; &lt;table width=96% style="border-spacing: 0; border-collapse: collapse; margin: 0 auto;"&gt; &lt;tr&gt; &lt;td style="padding: 0;"&gt; {TablaMateriales} &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td valign=top style="color: #555; font-family: Helvetica; font-size: 14px; text-align: center; padding-top: 30px; overflow: hidden; letter-spacing: normal;" align=center&gt; &lt;a clicktracking=off href=https://apps.agilice.com/ style="background-color: #00A7E1; color: #fff; text-decoration: none; border-radius: 4px; font-size: 17px; font-weight: 400; line-height: 26px; display: inline-block; margin: 0 0 20px; padding: 16px 25px 15px;"&gt;Ingresa a ofertar&lt;/a&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 20px 20px 5px;" bgcolor=#FFF align=left valign=top&gt; &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;No deje pasar esta Oportunidad de hacer Negocios. Para mayor información, ingrese al módulo de Cotizaciones de nuestro sistema.&lt;/p&gt; &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;Atentamente&lt;br&gt; &lt;strong&gt;Equipo Agilice&lt;/strong&gt;&lt;br&gt; &lt;a clicktracking=off href=https://apps.agilice.com&gt;https://apps.agilice.com&lt;/a&gt; &lt;br&gt; Mesa de Ayuda: +56 2 24861111&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center bgcolor=#fff style="border-left-style: solid; border-left-color: #dcdfe3; border-left-width: 1px; border-right-color: #dcdfe3; border-right-width: 1px; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt; &lt;tr&gt; &lt;td style="padding: 20px; border-top-width: 1px; border-top-color: #dcdfe3; border-top-style: solid; font-size: 11px; font-family: Helvetica; color: #666; background-color: #e9ecf0; border-bottom-width: 1px; border-bottom-style: solid; border-bottom-color: #dcdfe3;" bgcolor=#e9ecf0&gt; &lt;p&gt;Correo enviado a través de Agilice · Todos los Derechos Reservados&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/body&gt; &lt;/html&gt;','Invitación a los Proveedores para Participar en una Cotización Publicada.',131,2);</v>
       </c>
       <c r="T27" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20131, 'Redmat','iconstruye@iconstruye.com', '{NombreEmpresaCompradora} te invita a participar de la cotización N° {NumeroCotizacion}', '&lt;!DOCTYPE html&gt;_x000D_ &lt;html xmlns=http://www.w3.org/1999/xhtml&gt;_x000D_ &lt;head&gt;_x000D_ _x000D_ &lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;_x000D_ _x000D_ &lt;title&gt;INVITACIÓN A COTIZAR EN REDMAT&lt;/title&gt;_x000D_ &lt;meta name=viewport content="width=device-width, initial-scale=1.0"&gt;_x000D_ &lt;/head&gt;_x000D_ _x000D_ &lt;body leftmargin=0 topmargin=0 marginwidth=0 marginheight=0 yahoo=fix style="font-family: Helvetica, sans-serif; color: #666666; width: 100%; -webkit-font-smoothing: antialiased; background-color: #f2f5f9; margin: 0; padding: 0;" bgcolor=#f2f5f9&gt;_x000D_ _x000D_ _x000D_ &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center style="border-collapse: collapse;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td width=100% valign=top bgcolor=#f2f5f9 style="padding: 20px 0;"&gt;_x000D_ _x000D_ _x000D_ &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center style="border-bottom-style: solid; border-bottom-color: #dcdfe3; border-bottom-width: 1px; border-left-width: 1px; border-left-color: #dcdfe3; border-left-style: solid; border-right-width: 1px; border-right-color: #dcdfe3; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td width=100% bgcolor=#ffffff style="border-top-width: 2px; border-top-color: #083F75; border-top-style: solid; padding: 10px 0;"&gt;_x000D_ &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png style="width: 100%;"&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ _x000D_ _x000D_ &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center bgcolor=#FFF style="border-left-style: solid; border-left-color: #dcdfe3; border-left-width: 1px; border-right-color: #dcdfe3; border-right-width: 1px; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 10px 20px 5px;" bgcolor=#FFF align=left valign=top&gt;_x000D_ _x000D_ &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;Estimado (a): {NombreProveedor}&lt;/p&gt;_x000D_ _x000D_ &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;La empresa &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; lo ha invitado a participar de la siguiente cotización:&lt;/p&gt;_x000D_ _x000D_ &lt;ul&gt;_x000D_ &lt;li style="font-size: 0.9em; font-weight: 400; color: #3A5F84;"&gt;_x000D_ &lt;strong&gt;N° de Cotización:&lt;/strong&gt; {NumeroCotizacion}&lt;/li&gt;_x000D_ &lt;li style="font-size: 0.9em; font-weight: 400; color: #3A5F84;"&gt;_x000D_ &lt;strong&gt;Nombre de la cotización:&lt;/strong&gt; {NombreCotizacion}&lt;/li&gt;_x000D_ &lt;li style="font-size: 1em; font-weight: 600; color: #3A5F84;"&gt;_x000D_ &lt;strong&gt;Fecha de Cierre:&lt;/strong&gt; {FechaDeCierre}&lt;/li&gt;_x000D_ &lt;/ul&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 10px 20px 5px;" bgcolor=#FFF align=left valign=top&gt;_x000D_ &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;El detalle de los materiales a cotizar se encuentra en la siguiente tabla:&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ _x000D_ _x000D_ &lt;tr&gt;_x000D_ _x000D_ &lt;td style="text-align: center; color: #0d5369; font-family: Helvetica; font-size: 14px; line-height: 1.4em; overflow: hidden; letter-spacing: normal; padding-top: 0;" align=center&gt;_x000D_ &lt;table width=96% style="border-spacing: 0; border-collapse: collapse; margin: 0 auto;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td style="padding: 0;"&gt;_x000D_ {TablaMateriales}_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td valign=top style="color: #555; font-family: Helvetica; font-size: 14px; text-align: center; padding-top: 30px; overflow: hidden; letter-spacing: normal;" align=center&gt;_x000D_ &lt;a clicktracking=off href=https://redmat.iconstruye.com/ style="background-color: #F78E28; color: #fff; text-decoration: none; border-radius: 4px; font-size: 17px; font-weight: 400; line-height: 26px; display: inline-block; margin: 0 0 20px; padding: 16px 25px 15px;"&gt;Ingresa a ofertar&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 20px 20px 5px;" bgcolor=#FFF align=left valign=top&gt;_x000D_ &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;No deje pasar esta Oportunidad de hacer Negocios. Para mayor información, ingrese al módulo de Cotizaciones de nuestro sistema.&lt;/p&gt;_x000D_ &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;Atentamente&lt;br&gt;_x000D_ &lt;strong&gt;Equipo Redmat&lt;/strong&gt;&lt;br&gt;_x000D_ &lt;a clicktracking=off href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;br&gt;_x000D_ Mesa de Ayuda: +56 2 24861111&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt; _x000D_ &lt;/table&gt;_x000D_ _x000D_ _x000D_ &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center bgcolor=#fff style="border-left-style: solid; border-left-color: #dcdfe3; border-left-width: 1px; border-right-color: #dcdfe3; border-right-width: 1px; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td style="padding: 20px; border-top-width: 1px; border-top-color: #dcdfe3; border-top-style: solid; font-size: 11px; font-family: Helvetica; color: #666; background-color: #e9ecf0; border-bottom-width: 1px; border-bottom-style: solid; border-bottom-color: #dcdfe3;" bgcolor=#e9ecf0&gt;_x000D_ &lt;p&gt;Correo enviado a través de Redmat · Todos los Derechos Reservados&lt;/p&gt; _x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt; _x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt; _x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;','Invitación a los Proveedores para Participar en una Cotización Publicada.');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30131, 'Redmat','iconstruye@iconstruye.com', '{NombreEmpresaCompradora} te invita a participar de la cotización N° {NumeroCotizacion}', '&lt;!DOCTYPE html&gt;_x000D_ &lt;html xmlns=http://www.w3.org/1999/xhtml&gt;_x000D_ &lt;head&gt;_x000D_ _x000D_ &lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;_x000D_ _x000D_ &lt;title&gt;INVITACIÓN A COTIZAR EN REDMAT&lt;/title&gt;_x000D_ &lt;meta name=viewport content="width=device-width, initial-scale=1.0"&gt;_x000D_ &lt;/head&gt;_x000D_ _x000D_ &lt;body leftmargin=0 topmargin=0 marginwidth=0 marginheight=0 yahoo=fix style="font-family: Helvetica, sans-serif; color: #666666; width: 100%; -webkit-font-smoothing: antialiased; background-color: #f2f5f9; margin: 0; padding: 0;" bgcolor=#f2f5f9&gt;_x000D_ _x000D_ _x000D_ &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center style="border-collapse: collapse;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td width=100% valign=top bgcolor=#f2f5f9 style="padding: 20px 0;"&gt;_x000D_ _x000D_ _x000D_ &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center style="border-bottom-style: solid; border-bottom-color: #dcdfe3; border-bottom-width: 1px; border-left-width: 1px; border-left-color: #dcdfe3; border-left-style: solid; border-right-width: 1px; border-right-color: #dcdfe3; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td width=100% bgcolor=#ffffff style="border-top-width: 2px; border-top-color: #083F75; border-top-style: solid; padding: 10px 0;"&gt;_x000D_ &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png style="width: 100%;"&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ _x000D_ _x000D_ &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center bgcolor=#FFF style="border-left-style: solid; border-left-color: #dcdfe3; border-left-width: 1px; border-right-color: #dcdfe3; border-right-width: 1px; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 10px 20px 5px;" bgcolor=#FFF align=left valign=top&gt;_x000D_ _x000D_ &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;Estimado (a): {NombreProveedor}&lt;/p&gt;_x000D_ _x000D_ &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;La empresa &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; lo ha invitado a participar de la siguiente cotización:&lt;/p&gt;_x000D_ _x000D_ &lt;ul&gt;_x000D_ &lt;li style="font-size: 0.9em; font-weight: 400; color: #3A5F84;"&gt;_x000D_ &lt;strong&gt;N° de Cotización:&lt;/strong&gt; {NumeroCotizacion}&lt;/li&gt;_x000D_ &lt;li style="font-size: 0.9em; font-weight: 400; color: #3A5F84;"&gt;_x000D_ &lt;strong&gt;Nombre de la cotización:&lt;/strong&gt; {NombreCotizacion}&lt;/li&gt;_x000D_ &lt;li style="font-size: 1em; font-weight: 600; color: #3A5F84;"&gt;_x000D_ &lt;strong&gt;Fecha de Cierre:&lt;/strong&gt; {FechaDeCierre}&lt;/li&gt;_x000D_ &lt;/ul&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 10px 20px 5px;" bgcolor=#FFF align=left valign=top&gt;_x000D_ &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;El detalle de los materiales a cotizar se encuentra en la siguiente tabla:&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ _x000D_ _x000D_ &lt;tr&gt;_x000D_ _x000D_ &lt;td style="text-align: center; color: #0d5369; font-family: Helvetica; font-size: 14px; line-height: 1.4em; overflow: hidden; letter-spacing: normal; padding-top: 0;" align=center&gt;_x000D_ &lt;table width=96% style="border-spacing: 0; border-collapse: collapse; margin: 0 auto;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td style="padding: 0;"&gt;_x000D_ {TablaMateriales}_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td valign=top style="color: #555; font-family: Helvetica; font-size: 14px; text-align: center; padding-top: 30px; overflow: hidden; letter-spacing: normal;" align=center&gt;_x000D_ &lt;a clicktracking=off href=https://redmat.iconstruye.com/ style="background-color: #F78E28; color: #fff; text-decoration: none; border-radius: 4px; font-size: 17px; font-weight: 400; line-height: 26px; display: inline-block; margin: 0 0 20px; padding: 16px 25px 15px;"&gt;Ingresa a ofertar&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td style="color: #666; font-weight: normal; text-align: left; font-family: Helvetica, sans-serif; line-height: 24px; vertical-align: top; padding: 20px 20px 5px;" bgcolor=#FFF align=left valign=top&gt;_x000D_ &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;No deje pasar esta Oportunidad de hacer Negocios. Para mayor información, ingrese al módulo de Cotizaciones de nuestro sistema.&lt;/p&gt;_x000D_ &lt;p style="font-weight: 200; font-size: 14px; line-height: 1.7em; margin: 0 0 15px;"&gt;Atentamente&lt;br&gt;_x000D_ &lt;strong&gt;Equipo Redmat&lt;/strong&gt;&lt;br&gt;_x000D_ &lt;a clicktracking=off href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;br&gt;_x000D_ Mesa de Ayuda: +56 2 24861111&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt; _x000D_ &lt;/table&gt;_x000D_ _x000D_ _x000D_ &lt;table width=720 border=0 cellpadding=0 cellspacing=0 align=center bgcolor=#fff style="border-left-style: solid; border-left-color: #dcdfe3; border-left-width: 1px; border-right-color: #dcdfe3; border-right-width: 1px; border-right-style: solid; border-collapse: collapse; width: 780px !important; margin: 0 auto; padding: 0;"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td style="padding: 20px; border-top-width: 1px; border-top-color: #dcdfe3; border-top-style: solid; font-size: 11px; font-family: Helvetica; color: #666; background-color: #e9ecf0; border-bottom-width: 1px; border-bottom-style: solid; border-bottom-color: #dcdfe3;" bgcolor=#e9ecf0&gt;_x000D_ &lt;p&gt;Correo enviado a través de Redmat · Todos los Derechos Reservados&lt;/p&gt; _x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt; _x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt; _x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;','Invitación a los Proveedores para Participar en una Cotización Publicada.',131,3);</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>140</v>
       </c>
@@ -9017,15 +9028,15 @@
         <v>210</v>
       </c>
       <c r="S28" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20140, 'Agilice','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Sigro', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo iConstruye&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://sigro.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de iConstruye | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña portal Sigro');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20140, 'Agilice','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Sigro', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo iConstruye&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://sigro.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de iConstruye | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña portal Sigro',140,2);</v>
       </c>
       <c r="T28" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20140, 'Redmat','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Sigro', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo iConstruye&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://sigro.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de iConstruye | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña portal Sigro');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30140, 'Redmat','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Sigro', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo iConstruye&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://sigro.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de iConstruye | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña portal Sigro',140,3);</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>141</v>
       </c>
@@ -9081,15 +9092,15 @@
         <v>218</v>
       </c>
       <c r="S29" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20141, 'Agilice','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Besalco', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://besalco.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña portal Besalco');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20141, 'Agilice','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Besalco', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://besalco.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña portal Besalco',141,2);</v>
       </c>
       <c r="T29" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20141, 'Redmat','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Besalco', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://besalco.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña portal Besalco');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30141, 'Redmat','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Besalco', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://besalco.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña portal Besalco',141,3);</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>142</v>
       </c>
@@ -9145,15 +9156,15 @@
         <v>226</v>
       </c>
       <c r="S30" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20142, 'Agilice','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Icafal', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://icafal.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal Icafal');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20142, 'Agilice','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Icafal', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://icafal.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal Icafal',142,2);</v>
       </c>
       <c r="T30" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20142, 'Redmat','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Icafal', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://icafal.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal Icafal');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30142, 'Redmat','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de Icafal', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://icafal.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal Icafal',142,3);</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>18</v>
       </c>
@@ -9207,8 +9218,8 @@
         <v>232</v>
       </c>
       <c r="S31" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20018, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a &lt;nombsitio&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;_x000D_ &lt;title&gt;AGILICE&lt;/title&gt;_x000D_ &lt;style type=text/css&gt;* {margin: 0;font-family: "Helvetica Neue", Helvetica, Arial, sans-serif;box-sizing: border-box;font-size: 14px;}img {max-width: 100%;}body {-webkit-font-smoothing: antialiased;-webkit-text-size-adjust: none;width: 100% !important;height: 100%;line-height: 1.6em;}table td {vertical-align: top;}body {background-color: #f6f6f6;}.body-wrap {background-color: #f6f6f6;width: 100%;}.container {display: block !important;max-width: 600px !important;margin: 0 auto !important;clear: both !important;}.content {max-width: 600px;margin: 0 auto;display: block;padding: 20px;}.main {background-color: #fff;border-bottom: 2px solid #EAEAEA;border-radius: 3px;}.content-wrap {padding: 15px 20px;}.content-block {padding: 0 0 20px;}.header {width: 100%;margin-bottom: 20px;}.pre-footer {width: 100%;clear: both;color: #333;padding: 20px 0px;}.footer {width: 100%;clear: both;color: #999;padding: 15px;}.footer p, .footer a, .footer td {color: #999;font-size: 11px;}.resume-box {background: #FFF0E5;}h1, h2, h3 {color: #000;margin: 20px 0 0;line-height: 1.2em;font-weight: 400;}h1 {font-size: 20px;font-weight: 500;}h2 {font-size: 24px;}h3 {font-size: 18px;}h4 {font-size: 14px;font-weight: 600;}p, ul, ol {margin-bottom: 10px;font-weight: normal;}p li, ul li, ol li {margin-left: 5px;list-style-position: inside;line-height: 1.3em;}a {color: #348eda;text-decoration: underline;}.btn-primary {background:#0994FF; color:#fff !important; padding:10px 20px; text-decoration: none; border-radius:8px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight:bold;line-height: 23px;}.aligncenter {text-align: center;}.alignright {text-align: right;}.alignleft {text-align: left;}.clear {clear: both;}@media only screen and (max-width: 480px) {body {  padding: 0 !important;}h1, h2, h3, h4 { margin: 20px 0 5px !important;}h1 {  font-size: 22px !important;}h2 {  font-size: 18px !important;}h3 {  font-size: 16px !important;}.container {  padding: 0 !important;  width: 100% !important;}.content {  padding: 0 !important;}.content-wrap {  padding: 15px !important;}.mcnImage {max-width:100% !important;width:100% !important;} .img-app{margin-bottom: 10px;} table#banner td.w50{width: 50%;}a.button{width: 70px; margin-bottom: 10px;}span.sub-text{font-size: 16px;}}.sub-text{font-size: 18px;}a.button {_x000D_
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2018, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a &lt;nombsitio&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;_x000D_ &lt;title&gt;AGILICE&lt;/title&gt;_x000D_ &lt;style type=text/css&gt;* {margin: 0;font-family: "Helvetica Neue", Helvetica, Arial, sans-serif;box-sizing: border-box;font-size: 14px;}img {max-width: 100%;}body {-webkit-font-smoothing: antialiased;-webkit-text-size-adjust: none;width: 100% !important;height: 100%;line-height: 1.6em;}table td {vertical-align: top;}body {background-color: #f6f6f6;}.body-wrap {background-color: #f6f6f6;width: 100%;}.container {display: block !important;max-width: 600px !important;margin: 0 auto !important;clear: both !important;}.content {max-width: 600px;margin: 0 auto;display: block;padding: 20px;}.main {background-color: #fff;border-bottom: 2px solid #EAEAEA;border-radius: 3px;}.content-wrap {padding: 15px 20px;}.content-block {padding: 0 0 20px;}.header {width: 100%;margin-bottom: 20px;}.pre-footer {width: 100%;clear: both;color: #333;padding: 20px 0px;}.footer {width: 100%;clear: both;color: #999;padding: 15px;}.footer p, .footer a, .footer td {color: #999;font-size: 11px;}.resume-box {background: #FFF0E5;}h1, h2, h3 {color: #000;margin: 20px 0 0;line-height: 1.2em;font-weight: 400;}h1 {font-size: 20px;font-weight: 500;}h2 {font-size: 24px;}h3 {font-size: 18px;}h4 {font-size: 14px;font-weight: 600;}p, ul, ol {margin-bottom: 10px;font-weight: normal;}p li, ul li, ol li {margin-left: 5px;list-style-position: inside;line-height: 1.3em;}a {color: #348eda;text-decoration: underline;}.btn-primary {background:#0994FF; color:#fff !important; padding:10px 20px; text-decoration: none; border-radius:8px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight:bold;line-height: 23px;}.aligncenter {text-align: center;}.alignright {text-align: right;}.alignleft {text-align: left;}.clear {clear: both;}@media only screen and (max-width: 480px) {body {  padding: 0 !important;}h1, h2, h3, h4 { margin: 20px 0 5px !important;}h1 {  font-size: 22px !important;}h2 {  font-size: 18px !important;}h3 {  font-size: 16px !important;}.container {  padding: 0 !important;  width: 100% !important;}.content {  padding: 0 !important;}.content-wrap {  padding: 15px !important;}.mcnImage {max-width:100% !important;width:100% !important;} .img-app{margin-bottom: 10px;} table#banner td.w50{width: 50%;}a.button{width: 70px; margin-bottom: 10px;}span.sub-text{font-size: 16px;}}.sub-text{font-size: 18px;}a.button {_x000D_
     text-decoration: none;_x000D_
 }.img-app{border: 1px solid #00A7E1;_x000D_
     border-radius:8px;_x000D_
@@ -9216,11 +9227,11 @@
   	width:140px;_x000D_
   	height: auto;_x000D_
   	margin-right: 10px;_x000D_
-  	cursor: pointer;}&lt;/style&gt;_x000D_ &lt;/head&gt;_x000D_ &lt;body itemscope itemtype=http://schema.org/EmailMessage&gt;_x000D_ &lt;table class=body-wrap&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td&gt;&lt;/td&gt;_x000D_ &lt;td class=container width=600&gt;_x000D_ &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td&gt;_x000D_ &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td valign=top&gt;_x000D_ &lt;img align=center alt src=https://i.ibb.co/TcBfKbx/header-placeholder.png width=600 style="max-width: 600px;padding-bottom: 0;display: inline !important;vertical-align: bottom;border: 0;height: auto;outline: none;text-decoration: none;-ms-interpolation-mode: bicubic;" class=mcnImage&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;div class=content-wrap&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=content-block colspan=2&gt;_x000D_ &lt;h3&gt;¡Te damos la &lt;b style="font-size: 16px;"&gt;bienvenida a AGILICE!&lt;/b&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=content-block&gt;_x000D_ &lt;hr style="border-top: 1px solid #00A7E1;border-bottom: none;"&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td colspan=2&gt; _x000D_ &lt;p style=color:#000&gt;Hola &lt;b&gt;&lt;nombusuario&gt;&lt;/b&gt;,&lt;br&gt;tu cuenta de usuario para comenzar a operar en AGILICE ha sido creada con éxito. Estos son tus datos de registro:&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ _x000D_ &lt;div class="content-wrap resume-box"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td colspan=alignleft style="font-size: 16px;"&gt;_x000D_ &lt;span class=sub-text style="color: #00A7E1; font-weight: 700"&gt;Información de acceso&lt;/span&gt; &lt;br&gt;&lt;br&gt;_x000D_ &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Usuario:&lt;/b&gt; &lt;idusuario&gt;&lt;br&gt;&lt;/span&gt;_x000D_ &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Organización:&lt;/b&gt; &lt;nombempresa&gt;&lt;br&gt;&lt;/span&gt;_x000D_ &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Contraseña temporal:&lt;/b&gt; &lt;clave&gt;&lt;/span&gt;&lt;br&gt;&lt;br&gt;_x000D_ &lt;span style="font-size: 13px; color: #00A7E1;"&gt;Te recomendamos que al ingresar cambies tu contraseña&lt;/span&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ _x000D_ &lt;div class=content-wrap style="padding-top: 40px;"&gt;_x000D_ &lt;table width=100% cellspacing=0 cellpadding=0&gt;_x000D_ &lt;tr class=aligncenter&gt;_x000D_ &lt;td&gt;_x000D_ &lt;b style=color:#000&gt;¡Descubre todo lo que puedes hacer en el AGILICE y como mejoramos tu gestión!&lt;/b&gt;&lt;br&gt;&lt;br&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr class=aligncenter&gt;_x000D_ &lt;td&gt;_x000D_ &lt;a href=https://apps.agilice.com/index.html class=btn-primary&gt;Ingresa a AGILICE&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ _x000D_ &lt;div class=content-wrap&gt;_x000D_ &lt;table width=100% cellspacing=0 cellpadding=0&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=content-block&gt;&lt;p style=color:#000&gt;Saluda atentamente&lt;br&gt;&lt;b style=color:#000&gt;Equipo AGILICE &lt;br&gt;&lt;span style="color: #00A7E1;"&gt;AGILICE®&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;div class=pre-footer&gt;_x000D_ &lt;table id=banner width=100% style="background-color: #fff; padding: 15px 20px"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=w50&gt;_x000D_ &lt;p&gt;Ahora que posees una cuenta,&lt;br&gt;&lt;b&gt;descarga nuestra App mobile&lt;/b&gt;&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td class=alignright&gt;_x000D_ &lt;a href="https://play.google.com/store/apps/details?id=Agilice.Mobile&amp;hl=es_CL&amp;gl=US" target=_blank&gt;&lt;img align=center alt src=http://diseno.iconstruye.cl//mailing/templates/img/google-play.png width=100 class=img-app&gt;&lt;/a&gt;_x000D_ &lt;a href=https://apps.apple.com/cl/app/iconstruye/id1408881055 target=_blank&gt;&lt;img align=center alt src=http://diseno.iconstruye.cl//mailing/templates/img/app-store.png class=img-app&gt;&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ &lt;div class=footer&gt;_x000D_ &lt;table width=100%&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="aligncenter content-block"&gt;_x000D_ &lt;em style="font-size: 12px !important;"&gt;Correo enviado a través de &lt;a href="https://apps.agilice.com/index.html?ReturnUrl=%2fincludes%2fdefault.aspx" style="color: #00A7E1;"&gt;AGILICE&lt;/a&gt;®&amp;nbsp;·_x000D_ Copyright ©&amp;nbsp; Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;','Usuario Ingreso');</v>
+  	cursor: pointer;}&lt;/style&gt;_x000D_ &lt;/head&gt;_x000D_ &lt;body itemscope itemtype=http://schema.org/EmailMessage&gt;_x000D_ &lt;table class=body-wrap&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td&gt;&lt;/td&gt;_x000D_ &lt;td class=container width=600&gt;_x000D_ &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td&gt;_x000D_ &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td valign=top&gt;_x000D_ &lt;img align=center alt src=https://i.ibb.co/TcBfKbx/header-placeholder.png width=600 style="max-width: 600px;padding-bottom: 0;display: inline !important;vertical-align: bottom;border: 0;height: auto;outline: none;text-decoration: none;-ms-interpolation-mode: bicubic;" class=mcnImage&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;div class=content-wrap&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=content-block colspan=2&gt;_x000D_ &lt;h3&gt;¡Te damos la &lt;b style="font-size: 16px;"&gt;bienvenida a AGILICE!&lt;/b&gt;&lt;/h3&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=content-block&gt;_x000D_ &lt;hr style="border-top: 1px solid #00A7E1;border-bottom: none;"&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td colspan=2&gt; _x000D_ &lt;p style=color:#000&gt;Hola &lt;b&gt;&lt;nombusuario&gt;&lt;/b&gt;,&lt;br&gt;tu cuenta de usuario para comenzar a operar en AGILICE ha sido creada con éxito. Estos son tus datos de registro:&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ _x000D_ &lt;div class="content-wrap resume-box"&gt;_x000D_ &lt;table width=100% cellpadding=0 cellspacing=0&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td colspan=alignleft style="font-size: 16px;"&gt;_x000D_ &lt;span class=sub-text style="color: #00A7E1; font-weight: 700"&gt;Información de acceso&lt;/span&gt; &lt;br&gt;&lt;br&gt;_x000D_ &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Usuario:&lt;/b&gt; &lt;idusuario&gt;&lt;br&gt;&lt;/span&gt;_x000D_ &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Organización:&lt;/b&gt; &lt;nombempresa&gt;&lt;br&gt;&lt;/span&gt;_x000D_ &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Contraseña temporal:&lt;/b&gt; &lt;clave&gt;&lt;/span&gt;&lt;br&gt;&lt;br&gt;_x000D_ &lt;span style="font-size: 13px; color: #00A7E1;"&gt;Te recomendamos que al ingresar cambies tu contraseña&lt;/span&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ _x000D_ &lt;div class=content-wrap style="padding-top: 40px;"&gt;_x000D_ &lt;table width=100% cellspacing=0 cellpadding=0&gt;_x000D_ &lt;tr class=aligncenter&gt;_x000D_ &lt;td&gt;_x000D_ &lt;b style=color:#000&gt;¡Descubre todo lo que puedes hacer en el AGILICE y como mejoramos tu gestión!&lt;/b&gt;&lt;br&gt;&lt;br&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;tr class=aligncenter&gt;_x000D_ &lt;td&gt;_x000D_ &lt;a href=https://apps.agilice.com/index.html class=btn-primary&gt;Ingresa a AGILICE&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ _x000D_ &lt;div class=content-wrap&gt;_x000D_ &lt;table width=100% cellspacing=0 cellpadding=0&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=content-block&gt;&lt;p style=color:#000&gt;Saluda atentamente&lt;br&gt;&lt;b style=color:#000&gt;Equipo AGILICE &lt;br&gt;&lt;span style="color: #00A7E1;"&gt;AGILICE®&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;div class=pre-footer&gt;_x000D_ &lt;table id=banner width=100% style="background-color: #fff; padding: 15px 20px"&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class=w50&gt;_x000D_ &lt;p&gt;Ahora que posees una cuenta,&lt;br&gt;&lt;b&gt;descarga nuestra App mobile&lt;/b&gt;&lt;/p&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td class=alignright&gt;_x000D_ &lt;a href="https://play.google.com/store/apps/details?id=Agilice.Mobile&amp;hl=es_CL&amp;gl=US" target=_blank&gt;&lt;img align=center alt src=http://diseno.iconstruye.cl//mailing/templates/img/google-play.png width=100 class=img-app&gt;&lt;/a&gt;_x000D_ &lt;a href=https://apps.apple.com/cl/app/iconstruye/id1408881055 target=_blank&gt;&lt;img align=center alt src=http://diseno.iconstruye.cl//mailing/templates/img/app-store.png class=img-app&gt;&lt;/a&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ &lt;div class=footer&gt;_x000D_ &lt;table width=100%&gt;_x000D_ &lt;tr&gt;_x000D_ &lt;td class="aligncenter content-block"&gt;_x000D_ &lt;em style="font-size: 12px !important;"&gt;Correo enviado a través de &lt;a href="https://apps.agilice.com/index.html?ReturnUrl=%2fincludes%2fdefault.aspx" style="color: #00A7E1;"&gt;AGILICE&lt;/a&gt;®&amp;nbsp;·_x000D_ Copyright ©&amp;nbsp; Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/div&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;td&gt;_x000D_ &lt;/td&gt;_x000D_ &lt;/tr&gt;_x000D_ &lt;/table&gt;_x000D_ &lt;/body&gt;_x000D_ &lt;/html&gt;','Usuario Ingreso',18,2);</v>
       </c>
       <c r="T31" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20018, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a &lt;nombsitio&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;REDMAT&lt;/title&gt;&lt;style type=text/css&gt;* {margin: 0;font-family: "Helvetica Neue", Helvetica, Arial, sans-serif;box-sizing: border-box;font-size: 14px;}img {max-width: 100%;}body {-webkit-font-smoothing: antialiased;-webkit-text-size-adjust: none;width: 100% !important;height: 100%;line-height: 1.6em;}table td {vertical-align: top;}body {background-color: #f6f6f6;}.body-wrap {background-color: #f6f6f6;width: 100%;}.container {display: block !important;max-width: 600px !important;margin: 0 auto !important;clear: both !important;}.content {max-width: 600px;margin: 0 auto;display: block;padding: 20px;}.main {background-color: #fff;border-bottom: 2px solid #EAEAEA;border-radius: 3px;}.content-wrap {padding: 15px 20px;}.content-block {padding: 0 0 20px;}.header {width: 100%;margin-bottom: 20px;}.pre-footer {width: 100%;clear: both;color: #333;padding: 20px 0px;}.footer {width: 100%;clear: both;color: #999;padding: 15px;}.footer p, .footer a, .footer td {color: #999;font-size: 11px;}.resume-box {background: #FFF0E5;}h1, h2, h3 {color: #000;margin: 20px 0 0;line-height: 1.2em;font-weight: 400;}h1 {font-size: 20px;font-weight: 500;}h2 {font-size: 24px;}h3 {font-size: 18px;}h4 {font-size: 14px;font-weight: 600;}p, ul, ol {margin-bottom: 10px;font-weight: normal;}p li, ul li, ol li {margin-left: 5px;list-style-position: inside;line-height: 1.3em;}a {color: #F78E28;text-decoration: underline;}.btn-primary {background:#F78E28; color:#fff !important; padding:10px 20px; text-decoration: none; border-radius:8px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight:bold;line-height: 23px;}.aligncenter {text-align: center;}.alignright {text-align: right;}.alignleft {text-align: left;}.clear {clear: both;}@media only screen and (max-width: 480px) {body {  padding: 0 !important;}h1, h2, h3, h4 { margin: 20px 0 5px !important;}h1 {  font-size: 22px !important;}h2 {  font-size: 18px !important;}h3 {  font-size: 16px !important;}.container {  padding: 0 !important;  width: 100% !important;}.content {  padding: 0 !important;}.content-wrap {  padding: 15px !important;}.mcnImage {max-width:100% !important;width:100% !important;} .img-app{margin-bottom: 10px;} table#banner td.w50{width: 50%;}a.button{width: 70px; margin-bottom: 10px;}span.sub-text{font-size: 16px;}}.sub-text{font-size: 18px;}a.button {
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3018, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a &lt;nombsitio&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;REDMAT&lt;/title&gt;&lt;style type=text/css&gt;* {margin: 0;font-family: "Helvetica Neue", Helvetica, Arial, sans-serif;box-sizing: border-box;font-size: 14px;}img {max-width: 100%;}body {-webkit-font-smoothing: antialiased;-webkit-text-size-adjust: none;width: 100% !important;height: 100%;line-height: 1.6em;}table td {vertical-align: top;}body {background-color: #f6f6f6;}.body-wrap {background-color: #f6f6f6;width: 100%;}.container {display: block !important;max-width: 600px !important;margin: 0 auto !important;clear: both !important;}.content {max-width: 600px;margin: 0 auto;display: block;padding: 20px;}.main {background-color: #fff;border-bottom: 2px solid #EAEAEA;border-radius: 3px;}.content-wrap {padding: 15px 20px;}.content-block {padding: 0 0 20px;}.header {width: 100%;margin-bottom: 20px;}.pre-footer {width: 100%;clear: both;color: #333;padding: 20px 0px;}.footer {width: 100%;clear: both;color: #999;padding: 15px;}.footer p, .footer a, .footer td {color: #999;font-size: 11px;}.resume-box {background: #FFF0E5;}h1, h2, h3 {color: #000;margin: 20px 0 0;line-height: 1.2em;font-weight: 400;}h1 {font-size: 20px;font-weight: 500;}h2 {font-size: 24px;}h3 {font-size: 18px;}h4 {font-size: 14px;font-weight: 600;}p, ul, ol {margin-bottom: 10px;font-weight: normal;}p li, ul li, ol li {margin-left: 5px;list-style-position: inside;line-height: 1.3em;}a {color: #F78E28;text-decoration: underline;}.btn-primary {background:#F78E28; color:#fff !important; padding:10px 20px; text-decoration: none; border-radius:8px; margin: 10px 0;display:inline-block;font-size: 1.1em;font-weight:bold;line-height: 23px;}.aligncenter {text-align: center;}.alignright {text-align: right;}.alignleft {text-align: left;}.clear {clear: both;}@media only screen and (max-width: 480px) {body {  padding: 0 !important;}h1, h2, h3, h4 { margin: 20px 0 5px !important;}h1 {  font-size: 22px !important;}h2 {  font-size: 18px !important;}h3 {  font-size: 16px !important;}.container {  padding: 0 !important;  width: 100% !important;}.content {  padding: 0 !important;}.content-wrap {  padding: 15px !important;}.mcnImage {max-width:100% !important;width:100% !important;} .img-app{margin-bottom: 10px;} table#banner td.w50{width: 50%;}a.button{width: 70px; margin-bottom: 10px;}span.sub-text{font-size: 16px;}}.sub-text{font-size: 18px;}a.button {
     text-decoration: none;
 }.img-app{border: 1px solid #083F75;
     border-radius:8px;
@@ -9228,10 +9239,10 @@
   	width:140px;
   	height: auto;
   	margin-right: 10px;
-  	cursor: pointer;}&lt;/style&gt;&lt;/head&gt; &lt;body itemscope itemtype=http://schema.org/EmailMessage&gt; &lt;table class=body-wrap&gt; &lt;tr&gt; &lt;td&gt;&lt;/td&gt; &lt;td class=container width=600&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td valign=top&gt; &lt;img align=center alt src=https://i.ibb.co/TcBfKbx/header-placeholder.png width=600 style="max-width: 600px;padding-bottom: 0;display: inline !important;vertical-align: bottom;border: 0;height: auto;outline: none;text-decoration: none;-ms-interpolation-mode: bicubic;" class=mcnImage&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td class=content-block colspan=2&gt; &lt;h3&gt;¡Te damos la &lt;b style="font-size: 16px;"&gt;bienvenida a REDMAT!&lt;/b&gt;&lt;/h3&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td class=content-block&gt; &lt;hr style="border-top: 1px solid #083F75;border-bottom: none;"&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td colspan=2&gt; &lt;p style=color:#000&gt;Hola &lt;b&gt;&lt;nombusuario&gt;&lt;/b&gt;,&lt;br&gt;tu cuenta de usuario para comenzar a operar en REDMAT ha sido creada con éxito. Estos son tus datos de registro:&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div class="content-wrap resume-box"&gt; &lt;table width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td colspan=alignleft style="font-size: 16px;"&gt; &lt;span class=sub-text style="color: #083F75; font-weight: 700"&gt;Información de acceso&lt;/span&gt; &lt;br&gt;&lt;br&gt; &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Usuario:&lt;/b&gt; &lt;idusuario&gt;&lt;br&gt;&lt;/span&gt; &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Organización:&lt;/b&gt; &lt;nombempresa&gt;&lt;br&gt;&lt;/span&gt; &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Contraseña temporal:&lt;/b&gt; &lt;clave&gt;&lt;/span&gt;&lt;br&gt;&lt;br&gt; &lt;span style="font-size: 13px; color: #083F75;"&gt;Te recomendamos que al ingresar cambies tu contraseña&lt;/span&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div class=content-wrap style="padding-top: 40px;"&gt; &lt;table width=100% cellspacing=0 cellpadding=0&gt; &lt;tr class=aligncenter&gt; &lt;td&gt; &lt;b style=color:#000&gt;¡Descubre todo lo que puedes hacer en el REDMAT y como mejoramos tu gestión!&lt;/b&gt;&lt;br&gt;&lt;br&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr class=aligncenter&gt; &lt;td&gt; &lt;a href=https://redmat.iconstruye.com class=btn-primary&gt;Ingresa a REDMAT&lt;/a&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellspacing=0 cellpadding=0&gt; &lt;tr&gt; &lt;td class=content-block&gt;&lt;p style=color:#000&gt;Saluda atentamente&lt;br&gt;&lt;b style=color:#000&gt;Equipo REDMAT &lt;br&gt;&lt;span style="color: #083F75;"&gt;REDMAT®&lt;/span&gt;&lt;/b&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=footer&gt; &lt;table width=100%&gt; &lt;tr&gt; &lt;td class="aligncenter content-block"&gt; &lt;em style="font-size: 12px !important;"&gt;Correo enviado a través de &lt;a href="https://redmat.iconstruye.com/index.html?ReturnUrl=%2fincludes%2fdefault.aspx" style="color: #083F75;"&gt;REDMAT&lt;/a&gt;®&amp;nbsp;· Copyright ©&amp;nbsp; Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;td&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/body&gt; &lt;/html&gt;','Usuario Ingreso');</v>
+  	cursor: pointer;}&lt;/style&gt;&lt;/head&gt; &lt;body itemscope itemtype=http://schema.org/EmailMessage&gt; &lt;table class=body-wrap&gt; &lt;tr&gt; &lt;td&gt;&lt;/td&gt; &lt;td class=container width=600&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td&gt; &lt;table class=main width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td valign=top&gt; &lt;img align=center alt src=https://i.ibb.co/TcBfKbx/header-placeholder.png width=600 style="max-width: 600px;padding-bottom: 0;display: inline !important;vertical-align: bottom;border: 0;height: auto;outline: none;text-decoration: none;-ms-interpolation-mode: bicubic;" class=mcnImage&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td class=content-block colspan=2&gt; &lt;h3&gt;¡Te damos la &lt;b style="font-size: 16px;"&gt;bienvenida a REDMAT!&lt;/b&gt;&lt;/h3&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td class=content-block&gt; &lt;hr style="border-top: 1px solid #083F75;border-bottom: none;"&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;td colspan=2&gt; &lt;p style=color:#000&gt;Hola &lt;b&gt;&lt;nombusuario&gt;&lt;/b&gt;,&lt;br&gt;tu cuenta de usuario para comenzar a operar en REDMAT ha sido creada con éxito. Estos son tus datos de registro:&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div class="content-wrap resume-box"&gt; &lt;table width=100% cellpadding=0 cellspacing=0&gt; &lt;tr&gt; &lt;td colspan=alignleft style="font-size: 16px;"&gt; &lt;span class=sub-text style="color: #083F75; font-weight: 700"&gt;Información de acceso&lt;/span&gt; &lt;br&gt;&lt;br&gt; &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Usuario:&lt;/b&gt; &lt;idusuario&gt;&lt;br&gt;&lt;/span&gt; &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Organización:&lt;/b&gt; &lt;nombempresa&gt;&lt;br&gt;&lt;/span&gt; &lt;span class=text-notorious style=color:#000&gt;&lt;b&gt;Contraseña temporal:&lt;/b&gt; &lt;clave&gt;&lt;/span&gt;&lt;br&gt;&lt;br&gt; &lt;span style="font-size: 13px; color: #083F75;"&gt;Te recomendamos que al ingresar cambies tu contraseña&lt;/span&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div class=content-wrap style="padding-top: 40px;"&gt; &lt;table width=100% cellspacing=0 cellpadding=0&gt; &lt;tr class=aligncenter&gt; &lt;td&gt; &lt;b style=color:#000&gt;¡Descubre todo lo que puedes hacer en el REDMAT y como mejoramos tu gestión!&lt;/b&gt;&lt;br&gt;&lt;br&gt; &lt;/td&gt; &lt;/tr&gt; &lt;tr class=aligncenter&gt; &lt;td&gt; &lt;a href=https://redmat.iconstruye.com class=btn-primary&gt;Ingresa a REDMAT&lt;/a&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div class=content-wrap&gt; &lt;table width=100% cellspacing=0 cellpadding=0&gt; &lt;tr&gt; &lt;td class=content-block&gt;&lt;p style=color:#000&gt;Saluda atentamente&lt;br&gt;&lt;b style=color:#000&gt;Equipo REDMAT &lt;br&gt;&lt;span style="color: #083F75;"&gt;REDMAT®&lt;/span&gt;&lt;/b&gt;&lt;/p&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;div class=footer&gt; &lt;table width=100%&gt; &lt;tr&gt; &lt;td class="aligncenter content-block"&gt; &lt;em style="font-size: 12px !important;"&gt;Correo enviado a través de &lt;a href="https://redmat.iconstruye.com/index.html?ReturnUrl=%2fincludes%2fdefault.aspx" style="color: #083F75;"&gt;REDMAT&lt;/a&gt;®&amp;nbsp;· Copyright ©&amp;nbsp; Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;/td&gt; &lt;td&gt; &lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/body&gt; &lt;/html&gt;','Usuario Ingreso',18,3);</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>26</v>
       </c>
@@ -9285,15 +9296,15 @@
         <v>239</v>
       </c>
       <c r="S32" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20026, 'Agilice','iconstruye@iconstruye.com', 'Aviso de Modificación de Cotización', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarles, informamos a usted que la empresa &lt;nombempresa&gt; ha modificado la fecha de cierre de la Cotización &lt;numcz&gt;, &lt;nomcz&gt;. &lt;br&gt;Rogamos a usted tomar nota: &lt;br&gt;&lt;br&gt;Nueva Fecha de Cierre: &lt;fechacierre&gt;&lt;br&gt;Recomendamos revisar más antecedentes en el Módulo Cotizaciones.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cotizaciones, Modificación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2026, 'Agilice','iconstruye@iconstruye.com', 'Aviso de Modificación de Cotización', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarles, informamos a usted que la empresa &lt;nombempresa&gt; ha modificado la fecha de cierre de la Cotización &lt;numcz&gt;, &lt;nomcz&gt;. &lt;br&gt;Rogamos a usted tomar nota: &lt;br&gt;&lt;br&gt;Nueva Fecha de Cierre: &lt;fechacierre&gt;&lt;br&gt;Recomendamos revisar más antecedentes en el Módulo Cotizaciones.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cotizaciones, Modificación',26,2);</v>
       </c>
       <c r="T32" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20026, 'Redmat','iconstruye@iconstruye.com', 'Aviso de Modificación de Cotización', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarles, informamos a usted que la empresa &lt;nombempresa&gt; ha modificado la fecha de cierre de la Cotización &lt;numcz&gt;, &lt;nomcz&gt;. &lt;br&gt;Rogamos a usted tomar nota: &lt;br&gt;&lt;br&gt;Nueva Fecha de Cierre: &lt;fechacierre&gt;&lt;br&gt;Recomendamos revisar más antecedentes en el Módulo Cotizaciones.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cotizaciones, Modificación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3026, 'Redmat','iconstruye@iconstruye.com', 'Aviso de Modificación de Cotización', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarles, informamos a usted que la empresa &lt;nombempresa&gt; ha modificado la fecha de cierre de la Cotización &lt;numcz&gt;, &lt;nomcz&gt;. &lt;br&gt;Rogamos a usted tomar nota: &lt;br&gt;&lt;br&gt;Nueva Fecha de Cierre: &lt;fechacierre&gt;&lt;br&gt;Recomendamos revisar más antecedentes en el Módulo Cotizaciones.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cotizaciones, Modificación',26,3);</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>34</v>
       </c>
@@ -9347,15 +9358,15 @@
         <v>246</v>
       </c>
       <c r="S33" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20034, 'Agilice','iconstruye@iconstruye.com', 'Cancelación de Orden de Compra', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Cancelación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2034, 'Agilice','iconstruye@iconstruye.com', 'Cancelación de Orden de Compra', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Cancelación',34,2);</v>
       </c>
       <c r="T33" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20034, 'Redmat','iconstruye@iconstruye.com', 'Cancelación de Orden de Compra', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Cancelación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3034, 'Redmat','iconstruye@iconstruye.com', 'Cancelación de Orden de Compra', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Cancelación',34,3);</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>35</v>
       </c>
@@ -9409,15 +9420,15 @@
         <v>253</v>
       </c>
       <c r="S34" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20035, 'Agilice','iconstruye@iconstruye.com', 'Orden de compra no aceptada', 'Estimados Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; No ha Aceptado su Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más información, ingrese al módulo Compras.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, No Aceptada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2035, 'Agilice','iconstruye@iconstruye.com', 'Orden de compra no aceptada', 'Estimados Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; No ha Aceptado su Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más información, ingrese al módulo Compras.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, No Aceptada',35,2);</v>
       </c>
       <c r="T34" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20035, 'Redmat','iconstruye@iconstruye.com', 'Orden de compra no aceptada', 'Estimados Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; No ha Aceptado su Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más información, ingrese al módulo Compras.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, No Aceptada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3035, 'Redmat','iconstruye@iconstruye.com', 'Orden de compra no aceptada', 'Estimados Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; No ha Aceptado su Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más información, ingrese al módulo Compras.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, No Aceptada',35,3);</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>36</v>
       </c>
@@ -9471,15 +9482,15 @@
         <v>260</v>
       </c>
       <c r="S35" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20036, 'Agilice','iconstruye@iconstruye.com', 'Orden de Compra aceptada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;&lt;br&gt; Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha aceptado su Orden de Compra Nº&lt;numoc&gt;, &lt;nomoc&gt;, del Centro de Gestión &lt;nomborgc&gt;.&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt; Equipo Agilice&lt;br&gt;&lt;br&gt; &lt;link&gt;&lt;br&gt;&lt;br&gt; Mesa de Ayuda&lt;br&gt;&lt;br&gt; 486 11 11','Orden de Compra, Aceptada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2036, 'Agilice','iconstruye@iconstruye.com', 'Orden de Compra aceptada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;&lt;br&gt; Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha aceptado su Orden de Compra Nº&lt;numoc&gt;, &lt;nomoc&gt;, del Centro de Gestión &lt;nomborgc&gt;.&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt; Equipo Agilice&lt;br&gt;&lt;br&gt; &lt;link&gt;&lt;br&gt;&lt;br&gt; Mesa de Ayuda&lt;br&gt;&lt;br&gt; 486 11 11','Orden de Compra, Aceptada',36,2);</v>
       </c>
       <c r="T35" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20036, 'Redmat','iconstruye@iconstruye.com', 'Orden de Compra aceptada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;&lt;br&gt; Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha aceptado su Orden de Compra Nº&lt;numoc&gt;, &lt;nomoc&gt;, del Centro de Gestión &lt;nomborgc&gt;.&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt; Equipo Redmat&lt;br&gt;&lt;br&gt; &lt;link&gt;&lt;br&gt;&lt;br&gt; Mesa de Ayuda&lt;br&gt;&lt;br&gt; 486 11 11','Orden de Compra, Aceptada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3036, 'Redmat','iconstruye@iconstruye.com', 'Orden de Compra aceptada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;&lt;br&gt; Junto con saludarle, informamos a usted que la empresa &lt;nombproveedor&gt; ha aceptado su Orden de Compra Nº&lt;numoc&gt;, &lt;nomoc&gt;, del Centro de Gestión &lt;nomborgc&gt;.&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt; Equipo Redmat&lt;br&gt;&lt;br&gt; &lt;link&gt;&lt;br&gt;&lt;br&gt; Mesa de Ayuda&lt;br&gt;&lt;br&gt; 486 11 11','Orden de Compra, Aceptada',36,3);</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>37</v>
       </c>
@@ -9533,15 +9544,15 @@
         <v>267</v>
       </c>
       <c r="S36" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20037, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de cancelación de Orden de Compra', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; ha Solicitado a usted la Cancelación de la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo de Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Solicitud Cancelación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2037, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de cancelación de Orden de Compra', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; ha Solicitado a usted la Cancelación de la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo de Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Solicitud Cancelación',37,2);</v>
       </c>
       <c r="T36" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20037, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de cancelación de Orden de Compra', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; ha Solicitado a usted la Cancelación de la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo de Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Solicitud Cancelación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3037, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de cancelación de Orden de Compra', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; ha Solicitado a usted la Cancelación de la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo de Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Solicitud Cancelación',37,3);</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>40</v>
       </c>
@@ -9595,15 +9606,15 @@
         <v>274</v>
       </c>
       <c r="S37" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20040, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Materiales en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en su Lista de Administración.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborg&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Envío a Administración');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2040, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Materiales en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en su Lista de Administración.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborg&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Envío a Administración',40,2);</v>
       </c>
       <c r="T37" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20040, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Materiales en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en su Lista de Administración.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborg&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Envío a Administración');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3040, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Materiales en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en su Lista de Administración.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborg&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Envío a Administración',40,3);</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>41</v>
       </c>
@@ -9657,15 +9668,15 @@
         <v>281</v>
       </c>
       <c r="S38" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20041, 'Agilice','iconstruye@iconstruye.com', 'Notificación de Aprobación de Pedido de Materiales', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Pedido de Materiales generado por usted ha sido Aprobado.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Aprobación: &lt;fechaaprobacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Notifica Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2041, 'Agilice','iconstruye@iconstruye.com', 'Notificación de Aprobación de Pedido de Materiales', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Pedido de Materiales generado por usted ha sido Aprobado.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Aprobación: &lt;fechaaprobacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Notifica Aprobación',41,2);</v>
       </c>
       <c r="T38" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20041, 'Redmat','iconstruye@iconstruye.com', 'Notificación de Aprobación de Pedido de Materiales', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Pedido de Materiales generado por usted ha sido Aprobado.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Aprobación: &lt;fechaaprobacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Notifica Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3041, 'Redmat','iconstruye@iconstruye.com', 'Notificación de Aprobación de Pedido de Materiales', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Pedido de Materiales generado por usted ha sido Aprobado.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Aprobación: &lt;fechaaprobacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Notifica Aprobación',41,3);</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>42</v>
       </c>
@@ -9719,15 +9730,15 @@
         <v>288</v>
       </c>
       <c r="S39" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20042, 'Agilice','iconstruye@iconstruye.com', 'Envío de Orden de Compra a Proveedor No Integrado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;, deberá ser enviada por fax, ya que la empresa &lt;nombproveedor&gt; es un proveedor No Integrado, vale decir, no tiene contratados los servicios de Agilice y no podrá ver la OC por sistema. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Aviso PNI');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2042, 'Agilice','iconstruye@iconstruye.com', 'Envío de Orden de Compra a Proveedor No Integrado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;, deberá ser enviada por fax, ya que la empresa &lt;nombproveedor&gt; es un proveedor No Integrado, vale decir, no tiene contratados los servicios de Agilice y no podrá ver la OC por sistema. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Aviso PNI',42,2);</v>
       </c>
       <c r="T39" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20042, 'Redmat','iconstruye@iconstruye.com', 'Envío de Orden de Compra a Proveedor No Integrado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;, deberá ser enviada por fax, ya que la empresa &lt;nombproveedor&gt; es un proveedor No Integrado, vale decir, no tiene contratados los servicios de Redmat y no podrá ver la OC por sistema. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Aviso PNI');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3042, 'Redmat','iconstruye@iconstruye.com', 'Envío de Orden de Compra a Proveedor No Integrado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;, deberá ser enviada por fax, ya que la empresa &lt;nombproveedor&gt; es un proveedor No Integrado, vale decir, no tiene contratados los servicios de Redmat y no podrá ver la OC por sistema. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Aviso PNI',42,3);</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>43</v>
       </c>
@@ -9781,15 +9792,15 @@
         <v>295</v>
       </c>
       <c r="S40" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20043, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Materiales &lt;numpm&gt; Rechazado', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Materiales ha sido Rechazado.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Notifica Rechazo');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2043, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Materiales &lt;numpm&gt; Rechazado', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Materiales ha sido Rechazado.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Notifica Rechazo',43,2);</v>
       </c>
       <c r="T40" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20043, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Materiales &lt;numpm&gt; Rechazado', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Materiales ha sido Rechazado.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Notifica Rechazo');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3043, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Materiales &lt;numpm&gt; Rechazado', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Materiales ha sido Rechazado.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Notifica Rechazo',43,3);</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>44</v>
       </c>
@@ -9843,15 +9854,15 @@
         <v>302</v>
       </c>
       <c r="S41" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20044, 'Agilice','iconstruye@iconstruye.com', 'Pedido en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en su Lista de Administración.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborg&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Notifica Super Administrador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2044, 'Agilice','iconstruye@iconstruye.com', 'Pedido en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en su Lista de Administración.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborg&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Notifica Super Administrador',44,2);</v>
       </c>
       <c r="T41" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20044, 'Redmat','iconstruye@iconstruye.com', 'Pedido en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en su Lista de Administración.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborg&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Notifica Super Administrador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3044, 'Redmat','iconstruye@iconstruye.com', 'Pedido en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en su Lista de Administración.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborg&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Notifica Super Administrador',44,3);</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>45</v>
       </c>
@@ -9905,15 +9916,15 @@
         <v>309</v>
       </c>
       <c r="S42" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20045, 'Agilice','iconstruye@iconstruye.com', 'Asignación de Pedido de Materiales', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que le ha sido Asignado un nuevo Pedido de Materiales.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Asignación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2045, 'Agilice','iconstruye@iconstruye.com', 'Asignación de Pedido de Materiales', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que le ha sido Asignado un nuevo Pedido de Materiales.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Asignación',45,2);</v>
       </c>
       <c r="T42" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20045, 'Redmat','iconstruye@iconstruye.com', 'Asignación de Pedido de Materiales', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que le ha sido Asignado un nuevo Pedido de Materiales.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Asignación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3045, 'Redmat','iconstruye@iconstruye.com', 'Asignación de Pedido de Materiales', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que le ha sido Asignado un nuevo Pedido de Materiales.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Asignación',45,3);</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>47</v>
       </c>
@@ -9967,15 +9978,15 @@
         <v>316</v>
       </c>
       <c r="S43" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20047, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Solicitud de Regularización', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Regularización a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº Regularización: &lt;numrg&gt;&lt;br&gt;Nombre: &lt;nombreg&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;Para gestionar este documento, ingrese al módulo de Regularizaciones&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Solicitud de Regularización, Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2047, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Solicitud de Regularización', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Regularización a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº Regularización: &lt;numrg&gt;&lt;br&gt;Nombre: &lt;nombreg&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;Para gestionar este documento, ingrese al módulo de Regularizaciones&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Solicitud de Regularización, Envío a Aprobación',47,2);</v>
       </c>
       <c r="T43" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20047, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Solicitud de Regularización', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Regularización a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº Regularización: &lt;numrg&gt;&lt;br&gt;Nombre: &lt;nombreg&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;Para gestionar este documento, ingrese al módulo de Regularizaciones&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Solicitud de Regularización, Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3047, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Solicitud de Regularización', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Regularización a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº Regularización: &lt;numrg&gt;&lt;br&gt;Nombre: &lt;nombreg&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;Para gestionar este documento, ingrese al módulo de Regularizaciones&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Solicitud de Regularización, Envío a Aprobación',47,3);</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>48</v>
       </c>
@@ -10031,8 +10042,8 @@
         <v>324</v>
       </c>
       <c r="S44" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20048, 'Agilice','iconstruye@iconstruye.com', 'Factura en Espera de Aprobación', '&lt;!DOCTYPE html
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2048, 'Agilice','iconstruye@iconstruye.com', 'Factura en Espera de Aprobación', '&lt;!DOCTYPE html
 PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;AGILICE&lt;/title&gt;&lt;style type=text/css&gt;*{
 margin: 0;
 font-family: "Helvetica Neue", Helvetica, Arial, sans-serif;
@@ -10153,11 +10164,11 @@
 width: 100% !important;} .mcnImage{
 max-width: 100% !important;
 width: 100% !important;}}
-&lt;/style&gt;&lt;/head&gt;&lt;body itemscope itemtype=http://schema.org/EmailMessage&gt;&lt;table class=body-wrap&gt;&lt;tr&gt;&lt;td&gt;&lt;/td&gt;&lt;td class=container width=600&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td valign=top&gt;&lt;img align=center alt src=https://cl.iconstruye.com/images/banner-generico.jpg width=600 class=mcnImage&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Factura en espera de aprobación&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block colspan=2&gt;&lt;p&gt;Hola &lt;strong&gt;&lt;nombaprobador&gt;&lt;/strong&gt;,&lt;br&gt;Junto con saludar le informamos que tiene una nueva factura a la espera de aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo Aprobación: Supera el monto del comprador &lt;br&gt;&lt;br&gt;Recuerde que puede aprobar desde la APP de &lt;a href=https://apps.agilice.com&gt;AGILICE.com&lt;/a&gt;&lt;br&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;table width=100% cellspacing=0 cellpadding=0 class=resume-box&gt;&lt;tr&gt;&lt;td&gt;&lt;div class=content-wrap&gt;&lt;table&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Conoce las otras soluciones que tenemos para ti&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Con &lt;strong&gt;Rinde Ágil, &lt;/strong&gt;rinde tus gastos en cuestión de segundos. No más respaldos en papeles, digitaliza cada paso de la rendición de gastos de tu empresa.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="content-block aligncenter"&gt;&lt;span class=hs-cta-wrapper id=hs-cta-wrapper-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;span class="hs-cta-node hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9" id=hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;a href=https://cta-redirect.hubspot.com/cta/redirect/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9 target=_blank&gt;&lt;img class=hs-cta-img id=hs-cta-img-a826c11a-e3aa-46df-84a5-e53b35388aa9 style=border-width:0px; src=https://no-cache.hubspot.com/cta/default/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9.png alt="SOLICITA TU PRUEBA GRATIS AQUÍ"&gt;&lt;/a&gt;&lt;/span&gt;&lt;script charset=utf-8 src=https://js.hscta.net/cta/current.js&gt;&lt;/script&gt;&lt;script type=text/javascript&gt;hbspt.cta.load(5032552, "a826c11a-e3aa-46df-84a5-e53b35388aa9",{}); &lt;/script&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellspacing=0 cellpadding=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Saludos &lt;br&gt;&lt;strong&gt;Equipo AGILICE&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=footer&gt;&lt;table width=100%&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;¿Necesitas ayuda con este correo? &lt;a href=mailto:&gt;mesadeayuda@agilice.com&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;&lt;em&gt;Correo enviado a través de AGILICE®&amp;nbsp; Copyright © -Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;&lt;a href=[unsubscribe] style=color:#999;&gt;Si deseas salir del env&amp;iacute;o de emails de Agilice haz click aqu&amp;iacute;&lt;/a&gt;&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Factura, Envío a Aprobación');</v>
+&lt;/style&gt;&lt;/head&gt;&lt;body itemscope itemtype=http://schema.org/EmailMessage&gt;&lt;table class=body-wrap&gt;&lt;tr&gt;&lt;td&gt;&lt;/td&gt;&lt;td class=container width=600&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td valign=top&gt;&lt;img align=center alt src=https://cl.iconstruye.com/images/banner-generico.jpg width=600 class=mcnImage&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Factura en espera de aprobación&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block colspan=2&gt;&lt;p&gt;Hola &lt;strong&gt;&lt;nombaprobador&gt;&lt;/strong&gt;,&lt;br&gt;Junto con saludar le informamos que tiene una nueva factura a la espera de aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo Aprobación: Supera el monto del comprador &lt;br&gt;&lt;br&gt;Recuerde que puede aprobar desde la APP de &lt;a href=https://apps.agilice.com&gt;AGILICE.com&lt;/a&gt;&lt;br&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;table width=100% cellspacing=0 cellpadding=0 class=resume-box&gt;&lt;tr&gt;&lt;td&gt;&lt;div class=content-wrap&gt;&lt;table&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Conoce las otras soluciones que tenemos para ti&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Con &lt;strong&gt;Rinde Ágil, &lt;/strong&gt;rinde tus gastos en cuestión de segundos. No más respaldos en papeles, digitaliza cada paso de la rendición de gastos de tu empresa.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="content-block aligncenter"&gt;&lt;span class=hs-cta-wrapper id=hs-cta-wrapper-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;span class="hs-cta-node hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9" id=hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;a href=https://cta-redirect.hubspot.com/cta/redirect/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9 target=_blank&gt;&lt;img class=hs-cta-img id=hs-cta-img-a826c11a-e3aa-46df-84a5-e53b35388aa9 style=border-width:0px; src=https://no-cache.hubspot.com/cta/default/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9.png alt="SOLICITA TU PRUEBA GRATIS AQUÍ"&gt;&lt;/a&gt;&lt;/span&gt;&lt;script charset=utf-8 src=https://js.hscta.net/cta/current.js&gt;&lt;/script&gt;&lt;script type=text/javascript&gt;hbspt.cta.load(5032552, "a826c11a-e3aa-46df-84a5-e53b35388aa9",{}); &lt;/script&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellspacing=0 cellpadding=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Saludos &lt;br&gt;&lt;strong&gt;Equipo AGILICE&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=footer&gt;&lt;table width=100%&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;¿Necesitas ayuda con este correo? &lt;a href=mailto:&gt;mesadeayuda@agilice.com&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;&lt;em&gt;Correo enviado a través de AGILICE®&amp;nbsp; Copyright © -Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;&lt;a href=[unsubscribe] style=color:#999;&gt;Si deseas salir del env&amp;iacute;o de emails de Agilice haz click aqu&amp;iacute;&lt;/a&gt;&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Factura, Envío a Aprobación',48,2);</v>
       </c>
       <c r="T44" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20048, 'Redmat','iconstruye@iconstruye.com', 'Factura en Espera de Aprobación', '&lt;!DOCTYPE html
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3048, 'Redmat','iconstruye@iconstruye.com', 'Factura en Espera de Aprobación', '&lt;!DOCTYPE html
 PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;REDMAT&lt;/title&gt;&lt;style type=text/css&gt;*{
 margin: 0;
 font-family: "Helvetica Neue", Helvetica, Arial, sans-serif;
@@ -10278,10 +10289,10 @@
 width: 100% !important;} .mcnImage{
 max-width: 100% !important;
 width: 100% !important;}}
-&lt;/style&gt;&lt;/head&gt;&lt;body itemscope itemtype=http://schema.org/EmailMessage&gt;&lt;table class=body-wrap&gt;&lt;tr&gt;&lt;td&gt;&lt;/td&gt;&lt;td class=container width=600&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td valign=top&gt;&lt;img align=center alt src=https://cl.iconstruye.com/images/banner-generico.jpg width=600 class=mcnImage&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Factura en espera de aprobación&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block colspan=2&gt;&lt;p&gt;Hola &lt;strong&gt;&lt;nombaprobador&gt;&lt;/strong&gt;,&lt;br&gt;Junto con saludar le informamos que tiene una nueva factura a la espera de aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo Aprobación: Supera el monto del comprador &lt;br&gt;&lt;br&gt;Recuerde que puede aprobar desde la APP de &lt;a href=https://redmat.iconstruye.com&gt;REDMAT.com&lt;/a&gt;&lt;br&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;table width=100% cellspacing=0 cellpadding=0 class=resume-box&gt;&lt;tr&gt;&lt;td&gt;&lt;div class=content-wrap&gt;&lt;table&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Conoce las otras soluciones que tenemos para ti&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Con &lt;strong&gt;Rinde Ágil, &lt;/strong&gt;rinde tus gastos en cuestión de segundos. No más respaldos en papeles, digitaliza cada paso de la rendición de gastos de tu empresa.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="content-block aligncenter"&gt;&lt;span class=hs-cta-wrapper id=hs-cta-wrapper-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;span class="hs-cta-node hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9" id=hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;a href=https://cta-redirect.hubspot.com/cta/redirect/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9 target=_blank&gt;&lt;img class=hs-cta-img id=hs-cta-img-a826c11a-e3aa-46df-84a5-e53b35388aa9 style=border-width:0px; src=https://no-cache.hubspot.com/cta/default/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9.png alt="SOLICITA TU PRUEBA GRATIS AQUÍ"&gt;&lt;/a&gt;&lt;/span&gt;&lt;script charset=utf-8 src=https://js.hscta.net/cta/current.js&gt;&lt;/script&gt;&lt;script type=text/javascript&gt;hbspt.cta.load(5032552, "a826c11a-e3aa-46df-84a5-e53b35388aa9",{}); &lt;/script&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellspacing=0 cellpadding=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Saludos &lt;br&gt;&lt;strong&gt;Equipo REDMAT&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=footer&gt;&lt;table width=100%&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;¿Necesitas ayuda con este correo? &lt;a href=mailto:&gt;mesadeayuda@iconstruye.com&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;&lt;em&gt;Correo enviado a través de REDMAT®&amp;nbsp; Copyright © -Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;&lt;a href=[unsubscribe] style=color:#999;&gt;Si deseas salir del env&amp;iacute;o de emails de Redmat haz click aqu&amp;iacute;&lt;/a&gt;&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Factura, Envío a Aprobación');</v>
+&lt;/style&gt;&lt;/head&gt;&lt;body itemscope itemtype=http://schema.org/EmailMessage&gt;&lt;table class=body-wrap&gt;&lt;tr&gt;&lt;td&gt;&lt;/td&gt;&lt;td class=container width=600&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td valign=top&gt;&lt;img align=center alt src=https://cl.iconstruye.com/images/banner-generico.jpg width=600 class=mcnImage&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Factura en espera de aprobación&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block colspan=2&gt;&lt;p&gt;Hola &lt;strong&gt;&lt;nombaprobador&gt;&lt;/strong&gt;,&lt;br&gt;Junto con saludar le informamos que tiene una nueva factura a la espera de aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo Aprobación: Supera el monto del comprador &lt;br&gt;&lt;br&gt;Recuerde que puede aprobar desde la APP de &lt;a href=https://redmat.iconstruye.com&gt;REDMAT.com&lt;/a&gt;&lt;br&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;table width=100% cellspacing=0 cellpadding=0 class=resume-box&gt;&lt;tr&gt;&lt;td&gt;&lt;div class=content-wrap&gt;&lt;table&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Conoce las otras soluciones que tenemos para ti&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Con &lt;strong&gt;Rinde Ágil, &lt;/strong&gt;rinde tus gastos en cuestión de segundos. No más respaldos en papeles, digitaliza cada paso de la rendición de gastos de tu empresa.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="content-block aligncenter"&gt;&lt;span class=hs-cta-wrapper id=hs-cta-wrapper-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;span class="hs-cta-node hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9" id=hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;a href=https://cta-redirect.hubspot.com/cta/redirect/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9 target=_blank&gt;&lt;img class=hs-cta-img id=hs-cta-img-a826c11a-e3aa-46df-84a5-e53b35388aa9 style=border-width:0px; src=https://no-cache.hubspot.com/cta/default/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9.png alt="SOLICITA TU PRUEBA GRATIS AQUÍ"&gt;&lt;/a&gt;&lt;/span&gt;&lt;script charset=utf-8 src=https://js.hscta.net/cta/current.js&gt;&lt;/script&gt;&lt;script type=text/javascript&gt;hbspt.cta.load(5032552, "a826c11a-e3aa-46df-84a5-e53b35388aa9",{}); &lt;/script&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellspacing=0 cellpadding=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Saludos &lt;br&gt;&lt;strong&gt;Equipo REDMAT&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=footer&gt;&lt;table width=100%&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;¿Necesitas ayuda con este correo? &lt;a href=mailto:&gt;mesadeayuda@iconstruye.com&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;&lt;em&gt;Correo enviado a través de REDMAT®&amp;nbsp; Copyright © -Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;&lt;a href=[unsubscribe] style=color:#999;&gt;Si deseas salir del env&amp;iacute;o de emails de Redmat haz click aqu&amp;iacute;&lt;/a&gt;&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Factura, Envío a Aprobación',48,3);</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>49</v>
       </c>
@@ -10335,15 +10346,15 @@
         <v>331</v>
       </c>
       <c r="S45" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20049, 'Agilice','iconstruye@iconstruye.com', 'Factura Aprobada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Aprobada y se encuentra disponible para Pago.&lt;br&gt;&lt;br&gt;Proveedor: &lt;razonsocial&gt; &lt;br&gt;Nº Documento: &lt;numfc&gt; &lt;br&gt;Monto Factura: &lt;totalfactura&gt; &lt;br&gt;Tipo Documento: &lt;tipodoc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt; &lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Factura, Aprobada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2049, 'Agilice','iconstruye@iconstruye.com', 'Factura Aprobada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Aprobada y se encuentra disponible para Pago.&lt;br&gt;&lt;br&gt;Proveedor: &lt;razonsocial&gt; &lt;br&gt;Nº Documento: &lt;numfc&gt; &lt;br&gt;Monto Factura: &lt;totalfactura&gt; &lt;br&gt;Tipo Documento: &lt;tipodoc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt; &lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Factura, Aprobada',49,2);</v>
       </c>
       <c r="T45" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20049, 'Redmat','iconstruye@iconstruye.com', 'Factura Aprobada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Aprobada y se encuentra disponible para Pago.&lt;br&gt;&lt;br&gt;Proveedor: &lt;razonsocial&gt; &lt;br&gt;Nº Documento: &lt;numfc&gt; &lt;br&gt;Monto Factura: &lt;totalfactura&gt; &lt;br&gt;Tipo Documento: &lt;tipodoc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt; &lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Factura, Aprobada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3049, 'Redmat','iconstruye@iconstruye.com', 'Factura Aprobada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Aprobada y se encuentra disponible para Pago.&lt;br&gt;&lt;br&gt;Proveedor: &lt;razonsocial&gt; &lt;br&gt;Nº Documento: &lt;numfc&gt; &lt;br&gt;Monto Factura: &lt;totalfactura&gt; &lt;br&gt;Tipo Documento: &lt;tipodoc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt; &lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Factura, Aprobada',49,3);</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>50</v>
       </c>
@@ -10397,15 +10408,15 @@
         <v>338</v>
       </c>
       <c r="S46" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20050, 'Agilice','iconstruye@iconstruye.com', 'Factura Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Rechazada.&lt;br&gt;&lt;br&gt;Proveedor: &lt;razonsocial&gt; &lt;br&gt;Nº Documento: &lt;numfc&gt;&lt;br&gt;Monto Factura: &lt;totalfactura&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Rechazada por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Factura, Rechazo');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2050, 'Agilice','iconstruye@iconstruye.com', 'Factura Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Rechazada.&lt;br&gt;&lt;br&gt;Proveedor: &lt;razonsocial&gt; &lt;br&gt;Nº Documento: &lt;numfc&gt;&lt;br&gt;Monto Factura: &lt;totalfactura&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Rechazada por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Factura, Rechazo',50,2);</v>
       </c>
       <c r="T46" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20050, 'Redmat','iconstruye@iconstruye.com', 'Factura Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Rechazada.&lt;br&gt;&lt;br&gt;Proveedor: &lt;razonsocial&gt; &lt;br&gt;Nº Documento: &lt;numfc&gt;&lt;br&gt;Monto Factura: &lt;totalfactura&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Rechazada por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Factura, Rechazo');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3050, 'Redmat','iconstruye@iconstruye.com', 'Factura Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Rechazada.&lt;br&gt;&lt;br&gt;Proveedor: &lt;razonsocial&gt; &lt;br&gt;Nº Documento: &lt;numfc&gt;&lt;br&gt;Monto Factura: &lt;totalfactura&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Rechazada por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Factura, Rechazo',50,3);</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>51</v>
       </c>
@@ -10459,15 +10470,15 @@
         <v>344</v>
       </c>
       <c r="S47" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20051, 'Agilice','iconstruye@iconstruye.com', 'Recepción con Rechazos', 'Estimados Sres. Empresa &lt;nombproveedor&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; ha registrado un Rechazo en la Recepción de Productos de la Orden de Compra Nº &lt;numoc&gt; del Centro de Gestión &lt;orgc&gt;, asociado al documento de recepción &lt;numdoc&gt; de tipo &lt;tipodoc&gt;.&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Recepción con Rechazos');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2051, 'Agilice','iconstruye@iconstruye.com', 'Recepción con Rechazos', 'Estimados Sres. Empresa &lt;nombproveedor&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; ha registrado un Rechazo en la Recepción de Productos de la Orden de Compra Nº &lt;numoc&gt; del Centro de Gestión &lt;orgc&gt;, asociado al documento de recepción &lt;numdoc&gt; de tipo &lt;tipodoc&gt;.&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Recepción con Rechazos',51,2);</v>
       </c>
       <c r="T47" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20051, 'Redmat','iconstruye@iconstruye.com', 'Recepción con Rechazos', 'Estimados Sres. Empresa &lt;nombproveedor&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; ha registrado un Rechazo en la Recepción de Productos de la Orden de Compra Nº &lt;numoc&gt; del Centro de Gestión &lt;orgc&gt;, asociado al documento de recepción &lt;numdoc&gt; de tipo &lt;tipodoc&gt;.&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Recepción con Rechazos');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3051, 'Redmat','iconstruye@iconstruye.com', 'Recepción con Rechazos', 'Estimados Sres. Empresa &lt;nombproveedor&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; ha registrado un Rechazo en la Recepción de Productos de la Orden de Compra Nº &lt;numoc&gt; del Centro de Gestión &lt;orgc&gt;, asociado al documento de recepción &lt;numdoc&gt; de tipo &lt;tipodoc&gt;.&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Recepción con Rechazos',51,3);</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>78</v>
       </c>
@@ -10521,15 +10532,15 @@
         <v>351</v>
       </c>
       <c r="S48" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20078, 'Agilice','iconstruye@iconstruye.com', 'Estado de Pago Aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Estado de Pago, ha sido Aprobado.&lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Nº Estado Pago: &lt;numep&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación: &lt;fechacreacion&gt;&lt;br&gt;Nº Subcontrato: &lt;numsubcontrato&gt;&lt;br&gt;Nombre Subcontrato: &lt;nomsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Estado Pago, Notificación Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2078, 'Agilice','iconstruye@iconstruye.com', 'Estado de Pago Aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Estado de Pago, ha sido Aprobado.&lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Nº Estado Pago: &lt;numep&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación: &lt;fechacreacion&gt;&lt;br&gt;Nº Subcontrato: &lt;numsubcontrato&gt;&lt;br&gt;Nombre Subcontrato: &lt;nomsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Estado Pago, Notificación Aprobación',78,2);</v>
       </c>
       <c r="T48" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20078, 'Redmat','iconstruye@iconstruye.com', 'Estado de Pago Aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Estado de Pago, ha sido Aprobado.&lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Nº Estado Pago: &lt;numep&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación: &lt;fechacreacion&gt;&lt;br&gt;Nº Subcontrato: &lt;numsubcontrato&gt;&lt;br&gt;Nombre Subcontrato: &lt;nomsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Estado Pago, Notificación Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3078, 'Redmat','iconstruye@iconstruye.com', 'Estado de Pago Aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Estado de Pago, ha sido Aprobado.&lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Nº Estado Pago: &lt;numep&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación: &lt;fechacreacion&gt;&lt;br&gt;Nº Subcontrato: &lt;numsubcontrato&gt;&lt;br&gt;Nombre Subcontrato: &lt;nomsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Estado Pago, Notificación Aprobación',78,3);</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>92</v>
       </c>
@@ -10583,15 +10594,15 @@
         <v>356</v>
       </c>
       <c r="S49" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20092, 'Agilice','iconstruye@iconstruye.com', 'Solicitud Cancelacion OC', 'Estimado &lt;nombsolicitante&gt;: &lt;br&gt;&lt;br&gt; Junto con Saludarle, informamos a usted que se ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;. &lt;br&gt;&lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt; &lt;link&gt;&lt;br&gt;Mesa de Ayuda &lt;br&gt; 486 11 11','Cancelación OC Comprador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2092, 'Agilice','iconstruye@iconstruye.com', 'Solicitud Cancelacion OC', 'Estimado &lt;nombsolicitante&gt;: &lt;br&gt;&lt;br&gt; Junto con Saludarle, informamos a usted que se ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;. &lt;br&gt;&lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt; &lt;link&gt;&lt;br&gt;Mesa de Ayuda &lt;br&gt; 486 11 11','Cancelación OC Comprador',92,2);</v>
       </c>
       <c r="T49" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20092, 'Redmat','iconstruye@iconstruye.com', 'Solicitud Cancelacion OC', 'Estimado &lt;nombsolicitante&gt;: &lt;br&gt;&lt;br&gt; Junto con Saludarle, informamos a usted que se ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;. &lt;br&gt;&lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt; &lt;link&gt;&lt;br&gt;Mesa de Ayuda &lt;br&gt; 486 11 11','Cancelación OC Comprador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3092, 'Redmat','iconstruye@iconstruye.com', 'Solicitud Cancelacion OC', 'Estimado &lt;nombsolicitante&gt;: &lt;br&gt;&lt;br&gt; Junto con Saludarle, informamos a usted que se ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;. &lt;br&gt;&lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt; &lt;link&gt;&lt;br&gt;Mesa de Ayuda &lt;br&gt; 486 11 11','Cancelación OC Comprador',92,3);</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>52</v>
       </c>
@@ -10645,15 +10656,15 @@
         <v>363</v>
       </c>
       <c r="S50" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20052, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Factura (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo aprobación: Aprobador agregado al flujo &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Factura, Aprobador Agregado al Flujo');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2052, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Factura (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo aprobación: Aprobador agregado al flujo &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Factura, Aprobador Agregado al Flujo',52,2);</v>
       </c>
       <c r="T50" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20052, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Factura (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo aprobación: Aprobador agregado al flujo &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Factura, Aprobador Agregado al Flujo');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3052, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Factura (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Factura: &lt;numfc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Recepción: &lt;fecharecepcion&gt;&lt;br&gt;Tipo aprobación: Aprobador agregado al flujo &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Factura, Aprobador Agregado al Flujo',52,3);</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>60</v>
       </c>
@@ -10707,15 +10718,15 @@
         <v>370</v>
       </c>
       <c r="S51" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20060, 'Agilice','iconstruye@iconstruye.com', 'Asunto:  Aviso Subcontrato', 'Estimado Sr. &lt;nombusuario&gt;: &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Junto con saludarle, le avisamos que el &lt;fechaenvio&gt; usted recibió el subcontrato número &lt;numoc&gt;, generado por la empresa &lt;nombempresa&gt;. &lt;br&gt;_x000D_ Visite &lt;link&gt; para responderlo. &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente, &lt;br&gt;_x000D_ Agilice Mi brazo derecho &lt;br&gt;_x000D_ &lt;link&gt; &lt;br&gt;','Subcontrato, Aviso');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2060, 'Agilice','iconstruye@iconstruye.com', 'Asunto:  Aviso Subcontrato', 'Estimado Sr. &lt;nombusuario&gt;: &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Junto con saludarle, le avisamos que el &lt;fechaenvio&gt; usted recibió el subcontrato número &lt;numoc&gt;, generado por la empresa &lt;nombempresa&gt;. &lt;br&gt;_x000D_ Visite &lt;link&gt; para responderlo. &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente, &lt;br&gt;_x000D_ Agilice Mi brazo derecho &lt;br&gt;_x000D_ &lt;link&gt; &lt;br&gt;','Subcontrato, Aviso',60,2);</v>
       </c>
       <c r="T51" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20060, 'Redmat','iconstruye@iconstruye.com', 'Asunto:  Aviso Subcontrato', 'Estimado Sr. &lt;nombusuario&gt;: &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Junto con saludarle, le avisamos que el &lt;fechaenvio&gt; usted recibió el subcontrato número &lt;numoc&gt;, generado por la empresa &lt;nombempresa&gt;. &lt;br&gt;_x000D_ Visite &lt;link&gt; para responderlo. &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente, &lt;br&gt;_x000D_ Redmat Mi brazo derecho &lt;br&gt;_x000D_ &lt;link&gt; &lt;br&gt;','Subcontrato, Aviso');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3060, 'Redmat','iconstruye@iconstruye.com', 'Asunto:  Aviso Subcontrato', 'Estimado Sr. &lt;nombusuario&gt;: &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Junto con saludarle, le avisamos que el &lt;fechaenvio&gt; usted recibió el subcontrato número &lt;numoc&gt;, generado por la empresa &lt;nombempresa&gt;. &lt;br&gt;_x000D_ Visite &lt;link&gt; para responderlo. &lt;br&gt;_x000D_ &lt;br&gt;_x000D_ Atentamente, &lt;br&gt;_x000D_ Redmat Mi brazo derecho &lt;br&gt;_x000D_ &lt;link&gt; &lt;br&gt;','Subcontrato, Aviso',60,3);</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>65</v>
       </c>
@@ -10769,15 +10780,15 @@
         <v>377</v>
       </c>
       <c r="S52" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20065, 'Agilice','iconstruye@iconstruye.com', 'Preingreso Documento Rechazo', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Empresa &lt;nombempresa&gt; ha Rechazado el Preingreso de su &lt;tipodoc&gt;, Nº &lt;nrodoc&gt;.&lt;br&gt;&lt;br&gt;Para revisar más detalles, visite el módulo Preingreso de Documentos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Preingreso Documento, Rechazado Comprador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2065, 'Agilice','iconstruye@iconstruye.com', 'Preingreso Documento Rechazo', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Empresa &lt;nombempresa&gt; ha Rechazado el Preingreso de su &lt;tipodoc&gt;, Nº &lt;nrodoc&gt;.&lt;br&gt;&lt;br&gt;Para revisar más detalles, visite el módulo Preingreso de Documentos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Preingreso Documento, Rechazado Comprador',65,2);</v>
       </c>
       <c r="T52" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20065, 'Redmat','iconstruye@iconstruye.com', 'Preingreso Documento Rechazo', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Empresa &lt;nombempresa&gt; ha Rechazado el Preingreso de su &lt;tipodoc&gt;, Nº &lt;nrodoc&gt;.&lt;br&gt;&lt;br&gt;Para revisar más detalles, visite el módulo Preingreso de Documentos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Preingreso Documento, Rechazado Comprador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3065, 'Redmat','iconstruye@iconstruye.com', 'Preingreso Documento Rechazo', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Empresa &lt;nombempresa&gt; ha Rechazado el Preingreso de su &lt;tipodoc&gt;, Nº &lt;nrodoc&gt;.&lt;br&gt;&lt;br&gt;Para revisar más detalles, visite el módulo Preingreso de Documentos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Preingreso Documento, Rechazado Comprador',65,3);</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>66</v>
       </c>
@@ -10831,15 +10842,15 @@
         <v>384</v>
       </c>
       <c r="S53" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20066, 'Agilice','iconstruye@iconstruye.com', 'Preingreso Documento Aprobado', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Empresa &lt;nombempresa&gt; ha Aprobado el Preingreso de su &lt;tipodoc&gt;, N° &lt;nrodoc&gt;.&lt;br&gt;&lt;br&gt;Para revisar más detalles, visite el módulo Preingreso de Documentos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Preingreso Documento, Aprobado Comprador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2066, 'Agilice','iconstruye@iconstruye.com', 'Preingreso Documento Aprobado', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Empresa &lt;nombempresa&gt; ha Aprobado el Preingreso de su &lt;tipodoc&gt;, N° &lt;nrodoc&gt;.&lt;br&gt;&lt;br&gt;Para revisar más detalles, visite el módulo Preingreso de Documentos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Preingreso Documento, Aprobado Comprador',66,2);</v>
       </c>
       <c r="T53" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20066, 'Redmat','iconstruye@iconstruye.com', 'Preingreso Documento Aprobado', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Empresa &lt;nombempresa&gt; ha Aprobado el Preingreso de su &lt;tipodoc&gt;, N° &lt;nrodoc&gt;.&lt;br&gt;&lt;br&gt;Para revisar más detalles, visite el módulo Preingreso de Documentos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Preingreso Documento, Aprobado Comprador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3066, 'Redmat','iconstruye@iconstruye.com', 'Preingreso Documento Aprobado', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la Empresa &lt;nombempresa&gt; ha Aprobado el Preingreso de su &lt;tipodoc&gt;, N° &lt;nrodoc&gt;.&lt;br&gt;&lt;br&gt;Para revisar más detalles, visite el módulo Preingreso de Documentos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Preingreso Documento, Aprobado Comprador',66,3);</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>67</v>
       </c>
@@ -10893,15 +10904,15 @@
         <v>391</v>
       </c>
       <c r="S54" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20067, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Estado de Pago', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Estado de Pago en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt;&lt;br&gt;Nº Subcontrato: &lt;numsubcontrato&gt;&lt;br&gt;Nombre Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación solicitud: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Estado de Pago supera el gasto del comprador &lt;br&gt;&lt;br&gt;Para mayor información, ingrese al módulo de Subcontratos&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Estado Pago Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2067, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Estado de Pago', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Estado de Pago en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt;&lt;br&gt;Nº Subcontrato: &lt;numsubcontrato&gt;&lt;br&gt;Nombre Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación solicitud: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Estado de Pago supera el gasto del comprador &lt;br&gt;&lt;br&gt;Para mayor información, ingrese al módulo de Subcontratos&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Estado Pago Envío a Aprobación',67,2);</v>
       </c>
       <c r="T54" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20067, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Estado de Pago', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Estado de Pago en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt;&lt;br&gt;Nº Subcontrato: &lt;numsubcontrato&gt;&lt;br&gt;Nombre Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación solicitud: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Estado de Pago supera el gasto del comprador &lt;br&gt;&lt;br&gt;Para mayor información, ingrese al módulo de Subcontratos&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Estado Pago Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3067, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Estado de Pago', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Estado de Pago en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt;&lt;br&gt;Nº Subcontrato: &lt;numsubcontrato&gt;&lt;br&gt;Nombre Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación solicitud: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Estado de Pago supera el gasto del comprador &lt;br&gt;&lt;br&gt;Para mayor información, ingrese al módulo de Subcontratos&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Estado Pago Envío a Aprobación',67,3);</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>61</v>
       </c>
@@ -10955,15 +10966,15 @@
         <v>398</v>
       </c>
       <c r="S55" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20061, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Subcontrato', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Subcontrato en espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Subcontrato: &lt;numsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Subcontrato supera el gasto del comprador &lt;br&gt;Monto Contrato: &lt;montoaprobar&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2061, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Subcontrato', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Subcontrato en espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Subcontrato: &lt;numsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Subcontrato supera el gasto del comprador &lt;br&gt;Monto Contrato: &lt;montoaprobar&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Envío a Aprobación',61,2);</v>
       </c>
       <c r="T55" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20061, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Subcontrato', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Subcontrato en espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Subcontrato: &lt;numsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Subcontrato supera el gasto del comprador &lt;br&gt;Monto Contrato: &lt;montoaprobar&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3061, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Subcontrato', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Subcontrato en espera de su Aprobación.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Subcontrato: &lt;numsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Subcontrato supera el gasto del comprador &lt;br&gt;Monto Contrato: &lt;montoaprobar&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Envío a Aprobación',61,3);</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>62</v>
       </c>
@@ -11017,15 +11028,15 @@
         <v>405</v>
       </c>
       <c r="S56" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20062, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Subcontrato (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Subcontrato en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Envío a Aprobación Añadido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2062, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Subcontrato (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Subcontrato en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Envío a Aprobación Añadido',62,2);</v>
       </c>
       <c r="T56" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20062, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Subcontrato (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Subcontrato en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Envío a Aprobación Añadido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3062, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Subcontrato (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Subcontrato en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Envío a Aprobación Añadido',62,3);</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>63</v>
       </c>
@@ -11079,15 +11090,15 @@
         <v>412</v>
       </c>
       <c r="S57" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20063, 'Agilice','iconstruye@iconstruye.com', 'Subcontrato aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato generado por usted, ha sido Aprobado.&lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice &lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Aprobación Total');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2063, 'Agilice','iconstruye@iconstruye.com', 'Subcontrato aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato generado por usted, ha sido Aprobado.&lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice &lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Aprobación Total',63,2);</v>
       </c>
       <c r="T57" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20063, 'Redmat','iconstruye@iconstruye.com', 'Subcontrato aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato generado por usted, ha sido Aprobado.&lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat &lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Aprobación Total');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3063, 'Redmat','iconstruye@iconstruye.com', 'Subcontrato aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato generado por usted, ha sido Aprobado.&lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat &lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Aprobación Total',63,3);</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>64</v>
       </c>
@@ -11141,15 +11152,15 @@
         <v>419</v>
       </c>
       <c r="S58" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20064, 'Agilice','iconstruye@iconstruye.com', 'Subcontrato Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato generado por usted, ha sido Rechazado. &lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Rechazado Aprobador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2064, 'Agilice','iconstruye@iconstruye.com', 'Subcontrato Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato generado por usted, ha sido Rechazado. &lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Rechazado Aprobador',64,2);</v>
       </c>
       <c r="T58" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20064, 'Redmat','iconstruye@iconstruye.com', 'Subcontrato Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato generado por usted, ha sido Rechazado. &lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Rechazado Aprobador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3064, 'Redmat','iconstruye@iconstruye.com', 'Subcontrato Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato generado por usted, ha sido Rechazado. &lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Rechazado Aprobador',64,3);</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>77</v>
       </c>
@@ -11203,15 +11214,15 @@
         <v>426</v>
       </c>
       <c r="S59" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20077, 'Agilice','iconstruye@iconstruye.com', 'Linea de Pedido de Material Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludarle, le informamos que el Sr. &lt;nombaprobador&gt; ha eliminado una linea del Pedido de Material Solicitado por Ud. &lt;br&gt; &lt;br&gt; No. Pedido: &lt;numpm&gt; &lt;br&gt; Nombre Pedido: &lt;nompm&gt; &lt;br&gt; Organización: &lt;nomborgc&gt; &lt;br&gt; Fecha Rechazo: &lt;fechacreacion&gt; &lt;br&gt; Código Prod: &lt;cod&gt; &lt;br&gt; Cantidad : &lt;cantidad&gt; &lt;br&gt; Descripcion:&lt;descripcion&gt; &lt;br&gt; Glosa:&lt;glosa&gt; &lt;br&gt; &lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Eliminación de Linea de Pedido de Material');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2077, 'Agilice','iconstruye@iconstruye.com', 'Linea de Pedido de Material Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludarle, le informamos que el Sr. &lt;nombaprobador&gt; ha eliminado una linea del Pedido de Material Solicitado por Ud. &lt;br&gt; &lt;br&gt; No. Pedido: &lt;numpm&gt; &lt;br&gt; Nombre Pedido: &lt;nompm&gt; &lt;br&gt; Organización: &lt;nomborgc&gt; &lt;br&gt; Fecha Rechazo: &lt;fechacreacion&gt; &lt;br&gt; Código Prod: &lt;cod&gt; &lt;br&gt; Cantidad : &lt;cantidad&gt; &lt;br&gt; Descripcion:&lt;descripcion&gt; &lt;br&gt; Glosa:&lt;glosa&gt; &lt;br&gt; &lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Eliminación de Linea de Pedido de Material',77,2);</v>
       </c>
       <c r="T59" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20077, 'Redmat','iconstruye@iconstruye.com', 'Linea de Pedido de Material Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludarle, le informamos que el Sr. &lt;nombaprobador&gt; ha eliminado una linea del Pedido de Material Solicitado por Ud. &lt;br&gt; &lt;br&gt; No. Pedido: &lt;numpm&gt; &lt;br&gt; Nombre Pedido: &lt;nompm&gt; &lt;br&gt; Organización: &lt;nomborgc&gt; &lt;br&gt; Fecha Rechazo: &lt;fechacreacion&gt; &lt;br&gt; Código Prod: &lt;cod&gt; &lt;br&gt; Cantidad : &lt;cantidad&gt; &lt;br&gt; Descripcion:&lt;descripcion&gt; &lt;br&gt; Glosa:&lt;glosa&gt; &lt;br&gt; &lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Eliminación de Linea de Pedido de Material');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3077, 'Redmat','iconstruye@iconstruye.com', 'Linea de Pedido de Material Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludarle, le informamos que el Sr. &lt;nombaprobador&gt; ha eliminado una linea del Pedido de Material Solicitado por Ud. &lt;br&gt; &lt;br&gt; No. Pedido: &lt;numpm&gt; &lt;br&gt; Nombre Pedido: &lt;nompm&gt; &lt;br&gt; Organización: &lt;nomborgc&gt; &lt;br&gt; Fecha Rechazo: &lt;fechacreacion&gt; &lt;br&gt; Código Prod: &lt;cod&gt; &lt;br&gt; Cantidad : &lt;cantidad&gt; &lt;br&gt; Descripcion:&lt;descripcion&gt; &lt;br&gt; Glosa:&lt;glosa&gt; &lt;br&gt; &lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Eliminación de Linea de Pedido de Material',77,3);</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>79</v>
       </c>
@@ -11265,15 +11276,15 @@
         <v>433</v>
       </c>
       <c r="S60" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20079, 'Agilice','iconstruye@iconstruye.com', 'Estado de Pago Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Estado de Pago ingresado por usted ha sido Rechazado. &lt;br&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt; &lt;br&gt;Tipo Estado Pago: &lt;destipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha ingreso: &lt;fechacreacion&gt;.&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;N°: &lt;numsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Estado Pago, Notificación Rechazo');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2079, 'Agilice','iconstruye@iconstruye.com', 'Estado de Pago Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Estado de Pago ingresado por usted ha sido Rechazado. &lt;br&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt; &lt;br&gt;Tipo Estado Pago: &lt;destipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha ingreso: &lt;fechacreacion&gt;.&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;N°: &lt;numsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Estado Pago, Notificación Rechazo',79,2);</v>
       </c>
       <c r="T60" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20079, 'Redmat','iconstruye@iconstruye.com', 'Estado de Pago Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Estado de Pago ingresado por usted ha sido Rechazado. &lt;br&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt; &lt;br&gt;Tipo Estado Pago: &lt;destipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha ingreso: &lt;fechacreacion&gt;.&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;N°: &lt;numsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Estado Pago, Notificación Rechazo');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3079, 'Redmat','iconstruye@iconstruye.com', 'Estado de Pago Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Estado de Pago ingresado por usted ha sido Rechazado. &lt;br&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt; &lt;br&gt;Tipo Estado Pago: &lt;destipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha ingreso: &lt;fechacreacion&gt;.&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;N°: &lt;numsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Estado Pago, Notificación Rechazo',79,3);</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>80</v>
       </c>
@@ -11327,15 +11338,15 @@
         <v>439</v>
       </c>
       <c r="S61" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20080, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Estado de Pago (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Estado de Pago en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt;&lt;br&gt;Folio Subcontrato: &lt;foliosc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación solicitud: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Envío a Aprobación Añadido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2080, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Estado de Pago (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Estado de Pago en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt;&lt;br&gt;Folio Subcontrato: &lt;foliosc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación solicitud: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Envío a Aprobación Añadido',80,2);</v>
       </c>
       <c r="T61" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20080, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Estado de Pago (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Estado de Pago en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt;&lt;br&gt;Folio Subcontrato: &lt;foliosc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación solicitud: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Envío a Aprobación Añadido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3080, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Estado de Pago (Aprobador Agregado a Flujo)', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Estado de Pago en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Tipo Estado de Pago: &lt;destipodoc&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt;&lt;br&gt;Folio Subcontrato: &lt;foliosc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha creación solicitud: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Envío a Aprobación Añadido',80,3);</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>82</v>
       </c>
@@ -11389,15 +11400,15 @@
         <v>446</v>
       </c>
       <c r="S62" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20082, 'Agilice','iconstruye@iconstruye.com', 'Aviso de Stock Critico', 'Estimado Sr. &lt;nombreusu&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente producto se encuentra bajo el valor definido como Stock Crítico. &lt;br&gt;&lt;br&gt;Código: &lt;codigoitem&gt;&lt;br&gt;Descripción: &lt;descripcionitem&gt;&lt;br&gt;Bodega: &lt;nombrebodega&gt;&lt;br&gt;Centro de Gestión: &lt;nombreorg&gt;&lt;br&gt;Stock Actual: &lt;saldo&gt;&lt;br&gt;Stock Crítico: &lt;stockcritico&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Bodega, Aviso stock crítico');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2082, 'Agilice','iconstruye@iconstruye.com', 'Aviso de Stock Critico', 'Estimado Sr. &lt;nombreusu&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente producto se encuentra bajo el valor definido como Stock Crítico. &lt;br&gt;&lt;br&gt;Código: &lt;codigoitem&gt;&lt;br&gt;Descripción: &lt;descripcionitem&gt;&lt;br&gt;Bodega: &lt;nombrebodega&gt;&lt;br&gt;Centro de Gestión: &lt;nombreorg&gt;&lt;br&gt;Stock Actual: &lt;saldo&gt;&lt;br&gt;Stock Crítico: &lt;stockcritico&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Bodega, Aviso stock crítico',82,2);</v>
       </c>
       <c r="T62" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20082, 'Redmat','iconstruye@iconstruye.com', 'Aviso de Stock Critico', 'Estimado Sr. &lt;nombreusu&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente producto se encuentra bajo el valor definido como Stock Crítico. &lt;br&gt;&lt;br&gt;Código: &lt;codigoitem&gt;&lt;br&gt;Descripción: &lt;descripcionitem&gt;&lt;br&gt;Bodega: &lt;nombrebodega&gt;&lt;br&gt;Centro de Gestión: &lt;nombreorg&gt;&lt;br&gt;Stock Actual: &lt;saldo&gt;&lt;br&gt;Stock Crítico: &lt;stockcritico&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Bodega, Aviso stock crítico');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3082, 'Redmat','iconstruye@iconstruye.com', 'Aviso de Stock Critico', 'Estimado Sr. &lt;nombreusu&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente producto se encuentra bajo el valor definido como Stock Crítico. &lt;br&gt;&lt;br&gt;Código: &lt;codigoitem&gt;&lt;br&gt;Descripción: &lt;descripcionitem&gt;&lt;br&gt;Bodega: &lt;nombrebodega&gt;&lt;br&gt;Centro de Gestión: &lt;nombreorg&gt;&lt;br&gt;Stock Actual: &lt;saldo&gt;&lt;br&gt;Stock Crítico: &lt;stockcritico&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Bodega, Aviso stock crítico',82,3);</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>81</v>
       </c>
@@ -11451,15 +11462,15 @@
         <v>453</v>
       </c>
       <c r="S63" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20081, 'Agilice','iconstruye@iconstruye.com', 'Su Convenio ha sido Despublicado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Convenio ha finalizado su tiempo de Publicación. &lt;br&gt;&lt;br&gt;Nº Convenio: &lt;numcv&gt;&lt;br&gt;Nombre Convenio: &lt;nomcv&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Fecha Vigencia: &lt;fechavigencia&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Despublicación de Convenio');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2081, 'Agilice','iconstruye@iconstruye.com', 'Su Convenio ha sido Despublicado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Convenio ha finalizado su tiempo de Publicación. &lt;br&gt;&lt;br&gt;Nº Convenio: &lt;numcv&gt;&lt;br&gt;Nombre Convenio: &lt;nomcv&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Fecha Vigencia: &lt;fechavigencia&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Despublicación de Convenio',81,2);</v>
       </c>
       <c r="T63" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20081, 'Redmat','iconstruye@iconstruye.com', 'Su Convenio ha sido Despublicado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Convenio ha finalizado su tiempo de Publicación. &lt;br&gt;&lt;br&gt;Nº Convenio: &lt;numcv&gt;&lt;br&gt;Nombre Convenio: &lt;nomcv&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Fecha Vigencia: &lt;fechavigencia&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Despublicación de Convenio');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3081, 'Redmat','iconstruye@iconstruye.com', 'Su Convenio ha sido Despublicado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Convenio ha finalizado su tiempo de Publicación. &lt;br&gt;&lt;br&gt;Nº Convenio: &lt;numcv&gt;&lt;br&gt;Nombre Convenio: &lt;nomcv&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Fecha Vigencia: &lt;fechavigencia&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Despublicación de Convenio',81,3);</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>46</v>
       </c>
@@ -11513,15 +11524,15 @@
         <v>460</v>
       </c>
       <c r="S64" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20046, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Materiales Aprobador Añadido', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo. &lt;br&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Aprobador Añadido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2046, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Materiales Aprobador Añadido', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo. &lt;br&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Aprobador Añadido',46,2);</v>
       </c>
       <c r="T64" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20046, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Materiales Aprobador Añadido', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo. &lt;br&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Aprobador Añadido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3046, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Materiales Aprobador Añadido', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo. &lt;br&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Aprobador Añadido',46,3);</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>39</v>
       </c>
@@ -11575,15 +11586,15 @@
         <v>467</v>
       </c>
       <c r="S65" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20039, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Materiales en Espera de Aprobación', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2039, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Materiales en Espera de Aprobación', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido Materiales, Envío a Aprobación',39,2);</v>
       </c>
       <c r="T65" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20039, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Materiales en Espera de Aprobación', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3039, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Materiales en Espera de Aprobación', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Materiales.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido Materiales, Envío a Aprobación',39,3);</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>81</v>
       </c>
@@ -11637,15 +11648,15 @@
         <v>453</v>
       </c>
       <c r="S66" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20081, 'Agilice','iconstruye@iconstruye.com', 'Su Convenio ha sido Despublicado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Convenio ha finalizado su tiempo de Publicación. &lt;br&gt;&lt;br&gt;Nº Convenio: &lt;numcv&gt;&lt;br&gt;Nombre Convenio: &lt;nomcv&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Fecha Vigencia: &lt;fechavigencia&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Despublicación de Convenio');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2081, 'Agilice','iconstruye@iconstruye.com', 'Su Convenio ha sido Despublicado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Convenio ha finalizado su tiempo de Publicación. &lt;br&gt;&lt;br&gt;Nº Convenio: &lt;numcv&gt;&lt;br&gt;Nombre Convenio: &lt;nomcv&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Fecha Vigencia: &lt;fechavigencia&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Despublicación de Convenio',81,2);</v>
       </c>
       <c r="T66" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20081, 'Redmat','iconstruye@iconstruye.com', 'Su Convenio ha sido Despublicado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Convenio ha finalizado su tiempo de Publicación. &lt;br&gt;&lt;br&gt;Nº Convenio: &lt;numcv&gt;&lt;br&gt;Nombre Convenio: &lt;nomcv&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Fecha Vigencia: &lt;fechavigencia&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Despublicación de Convenio');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3081, 'Redmat','iconstruye@iconstruye.com', 'Su Convenio ha sido Despublicado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Convenio ha finalizado su tiempo de Publicación. &lt;br&gt;&lt;br&gt;Nº Convenio: &lt;numcv&gt;&lt;br&gt;Nombre Convenio: &lt;nomcv&gt;&lt;br&gt;Empresa: &lt;nombempresa&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Fecha Vigencia: &lt;fechavigencia&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Despublicación de Convenio',81,3);</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>83</v>
       </c>
@@ -11699,15 +11710,15 @@
         <v>473</v>
       </c>
       <c r="S67" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20083, 'Agilice','iconstruye@iconstruye.com', 'Generación Automatica de Bodega', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que en el Centro de Gestión &lt;nombrecg&gt; se ha generado automáticamente una Bodega, solicitamos a usted verificar los datos asociados. &lt;br&gt;&lt;br&gt;Código Bodega: 001&lt;br&gt;Nombre Bodega: &lt;nombrebod&gt;&lt;br&gt;Encargado Bodega: &lt;nombencargado&gt;&lt;br&gt;Comentarios: Bodega generada automáticamente por el sistema &lt;br&gt;Prefijo de Entrada: E-&lt;br&gt;Correlativo de Entrada: 1&lt;br&gt;Prefijo de Salida: S-&lt;br&gt;Correlativo de Salida: 1&lt;br&gt;&lt;br&gt;Para revisar o modificar estos antecedentes, visite el módulo Bodega. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Generación Automatica de Bodega');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2083, 'Agilice','iconstruye@iconstruye.com', 'Generación Automatica de Bodega', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que en el Centro de Gestión &lt;nombrecg&gt; se ha generado automáticamente una Bodega, solicitamos a usted verificar los datos asociados. &lt;br&gt;&lt;br&gt;Código Bodega: 001&lt;br&gt;Nombre Bodega: &lt;nombrebod&gt;&lt;br&gt;Encargado Bodega: &lt;nombencargado&gt;&lt;br&gt;Comentarios: Bodega generada automáticamente por el sistema &lt;br&gt;Prefijo de Entrada: E-&lt;br&gt;Correlativo de Entrada: 1&lt;br&gt;Prefijo de Salida: S-&lt;br&gt;Correlativo de Salida: 1&lt;br&gt;&lt;br&gt;Para revisar o modificar estos antecedentes, visite el módulo Bodega. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Generación Automatica de Bodega',83,2);</v>
       </c>
       <c r="T67" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20083, 'Redmat','iconstruye@iconstruye.com', 'Generación Automatica de Bodega', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que en el Centro de Gestión &lt;nombrecg&gt; se ha generado automáticamente una Bodega, solicitamos a usted verificar los datos asociados. &lt;br&gt;&lt;br&gt;Código Bodega: 001&lt;br&gt;Nombre Bodega: &lt;nombrebod&gt;&lt;br&gt;Encargado Bodega: &lt;nombencargado&gt;&lt;br&gt;Comentarios: Bodega generada automáticamente por el sistema &lt;br&gt;Prefijo de Entrada: E-&lt;br&gt;Correlativo de Entrada: 1&lt;br&gt;Prefijo de Salida: S-&lt;br&gt;Correlativo de Salida: 1&lt;br&gt;&lt;br&gt;Para revisar o modificar estos antecedentes, visite el módulo Bodega. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Generación Automatica de Bodega');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3083, 'Redmat','iconstruye@iconstruye.com', 'Generación Automatica de Bodega', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que en el Centro de Gestión &lt;nombrecg&gt; se ha generado automáticamente una Bodega, solicitamos a usted verificar los datos asociados. &lt;br&gt;&lt;br&gt;Código Bodega: 001&lt;br&gt;Nombre Bodega: &lt;nombrebod&gt;&lt;br&gt;Encargado Bodega: &lt;nombencargado&gt;&lt;br&gt;Comentarios: Bodega generada automáticamente por el sistema &lt;br&gt;Prefijo de Entrada: E-&lt;br&gt;Correlativo de Entrada: 1&lt;br&gt;Prefijo de Salida: S-&lt;br&gt;Correlativo de Salida: 1&lt;br&gt;&lt;br&gt;Para revisar o modificar estos antecedentes, visite el módulo Bodega. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Generación Automatica de Bodega',83,3);</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>84</v>
       </c>
@@ -11761,15 +11772,15 @@
         <v>480</v>
       </c>
       <c r="S68" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20084, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de facturas', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt;, ha Aprobado la Factura &lt;numerofactura&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Aprobación de facturas Proveedor');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2084, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de facturas', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt;, ha Aprobado la Factura &lt;numerofactura&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Aprobación de facturas Proveedor',84,2);</v>
       </c>
       <c r="T68" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20084, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de facturas', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt;, ha Aprobado la Factura &lt;numerofactura&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Aprobación de facturas Proveedor');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3084, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de facturas', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt;, ha Aprobado la Factura &lt;numerofactura&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Aprobación de facturas Proveedor',84,3);</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>85</v>
       </c>
@@ -11823,15 +11834,15 @@
         <v>487</v>
       </c>
       <c r="S69" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20085, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de Nota Corrección', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt; usted recibió una solicitud de &lt;tiponota&gt;, de la empresa &lt;nombempresa&gt;, correspondiente a la factura número &lt;numfactura&gt;, por concepto de &lt;motivo&gt;.&lt;br&gt;&lt;br&gt;Los Documentos de Recepción afectados son: &lt;docrecp&gt;.&lt;br&gt;Las Órdenes de Compra afectadas son: &lt;dococ&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Solicitud de Nota Corrección Proveedor');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2085, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de Nota Corrección', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt; usted recibió una solicitud de &lt;tiponota&gt;, de la empresa &lt;nombempresa&gt;, correspondiente a la factura número &lt;numfactura&gt;, por concepto de &lt;motivo&gt;.&lt;br&gt;&lt;br&gt;Los Documentos de Recepción afectados son: &lt;docrecp&gt;.&lt;br&gt;Las Órdenes de Compra afectadas son: &lt;dococ&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Solicitud de Nota Corrección Proveedor',85,2);</v>
       </c>
       <c r="T69" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20085, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de Nota Corrección', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt; usted recibió una solicitud de &lt;tiponota&gt;, de la empresa &lt;nombempresa&gt;, correspondiente a la factura número &lt;numfactura&gt;, por concepto de &lt;motivo&gt;.&lt;br&gt;&lt;br&gt;Los Documentos de Recepción afectados son: &lt;docrecp&gt;.&lt;br&gt;Las Órdenes de Compra afectadas son: &lt;dococ&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Solicitud de Nota Corrección Proveedor');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3085, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de Nota Corrección', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt; usted recibió una solicitud de &lt;tiponota&gt;, de la empresa &lt;nombempresa&gt;, correspondiente a la factura número &lt;numfactura&gt;, por concepto de &lt;motivo&gt;.&lt;br&gt;&lt;br&gt;Los Documentos de Recepción afectados son: &lt;docrecp&gt;.&lt;br&gt;Las Órdenes de Compra afectadas son: &lt;dococ&gt;.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Solicitud de Nota Corrección Proveedor',85,3);</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>86</v>
       </c>
@@ -11885,15 +11896,15 @@
         <v>494</v>
       </c>
       <c r="S70" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20086, 'Agilice','iconstruye@iconstruye.com', 'Cancelación de Solicitud de Nota Corrección', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt; ha Cancelado la Solicitud de &lt;tiponota&gt;, correspondiente a la factura número &lt;numfactura&gt;.&lt;br&gt;&lt;br&gt;Para revisar más antecedentes, ingrese al módulo de Facturación &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Solicitud de Nota Corrección Proveedor');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2086, 'Agilice','iconstruye@iconstruye.com', 'Cancelación de Solicitud de Nota Corrección', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt; ha Cancelado la Solicitud de &lt;tiponota&gt;, correspondiente a la factura número &lt;numfactura&gt;.&lt;br&gt;&lt;br&gt;Para revisar más antecedentes, ingrese al módulo de Facturación &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Solicitud de Nota Corrección Proveedor',86,2);</v>
       </c>
       <c r="T70" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20086, 'Redmat','iconstruye@iconstruye.com', 'Cancelación de Solicitud de Nota Corrección', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt; ha Cancelado la Solicitud de &lt;tiponota&gt;, correspondiente a la factura número &lt;numfactura&gt;.&lt;br&gt;&lt;br&gt;Para revisar más antecedentes, ingrese al módulo de Facturación &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Solicitud de Nota Corrección Proveedor');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3086, 'Redmat','iconstruye@iconstruye.com', 'Cancelación de Solicitud de Nota Corrección', 'Estimado Sr. &lt;nombreproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt; ha Cancelado la Solicitud de &lt;tiponota&gt;, correspondiente a la factura número &lt;numfactura&gt;.&lt;br&gt;&lt;br&gt;Para revisar más antecedentes, ingrese al módulo de Facturación &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Solicitud de Nota Corrección Proveedor',86,3);</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>87</v>
       </c>
@@ -11947,15 +11958,15 @@
         <v>501</v>
       </c>
       <c r="S71" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20087, 'Agilice','iconstruye@iconstruye.com', 'FACTURA CANCELADA', 'Estimado Sr. Usuario:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Cancelada.&lt;br&gt;&lt;br&gt;Nº Factura: &lt;numfactura&gt;&lt;br&gt;Folio Único: &lt;foliounico&gt;&lt;br&gt;Centro Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt;&lt;br&gt;Cancelada por: &lt;nomusuariocanc&gt;&lt;br&gt;Comentarios: &lt;comentarios&gt;&lt;br&gt;Información Asociada a la Factura (notas): &lt;infoasocnotas&gt;&lt;br&gt;&lt;br&gt;Para revisar más antecedentes, ingrese al módulo Factura. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;2 486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Factura');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2087, 'Agilice','iconstruye@iconstruye.com', 'FACTURA CANCELADA', 'Estimado Sr. Usuario:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Cancelada.&lt;br&gt;&lt;br&gt;Nº Factura: &lt;numfactura&gt;&lt;br&gt;Folio Único: &lt;foliounico&gt;&lt;br&gt;Centro Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt;&lt;br&gt;Cancelada por: &lt;nomusuariocanc&gt;&lt;br&gt;Comentarios: &lt;comentarios&gt;&lt;br&gt;Información Asociada a la Factura (notas): &lt;infoasocnotas&gt;&lt;br&gt;&lt;br&gt;Para revisar más antecedentes, ingrese al módulo Factura. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;2 486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Factura',87,2);</v>
       </c>
       <c r="T71" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20087, 'Redmat','iconstruye@iconstruye.com', 'FACTURA CANCELADA', 'Estimado Sr. Usuario:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Cancelada.&lt;br&gt;&lt;br&gt;Nº Factura: &lt;numfactura&gt;&lt;br&gt;Folio Único: &lt;foliounico&gt;&lt;br&gt;Centro Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt;&lt;br&gt;Cancelada por: &lt;nomusuariocanc&gt;&lt;br&gt;Comentarios: &lt;comentarios&gt;&lt;br&gt;Información Asociada a la Factura (notas): &lt;infoasocnotas&gt;&lt;br&gt;&lt;br&gt;Para revisar más antecedentes, ingrese al módulo Factura. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;2 486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Factura');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3087, 'Redmat','iconstruye@iconstruye.com', 'FACTURA CANCELADA', 'Estimado Sr. Usuario:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la siguiente Factura ha sido Cancelada.&lt;br&gt;&lt;br&gt;Nº Factura: &lt;numfactura&gt;&lt;br&gt;Folio Único: &lt;foliounico&gt;&lt;br&gt;Centro Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt;&lt;br&gt;Cancelada por: &lt;nomusuariocanc&gt;&lt;br&gt;Comentarios: &lt;comentarios&gt;&lt;br&gt;Información Asociada a la Factura (notas): &lt;infoasocnotas&gt;&lt;br&gt;&lt;br&gt;Para revisar más antecedentes, ingrese al módulo Factura. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;2 486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Factura',87,3);</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>88</v>
       </c>
@@ -12009,15 +12020,15 @@
         <v>508</v>
       </c>
       <c r="S72" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20088, 'Agilice','iconstruye@iconstruye.com', 'NOTA DE CORRECCION CANCELADA', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente documento ha sido Cancelado&lt;br&gt;&lt;br&gt;N° Documento: &lt;numfactura&gt;&lt;br&gt;Tipo Documento: &lt;tipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt;&lt;br&gt;Cancelado por: &lt;nomusuariocanc&gt;&lt;br&gt;Comentarios: &lt;comentarios&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Nota de Correccion');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2088, 'Agilice','iconstruye@iconstruye.com', 'NOTA DE CORRECCION CANCELADA', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente documento ha sido Cancelado&lt;br&gt;&lt;br&gt;N° Documento: &lt;numfactura&gt;&lt;br&gt;Tipo Documento: &lt;tipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt;&lt;br&gt;Cancelado por: &lt;nomusuariocanc&gt;&lt;br&gt;Comentarios: &lt;comentarios&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Nota de Correccion',88,2);</v>
       </c>
       <c r="T72" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20088, 'Redmat','iconstruye@iconstruye.com', 'NOTA DE CORRECCION CANCELADA', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente documento ha sido Cancelado&lt;br&gt;&lt;br&gt;N° Documento: &lt;numfactura&gt;&lt;br&gt;Tipo Documento: &lt;tipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt;&lt;br&gt;Cancelado por: &lt;nomusuariocanc&gt;&lt;br&gt;Comentarios: &lt;comentarios&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Nota de Correccion');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3088, 'Redmat','iconstruye@iconstruye.com', 'NOTA DE CORRECCION CANCELADA', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente documento ha sido Cancelado&lt;br&gt;&lt;br&gt;N° Documento: &lt;numfactura&gt;&lt;br&gt;Tipo Documento: &lt;tipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha de Ingreso: &lt;fechacreacion&gt;&lt;br&gt;Cancelado por: &lt;nomusuariocanc&gt;&lt;br&gt;Comentarios: &lt;comentarios&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Nota de Correccion',88,3);</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>83</v>
       </c>
@@ -12071,15 +12082,15 @@
         <v>473</v>
       </c>
       <c r="S73" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20083, 'Agilice','iconstruye@iconstruye.com', 'Generación Automatica de Bodega', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que en el Centro de Gestión &lt;nombrecg&gt; se ha generado automáticamente una Bodega, solicitamos a usted verificar los datos asociados. &lt;br&gt;&lt;br&gt;Código Bodega: 001&lt;br&gt;Nombre Bodega: &lt;nombrebod&gt;&lt;br&gt;Encargado Bodega: &lt;nombencargado&gt;&lt;br&gt;Comentarios: Bodega generada automáticamente por el sistema &lt;br&gt;Prefijo de Entrada: E-&lt;br&gt;Correlativo de Entrada: 1&lt;br&gt;Prefijo de Salida: S-&lt;br&gt;Correlativo de Salida: 1&lt;br&gt;&lt;br&gt;Para revisar o modificar estos antecedentes, visite el módulo Bodega. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Generación Automatica de Bodega');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2083, 'Agilice','iconstruye@iconstruye.com', 'Generación Automatica de Bodega', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que en el Centro de Gestión &lt;nombrecg&gt; se ha generado automáticamente una Bodega, solicitamos a usted verificar los datos asociados. &lt;br&gt;&lt;br&gt;Código Bodega: 001&lt;br&gt;Nombre Bodega: &lt;nombrebod&gt;&lt;br&gt;Encargado Bodega: &lt;nombencargado&gt;&lt;br&gt;Comentarios: Bodega generada automáticamente por el sistema &lt;br&gt;Prefijo de Entrada: E-&lt;br&gt;Correlativo de Entrada: 1&lt;br&gt;Prefijo de Salida: S-&lt;br&gt;Correlativo de Salida: 1&lt;br&gt;&lt;br&gt;Para revisar o modificar estos antecedentes, visite el módulo Bodega. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Generación Automatica de Bodega',83,2);</v>
       </c>
       <c r="T73" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20083, 'Redmat','iconstruye@iconstruye.com', 'Generación Automatica de Bodega', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que en el Centro de Gestión &lt;nombrecg&gt; se ha generado automáticamente una Bodega, solicitamos a usted verificar los datos asociados. &lt;br&gt;&lt;br&gt;Código Bodega: 001&lt;br&gt;Nombre Bodega: &lt;nombrebod&gt;&lt;br&gt;Encargado Bodega: &lt;nombencargado&gt;&lt;br&gt;Comentarios: Bodega generada automáticamente por el sistema &lt;br&gt;Prefijo de Entrada: E-&lt;br&gt;Correlativo de Entrada: 1&lt;br&gt;Prefijo de Salida: S-&lt;br&gt;Correlativo de Salida: 1&lt;br&gt;&lt;br&gt;Para revisar o modificar estos antecedentes, visite el módulo Bodega. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Generación Automatica de Bodega');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3083, 'Redmat','iconstruye@iconstruye.com', 'Generación Automatica de Bodega', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que en el Centro de Gestión &lt;nombrecg&gt; se ha generado automáticamente una Bodega, solicitamos a usted verificar los datos asociados. &lt;br&gt;&lt;br&gt;Código Bodega: 001&lt;br&gt;Nombre Bodega: &lt;nombrebod&gt;&lt;br&gt;Encargado Bodega: &lt;nombencargado&gt;&lt;br&gt;Comentarios: Bodega generada automáticamente por el sistema &lt;br&gt;Prefijo de Entrada: E-&lt;br&gt;Correlativo de Entrada: 1&lt;br&gt;Prefijo de Salida: S-&lt;br&gt;Correlativo de Salida: 1&lt;br&gt;&lt;br&gt;Para revisar o modificar estos antecedentes, visite el módulo Bodega. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Generación Automatica de Bodega',83,3);</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>90</v>
       </c>
@@ -12135,17 +12146,17 @@
         <v>517</v>
       </c>
       <c r="S74" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20090, 'Agilice','b2bsalfa@iconstruye.com', 'Nueva OC de SALFACORP &lt;numoc&gt;', '&lt;div style=width:600px;&gt; &lt;p style="font-family:Arial; font-size:12px; text-
-align:left;"&gt;&lt;b&gt;Estimados Sr. &lt;nombreproveedor&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt; Por encargo del &lt;b&gt;Holding Salfacorp&lt;/b&gt; le informamos que el día &lt;fechaenvio&gt; le ha generado la orden de compra N° &lt;numoc&gt;. Para visualizar haga &lt;link&gt;.&lt;br&gt;&lt;br&gt;Para aceptar o rechazar esta orden de compra debe responder este correo, &lt;b&gt;como plazo máximo dentro de 8 horas hábiles&lt;/b&gt;, señalando claramente su decisión. En caso de rechazar la OC debe explicar claramente las razones del rechazo.&lt;br&gt;En caso de cualquier duda o consulta póngase en contacto con Agilice - B2B SALFA al 24861220 o al e-mail &lt;a mailto=b2bsalfa@iconstruye.com&gt;b2bsalfa@iconstruye.com&lt;/a&gt;.&lt;br&gt;&lt;br&gt;&lt;b&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra, responda este correo indicado el nombre y correo electrónico del contacto.&lt;/b&gt;&lt;br&gt;&lt;br&gt;&lt;b&gt;Al aceptar la OC "Preliminar" accederá a la OC oficial de SALFACORP documento válido para proceso de facturación y pago.&lt;/span&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;&lt;a href=https://apps.agilice.com/ &gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://apps.agilice.com/ &gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Agilice y realizar en línea la gestión completa de sus negocios con SALFACORP a través de &lt;a href=https://apps.agilice.com/ &gt;https://apps.agilice.com/&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Agilice, S.A.&lt;br&gt;Servicio de Activación de Órdenes de Compra.&lt;/b&gt;&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;&lt;br&gt;&lt;br&gt; &lt;span style=font-size:10px;&gt;&lt;b&gt;PD1: Recomendamos la utilización de Internet Explorer 7 ó superior.&lt;/span&gt;&lt;/b&gt;&lt;br&gt; &lt;span style=font-size:10px;&gt;&lt;b&gt;PD2: Para visualizar la orden, debe tener Adobe Acrobat (TM) Reader instalado en su computador. &lt;a href=http://get.adobe.com/es/reader&gt;Descarguelo aquí&lt;/a&gt;.&lt;/span&gt;&lt;/b&gt; &lt;/p&gt; &lt;/div&gt; ','Envio OC sistema de Integracion');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2090, 'Agilice','b2bsalfa@iconstruye.com', 'Nueva OC de SALFACORP &lt;numoc&gt;', '&lt;div style=width:600px;&gt; &lt;p style="font-family:Arial; font-size:12px; text-
+align:left;"&gt;&lt;b&gt;Estimados Sr. &lt;nombreproveedor&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt; Por encargo del &lt;b&gt;Holding Salfacorp&lt;/b&gt; le informamos que el día &lt;fechaenvio&gt; le ha generado la orden de compra N° &lt;numoc&gt;. Para visualizar haga &lt;link&gt;.&lt;br&gt;&lt;br&gt;Para aceptar o rechazar esta orden de compra debe responder este correo, &lt;b&gt;como plazo máximo dentro de 8 horas hábiles&lt;/b&gt;, señalando claramente su decisión. En caso de rechazar la OC debe explicar claramente las razones del rechazo.&lt;br&gt;En caso de cualquier duda o consulta póngase en contacto con Agilice - B2B SALFA al 24861220 o al e-mail &lt;a mailto=b2bsalfa@iconstruye.com&gt;b2bsalfa@iconstruye.com&lt;/a&gt;.&lt;br&gt;&lt;br&gt;&lt;b&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra, responda este correo indicado el nombre y correo electrónico del contacto.&lt;/b&gt;&lt;br&gt;&lt;br&gt;&lt;b&gt;Al aceptar la OC "Preliminar" accederá a la OC oficial de SALFACORP documento válido para proceso de facturación y pago.&lt;/span&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;&lt;a href=https://apps.agilice.com/ &gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://apps.agilice.com/ &gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Agilice y realizar en línea la gestión completa de sus negocios con SALFACORP a través de &lt;a href=https://apps.agilice.com/ &gt;https://apps.agilice.com/&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Agilice, S.A.&lt;br&gt;Servicio de Activación de Órdenes de Compra.&lt;/b&gt;&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;&lt;br&gt;&lt;br&gt; &lt;span style=font-size:10px;&gt;&lt;b&gt;PD1: Recomendamos la utilización de Internet Explorer 7 ó superior.&lt;/span&gt;&lt;/b&gt;&lt;br&gt; &lt;span style=font-size:10px;&gt;&lt;b&gt;PD2: Para visualizar la orden, debe tener Adobe Acrobat (TM) Reader instalado en su computador. &lt;a href=http://get.adobe.com/es/reader&gt;Descarguelo aquí&lt;/a&gt;.&lt;/span&gt;&lt;/b&gt; &lt;/p&gt; &lt;/div&gt; ','Envio OC sistema de Integracion',90,2);</v>
       </c>
       <c r="T74" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20090, 'Redmat','b2bsalfa@iconstruye.com', 'Nueva OC de SALFACORP &lt;numoc&gt;', '&lt;div style=width:600px;&gt; &lt;p style="font-family:Arial; font-size:12px; text-
-align:left;"&gt;&lt;b&gt;Estimados Sr. &lt;nombreproveedor&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt; Por encargo del &lt;b&gt;Holding Salfacorp&lt;/b&gt; le informamos que el día &lt;fechaenvio&gt; le ha generado la orden de compra N° &lt;numoc&gt;. Para visualizar haga &lt;link&gt;.&lt;br&gt;&lt;br&gt;Para aceptar o rechazar esta orden de compra debe responder este correo, &lt;b&gt;como plazo máximo dentro de 8 horas hábiles&lt;/b&gt;, señalando claramente su decisión. En caso de rechazar la OC debe explicar claramente las razones del rechazo.&lt;br&gt;En caso de cualquier duda o consulta póngase en contacto con Redmat - B2B SALFA al 24861220 o al e-mail &lt;a mailto=b2bsalfa@iconstruye.com&gt;b2bsalfa@iconstruye.com&lt;/a&gt;.&lt;br&gt;&lt;br&gt;&lt;b&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra, responda este correo indicado el nombre y correo electrónico del contacto.&lt;/b&gt;&lt;br&gt;&lt;br&gt;&lt;b&gt;Al aceptar la OC "Preliminar" accederá a la OC oficial de SALFACORP documento válido para proceso de facturación y pago.&lt;/span&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;&lt;a href=https://redmat.iconstruye.com/ &gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://redmat.iconstruye.com/ &gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Redmat y realizar en línea la gestión completa de sus negocios con SALFACORP a través de &lt;a href=https://redmat.iconstruye.com/ &gt;https://redmat.iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Redmat, S.A.&lt;br&gt;Servicio de Activación de Órdenes de Compra.&lt;/b&gt;&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;&lt;br&gt;&lt;br&gt; &lt;span style=font-size:10px;&gt;&lt;b&gt;PD1: Recomendamos la utilización de Internet Explorer 7 ó superior.&lt;/span&gt;&lt;/b&gt;&lt;br&gt; &lt;span style=font-size:10px;&gt;&lt;b&gt;PD2: Para visualizar la orden, debe tener Adobe Acrobat (TM) Reader instalado en su computador. &lt;a href=http://get.adobe.com/es/reader&gt;Descarguelo aquí&lt;/a&gt;.&lt;/span&gt;&lt;/b&gt; &lt;/p&gt; &lt;/div&gt; ','Envio OC sistema de Integracion');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3090, 'Redmat','b2bsalfa@iconstruye.com', 'Nueva OC de SALFACORP &lt;numoc&gt;', '&lt;div style=width:600px;&gt; &lt;p style="font-family:Arial; font-size:12px; text-
+align:left;"&gt;&lt;b&gt;Estimados Sr. &lt;nombreproveedor&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt; Por encargo del &lt;b&gt;Holding Salfacorp&lt;/b&gt; le informamos que el día &lt;fechaenvio&gt; le ha generado la orden de compra N° &lt;numoc&gt;. Para visualizar haga &lt;link&gt;.&lt;br&gt;&lt;br&gt;Para aceptar o rechazar esta orden de compra debe responder este correo, &lt;b&gt;como plazo máximo dentro de 8 horas hábiles&lt;/b&gt;, señalando claramente su decisión. En caso de rechazar la OC debe explicar claramente las razones del rechazo.&lt;br&gt;En caso de cualquier duda o consulta póngase en contacto con Redmat - B2B SALFA al 24861220 o al e-mail &lt;a mailto=b2bsalfa@iconstruye.com&gt;b2bsalfa@iconstruye.com&lt;/a&gt;.&lt;br&gt;&lt;br&gt;&lt;b&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra, responda este correo indicado el nombre y correo electrónico del contacto.&lt;/b&gt;&lt;br&gt;&lt;br&gt;&lt;b&gt;Al aceptar la OC "Preliminar" accederá a la OC oficial de SALFACORP documento válido para proceso de facturación y pago.&lt;/span&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;&lt;a href=https://redmat.iconstruye.com/ &gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://redmat.iconstruye.com/ &gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Redmat y realizar en línea la gestión completa de sus negocios con SALFACORP a través de &lt;a href=https://redmat.iconstruye.com/ &gt;https://redmat.iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Redmat, S.A.&lt;br&gt;Servicio de Activación de Órdenes de Compra.&lt;/b&gt;&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;&lt;br&gt;&lt;br&gt; &lt;span style=font-size:10px;&gt;&lt;b&gt;PD1: Recomendamos la utilización de Internet Explorer 7 ó superior.&lt;/span&gt;&lt;/b&gt;&lt;br&gt; &lt;span style=font-size:10px;&gt;&lt;b&gt;PD2: Para visualizar la orden, debe tener Adobe Acrobat (TM) Reader instalado en su computador. &lt;a href=http://get.adobe.com/es/reader&gt;Descarguelo aquí&lt;/a&gt;.&lt;/span&gt;&lt;/b&gt; &lt;/p&gt; &lt;/div&gt; ','Envio OC sistema de Integracion',90,3);</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>93</v>
       </c>
@@ -12199,15 +12210,15 @@
         <v>524</v>
       </c>
       <c r="S75" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20093, 'Agilice','iconstruye@iconstruye.com', 'Línea de Pedido de Material Cancelada', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que una línea del siguiente Pedido de Material ha sido Cancelada. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Código Producto: &lt;cod&gt;&lt;br&gt;Cantidad: &lt;cantidad&gt;&lt;br&gt;Descripción: &lt;descripcion&gt;&lt;br&gt;Comentario: &lt;motivocancelacion&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Línea de Pedido de Material');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2093, 'Agilice','iconstruye@iconstruye.com', 'Línea de Pedido de Material Cancelada', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que una línea del siguiente Pedido de Material ha sido Cancelada. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Código Producto: &lt;cod&gt;&lt;br&gt;Cantidad: &lt;cantidad&gt;&lt;br&gt;Descripción: &lt;descripcion&gt;&lt;br&gt;Comentario: &lt;motivocancelacion&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Línea de Pedido de Material',93,2);</v>
       </c>
       <c r="T75" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20093, 'Redmat','iconstruye@iconstruye.com', 'Línea de Pedido de Material Cancelada', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que una línea del siguiente Pedido de Material ha sido Cancelada. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Código Producto: &lt;cod&gt;&lt;br&gt;Cantidad: &lt;cantidad&gt;&lt;br&gt;Descripción: &lt;descripcion&gt;&lt;br&gt;Comentario: &lt;motivocancelacion&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Línea de Pedido de Material');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3093, 'Redmat','iconstruye@iconstruye.com', 'Línea de Pedido de Material Cancelada', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que una línea del siguiente Pedido de Material ha sido Cancelada. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Código Producto: &lt;cod&gt;&lt;br&gt;Cantidad: &lt;cantidad&gt;&lt;br&gt;Descripción: &lt;descripcion&gt;&lt;br&gt;Comentario: &lt;motivocancelacion&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Línea de Pedido de Material',93,3);</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>94</v>
       </c>
@@ -12261,15 +12272,15 @@
         <v>530</v>
       </c>
       <c r="S76" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20094, 'Agilice','iconstruye@iconstruye.com', 'Orden de Compra Cancelada', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el usuario(a) &lt;usuariocancela&gt; ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Orden de Compra');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2094, 'Agilice','iconstruye@iconstruye.com', 'Orden de Compra Cancelada', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el usuario(a) &lt;usuariocancela&gt; ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Orden de Compra',94,2);</v>
       </c>
       <c r="T76" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20094, 'Redmat','iconstruye@iconstruye.com', 'Orden de Compra Cancelada', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el usuario(a) &lt;usuariocancela&gt; ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Orden de Compra');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3094, 'Redmat','iconstruye@iconstruye.com', 'Orden de Compra Cancelada', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el usuario(a) &lt;usuariocancela&gt; ha Cancelado la Orden de Compra Nº &lt;numoc&gt;, &lt;nomoc&gt;.&lt;br&gt;&lt;br&gt;Para más antecedentes, ingrese al módulo Compras. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Orden de Compra',94,3);</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <v>91</v>
       </c>
@@ -12323,15 +12334,15 @@
         <v>537</v>
       </c>
       <c r="S77" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20091, 'Agilice','iconstruye@iconstruye.com', 'Traspaso Por Recibir &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Traspaso por Recibir:&lt;br&gt;&lt;br&gt;Usuario: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá Aceptar este traspaso ingresando al módulo Bodega, opción Traspasos por Recibir. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Notificacion de traspaso');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2091, 'Agilice','iconstruye@iconstruye.com', 'Traspaso Por Recibir &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Traspaso por Recibir:&lt;br&gt;&lt;br&gt;Usuario: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá Aceptar este traspaso ingresando al módulo Bodega, opción Traspasos por Recibir. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Notificacion de traspaso',91,2);</v>
       </c>
       <c r="T77" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20091, 'Redmat','iconstruye@iconstruye.com', 'Traspaso Por Recibir &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Traspaso por Recibir:&lt;br&gt;&lt;br&gt;Usuario: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá Aceptar este traspaso ingresando al módulo Bodega, opción Traspasos por Recibir. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Notificacion de traspaso');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3091, 'Redmat','iconstruye@iconstruye.com', 'Traspaso Por Recibir &lt;numtraspaso&gt;', 'Estimado(a) Sr(a). &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Traspaso por Recibir:&lt;br&gt;&lt;br&gt;Usuario: &lt;nombre de quien hace el traspaso&gt;&lt;br&gt;N° del Traspaso: &lt;numtraspaso&gt;&lt;br&gt;N° del Documento: &lt;numrespaldo&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha del Traspaso: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá Aceptar este traspaso ingresando al módulo Bodega, opción Traspasos por Recibir. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Notificacion de traspaso',91,3);</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
         <v>95</v>
       </c>
@@ -12385,15 +12396,15 @@
         <v>544</v>
       </c>
       <c r="S78" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20095, 'Agilice','iconstruye@iconstruye.com', 'Nueva OC &lt;numoc&gt;', 'Estimado Sres. &lt;nombreproveedor&gt;: &lt;br&gt; &lt;br&gt;Junto con saludarle, le informamos que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt; le ha enviado la Orden de Compra número &lt;numoc&gt;. &lt;br&gt; &lt;br&gt;Para Aceptarla o Rechazarla, ingrese a &lt;link&gt;&lt;br&gt; &lt;br&gt; Atentamente, &lt;br&gt; Equipo Agilice','Orden de Compra, Aviso');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2095, 'Agilice','iconstruye@iconstruye.com', 'Nueva OC &lt;numoc&gt;', 'Estimado Sres. &lt;nombreproveedor&gt;: &lt;br&gt; &lt;br&gt;Junto con saludarle, le informamos que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt; le ha enviado la Orden de Compra número &lt;numoc&gt;. &lt;br&gt; &lt;br&gt;Para Aceptarla o Rechazarla, ingrese a &lt;link&gt;&lt;br&gt; &lt;br&gt; Atentamente, &lt;br&gt; Equipo Agilice','Orden de Compra, Aviso',95,2);</v>
       </c>
       <c r="T78" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20095, 'Redmat','iconstruye@iconstruye.com', 'Nueva OC &lt;numoc&gt;', 'Estimado Sres. &lt;nombreproveedor&gt;: &lt;br&gt; &lt;br&gt;Junto con saludarle, le informamos que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt; le ha enviado la Orden de Compra número &lt;numoc&gt;. &lt;br&gt; &lt;br&gt;Para Aceptarla o Rechazarla, ingrese a &lt;link&gt;&lt;br&gt; &lt;br&gt; Atentamente, &lt;br&gt; Equipo Redmat','Orden de Compra, Aviso');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3095, 'Redmat','iconstruye@iconstruye.com', 'Nueva OC &lt;numoc&gt;', 'Estimado Sres. &lt;nombreproveedor&gt;: &lt;br&gt; &lt;br&gt;Junto con saludarle, le informamos que el &lt;fechaenvio&gt;, la empresa &lt;nombempresa&gt; le ha enviado la Orden de Compra número &lt;numoc&gt;. &lt;br&gt; &lt;br&gt;Para Aceptarla o Rechazarla, ingrese a &lt;link&gt;&lt;br&gt; &lt;br&gt; Atentamente, &lt;br&gt; Equipo Redmat','Orden de Compra, Aviso',95,3);</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
         <v>100</v>
       </c>
@@ -12447,15 +12458,15 @@
         <v>550</v>
       </c>
       <c r="S79" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20100, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Materiales con Presupuesto Excedido', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que se ha creado un Pedido de Material con presupuesto excedido. &lt;br&gt;&lt;br&gt;Nombre PM: &lt;nompm&gt;&lt;br&gt;Centro de Gestión:&lt;nomorgc&gt;&lt;br&gt;Usuario creador del PM: &lt;usuariopm&gt;&lt;br&gt;Fecha creación PM:&lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;Para ver el documento, visite nuestro m&amp;oacute;dulo de Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido de Materiales con Presupuesto Excedido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20100, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Materiales con Presupuesto Excedido', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que se ha creado un Pedido de Material con presupuesto excedido. &lt;br&gt;&lt;br&gt;Nombre PM: &lt;nompm&gt;&lt;br&gt;Centro de Gestión:&lt;nomorgc&gt;&lt;br&gt;Usuario creador del PM: &lt;usuariopm&gt;&lt;br&gt;Fecha creación PM:&lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;Para ver el documento, visite nuestro m&amp;oacute;dulo de Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido de Materiales con Presupuesto Excedido',100,2);</v>
       </c>
       <c r="T79" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20100, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Materiales con Presupuesto Excedido', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que se ha creado un Pedido de Material con presupuesto excedido. &lt;br&gt;&lt;br&gt;Nombre PM: &lt;nompm&gt;&lt;br&gt;Centro de Gestión:&lt;nomorgc&gt;&lt;br&gt;Usuario creador del PM: &lt;usuariopm&gt;&lt;br&gt;Fecha creación PM:&lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;Para ver el documento, visite nuestro m&amp;oacute;dulo de Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido de Materiales con Presupuesto Excedido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30100, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Materiales con Presupuesto Excedido', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que se ha creado un Pedido de Material con presupuesto excedido. &lt;br&gt;&lt;br&gt;Nombre PM: &lt;nompm&gt;&lt;br&gt;Centro de Gestión:&lt;nomorgc&gt;&lt;br&gt;Usuario creador del PM: &lt;usuariopm&gt;&lt;br&gt;Fecha creación PM:&lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;Para ver el documento, visite nuestro m&amp;oacute;dulo de Pedido de Materiales. &lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido de Materiales con Presupuesto Excedido',100,3);</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80" s="6">
         <v>70</v>
       </c>
@@ -12509,15 +12520,15 @@
         <v>557</v>
       </c>
       <c r="S80" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20070, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Pedido de Equipos', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Equipos en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido de Equipos envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2070, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de Pedido de Equipos', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Equipos en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido de Equipos envío a Aprobación',70,2);</v>
       </c>
       <c r="T80" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20070, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Pedido de Equipos', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Equipos en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido de Equipos envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3070, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de Pedido de Equipos', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Equipos en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido de Equipos envío a Aprobación',70,3);</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
         <v>96</v>
       </c>
@@ -12569,15 +12580,15 @@
         <v>564</v>
       </c>
       <c r="S81" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20096, 'Agilice','iconstruye@iconstruye.com', 'Aviso Vencimiento de &lt;TIPOGARANTIA&gt;', 'Estimado Sr.(a) &lt;nombreusuario&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos a usted que para el siguiente subcontrato existe una garantía por expirar, los datos son: &lt;br&gt;&lt;br&gt;Centro de Gestión: &lt;nombreorgc&gt;&lt;br&gt;Nº del Subcontrato: &lt;numerosubcontrato&gt;&lt;br&gt;Nombre del Subcontrato: &lt;nombresubcontrato&gt;&lt;br&gt;Tipo de Garantía: &lt;tipogarantia&gt;&lt;br&gt;Tipo de Documento: &lt;tipodocumento&gt;&lt;br&gt;Fecha de Vencimiento: &lt;fechavencimiento&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentemente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;4861111','Aviso de Vencimiento de Garantia');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2096, 'Agilice','iconstruye@iconstruye.com', 'Aviso Vencimiento de &lt;TIPOGARANTIA&gt;', 'Estimado Sr.(a) &lt;nombreusuario&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos a usted que para el siguiente subcontrato existe una garantía por expirar, los datos son: &lt;br&gt;&lt;br&gt;Centro de Gestión: &lt;nombreorgc&gt;&lt;br&gt;Nº del Subcontrato: &lt;numerosubcontrato&gt;&lt;br&gt;Nombre del Subcontrato: &lt;nombresubcontrato&gt;&lt;br&gt;Tipo de Garantía: &lt;tipogarantia&gt;&lt;br&gt;Tipo de Documento: &lt;tipodocumento&gt;&lt;br&gt;Fecha de Vencimiento: &lt;fechavencimiento&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentemente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;4861111','Aviso de Vencimiento de Garantia',96,2);</v>
       </c>
       <c r="T81" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20096, 'Redmat','iconstruye@iconstruye.com', 'Aviso Vencimiento de &lt;TIPOGARANTIA&gt;', 'Estimado Sr.(a) &lt;nombreusuario&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos a usted que para el siguiente subcontrato existe una garantía por expirar, los datos son: &lt;br&gt;&lt;br&gt;Centro de Gestión: &lt;nombreorgc&gt;&lt;br&gt;Nº del Subcontrato: &lt;numerosubcontrato&gt;&lt;br&gt;Nombre del Subcontrato: &lt;nombresubcontrato&gt;&lt;br&gt;Tipo de Garantía: &lt;tipogarantia&gt;&lt;br&gt;Tipo de Documento: &lt;tipodocumento&gt;&lt;br&gt;Fecha de Vencimiento: &lt;fechavencimiento&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentemente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;4861111','Aviso de Vencimiento de Garantia');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3096, 'Redmat','iconstruye@iconstruye.com', 'Aviso Vencimiento de &lt;TIPOGARANTIA&gt;', 'Estimado Sr.(a) &lt;nombreusuario&gt;: &lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos a usted que para el siguiente subcontrato existe una garantía por expirar, los datos son: &lt;br&gt;&lt;br&gt;Centro de Gestión: &lt;nombreorgc&gt;&lt;br&gt;Nº del Subcontrato: &lt;numerosubcontrato&gt;&lt;br&gt;Nombre del Subcontrato: &lt;nombresubcontrato&gt;&lt;br&gt;Tipo de Garantía: &lt;tipogarantia&gt;&lt;br&gt;Tipo de Documento: &lt;tipodocumento&gt;&lt;br&gt;Fecha de Vencimiento: &lt;fechavencimiento&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentemente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;4861111','Aviso de Vencimiento de Garantia',96,3);</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <v>97</v>
       </c>
@@ -12631,15 +12642,15 @@
         <v>570</v>
       </c>
       <c r="S82" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20097, 'Agilice','iconstruye@iconstruye.com', 'Aviso Modificación Linea Convenio', 'Estimado Sr. &lt;usradminconvenio&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombreproveedor&gt; ha realizado una modificación en el Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt; Para Aceptar o Rechazar esta modificación, ingrese a &lt;link&gt; &lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Aviso Modificación Linea Convenio');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2097, 'Agilice','iconstruye@iconstruye.com', 'Aviso Modificación Linea Convenio', 'Estimado Sr. &lt;usradminconvenio&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombreproveedor&gt; ha realizado una modificación en el Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt; Para Aceptar o Rechazar esta modificación, ingrese a &lt;link&gt; &lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Aviso Modificación Linea Convenio',97,2);</v>
       </c>
       <c r="T82" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20097, 'Redmat','iconstruye@iconstruye.com', 'Aviso Modificación Linea Convenio', 'Estimado Sr. &lt;usradminconvenio&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombreproveedor&gt; ha realizado una modificación en el Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt; Para Aceptar o Rechazar esta modificación, ingrese a &lt;link&gt; &lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Aviso Modificación Linea Convenio');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3097, 'Redmat','iconstruye@iconstruye.com', 'Aviso Modificación Linea Convenio', 'Estimado Sr. &lt;usradminconvenio&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombreproveedor&gt; ha realizado una modificación en el Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt; Para Aceptar o Rechazar esta modificación, ingrese a &lt;link&gt; &lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Aviso Modificación Linea Convenio',97,3);</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
         <v>98</v>
       </c>
@@ -12693,15 +12704,15 @@
         <v>576</v>
       </c>
       <c r="S83" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20098, 'Agilice','iconstruye@iconstruye.com', 'Rechazo Modificación Linea Convenio', 'Estimados Sr. &lt;usrproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombrecomprador&gt; No ha Aceptado la modificación del Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Rechazo Modificación Linea Convenio');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2098, 'Agilice','iconstruye@iconstruye.com', 'Rechazo Modificación Linea Convenio', 'Estimados Sr. &lt;usrproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombrecomprador&gt; No ha Aceptado la modificación del Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Rechazo Modificación Linea Convenio',98,2);</v>
       </c>
       <c r="T83" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20098, 'Redmat','iconstruye@iconstruye.com', 'Rechazo Modificación Linea Convenio', 'Estimados Sr. &lt;usrproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombrecomprador&gt; No ha Aceptado la modificación del Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Rechazo Modificación Linea Convenio');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3098, 'Redmat','iconstruye@iconstruye.com', 'Rechazo Modificación Linea Convenio', 'Estimados Sr. &lt;usrproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombrecomprador&gt; No ha Aceptado la modificación del Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Rechazo Modificación Linea Convenio',98,3);</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
         <v>99</v>
       </c>
@@ -12755,15 +12766,15 @@
         <v>582</v>
       </c>
       <c r="S84" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20099, 'Agilice','iconstruye@iconstruye.com', 'Aprobación Modificación Linea Convenio', 'Estimados Sr. &lt;usrproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombrecomprador&gt; aceptó la modificación del Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Aprobación Modificación Linea Convenio');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2099, 'Agilice','iconstruye@iconstruye.com', 'Aprobación Modificación Linea Convenio', 'Estimados Sr. &lt;usrproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombrecomprador&gt; aceptó la modificación del Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Aprobación Modificación Linea Convenio',99,2);</v>
       </c>
       <c r="T84" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20099, 'Redmat','iconstruye@iconstruye.com', 'Aprobación Modificación Linea Convenio', 'Estimados Sr. &lt;usrproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombrecomprador&gt; aceptó la modificación del Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Aprobación Modificación Linea Convenio');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3099, 'Redmat','iconstruye@iconstruye.com', 'Aprobación Modificación Linea Convenio', 'Estimados Sr. &lt;usrproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombrecomprador&gt; aceptó la modificación del Convenio &lt;nombreconvenio&gt;, para el producto &lt;codigomaestro&gt; &lt;descripcion&gt;.&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Aprobación Modificación Linea Convenio',99,3);</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
         <v>101</v>
       </c>
@@ -12815,15 +12826,15 @@
         <v>589</v>
       </c>
       <c r="S85" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20101, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Material Cancelado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Material ha sido Cancelado. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Cancelación: &lt;fechacancelacion&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;motivocancelacion&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Pedido de Material');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20101, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Material Cancelado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Material ha sido Cancelado. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Cancelación: &lt;fechacancelacion&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;motivocancelacion&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cancelación de Pedido de Material',101,2);</v>
       </c>
       <c r="T85" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20101, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Material Cancelado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Material ha sido Cancelado. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Cancelación: &lt;fechacancelacion&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;motivocancelacion&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Pedido de Material');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30101, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Material Cancelado', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Material ha sido Cancelado. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpm&gt;&lt;br&gt;Nombre Pedido: &lt;nompm&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Cancelación: &lt;fechacancelacion&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;motivocancelacion&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cancelación de Pedido de Material',101,3);</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
         <v>74</v>
       </c>
@@ -12877,15 +12888,15 @@
         <v>595</v>
       </c>
       <c r="S86" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20074, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Equipos Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Equipos ha sido Rechazado.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Equipos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido de Equipos Rechazado');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2074, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Equipos Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Equipos ha sido Rechazado.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Equipos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido de Equipos Rechazado',74,2);</v>
       </c>
       <c r="T86" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20074, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Equipos Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Equipos ha sido Rechazado.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Equipos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido de Equipos Rechazado');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3074, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Equipos Rechazado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que el siguiente Pedido de Equipos ha sido Rechazado.&lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Rechazo: &lt;fechaaprobacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para mayores antecedentes, ingrese al módulo Pedido de Equipos. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido de Equipos Rechazado',74,3);</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <v>73</v>
       </c>
@@ -12939,15 +12950,15 @@
         <v>601</v>
       </c>
       <c r="S87" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20073, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Equipos Aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Pedido de Materiales generado por usted ha sido Aprobado.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Aprobación: &lt;fechaaprobacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido de Equipos Aprobado');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2073, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Equipos Aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Pedido de Materiales generado por usted ha sido Aprobado.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Aprobación: &lt;fechaaprobacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido de Equipos Aprobado',73,2);</v>
       </c>
       <c r="T87" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20073, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Equipos Aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Pedido de Materiales generado por usted ha sido Aprobado.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Aprobación: &lt;fechaaprobacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido de Equipos Aprobado');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3073, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Equipos Aprobado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Pedido de Materiales generado por usted ha sido Aprobado.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Aprobación: &lt;fechaaprobacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido de Equipos Aprobado',73,3);</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <v>71</v>
       </c>
@@ -13001,15 +13012,15 @@
         <v>607</v>
       </c>
       <c r="S88" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20071, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Equipos Aprobador Añadido', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo. &lt;br&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido de Equipos Aprobador Añadido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2071, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Equipos Aprobador Añadido', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo. &lt;br&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Pedido de Equipos Aprobador Añadido',71,2);</v>
       </c>
       <c r="T88" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20071, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Equipos Aprobador Añadido', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo. &lt;br&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido de Equipos Aprobador Añadido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3071, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Equipos Aprobador Añadido', 'Estimado Sr. &lt;nombaprobador&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene un nuevo Pedido de Materiales en espera de su Aprobación. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo. &lt;br&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Pedido de Equipos Aprobador Añadido',71,3);</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
         <v>102</v>
       </c>
@@ -13063,15 +13074,15 @@
         <v>613</v>
       </c>
       <c r="S89" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20102, 'Agilice','iconstruye@iconstruye.com', 'Línea de Pedido de Equipos Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludarle, le informamos que el Sr. &lt;nombaprobador&gt; ha eliminado una línea del Pedido de Equipos solicitado por Ud. &lt;br&gt; &lt;br&gt; No. Pedido: &lt;numpe&gt; &lt;br&gt; Nombre Pedido: &lt;nompe&gt; &lt;br&gt; Organización: &lt;nomborgc&gt; &lt;br&gt; Fecha Rechazo: &lt;fechacreacion&gt; &lt;br&gt; Código Prod: &lt;cod&gt; &lt;br&gt; Cantidad : &lt;cantidad&gt; &lt;br&gt; Descripción:&lt;descripcion&gt; &lt;br&gt; Glosa:&lt;glosa&gt; &lt;br&gt; &lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Línea de Pedido de Equipos Rechazada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20102, 'Agilice','iconstruye@iconstruye.com', 'Línea de Pedido de Equipos Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludarle, le informamos que el Sr. &lt;nombaprobador&gt; ha eliminado una línea del Pedido de Equipos solicitado por Ud. &lt;br&gt; &lt;br&gt; No. Pedido: &lt;numpe&gt; &lt;br&gt; Nombre Pedido: &lt;nompe&gt; &lt;br&gt; Organización: &lt;nomborgc&gt; &lt;br&gt; Fecha Rechazo: &lt;fechacreacion&gt; &lt;br&gt; Código Prod: &lt;cod&gt; &lt;br&gt; Cantidad : &lt;cantidad&gt; &lt;br&gt; Descripción:&lt;descripcion&gt; &lt;br&gt; Glosa:&lt;glosa&gt; &lt;br&gt; &lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Línea de Pedido de Equipos Rechazada',102,2);</v>
       </c>
       <c r="T89" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20102, 'Redmat','iconstruye@iconstruye.com', 'Línea de Pedido de Equipos Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludarle, le informamos que el Sr. &lt;nombaprobador&gt; ha eliminado una línea del Pedido de Equipos solicitado por Ud. &lt;br&gt; &lt;br&gt; No. Pedido: &lt;numpe&gt; &lt;br&gt; Nombre Pedido: &lt;nompe&gt; &lt;br&gt; Organización: &lt;nomborgc&gt; &lt;br&gt; Fecha Rechazo: &lt;fechacreacion&gt; &lt;br&gt; Código Prod: &lt;cod&gt; &lt;br&gt; Cantidad : &lt;cantidad&gt; &lt;br&gt; Descripción:&lt;descripcion&gt; &lt;br&gt; Glosa:&lt;glosa&gt; &lt;br&gt; &lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Línea de Pedido de Equipos Rechazada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30102, 'Redmat','iconstruye@iconstruye.com', 'Línea de Pedido de Equipos Rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludarle, le informamos que el Sr. &lt;nombaprobador&gt; ha eliminado una línea del Pedido de Equipos solicitado por Ud. &lt;br&gt; &lt;br&gt; No. Pedido: &lt;numpe&gt; &lt;br&gt; Nombre Pedido: &lt;nompe&gt; &lt;br&gt; Organización: &lt;nomborgc&gt; &lt;br&gt; Fecha Rechazo: &lt;fechacreacion&gt; &lt;br&gt; Código Prod: &lt;cod&gt; &lt;br&gt; Cantidad : &lt;cantidad&gt; &lt;br&gt; Descripción:&lt;descripcion&gt; &lt;br&gt; Glosa:&lt;glosa&gt; &lt;br&gt; &lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Línea de Pedido de Equipos Rechazada',102,3);</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
         <v>76</v>
       </c>
@@ -13125,15 +13136,15 @@
         <v>619</v>
       </c>
       <c r="S90" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20076, 'Agilice','iconstruye@iconstruye.com', 'Asignación de Pedido de Equipos', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que se le ha sido Asignado un nuevo Pedido de Equipos.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpe&gt;/&lt;numlineape&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Asignación de Pedido de Equipos');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2076, 'Agilice','iconstruye@iconstruye.com', 'Asignación de Pedido de Equipos', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que se le ha sido Asignado un nuevo Pedido de Equipos.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpe&gt;/&lt;numlineape&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Asignación de Pedido de Equipos',76,2);</v>
       </c>
       <c r="T90" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20076, 'Redmat','iconstruye@iconstruye.com', 'Asignación de Pedido de Equipos', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que se le ha sido Asignado un nuevo Pedido de Equipos.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpe&gt;/&lt;numlineape&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Asignación de Pedido de Equipos');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3076, 'Redmat','iconstruye@iconstruye.com', 'Asignación de Pedido de Equipos', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que se le ha sido Asignado un nuevo Pedido de Equipos.&lt;br&gt;&lt;br&gt;N° Pedido: &lt;numpe&gt;/&lt;numlineape&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha: &lt;fechacreacion&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;&lt;br&gt;Para revisarlo, visite el módulo Pedido de Equipos.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Asignación de Pedido de Equipos',76,3);</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
         <v>103</v>
       </c>
@@ -13187,15 +13198,15 @@
         <v>625</v>
       </c>
       <c r="S91" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20103, 'Agilice','iconstruye@iconstruye.com', 'Línea de Pedido de Equipos Cancelada', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que una línea del siguiente Pedido de Equipo ha sido Cancelada. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;/&lt;numlineape&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Cancelación: &lt;fechacreacion&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Código Producto: &lt;cod&gt;&lt;br&gt;Cantidad: &lt;cantidad&gt;&lt;br&gt;Descripción: &lt;descripcion&gt;&lt;br&gt;Comentario: &lt;agregar aquí el motivo de la cancelación&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Línea de Pedido de Equipos Cancelada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20103, 'Agilice','iconstruye@iconstruye.com', 'Línea de Pedido de Equipos Cancelada', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que una línea del siguiente Pedido de Equipo ha sido Cancelada. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;/&lt;numlineape&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Cancelación: &lt;fechacreacion&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Código Producto: &lt;cod&gt;&lt;br&gt;Cantidad: &lt;cantidad&gt;&lt;br&gt;Descripción: &lt;descripcion&gt;&lt;br&gt;Comentario: &lt;agregar aquí el motivo de la cancelación&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Línea de Pedido de Equipos Cancelada',103,2);</v>
       </c>
       <c r="T91" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20103, 'Redmat','iconstruye@iconstruye.com', 'Línea de Pedido de Equipos Cancelada', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que una línea del siguiente Pedido de Equipo ha sido Cancelada. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;/&lt;numlineape&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Cancelación: &lt;fechacreacion&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Código Producto: &lt;cod&gt;&lt;br&gt;Cantidad: &lt;cantidad&gt;&lt;br&gt;Descripción: &lt;descripcion&gt;&lt;br&gt;Comentario: &lt;agregar aquí el motivo de la cancelación&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Línea de Pedido de Equipos Cancelada');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30103, 'Redmat','iconstruye@iconstruye.com', 'Línea de Pedido de Equipos Cancelada', 'Estimado Sr.:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que una línea del siguiente Pedido de Equipo ha sido Cancelada. &lt;br&gt;&lt;br&gt;Nº Pedido: &lt;numpe&gt;/&lt;numlineape&gt;&lt;br&gt;Nombre Pedido: &lt;nompe&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Cancelación: &lt;fechacreacion&gt;&lt;br&gt;Cancelado por: &lt;nombaprobador&gt;&lt;br&gt;Código Producto: &lt;cod&gt;&lt;br&gt;Cantidad: &lt;cantidad&gt;&lt;br&gt;Descripción: &lt;descripcion&gt;&lt;br&gt;Comentario: &lt;agregar aquí el motivo de la cancelación&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Línea de Pedido de Equipos Cancelada',103,3);</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
         <v>75</v>
       </c>
@@ -13249,15 +13260,15 @@
         <v>632</v>
       </c>
       <c r="S92" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20075, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Equipos en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;: &lt;br&gt; &lt;br&gt; Tiene un nuevo Pedido de Equipos esperando en su Lista de Administración. &lt;br&gt; &lt;br&gt; No. Pedido : &lt;numpm&gt; &lt;br&gt; Nombre Pedido : &lt;nompm&gt; &lt;br&gt; Organización : &lt;nomborgc&gt; &lt;br&gt; Fecha: &lt;fechacreacion&gt; &lt;br&gt; &lt;br&gt; Solicitante: &lt;nombsolicitante&gt; &lt;br&gt; &lt;br&gt; Para verlo, visite nuestro módulo de Pedido de Equipos. &lt;br&gt; &lt;br&gt; &lt;br&gt; Atentamente, &lt;br&gt; &lt;br&gt; Agilice &lt;br&gt; Mi brazo derecho &lt;br&gt; &lt;link&gt; &lt;br&gt;','Pedido Equipos, Notifica Super Administrador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2075, 'Agilice','iconstruye@iconstruye.com', 'Pedido de Equipos en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;: &lt;br&gt; &lt;br&gt; Tiene un nuevo Pedido de Equipos esperando en su Lista de Administración. &lt;br&gt; &lt;br&gt; No. Pedido : &lt;numpm&gt; &lt;br&gt; Nombre Pedido : &lt;nompm&gt; &lt;br&gt; Organización : &lt;nomborgc&gt; &lt;br&gt; Fecha: &lt;fechacreacion&gt; &lt;br&gt; &lt;br&gt; Solicitante: &lt;nombsolicitante&gt; &lt;br&gt; &lt;br&gt; Para verlo, visite nuestro módulo de Pedido de Equipos. &lt;br&gt; &lt;br&gt; &lt;br&gt; Atentamente, &lt;br&gt; &lt;br&gt; Agilice &lt;br&gt; Mi brazo derecho &lt;br&gt; &lt;link&gt; &lt;br&gt;','Pedido Equipos, Notifica Super Administrador',75,2);</v>
       </c>
       <c r="T92" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20075, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Equipos en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;: &lt;br&gt; &lt;br&gt; Tiene un nuevo Pedido de Equipos esperando en su Lista de Administración. &lt;br&gt; &lt;br&gt; No. Pedido : &lt;numpm&gt; &lt;br&gt; Nombre Pedido : &lt;nompm&gt; &lt;br&gt; Organización : &lt;nomborgc&gt; &lt;br&gt; Fecha: &lt;fechacreacion&gt; &lt;br&gt; &lt;br&gt; Solicitante: &lt;nombsolicitante&gt; &lt;br&gt; &lt;br&gt; Para verlo, visite nuestro módulo de Pedido de Equipos. &lt;br&gt; &lt;br&gt; &lt;br&gt; Atentamente, &lt;br&gt; &lt;br&gt; Redmat &lt;br&gt; Mi brazo derecho &lt;br&gt; &lt;link&gt; &lt;br&gt;','Pedido Equipos, Notifica Super Administrador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3075, 'Redmat','iconstruye@iconstruye.com', 'Pedido de Equipos en Lista de Administración', 'Estimado Sr. &lt;nombaprobador&gt;: &lt;br&gt; &lt;br&gt; Tiene un nuevo Pedido de Equipos esperando en su Lista de Administración. &lt;br&gt; &lt;br&gt; No. Pedido : &lt;numpm&gt; &lt;br&gt; Nombre Pedido : &lt;nompm&gt; &lt;br&gt; Organización : &lt;nomborgc&gt; &lt;br&gt; Fecha: &lt;fechacreacion&gt; &lt;br&gt; &lt;br&gt; Solicitante: &lt;nombsolicitante&gt; &lt;br&gt; &lt;br&gt; Para verlo, visite nuestro módulo de Pedido de Equipos. &lt;br&gt; &lt;br&gt; &lt;br&gt; Atentamente, &lt;br&gt; &lt;br&gt; Redmat &lt;br&gt; Mi brazo derecho &lt;br&gt; &lt;link&gt; &lt;br&gt;','Pedido Equipos, Notifica Super Administrador',75,3);</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <v>104</v>
       </c>
@@ -13311,15 +13322,15 @@
         <v>639</v>
       </c>
       <c r="S93" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20104, 'Agilice','iconstruye@iconstruye.com', 'Verificación Archivo Excel Carga Presupuesto', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;El proceso de verificación de la planilla a cargar &lt;nombreplanilla&gt; contiene los siguientes recursos que no se encuentran en el maestro de materiales del centro de gestión &lt;centrogestion&gt;:&lt;br&gt;&lt;br&gt;&lt;recursos&gt;&lt;br&gt;&lt;br&gt;Para poder realizar la carga de su presupuesto deberá revisar los recursos informados y solicitar la creación si corresponde.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Presupuesto, Error Carga planilla');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20104, 'Agilice','iconstruye@iconstruye.com', 'Verificación Archivo Excel Carga Presupuesto', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;El proceso de verificación de la planilla a cargar &lt;nombreplanilla&gt; contiene los siguientes recursos que no se encuentran en el maestro de materiales del centro de gestión &lt;centrogestion&gt;:&lt;br&gt;&lt;br&gt;&lt;recursos&gt;&lt;br&gt;&lt;br&gt;Para poder realizar la carga de su presupuesto deberá revisar los recursos informados y solicitar la creación si corresponde.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Presupuesto, Error Carga planilla',104,2);</v>
       </c>
       <c r="T93" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20104, 'Redmat','iconstruye@iconstruye.com', 'Verificación Archivo Excel Carga Presupuesto', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;El proceso de verificación de la planilla a cargar &lt;nombreplanilla&gt; contiene los siguientes recursos que no se encuentran en el maestro de materiales del centro de gestión &lt;centrogestion&gt;:&lt;br&gt;&lt;br&gt;&lt;recursos&gt;&lt;br&gt;&lt;br&gt;Para poder realizar la carga de su presupuesto deberá revisar los recursos informados y solicitar la creación si corresponde.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Presupuesto, Error Carga planilla');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30104, 'Redmat','iconstruye@iconstruye.com', 'Verificación Archivo Excel Carga Presupuesto', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;El proceso de verificación de la planilla a cargar &lt;nombreplanilla&gt; contiene los siguientes recursos que no se encuentran en el maestro de materiales del centro de gestión &lt;centrogestion&gt;:&lt;br&gt;&lt;br&gt;&lt;recursos&gt;&lt;br&gt;&lt;br&gt;Para poder realizar la carga de su presupuesto deberá revisar los recursos informados y solicitar la creación si corresponde.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Presupuesto, Error Carga planilla',104,3);</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
         <v>105</v>
       </c>
@@ -13373,15 +13384,15 @@
         <v>645</v>
       </c>
       <c r="S94" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20105, 'Agilice','iconstruye@iconstruye.com', 'Aviso Orden Despacho', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Orden de Despacho:&lt;br&gt;&lt;br&gt;Usuario: &lt;nombreusuarioorigen&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha Solicitud Despacho: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá generar el Despacho ingresando al módulo Bodega, opción Salida/Despachos Pendientes. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Aviso Orden Despacho');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20105, 'Agilice','iconstruye@iconstruye.com', 'Aviso Orden Despacho', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Orden de Despacho:&lt;br&gt;&lt;br&gt;Usuario: &lt;nombreusuarioorigen&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha Solicitud Despacho: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá generar el Despacho ingresando al módulo Bodega, opción Salida/Despachos Pendientes. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Aviso Orden Despacho',105,2);</v>
       </c>
       <c r="T94" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20105, 'Redmat','iconstruye@iconstruye.com', 'Aviso Orden Despacho', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Orden de Despacho:&lt;br&gt;&lt;br&gt;Usuario: &lt;nombreusuarioorigen&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha Solicitud Despacho: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá generar el Despacho ingresando al módulo Bodega, opción Salida/Despachos Pendientes. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Aviso Orden Despacho');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30105, 'Redmat','iconstruye@iconstruye.com', 'Aviso Orden Despacho', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Orden de Despacho:&lt;br&gt;&lt;br&gt;Usuario: &lt;nombreusuarioorigen&gt;&lt;br&gt;Centro de Gestión de origen: &lt;nomorgc&gt;&lt;br&gt;Fecha Solicitud Despacho: &lt;fechaenvio&gt;&lt;br&gt;Centro de Gestión de destino: &lt;nomorgcdestino&gt;&lt;br&gt;&lt;br&gt;Podrá generar el Despacho ingresando al módulo Bodega, opción Salida/Despachos Pendientes. En caso de requerir información adicional, comuníquese con nosotros al 486 11 11.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Aviso Orden Despacho',105,3);</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
         <v>106</v>
       </c>
@@ -13435,15 +13446,15 @@
         <v>651</v>
       </c>
       <c r="S95" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20106, 'Agilice','iconstruye@iconstruye.com', 'Subcontrato aprobado', 'Estimado(a) Sr(a).:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato se encuentra ingresado en iconstruye, y disponible para ser impreso.&lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice &lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Receptor Mensajeria');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20106, 'Agilice','iconstruye@iconstruye.com', 'Subcontrato aprobado', 'Estimado(a) Sr(a).:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato se encuentra ingresado en iconstruye, y disponible para ser impreso.&lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice &lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Subcontrato, Receptor Mensajeria',106,2);</v>
       </c>
       <c r="T95" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20106, 'Redmat','iconstruye@iconstruye.com', 'Subcontrato aprobado', 'Estimado(a) Sr(a).:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato se encuentra ingresado en iconstruye, y disponible para ser impreso.&lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat &lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Receptor Mensajeria');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30106, 'Redmat','iconstruye@iconstruye.com', 'Subcontrato aprobado', 'Estimado(a) Sr(a).:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Subcontrato se encuentra ingresado en iconstruye, y disponible para ser impreso.&lt;br&gt;&lt;br&gt;Nº Subcontrato: &lt;numsc&gt;&lt;br&gt;Nombre: &lt;nomsc&gt; &lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha Solicitud: &lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat &lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Subcontrato, Receptor Mensajeria',106,3);</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
         <v>107</v>
       </c>
@@ -13499,15 +13510,15 @@
         <v>659</v>
       </c>
       <c r="S96" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20107, 'Agilice','b2bsalfa@iconstruye.com', ' NUEVA OC  SALFA - &lt;numoc&gt;', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el &lt;fechaenvio&gt; SALFA le ha enviado la Orden de Compra Nº &lt;numoc&gt;.&lt;br&gt;&lt;br&gt;A nombre de Don Andrés Delpiano, Gerente de Abastecimiento de SALFA, le solicitamos Aceptar esta OC, en el menor tiempo posible, en &lt;link&gt; o desde su dispositivo móvil en &lt;link2&gt;.&lt;br&gt;&lt;br&gt;En caso de rechazo, SALFA necesita que indique claramente en los comentarios las razones de esta decisión.&lt;br&gt;&lt;br&gt;En caso de cualquier duda o consulta póngase en contacto con nuestra Mesa de Activación de OC en Agilice al fono 4861220 o por mail b2bsalfa@iconstruye.com&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Servicio Activación de OC&lt;br&gt;B2B SALFA Agilice&lt;br&gt;&lt;img height=28px width=124px src=https://apps.agilice.com/img/logo-agilice.png img&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;img height=28px width=124px src=http://cl.iconstruye.com/images/logo_salfa.jpg img&gt;','Orden de Compra, Aviso Proveedor (Sólo SALFA)');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20107, 'Agilice','b2bsalfa@iconstruye.com', ' NUEVA OC  SALFA - &lt;numoc&gt;', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el &lt;fechaenvio&gt; SALFA le ha enviado la Orden de Compra Nº &lt;numoc&gt;.&lt;br&gt;&lt;br&gt;A nombre de Don Andrés Delpiano, Gerente de Abastecimiento de SALFA, le solicitamos Aceptar esta OC, en el menor tiempo posible, en &lt;link&gt; o desde su dispositivo móvil en &lt;link2&gt;.&lt;br&gt;&lt;br&gt;En caso de rechazo, SALFA necesita que indique claramente en los comentarios las razones de esta decisión.&lt;br&gt;&lt;br&gt;En caso de cualquier duda o consulta póngase en contacto con nuestra Mesa de Activación de OC en Agilice al fono 4861220 o por mail b2bsalfa@iconstruye.com&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Servicio Activación de OC&lt;br&gt;B2B SALFA Agilice&lt;br&gt;&lt;img height=28px width=124px src=https://apps.agilice.com/img/logo-agilice.png img&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;img height=28px width=124px src=http://cl.iconstruye.com/images/logo_salfa.jpg img&gt;','Orden de Compra, Aviso Proveedor (Sólo SALFA)',107,2);</v>
       </c>
       <c r="T96" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20107, 'Redmat','b2bsalfa@iconstruye.com', ' NUEVA OC  SALFA - &lt;numoc&gt;', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el &lt;fechaenvio&gt; SALFA le ha enviado la Orden de Compra Nº &lt;numoc&gt;.&lt;br&gt;&lt;br&gt;A nombre de Don Andrés Delpiano, Gerente de Abastecimiento de SALFA, le solicitamos Aceptar esta OC, en el menor tiempo posible, en &lt;link&gt; o desde su dispositivo móvil en &lt;link2&gt;.&lt;br&gt;&lt;br&gt;En caso de rechazo, SALFA necesita que indique claramente en los comentarios las razones de esta decisión.&lt;br&gt;&lt;br&gt;En caso de cualquier duda o consulta póngase en contacto con nuestra Mesa de Activación de OC en Redmat al fono 4861220 o por mail b2bsalfa@iconstruye.com&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Servicio Activación de OC&lt;br&gt;B2B SALFA Redmat&lt;br&gt;&lt;img height=28px width=124px src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;img height=28px width=124px src=http://cl.iconstruye.com/images/logo_salfa.jpg img&gt;','Orden de Compra, Aviso Proveedor (Sólo SALFA)');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30107, 'Redmat','b2bsalfa@iconstruye.com', ' NUEVA OC  SALFA - &lt;numoc&gt;', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el &lt;fechaenvio&gt; SALFA le ha enviado la Orden de Compra Nº &lt;numoc&gt;.&lt;br&gt;&lt;br&gt;A nombre de Don Andrés Delpiano, Gerente de Abastecimiento de SALFA, le solicitamos Aceptar esta OC, en el menor tiempo posible, en &lt;link&gt; o desde su dispositivo móvil en &lt;link2&gt;.&lt;br&gt;&lt;br&gt;En caso de rechazo, SALFA necesita que indique claramente en los comentarios las razones de esta decisión.&lt;br&gt;&lt;br&gt;En caso de cualquier duda o consulta póngase en contacto con nuestra Mesa de Activación de OC en Redmat al fono 4861220 o por mail b2bsalfa@iconstruye.com&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Servicio Activación de OC&lt;br&gt;B2B SALFA Redmat&lt;br&gt;&lt;img height=28px width=124px src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;img height=28px width=124px src=http://cl.iconstruye.com/images/logo_salfa.jpg img&gt;','Orden de Compra, Aviso Proveedor (Sólo SALFA)',107,3);</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
         <v>108</v>
       </c>
@@ -13561,15 +13572,15 @@
         <v>666</v>
       </c>
       <c r="S97" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20108, 'Agilice','iconstruye@iconstruye.com', 'Solicitud VºBº Ajuste de Factura', 'Estimado Sr. &lt;nombredestino&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su V°B° de ajustes.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombresolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfactura&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Envío: &lt;fechaenvio&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Solicitud VºBº Ajuste Factura');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20108, 'Agilice','iconstruye@iconstruye.com', 'Solicitud VºBº Ajuste de Factura', 'Estimado Sr. &lt;nombredestino&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su V°B° de ajustes.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombresolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfactura&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Envío: &lt;fechaenvio&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Solicitud VºBº Ajuste Factura',108,2);</v>
       </c>
       <c r="T97" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20108, 'Redmat','iconstruye@iconstruye.com', 'Solicitud VºBº Ajuste de Factura', 'Estimado Sr. &lt;nombredestino&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su V°B° de ajustes.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombresolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfactura&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Envío: &lt;fechaenvio&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Solicitud VºBº Ajuste Factura');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30108, 'Redmat','iconstruye@iconstruye.com', 'Solicitud VºBº Ajuste de Factura', 'Estimado Sr. &lt;nombredestino&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Factura a la espera de su V°B° de ajustes.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombresolicitante&gt;&lt;br&gt;N° de Factura: &lt;numfactura&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Envío: &lt;fechaenvio&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Solicitud VºBº Ajuste Factura',108,3);</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
         <v>110</v>
       </c>
@@ -13623,15 +13634,15 @@
         <v>672</v>
       </c>
       <c r="S98" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20110, 'Agilice','iconstruye@iconstruye.com', 'Mail Unitario Proveedor IR', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; La empresa &lt;b&gt;&lt;nombre_empresa_c&gt;&lt;/b&gt; ha enviado el siguiente mensaje, a través del Registro de Proveedores de Agilice: &lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;mensaje&gt;&lt;/p&gt; &lt;br&gt; Cualquier consulta asociada al contenido de este mensaje, debe ser gestionado con la empresa que lo emite. &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Mail Unitario Proveedor IR');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20110, 'Agilice','iconstruye@iconstruye.com', 'Mail Unitario Proveedor IR', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; La empresa &lt;b&gt;&lt;nombre_empresa_c&gt;&lt;/b&gt; ha enviado el siguiente mensaje, a través del Registro de Proveedores de Agilice: &lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;mensaje&gt;&lt;/p&gt; &lt;br&gt; Cualquier consulta asociada al contenido de este mensaje, debe ser gestionado con la empresa que lo emite. &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Mail Unitario Proveedor IR',110,2);</v>
       </c>
       <c r="T98" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20110, 'Redmat','iconstruye@iconstruye.com', 'Mail Unitario Proveedor IR', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; La empresa &lt;b&gt;&lt;nombre_empresa_c&gt;&lt;/b&gt; ha enviado el siguiente mensaje, a través del Registro de Proveedores de Redmat: &lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;mensaje&gt;&lt;/p&gt; &lt;br&gt; Cualquier consulta asociada al contenido de este mensaje, debe ser gestionado con la empresa que lo emite. &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Mail Unitario Proveedor IR');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30110, 'Redmat','iconstruye@iconstruye.com', 'Mail Unitario Proveedor IR', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; La empresa &lt;b&gt;&lt;nombre_empresa_c&gt;&lt;/b&gt; ha enviado el siguiente mensaje, a través del Registro de Proveedores de Redmat: &lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;mensaje&gt;&lt;/p&gt; &lt;br&gt; Cualquier consulta asociada al contenido de este mensaje, debe ser gestionado con la empresa que lo emite. &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Mail Unitario Proveedor IR',110,3);</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
         <v>111</v>
       </c>
@@ -13685,15 +13696,15 @@
         <v>672</v>
       </c>
       <c r="S99" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20111, 'Agilice','iconstruye@iconstruye.com', 'Mail Grupo Proveedor IR', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; La empresa &lt;b&gt;&lt;nombre_empresa_c&gt;&lt;/b&gt; ha enviado el siguiente mensaje, a través del Registro de Proveedores de Agilice: &lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;mensaje&gt;&lt;/p&gt; &lt;br&gt; Cualquier consulta asociada al contenido de este mensaje, debe ser gestionado con la empresa que lo emite. &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Mail Grupo Proveedor IR');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20111, 'Agilice','iconstruye@iconstruye.com', 'Mail Grupo Proveedor IR', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; La empresa &lt;b&gt;&lt;nombre_empresa_c&gt;&lt;/b&gt; ha enviado el siguiente mensaje, a través del Registro de Proveedores de Agilice: &lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;mensaje&gt;&lt;/p&gt; &lt;br&gt; Cualquier consulta asociada al contenido de este mensaje, debe ser gestionado con la empresa que lo emite. &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Mail Grupo Proveedor IR',111,2);</v>
       </c>
       <c r="T99" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20111, 'Redmat','iconstruye@iconstruye.com', 'Mail Grupo Proveedor IR', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; La empresa &lt;b&gt;&lt;nombre_empresa_c&gt;&lt;/b&gt; ha enviado el siguiente mensaje, a través del Registro de Proveedores de Redmat: &lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;mensaje&gt;&lt;/p&gt; &lt;br&gt; Cualquier consulta asociada al contenido de este mensaje, debe ser gestionado con la empresa que lo emite. &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Mail Grupo Proveedor IR');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30111, 'Redmat','iconstruye@iconstruye.com', 'Mail Grupo Proveedor IR', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; La empresa &lt;b&gt;&lt;nombre_empresa_c&gt;&lt;/b&gt; ha enviado el siguiente mensaje, a través del Registro de Proveedores de Redmat: &lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;mensaje&gt;&lt;/p&gt; &lt;br&gt; Cualquier consulta asociada al contenido de este mensaje, debe ser gestionado con la empresa que lo emite. &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Mail Grupo Proveedor IR',111,3);</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <v>112</v>
       </c>
@@ -13747,15 +13758,15 @@
         <v>680</v>
       </c>
       <c r="S100" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20112, 'Agilice','iconstruye@iconstruye.com', 'Aviso de Vencimiento de Archivo en IRegistro', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; El Registro de Proveedores de Agilice informa que el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; ubicado en &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, vencerá el día &lt;b&gt;&lt;fecha_vencimiento&gt;&lt;/b&gt;, por lo cual solicitamos gestionar una nueva versión del mismo, si es que corresponde. &lt;/p&gt; &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Mail Vencimiento Archivo IR');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20112, 'Agilice','iconstruye@iconstruye.com', 'Aviso de Vencimiento de Archivo en IRegistro', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; El Registro de Proveedores de Agilice informa que el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; ubicado en &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, vencerá el día &lt;b&gt;&lt;fecha_vencimiento&gt;&lt;/b&gt;, por lo cual solicitamos gestionar una nueva versión del mismo, si es que corresponde. &lt;/p&gt; &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Mail Vencimiento Archivo IR',112,2);</v>
       </c>
       <c r="T100" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20112, 'Redmat','iconstruye@iconstruye.com', 'Aviso de Vencimiento de Archivo en IRegistro', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; El Registro de Proveedores de Redmat informa que el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; ubicado en &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, vencerá el día &lt;b&gt;&lt;fecha_vencimiento&gt;&lt;/b&gt;, por lo cual solicitamos gestionar una nueva versión del mismo, si es que corresponde. &lt;/p&gt; &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Mail Vencimiento Archivo IR');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30112, 'Redmat','iconstruye@iconstruye.com', 'Aviso de Vencimiento de Archivo en IRegistro', 'Estimados Srs: &lt;br&gt; &lt;b&gt;&lt;usrproveedor&gt;&lt;/b&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt; El Registro de Proveedores de Redmat informa que el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; ubicado en &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, vencerá el día &lt;b&gt;&lt;fecha_vencimiento&gt;&lt;/b&gt;, por lo cual solicitamos gestionar una nueva versión del mismo, si es que corresponde. &lt;/p&gt; &lt;br&gt;&lt;br&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt; &lt;link&gt; &lt;br&gt; Mesa de Ayuda &lt;br&gt; 486 11 11 &lt;br&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Mail Vencimiento Archivo IR',112,3);</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A101" s="6">
         <v>113</v>
       </c>
@@ -13809,15 +13820,15 @@
         <v>687</v>
       </c>
       <c r="S101" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20113, 'Agilice','iconstruye@iconstruye.com', 'Aviso de Creación de Material', '&lt;div style=width:600px;&gt;&lt;p style="font-family:Arial; font-size:12px; text-align:left;"&gt;&lt;b&gt;Estimado Sr(a). &lt;usuariosolicitante&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de creación de código enviada el día &lt;fechaenvio&gt;, del centro de gestión &lt;nomorgc&gt; a sido aprobada por el usuario &lt;nomusuarioatiende&gt;.&lt;b&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;MATERIAL SOLICITADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Descripción:&lt;/td&gt;&lt;td&gt;&lt;descripcion1&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;b&gt;MATERIAL CREADO&lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Código: &lt;/td&gt;&lt;td&gt;&lt;codigo2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Descripción: &lt;/td&gt;&lt;td&gt;&lt;descripcion2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad2&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Estado: &lt;/td&gt;&lt;td&gt;&lt;estadomaterial&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Agilice S.A. &lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se crea los materiales solicitados y que estan pendientes');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20113, 'Agilice','iconstruye@iconstruye.com', 'Aviso de Creación de Material', '&lt;div style=width:600px;&gt;&lt;p style="font-family:Arial; font-size:12px; text-align:left;"&gt;&lt;b&gt;Estimado Sr(a). &lt;usuariosolicitante&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de creación de código enviada el día &lt;fechaenvio&gt;, del centro de gestión &lt;nomorgc&gt; a sido aprobada por el usuario &lt;nomusuarioatiende&gt;.&lt;b&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;MATERIAL SOLICITADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Descripción:&lt;/td&gt;&lt;td&gt;&lt;descripcion1&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;b&gt;MATERIAL CREADO&lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Código: &lt;/td&gt;&lt;td&gt;&lt;codigo2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Descripción: &lt;/td&gt;&lt;td&gt;&lt;descripcion2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad2&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Estado: &lt;/td&gt;&lt;td&gt;&lt;estadomaterial&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Agilice S.A. &lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se crea los materiales solicitados y que estan pendientes',113,2);</v>
       </c>
       <c r="T101" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20113, 'Redmat','iconstruye@iconstruye.com', 'Aviso de Creación de Material', '&lt;div style=width:600px;&gt;&lt;p style="font-family:Arial; font-size:12px; text-align:left;"&gt;&lt;b&gt;Estimado Sr(a). &lt;usuariosolicitante&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de creación de código enviada el día &lt;fechaenvio&gt;, del centro de gestión &lt;nomorgc&gt; a sido aprobada por el usuario &lt;nomusuarioatiende&gt;.&lt;b&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;MATERIAL SOLICITADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Descripción:&lt;/td&gt;&lt;td&gt;&lt;descripcion1&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;b&gt;MATERIAL CREADO&lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Código: &lt;/td&gt;&lt;td&gt;&lt;codigo2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Descripción: &lt;/td&gt;&lt;td&gt;&lt;descripcion2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad2&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Estado: &lt;/td&gt;&lt;td&gt;&lt;estadomaterial&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Redmat S.A. &lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se crea los materiales solicitados y que estan pendientes');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30113, 'Redmat','iconstruye@iconstruye.com', 'Aviso de Creación de Material', '&lt;div style=width:600px;&gt;&lt;p style="font-family:Arial; font-size:12px; text-align:left;"&gt;&lt;b&gt;Estimado Sr(a). &lt;usuariosolicitante&gt;&lt;/b&gt;&lt;br&gt;&lt;br&gt;La solicitud de creación de código enviada el día &lt;fechaenvio&gt;, del centro de gestión &lt;nomorgc&gt; a sido aprobada por el usuario &lt;nomusuarioatiende&gt;.&lt;b&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;MATERIAL SOLICITADO &lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Descripción:&lt;/td&gt;&lt;td&gt;&lt;descripcion1&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;b&gt;MATERIAL CREADO&lt;/b&gt;&lt;table style="font-family:Arial; font-size:12px; text-align:left;" border=0&gt;&lt;tr&gt;&lt;td&gt;Código: &lt;/td&gt;&lt;td&gt;&lt;codigo2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Descripción: &lt;/td&gt;&lt;td&gt;&lt;descripcion2&gt;&lt;/td&gt;&lt;tr&gt;&lt;td&gt;Unidad: &lt;/td&gt;&lt;td&gt;&lt;unidad2&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Estado: &lt;/td&gt;&lt;td&gt;&lt;estadomaterial&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atte,&lt;br&gt;Redmat S.A. &lt;br&gt;&lt;/p&gt;&lt;/div&gt;','Se envia cuando se crea los materiales solicitados y que estan pendientes',113,3);</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
         <v>114</v>
       </c>
@@ -13871,15 +13882,15 @@
         <v>694</v>
       </c>
       <c r="S102" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20114, 'Agilice','iconstruye@iconstruye.com', 'Nuevo Documento IR', 'Estimados Srs:&lt;br&gt;&lt;br&gt;&lt;p&gt; El Registro de Proveedores de Agilice informa que se ha agregado el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; a la carpeta &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, quedando disponible para su revisión.&lt;/p&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Mail aviso nuevo documento agregado');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20114, 'Agilice','iconstruye@iconstruye.com', 'Nuevo Documento IR', 'Estimados Srs:&lt;br&gt;&lt;br&gt;&lt;p&gt; El Registro de Proveedores de Agilice informa que se ha agregado el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; a la carpeta &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, quedando disponible para su revisión.&lt;/p&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Mail aviso nuevo documento agregado',114,2);</v>
       </c>
       <c r="T102" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20114, 'Redmat','iconstruye@iconstruye.com', 'Nuevo Documento IR', 'Estimados Srs:&lt;br&gt;&lt;br&gt;&lt;p&gt; El Registro de Proveedores de Redmat informa que se ha agregado el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; a la carpeta &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, quedando disponible para su revisión.&lt;/p&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Mail aviso nuevo documento agregado');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30114, 'Redmat','iconstruye@iconstruye.com', 'Nuevo Documento IR', 'Estimados Srs:&lt;br&gt;&lt;br&gt;&lt;p&gt; El Registro de Proveedores de Redmat informa que se ha agregado el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; a la carpeta &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, quedando disponible para su revisión.&lt;/p&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Mail aviso nuevo documento agregado',114,3);</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
         <v>115</v>
       </c>
@@ -13933,15 +13944,15 @@
         <v>700</v>
       </c>
       <c r="S103" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20115, 'Agilice','iconstruye@iconstruye.com', 'Eliminación Documento IR', 'Estimados Srs:&lt;br&gt;&lt;br&gt;&lt;p&gt; El Registro de Proveedores de Agilice informa que se ha eliminado el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; de la carpeta &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, por lo cual no estará disponible nuevamente.&lt;/p&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Mail aviso nuevo documento agregado');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20115, 'Agilice','iconstruye@iconstruye.com', 'Eliminación Documento IR', 'Estimados Srs:&lt;br&gt;&lt;br&gt;&lt;p&gt; El Registro de Proveedores de Agilice informa que se ha eliminado el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; de la carpeta &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, por lo cual no estará disponible nuevamente.&lt;/p&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Mail aviso nuevo documento agregado',115,2);</v>
       </c>
       <c r="T103" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20115, 'Redmat','iconstruye@iconstruye.com', 'Eliminación Documento IR', 'Estimados Srs:&lt;br&gt;&lt;br&gt;&lt;p&gt; El Registro de Proveedores de Redmat informa que se ha eliminado el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; de la carpeta &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, por lo cual no estará disponible nuevamente.&lt;/p&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Mail aviso nuevo documento agregado');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30115, 'Redmat','iconstruye@iconstruye.com', 'Eliminación Documento IR', 'Estimados Srs:&lt;br&gt;&lt;br&gt;&lt;p&gt; El Registro de Proveedores de Redmat informa que se ha eliminado el archivo &lt;b&gt;&lt;nombre_archivo&gt;&lt;/b&gt; de la carpeta &lt;b&gt;&lt;nombrecarpeta&gt;&lt;/b&gt;, creada por la empresa &lt;b&gt;&lt;nombre_empresa_duena_carpeta&gt;&lt;/b&gt;, por lo cual no estará disponible nuevamente.&lt;/p&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Mail aviso nuevo documento agregado',115,3);</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
         <v>116</v>
       </c>
@@ -13995,15 +14006,15 @@
         <v>707</v>
       </c>
       <c r="S104" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20116, 'Agilice','iconstruye@iconstruye.com', 'Estado de Pago Cancelado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Estado de Pago ha sido Cancelado. &lt;br&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt; &lt;br&gt;Tipo Estado Pago: &lt;destipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha ingreso: &lt;fechacreacion&gt;.&lt;br&gt;Comentario: &lt;cancelado&gt;&lt;br&gt;Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;N°: &lt;numsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Estado Pago, Notificación Cancelado');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20116, 'Agilice','iconstruye@iconstruye.com', 'Estado de Pago Cancelado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Estado de Pago ha sido Cancelado. &lt;br&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt; &lt;br&gt;Tipo Estado Pago: &lt;destipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha ingreso: &lt;fechacreacion&gt;.&lt;br&gt;Comentario: &lt;cancelado&gt;&lt;br&gt;Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;N°: &lt;numsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Estado Pago, Notificación Cancelado',116,2);</v>
       </c>
       <c r="T104" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20116, 'Redmat','iconstruye@iconstruye.com', 'Estado de Pago Cancelado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Estado de Pago ha sido Cancelado. &lt;br&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt; &lt;br&gt;Tipo Estado Pago: &lt;destipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha ingreso: &lt;fechacreacion&gt;.&lt;br&gt;Comentario: &lt;cancelado&gt;&lt;br&gt;Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;N°: &lt;numsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Estado Pago, Notificación Cancelado');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30116, 'Redmat','iconstruye@iconstruye.com', 'Estado de Pago Cancelado', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos que el siguiente Estado de Pago ha sido Cancelado. &lt;br&gt;&lt;br&gt;N° Estado Pago: &lt;numep&gt; &lt;br&gt;Tipo Estado Pago: &lt;destipodoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt; &lt;br&gt;Fecha ingreso: &lt;fechacreacion&gt;.&lt;br&gt;Comentario: &lt;cancelado&gt;&lt;br&gt;Subcontrato: &lt;nomsubcontrato&gt;&lt;br&gt;N°: &lt;numsubcontrato&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Estado Pago, Notificación Cancelado',116,3);</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
         <v>19</v>
       </c>
@@ -14057,15 +14068,15 @@
         <v>714</v>
       </c>
       <c r="S105" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20019, 'Agilice','iconstruye@iconstruye.com', '&lt;nombsitio&gt; le recuerda su contraseña', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le recordamos que que sus datos de acceso a nuestro sistema son:&lt;br&gt;&lt;br&gt;Usuario: &lt;idusuario&gt;&lt;br&gt;Organización: &lt;nombempresa&gt;&lt;br&gt;Clave: &lt;clave&gt;&lt;br&gt;&lt;br&gt;En caso de requerir información adicional, comuníquese con nosotros al &lt;fonocontacto&gt;. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo &lt;nombsitio&gt;&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;fonocontacto&gt;&lt;br&gt;&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Usuario Contraseña');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2019, 'Agilice','iconstruye@iconstruye.com', '&lt;nombsitio&gt; le recuerda su contraseña', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le recordamos que que sus datos de acceso a nuestro sistema son:&lt;br&gt;&lt;br&gt;Usuario: &lt;idusuario&gt;&lt;br&gt;Organización: &lt;nombempresa&gt;&lt;br&gt;Clave: &lt;clave&gt;&lt;br&gt;&lt;br&gt;En caso de requerir información adicional, comuníquese con nosotros al &lt;fonocontacto&gt;. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo &lt;nombsitio&gt;&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;fonocontacto&gt;&lt;br&gt;&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Usuario Contraseña',19,2);</v>
       </c>
       <c r="T105" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20019, 'Redmat','iconstruye@iconstruye.com', '&lt;nombsitio&gt; le recuerda su contraseña', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le recordamos que que sus datos de acceso a nuestro sistema son:&lt;br&gt;&lt;br&gt;Usuario: &lt;idusuario&gt;&lt;br&gt;Organización: &lt;nombempresa&gt;&lt;br&gt;Clave: &lt;clave&gt;&lt;br&gt;&lt;br&gt;En caso de requerir información adicional, comuníquese con nosotros al &lt;fonocontacto&gt;. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo &lt;nombsitio&gt;&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;fonocontacto&gt;&lt;br&gt;&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Usuario Contraseña');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3019, 'Redmat','iconstruye@iconstruye.com', '&lt;nombsitio&gt; le recuerda su contraseña', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le recordamos que que sus datos de acceso a nuestro sistema son:&lt;br&gt;&lt;br&gt;Usuario: &lt;idusuario&gt;&lt;br&gt;Organización: &lt;nombempresa&gt;&lt;br&gt;Clave: &lt;clave&gt;&lt;br&gt;&lt;br&gt;En caso de requerir información adicional, comuníquese con nosotros al &lt;fonocontacto&gt;. &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo &lt;nombsitio&gt;&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;fonocontacto&gt;&lt;br&gt;&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Usuario Contraseña',19,3);</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
         <v>20</v>
       </c>
@@ -14121,15 +14132,15 @@
         <v>720</v>
       </c>
       <c r="S106" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20020, 'Agilice','iconstruye@iconstruye.com', 'Nueva OC &lt;numoc&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;AGILICE&lt;/title&gt;&lt;style type=text/css&gt;*{ margin: 0; font-family: "Helvetica Neue", Helvetica, Arial, sans-serif; box-sizing: border-box; font-size: 14px;} img{ max-width: 100%;} body{ -webkit-font-smoothing: antialiased; -webkit-text-size-adjust: none; width: 100% !important; height: 100%; line-height: 1.6em;} table td{ vertical-align: top;} body{ background-color: #f6f6f6;} .body-wrap{ background-color: #f6f6f6; width: 100%;} .container{ display: block !important; max-width: 600px !important; margin: 0 auto !important; clear: both !important;} .content{ max-width: 600px; margin: 0 auto; display: block; padding: 20px;} .main{ background-color: #fff; border: 1px solid #e9e9e9; border-radius: 3px;} .content-wrap{ padding: 20px;} .content-block{ padding: 0 0 20px;} .header{ width: 100%; margin-bottom: 20px;} .footer{ width: 100%; clear: both; color: #999; padding: 20px;} .footer p, .footer a, .footer td{ color: #999; font-size: 12px;} .resume-box{ background: #EBF6FF;} h1, h2, h3{ font-family: "Helvetica Neue", Helvetica, Arial, "Lucida Grande", sans-serif; color: #000; margin: 20px 0 0; line-height: 1.2em; font-weight: 400;} h1{ font-size: 20px; font-weight: 500;} h2{ font-size: 24px;} h3{ font-size: 18px;} h4{ font-size: 14px; font-weight: 600;} p, ul, ol{ margin-bottom: 10px; font-weight: normal;} p li, ul li, ol li{ margin-left: 5px; list-style-position: inside; line-height: 1.3em;} a{ color: #348eda; text-decoration: underline;} .btn-primary{ text-decoration: none; color: #FFF; background-color: #0284d3; padding: 10px 20px; line-height: 2em; font-weight: 400; font-size: 1.1em; text-align: center; cursor: pointer; display: inline-block; border-radius: 5px; text-transform: capitalize;} .last{ margin-bottom: 0;} .first{ margin-top: 0;} .aligncenter{ text-align: center;} .alignright{ text-align: right;} .alignleft{ text-align: left;} .clear{ clear: both;} .alert{ font-size: 16px; color: #fff; font-weight: 500; padding: 20px; text-align: center; border-radius: 3px 3px 0 0;} .alert a{ color: #fff; text-decoration: none; font-weight: 500; font-size: 16px;} .alert.alert-warning{ background-color: #FF9F00;} .alert.alert-bad{ background-color: #D0021B;} .alert.alert-good{ background-color: #68B90F;} .invoice{ margin: 40px auto; text-align: left; width: 80%;} .invoice td{ padding: 5px 0;} .invoice .invoice-items{ width: 100%;} .invoice .invoice-items td{ border-top: #eee 1px solid;} .invoice .invoice-items .total td{ border-top: 2px solid #333; border-bottom: 2px solid #333; font-weight: 700;} @media only screen and (max-width: 640px){ body{ padding: 0 !important;} h1, h2, h3, h4{ font-weight: 800 !important; margin: 20px 0 5px !important;} h1{ font-size: 22px !important;} h2{ font-size: 18px !important;} h3{ font-size: 16px !important;} .container{ padding: 0 !important; width: 100% !important;} .content{ padding: 0 !important;} .content-wrap{ padding: 10px !important;} .invoice{ width: 100% !important;} .mcnImage{ max-width: 100% !important; width: 100% !important;}} &lt;/style&gt;&lt;/head&gt;&lt;body itemscope itemtype=http://schema.org/EmailMessage&gt;&lt;table class=body-wrap&gt;&lt;tr&gt;&lt;td&gt;&lt;/td&gt;&lt;td class=container width=600&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td valign=top&gt;&lt;img align=center alt src=https://cl.iconstruye.com/images/banner-generico.jpg width=600 class=mcnImage&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h1&gt;Has recibido una nueva Orden de compra.&lt;/h1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Hola &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;,&lt;br&gt;Junto con saludar le informamos que el &lt;fechaenvio&gt;, la empresa &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;enviado a usted la Orden de Compra número &lt;strong&gt;&lt;numoc&gt;&lt;/strong&gt;.&lt;br&gt;&lt;br&gt;Recuerde siempre Aceptar o Rechazar este documento desde &lt;a href=https://apps.agilice.com&gt;https://apps.agilice.com&lt;/a&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;table width=100% cellspacing=0 cellpadding=0 class=resume-box&gt;&lt;tr&gt;&lt;td&gt;&lt;div class=content-wrap&gt;&lt;table&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Conoce las otras soluciones que tenemos para ti&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Con &lt;strong&gt;Rinde Ágil, &lt;/strong&gt;rinde tus gastos en cuestión de segundos. No más respaldos en papeles, digitaliza cada paso de la rendición de gastos de tu empresa.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="content-block aligncenter"&gt;&lt;span class=hs-cta-wrapper id=hs-cta-wrapper-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;span class="hs-cta-node hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9" id=hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;a href=https://cta-redirect.hubspot.com/cta/redirect/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9 target=_blank&gt;&lt;img class=hs-cta-img id=hs-cta-img-a826c11a-e3aa-46df-84a5-e53b35388aa9 style=border-width:0px; src=https://no-cache.hubspot.com/cta/default/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9.png alt="SOLICITA TU PRUEBA GRATIS AQUÍ"&gt;&lt;/a&gt;&lt;/span&gt;&lt;script charset=utf-8 src=https://js.hscta.net/cta/current.js&gt;&lt;/script&gt;&lt;script type=text/javascript&gt;hbspt.cta.load(5032552, "a826c11a-e3aa-46df-84a5-e53b35388aa9",{}); &lt;/script&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellspacing=0 cellpadding=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Saludos &lt;br&gt;&lt;strong&gt;Equipo AGILICE&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=footer&gt;&lt;table width=100%&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;¿Necesitas ayuda con este correo? &lt;a href=mailto:&gt;mesadeayuda@agilice.com&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;&lt;em&gt;Correo enviado a través de AGILICE®&amp;nbsp; Copyright © -Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;&lt;a href=[unsubscribe] style=color:#999;&gt;Si deseas salir del env&amp;iacute;o de emails de Agilice haz click aqu&amp;iacute;&lt;/a&gt;&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;f','Orden de Compra, Aviso');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2020, 'Agilice','iconstruye@iconstruye.com', 'Nueva OC &lt;numoc&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;AGILICE&lt;/title&gt;&lt;style type=text/css&gt;*{ margin: 0; font-family: "Helvetica Neue", Helvetica, Arial, sans-serif; box-sizing: border-box; font-size: 14px;} img{ max-width: 100%;} body{ -webkit-font-smoothing: antialiased; -webkit-text-size-adjust: none; width: 100% !important; height: 100%; line-height: 1.6em;} table td{ vertical-align: top;} body{ background-color: #f6f6f6;} .body-wrap{ background-color: #f6f6f6; width: 100%;} .container{ display: block !important; max-width: 600px !important; margin: 0 auto !important; clear: both !important;} .content{ max-width: 600px; margin: 0 auto; display: block; padding: 20px;} .main{ background-color: #fff; border: 1px solid #e9e9e9; border-radius: 3px;} .content-wrap{ padding: 20px;} .content-block{ padding: 0 0 20px;} .header{ width: 100%; margin-bottom: 20px;} .footer{ width: 100%; clear: both; color: #999; padding: 20px;} .footer p, .footer a, .footer td{ color: #999; font-size: 12px;} .resume-box{ background: #EBF6FF;} h1, h2, h3{ font-family: "Helvetica Neue", Helvetica, Arial, "Lucida Grande", sans-serif; color: #000; margin: 20px 0 0; line-height: 1.2em; font-weight: 400;} h1{ font-size: 20px; font-weight: 500;} h2{ font-size: 24px;} h3{ font-size: 18px;} h4{ font-size: 14px; font-weight: 600;} p, ul, ol{ margin-bottom: 10px; font-weight: normal;} p li, ul li, ol li{ margin-left: 5px; list-style-position: inside; line-height: 1.3em;} a{ color: #348eda; text-decoration: underline;} .btn-primary{ text-decoration: none; color: #FFF; background-color: #0284d3; padding: 10px 20px; line-height: 2em; font-weight: 400; font-size: 1.1em; text-align: center; cursor: pointer; display: inline-block; border-radius: 5px; text-transform: capitalize;} .last{ margin-bottom: 0;} .first{ margin-top: 0;} .aligncenter{ text-align: center;} .alignright{ text-align: right;} .alignleft{ text-align: left;} .clear{ clear: both;} .alert{ font-size: 16px; color: #fff; font-weight: 500; padding: 20px; text-align: center; border-radius: 3px 3px 0 0;} .alert a{ color: #fff; text-decoration: none; font-weight: 500; font-size: 16px;} .alert.alert-warning{ background-color: #FF9F00;} .alert.alert-bad{ background-color: #D0021B;} .alert.alert-good{ background-color: #68B90F;} .invoice{ margin: 40px auto; text-align: left; width: 80%;} .invoice td{ padding: 5px 0;} .invoice .invoice-items{ width: 100%;} .invoice .invoice-items td{ border-top: #eee 1px solid;} .invoice .invoice-items .total td{ border-top: 2px solid #333; border-bottom: 2px solid #333; font-weight: 700;} @media only screen and (max-width: 640px){ body{ padding: 0 !important;} h1, h2, h3, h4{ font-weight: 800 !important; margin: 20px 0 5px !important;} h1{ font-size: 22px !important;} h2{ font-size: 18px !important;} h3{ font-size: 16px !important;} .container{ padding: 0 !important; width: 100% !important;} .content{ padding: 0 !important;} .content-wrap{ padding: 10px !important;} .invoice{ width: 100% !important;} .mcnImage{ max-width: 100% !important; width: 100% !important;}} &lt;/style&gt;&lt;/head&gt;&lt;body itemscope itemtype=http://schema.org/EmailMessage&gt;&lt;table class=body-wrap&gt;&lt;tr&gt;&lt;td&gt;&lt;/td&gt;&lt;td class=container width=600&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td valign=top&gt;&lt;img align=center alt src=https://cl.iconstruye.com/images/banner-generico.jpg width=600 class=mcnImage&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h1&gt;Has recibido una nueva Orden de compra.&lt;/h1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Hola &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;,&lt;br&gt;Junto con saludar le informamos que el &lt;fechaenvio&gt;, la empresa &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;enviado a usted la Orden de Compra número &lt;strong&gt;&lt;numoc&gt;&lt;/strong&gt;.&lt;br&gt;&lt;br&gt;Recuerde siempre Aceptar o Rechazar este documento desde &lt;a href=https://apps.agilice.com&gt;https://apps.agilice.com&lt;/a&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;table width=100% cellspacing=0 cellpadding=0 class=resume-box&gt;&lt;tr&gt;&lt;td&gt;&lt;div class=content-wrap&gt;&lt;table&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Conoce las otras soluciones que tenemos para ti&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Con &lt;strong&gt;Rinde Ágil, &lt;/strong&gt;rinde tus gastos en cuestión de segundos. No más respaldos en papeles, digitaliza cada paso de la rendición de gastos de tu empresa.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="content-block aligncenter"&gt;&lt;span class=hs-cta-wrapper id=hs-cta-wrapper-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;span class="hs-cta-node hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9" id=hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;a href=https://cta-redirect.hubspot.com/cta/redirect/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9 target=_blank&gt;&lt;img class=hs-cta-img id=hs-cta-img-a826c11a-e3aa-46df-84a5-e53b35388aa9 style=border-width:0px; src=https://no-cache.hubspot.com/cta/default/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9.png alt="SOLICITA TU PRUEBA GRATIS AQUÍ"&gt;&lt;/a&gt;&lt;/span&gt;&lt;script charset=utf-8 src=https://js.hscta.net/cta/current.js&gt;&lt;/script&gt;&lt;script type=text/javascript&gt;hbspt.cta.load(5032552, "a826c11a-e3aa-46df-84a5-e53b35388aa9",{}); &lt;/script&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellspacing=0 cellpadding=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Saludos &lt;br&gt;&lt;strong&gt;Equipo AGILICE&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=footer&gt;&lt;table width=100%&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;¿Necesitas ayuda con este correo? &lt;a href=mailto:&gt;mesadeayuda@agilice.com&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;&lt;em&gt;Correo enviado a través de AGILICE®&amp;nbsp; Copyright © -Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;&lt;a href=[unsubscribe] style=color:#999;&gt;Si deseas salir del env&amp;iacute;o de emails de Agilice haz click aqu&amp;iacute;&lt;/a&gt;&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;f','Orden de Compra, Aviso',20,2);</v>
       </c>
       <c r="T106" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20020, 'Redmat','iconstruye@iconstruye.com', 'Nueva OC &lt;numoc&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;redmat&lt;/title&gt;&lt;style type=text/css&gt;*{ margin: 0; font-family: "Helvetica Neue", Helvetica, Arial, sans-serif; box-sizing: border-box; font-size: 14px;} img{ max-width: 100%;} body{ -webkit-font-smoothing: antialiased; -webkit-text-size-adjust: none; width: 100% !important; height: 100%; line-height: 1.6em;} table td{ vertical-align: top;} body{ background-color: #f6f6f6;} .body-wrap{ background-color: #f6f6f6; width: 100%;} .container{ display: block !important; max-width: 600px !important; margin: 0 auto !important; clear: both !important;} .content{ max-width: 600px; margin: 0 auto; display: block; padding: 20px;} .main{ background-color: #fff; border: 1px solid #e9e9e9; border-radius: 3px;} .content-wrap{ padding: 20px;} .content-block{ padding: 0 0 20px;} .header{ width: 100%; margin-bottom: 20px;} .footer{ width: 100%; clear: both; color: #999; padding: 20px;} .footer p, .footer a, .footer td{ color: #999; font-size: 12px;} .resume-box{ background: #EBF6FF;} h1, h2, h3{ font-family: "Helvetica Neue", Helvetica, Arial, "Lucida Grande", sans-serif; color: #000; margin: 20px 0 0; line-height: 1.2em; font-weight: 400;} h1{ font-size: 20px; font-weight: 500;} h2{ font-size: 24px;} h3{ font-size: 18px;} h4{ font-size: 14px; font-weight: 600;} p, ul, ol{ margin-bottom: 10px; font-weight: normal;} p li, ul li, ol li{ margin-left: 5px; list-style-position: inside; line-height: 1.3em;} a{ color: #348eda; text-decoration: underline;} .btn-primary{ text-decoration: none; color: #FFF; background-color: #0284d3; padding: 10px 20px; line-height: 2em; font-weight: 400; font-size: 1.1em; text-align: center; cursor: pointer; display: inline-block; border-radius: 5px; text-transform: capitalize;} .last{ margin-bottom: 0;} .first{ margin-top: 0;} .aligncenter{ text-align: center;} .alignright{ text-align: right;} .alignleft{ text-align: left;} .clear{ clear: both;} .alert{ font-size: 16px; color: #fff; font-weight: 500; padding: 20px; text-align: center; border-radius: 3px 3px 0 0;} .alert a{ color: #fff; text-decoration: none; font-weight: 500; font-size: 16px;} .alert.alert-warning{ background-color: #FF9F00;} .alert.alert-bad{ background-color: #D0021B;} .alert.alert-good{ background-color: #68B90F;} .invoice{ margin: 40px auto; text-align: left; width: 80%;} .invoice td{ padding: 5px 0;} .invoice .invoice-items{ width: 100%;} .invoice .invoice-items td{ border-top: #eee 1px solid;} .invoice .invoice-items .total td{ border-top: 2px solid #333; border-bottom: 2px solid #333; font-weight: 700;} @media only screen and (max-width: 640px){ body{ padding: 0 !important;} h1, h2, h3, h4{ font-weight: 800 !important; margin: 20px 0 5px !important;} h1{ font-size: 22px !important;} h2{ font-size: 18px !important;} h3{ font-size: 16px !important;} .container{ padding: 0 !important; width: 100% !important;} .content{ padding: 0 !important;} .content-wrap{ padding: 10px !important;} .invoice{ width: 100% !important;} .mcnImage{ max-width: 100% !important; width: 100% !important;}} &lt;/style&gt;&lt;/head&gt;&lt;body itemscope itemtype=http://schema.org/EmailMessage&gt;&lt;table class=body-wrap&gt;&lt;tr&gt;&lt;td&gt;&lt;/td&gt;&lt;td class=container width=600&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td valign=top&gt;&lt;img align=center alt src=https://cl.iconstruye.com/images/banner-generico.jpg width=600 class=mcnImage&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h1&gt;Has recibido una nueva Orden de compra.&lt;/h1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Hola &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;,&lt;br&gt;Junto con saludar le informamos que el &lt;fechaenvio&gt;, la empresa &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;enviado a usted la Orden de Compra número &lt;strong&gt;&lt;numoc&gt;&lt;/strong&gt;.&lt;br&gt;&lt;br&gt;Recuerde siempre Aceptar o Rechazar este documento desde &lt;a href=https://redmat.iconstruye.com&gt;https://redmat.iconstruye.com&lt;/a&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;table width=100% cellspacing=0 cellpadding=0 class=resume-box&gt;&lt;tr&gt;&lt;td&gt;&lt;div class=content-wrap&gt;&lt;table&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Conoce las otras soluciones que tenemos para ti&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Con &lt;strong&gt;Rinde Ágil, &lt;/strong&gt;rinde tus gastos en cuestión de segundos. No más respaldos en papeles, digitaliza cada paso de la rendición de gastos de tu empresa.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="content-block aligncenter"&gt;&lt;span class=hs-cta-wrapper id=hs-cta-wrapper-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;span class="hs-cta-node hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9" id=hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;a href=https://cta-redirect.hubspot.com/cta/redirect/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9 target=_blank&gt;&lt;img class=hs-cta-img id=hs-cta-img-a826c11a-e3aa-46df-84a5-e53b35388aa9 style=border-width:0px; src=https://no-cache.hubspot.com/cta/default/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9.png alt="SOLICITA TU PRUEBA GRATIS AQUÍ"&gt;&lt;/a&gt;&lt;/span&gt;&lt;script charset=utf-8 src=https://js.hscta.net/cta/current.js&gt;&lt;/script&gt;&lt;script type=text/javascript&gt;hbspt.cta.load(5032552, "a826c11a-e3aa-46df-84a5-e53b35388aa9",{}); &lt;/script&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellspacing=0 cellpadding=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Saludos &lt;br&gt;&lt;strong&gt;Equipo Redmat&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=footer&gt;&lt;table width=100%&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;¿Necesitas ayuda con este correo? &lt;a href=mailto:&gt;mesadeayuda@iconstruye.com&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;&lt;em&gt;Correo enviado a través de Redmat®&amp;nbsp; Copyright © -Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;&lt;a href=[unsubscribe] style=color:#999;&gt;Si deseas salir del env&amp;iacute;o de emails de redmat haz click aqu&amp;iacute;&lt;/a&gt;&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Orden de Compra, Aviso');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3020, 'Redmat','iconstruye@iconstruye.com', 'Nueva OC &lt;numoc&gt;', '&lt;!DOCTYPE html PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN" "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;&lt;html xmlns=http://www.w3.org/1999/xhtml&gt;&lt;head&gt;&lt;meta name=viewport content="width=device-width"&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;title&gt;redmat&lt;/title&gt;&lt;style type=text/css&gt;*{ margin: 0; font-family: "Helvetica Neue", Helvetica, Arial, sans-serif; box-sizing: border-box; font-size: 14px;} img{ max-width: 100%;} body{ -webkit-font-smoothing: antialiased; -webkit-text-size-adjust: none; width: 100% !important; height: 100%; line-height: 1.6em;} table td{ vertical-align: top;} body{ background-color: #f6f6f6;} .body-wrap{ background-color: #f6f6f6; width: 100%;} .container{ display: block !important; max-width: 600px !important; margin: 0 auto !important; clear: both !important;} .content{ max-width: 600px; margin: 0 auto; display: block; padding: 20px;} .main{ background-color: #fff; border: 1px solid #e9e9e9; border-radius: 3px;} .content-wrap{ padding: 20px;} .content-block{ padding: 0 0 20px;} .header{ width: 100%; margin-bottom: 20px;} .footer{ width: 100%; clear: both; color: #999; padding: 20px;} .footer p, .footer a, .footer td{ color: #999; font-size: 12px;} .resume-box{ background: #EBF6FF;} h1, h2, h3{ font-family: "Helvetica Neue", Helvetica, Arial, "Lucida Grande", sans-serif; color: #000; margin: 20px 0 0; line-height: 1.2em; font-weight: 400;} h1{ font-size: 20px; font-weight: 500;} h2{ font-size: 24px;} h3{ font-size: 18px;} h4{ font-size: 14px; font-weight: 600;} p, ul, ol{ margin-bottom: 10px; font-weight: normal;} p li, ul li, ol li{ margin-left: 5px; list-style-position: inside; line-height: 1.3em;} a{ color: #348eda; text-decoration: underline;} .btn-primary{ text-decoration: none; color: #FFF; background-color: #0284d3; padding: 10px 20px; line-height: 2em; font-weight: 400; font-size: 1.1em; text-align: center; cursor: pointer; display: inline-block; border-radius: 5px; text-transform: capitalize;} .last{ margin-bottom: 0;} .first{ margin-top: 0;} .aligncenter{ text-align: center;} .alignright{ text-align: right;} .alignleft{ text-align: left;} .clear{ clear: both;} .alert{ font-size: 16px; color: #fff; font-weight: 500; padding: 20px; text-align: center; border-radius: 3px 3px 0 0;} .alert a{ color: #fff; text-decoration: none; font-weight: 500; font-size: 16px;} .alert.alert-warning{ background-color: #FF9F00;} .alert.alert-bad{ background-color: #D0021B;} .alert.alert-good{ background-color: #68B90F;} .invoice{ margin: 40px auto; text-align: left; width: 80%;} .invoice td{ padding: 5px 0;} .invoice .invoice-items{ width: 100%;} .invoice .invoice-items td{ border-top: #eee 1px solid;} .invoice .invoice-items .total td{ border-top: 2px solid #333; border-bottom: 2px solid #333; font-weight: 700;} @media only screen and (max-width: 640px){ body{ padding: 0 !important;} h1, h2, h3, h4{ font-weight: 800 !important; margin: 20px 0 5px !important;} h1{ font-size: 22px !important;} h2{ font-size: 18px !important;} h3{ font-size: 16px !important;} .container{ padding: 0 !important; width: 100% !important;} .content{ padding: 0 !important;} .content-wrap{ padding: 10px !important;} .invoice{ width: 100% !important;} .mcnImage{ max-width: 100% !important; width: 100% !important;}} &lt;/style&gt;&lt;/head&gt;&lt;body itemscope itemtype=http://schema.org/EmailMessage&gt;&lt;table class=body-wrap&gt;&lt;tr&gt;&lt;td&gt;&lt;/td&gt;&lt;td class=container width=600&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td&gt;&lt;table class=main width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td valign=top&gt;&lt;img align=center alt src=https://cl.iconstruye.com/images/banner-generico.jpg width=600 class=mcnImage&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellpadding=0 cellspacing=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h1&gt;Has recibido una nueva Orden de compra.&lt;/h1&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Hola &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;,&lt;br&gt;Junto con saludar le informamos que el &lt;fechaenvio&gt;, la empresa &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;enviado a usted la Orden de Compra número &lt;strong&gt;&lt;numoc&gt;&lt;/strong&gt;.&lt;br&gt;&lt;br&gt;Recuerde siempre Aceptar o Rechazar este documento desde &lt;a href=https://redmat.iconstruye.com&gt;https://redmat.iconstruye.com&lt;/a&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;table width=100% cellspacing=0 cellpadding=0 class=resume-box&gt;&lt;tr&gt;&lt;td&gt;&lt;div class=content-wrap&gt;&lt;table&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;h3&gt;Conoce las otras soluciones que tenemos para ti&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Con &lt;strong&gt;Rinde Ágil, &lt;/strong&gt;rinde tus gastos en cuestión de segundos. No más respaldos en papeles, digitaliza cada paso de la rendición de gastos de tu empresa.&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="content-block aligncenter"&gt;&lt;span class=hs-cta-wrapper id=hs-cta-wrapper-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;span class="hs-cta-node hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9" id=hs-cta-a826c11a-e3aa-46df-84a5-e53b35388aa9&gt;&lt;a href=https://cta-redirect.hubspot.com/cta/redirect/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9 target=_blank&gt;&lt;img class=hs-cta-img id=hs-cta-img-a826c11a-e3aa-46df-84a5-e53b35388aa9 style=border-width:0px; src=https://no-cache.hubspot.com/cta/default/5032552/a826c11a-e3aa-46df-84a5-e53b35388aa9.png alt="SOLICITA TU PRUEBA GRATIS AQUÍ"&gt;&lt;/a&gt;&lt;/span&gt;&lt;script charset=utf-8 src=https://js.hscta.net/cta/current.js&gt;&lt;/script&gt;&lt;script type=text/javascript&gt;hbspt.cta.load(5032552, "a826c11a-e3aa-46df-84a5-e53b35388aa9",{}); &lt;/script&gt;&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=content-wrap&gt;&lt;table width=100% cellspacing=0 cellpadding=0&gt;&lt;tr&gt;&lt;td class=content-block&gt;&lt;p&gt;Saludos &lt;br&gt;&lt;strong&gt;Equipo Redmat&lt;/strong&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;div class=footer&gt;&lt;table width=100%&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;¿Necesitas ayuda con este correo? &lt;a href=mailto:&gt;mesadeayuda@iconstruye.com&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class="aligncenter content-block"&gt;&lt;em&gt;Correo enviado a través de Redmat®&amp;nbsp; Copyright © -Todos los Derechos Reservados&lt;/em&gt;&lt;br&gt;&lt;p&gt;&lt;span style="font-size: 12px;"&gt;&lt;a href=[unsubscribe] style=color:#999;&gt;Si deseas salir del env&amp;iacute;o de emails de redmat haz click aqu&amp;iacute;&lt;/a&gt;&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/body&gt;&lt;/html&gt;','Orden de Compra, Aviso',20,3);</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
         <v>21</v>
       </c>
@@ -14183,17 +14194,17 @@
         <v>727</v>
       </c>
       <c r="S107" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20021, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de OC &lt;numoc&gt;', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Orden de Compra pendiente de Aprobar.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: OC Supera el gasto del comprador&lt;br&gt;Monto a Aprobar: &lt;montoaprobar&gt;&lt;br&gt;&lt;br&gt;Podrá Aprobar este documento desde &lt;link&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt; &lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;+56 22 486 11 11&lt;br&gt;&lt;img src="
-                https://apps.agilice.com/img/logo-agilice.png" img&gt;','Orden de Compra, Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2021, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de OC &lt;numoc&gt;', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Orden de Compra pendiente de Aprobar.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: OC Supera el gasto del comprador&lt;br&gt;Monto a Aprobar: &lt;montoaprobar&gt;&lt;br&gt;&lt;br&gt;Podrá Aprobar este documento desde &lt;link&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt; &lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;+56 22 486 11 11&lt;br&gt;&lt;img src="
+                https://apps.agilice.com/img/logo-agilice.png" img&gt;','Orden de Compra, Envío a Aprobación',21,2);</v>
       </c>
       <c r="T107" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20021, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de OC &lt;numoc&gt;', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Orden de Compra pendiente de Aprobar.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: OC Supera el gasto del comprador&lt;br&gt;Monto a Aprobar: &lt;montoaprobar&gt;&lt;br&gt;&lt;br&gt;Podrá Aprobar este documento desde &lt;link&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt; &lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;+56 22 486 11 11&lt;br&gt;&lt;img src="
-                https://redmat.iconstruye.com/img/logo-redmat.png" img&gt;','Orden de Compra, Envío a Aprobación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3021, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de OC &lt;numoc&gt;', 'Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que tiene una nueva Orden de Compra pendiente de Aprobar.&lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;N° de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: OC Supera el gasto del comprador&lt;br&gt;Monto a Aprobar: &lt;montoaprobar&gt;&lt;br&gt;&lt;br&gt;Podrá Aprobar este documento desde &lt;link&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt; &lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;+56 22 486 11 11&lt;br&gt;&lt;img src="
+                https://redmat.iconstruye.com/img/logo-redmat.png" img&gt;','Orden de Compra, Envío a Aprobación',21,3);</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
         <v>22</v>
       </c>
@@ -14247,15 +14258,15 @@
         <v>734</v>
       </c>
       <c r="S108" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20022, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de OC &lt;numoc&gt; (Aprobador Agregado a Flujo)', '&lt;div id=header&gt;_x000D_ &lt;/div&gt;_x000D_ &lt;div id=body&gt;_x000D_ Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que ha sido invitado a participar en el flujo de aprobación de una Orden de Compra. &lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;Podrá Aprobar este documento ya sea desde &lt;link&gt; o bien ingresando desde su dispositivo móvil a &lt;link2&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, _x000D_ &lt;/div&gt;_x000D_ &lt;div id=footer&gt;_x000D_ &lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;_x000D_ &lt;/div&gt;','Orden de Compra, Envío a Aprobación Añadido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2022, 'Agilice','iconstruye@iconstruye.com', 'Aprobación de OC &lt;numoc&gt; (Aprobador Agregado a Flujo)', '&lt;div id=header&gt;_x000D_ &lt;/div&gt;_x000D_ &lt;div id=body&gt;_x000D_ Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que ha sido invitado a participar en el flujo de aprobación de una Orden de Compra. &lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;Podrá Aprobar este documento ya sea desde &lt;link&gt; o bien ingresando desde su dispositivo móvil a &lt;link2&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, _x000D_ &lt;/div&gt;_x000D_ &lt;div id=footer&gt;_x000D_ &lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;_x000D_ &lt;/div&gt;','Orden de Compra, Envío a Aprobación Añadido',22,2);</v>
       </c>
       <c r="T108" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20022, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de OC &lt;numoc&gt; (Aprobador Agregado a Flujo)', '&lt;div id=header&gt;_x000D_ &lt;/div&gt;_x000D_ &lt;div id=body&gt;_x000D_ Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que ha sido invitado a participar en el flujo de aprobación de una Orden de Compra. &lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;Podrá Aprobar este documento ya sea desde &lt;link&gt; o bien ingresando desde su dispositivo móvil a &lt;link2&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, _x000D_ &lt;/div&gt;_x000D_ &lt;div id=footer&gt;_x000D_ &lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;_x000D_ &lt;/div&gt;','Orden de Compra, Envío a Aprobación Añadido');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3022, 'Redmat','iconstruye@iconstruye.com', 'Aprobación de OC &lt;numoc&gt; (Aprobador Agregado a Flujo)', '&lt;div id=header&gt;_x000D_ &lt;/div&gt;_x000D_ &lt;div id=body&gt;_x000D_ Estimado Sr. &lt;nombusuario&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que ha sido invitado a participar en el flujo de aprobación de una Orden de Compra. &lt;br&gt;&lt;br&gt;Solicitante: &lt;nombsolicitante&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomorgc&gt;&lt;br&gt;Fecha Creación: &lt;fechacreacion&gt;&lt;br&gt;Tipo de Aprobación: Aprobador agregado al flujo.&lt;br&gt;&lt;br&gt;Podrá Aprobar este documento ya sea desde &lt;link&gt; o bien ingresando desde su dispositivo móvil a &lt;link2&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, _x000D_ &lt;/div&gt;_x000D_ &lt;div id=footer&gt;_x000D_ &lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;_x000D_ &lt;/div&gt;','Orden de Compra, Envío a Aprobación Añadido',22,3);</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A109" s="6">
         <v>23</v>
       </c>
@@ -14309,15 +14320,15 @@
         <v>741</v>
       </c>
       <c r="S109" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20023, 'Agilice','iconstruye@iconstruye.com', 'Orden de Compra  aprobada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Solicitud de Compra generada por usted ha sido Aprobada y enviada al proveedor. &lt;br&gt;&lt;br&gt;N° de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha envío solicitud: &lt;fechacreacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Aprobación Total');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2023, 'Agilice','iconstruye@iconstruye.com', 'Orden de Compra  aprobada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Solicitud de Compra generada por usted ha sido Aprobada y enviada al proveedor. &lt;br&gt;&lt;br&gt;N° de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha envío solicitud: &lt;fechacreacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Aprobación Total',23,2);</v>
       </c>
       <c r="T109" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20023, 'Redmat','iconstruye@iconstruye.com', 'Orden de Compra  aprobada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Solicitud de Compra generada por usted ha sido Aprobada y enviada al proveedor. &lt;br&gt;&lt;br&gt;N° de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha envío solicitud: &lt;fechacreacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Aprobación Total');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3023, 'Redmat','iconstruye@iconstruye.com', 'Orden de Compra  aprobada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Solicitud de Compra generada por usted ha sido Aprobada y enviada al proveedor. &lt;br&gt;&lt;br&gt;N° de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha envío solicitud: &lt;fechacreacion&gt;&lt;br&gt;Aprobador: &lt;nombaprobador&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente, &lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt; &lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Aprobación Total',23,3);</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A110" s="6">
         <v>24</v>
       </c>
@@ -14371,15 +14382,15 @@
         <v>748</v>
       </c>
       <c r="S110" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20024, 'Agilice','iconstruye@iconstruye.com', 'Orden de Compra rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Orden de Compra generada por usted ha sido Rechazada. &lt;br&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha envío OC: &lt;fechacreacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para revisar mayores antecedentes, ingrese al módulo Compras de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Rechazada Aprobador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2024, 'Agilice','iconstruye@iconstruye.com', 'Orden de Compra rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Orden de Compra generada por usted ha sido Rechazada. &lt;br&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha envío OC: &lt;fechacreacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para revisar mayores antecedentes, ingrese al módulo Compras de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Orden de Compra, Rechazada Aprobador',24,2);</v>
       </c>
       <c r="T110" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20024, 'Redmat','iconstruye@iconstruye.com', 'Orden de Compra rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Orden de Compra generada por usted ha sido Rechazada. &lt;br&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha envío OC: &lt;fechacreacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para revisar mayores antecedentes, ingrese al módulo Compras de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Rechazada Aprobador');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3024, 'Redmat','iconstruye@iconstruye.com', 'Orden de Compra rechazada', 'Estimado Sr. &lt;nombsolicitante&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, le informamos que la siguiente Orden de Compra generada por usted ha sido Rechazada. &lt;br&gt;&lt;br&gt;Nº de OC: &lt;numoc&gt;&lt;br&gt;Nombre OC: &lt;nomoc&gt;&lt;br&gt;Centro de Gestión: &lt;nomborgc&gt;&lt;br&gt;Fecha envío OC: &lt;fechacreacion&gt;&lt;br&gt;Rechazado por: &lt;nombaprobador&gt;&lt;br&gt;Comentario: &lt;rechazo&gt;&lt;br&gt;&lt;br&gt;Para revisar mayores antecedentes, ingrese al módulo Compras de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Orden de Compra, Rechazada Aprobador',24,3);</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A111" s="6">
         <v>25</v>
       </c>
@@ -14433,15 +14444,15 @@
         <v>755</v>
       </c>
       <c r="S111" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20025, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de Cotización', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; lo ha invitado a participar de la siguiente Cotización. &lt;br&gt;&lt;br&gt;Nº de Cotización: &lt;numcz&gt;&lt;br&gt;Nombre Cotización: &lt;nomcz&gt;&lt;br&gt;Fecha de cierre: &lt;fechacierre&gt;&lt;br&gt;&lt;br&gt;No deje pasar esta Oportunidad de hacer Negocios. Para mayor información, ingrese al módulo Cotizaciones de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cotizaciones, Publicación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (2025, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de Cotización', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; lo ha invitado a participar de la siguiente Cotización. &lt;br&gt;&lt;br&gt;Nº de Cotización: &lt;numcz&gt;&lt;br&gt;Nombre Cotización: &lt;nomcz&gt;&lt;br&gt;Fecha de cierre: &lt;fechacierre&gt;&lt;br&gt;&lt;br&gt;No deje pasar esta Oportunidad de hacer Negocios. Para mayor información, ingrese al módulo Cotizaciones de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;','Cotizaciones, Publicación',25,2);</v>
       </c>
       <c r="T111" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20025, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de Cotización', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; lo ha invitado a participar de la siguiente Cotización. &lt;br&gt;&lt;br&gt;Nº de Cotización: &lt;numcz&gt;&lt;br&gt;Nombre Cotización: &lt;nomcz&gt;&lt;br&gt;Fecha de cierre: &lt;fechacierre&gt;&lt;br&gt;&lt;br&gt;No deje pasar esta Oportunidad de hacer Negocios. Para mayor información, ingrese al módulo Cotizaciones de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cotizaciones, Publicación');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (3025, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de Cotización', 'Estimados Sres. &lt;nombproveedor&gt;:&lt;br&gt;&lt;br&gt;Junto con saludarle, informamos a usted que la empresa &lt;nombempresa&gt; lo ha invitado a participar de la siguiente Cotización. &lt;br&gt;&lt;br&gt;Nº de Cotización: &lt;numcz&gt;&lt;br&gt;Nombre Cotización: &lt;nomcz&gt;&lt;br&gt;Fecha de cierre: &lt;fechacierre&gt;&lt;br&gt;&lt;br&gt;No deje pasar esta Oportunidad de hacer Negocios. Para mayor información, ingrese al módulo Cotizaciones de nuestro sistema.&lt;br&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;','Cotizaciones, Publicación',25,3);</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A112" s="6">
         <v>1000</v>
       </c>
@@ -14495,15 +14506,15 @@
         <v>762</v>
       </c>
       <c r="S112" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (21000, 'Agilice','B2belectrafk@iconstruye.com', 'Nueva(s) Órden(es) de Compra de {EmpresaCompradora}', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;    body {     font-family: Arial, Helvetica, sans-serif;     font-size: small;     padding: 12px;    }      p {     text-align: justify;    }      p.parrafo {     text-indent: 24px;    }   &lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;&lt;strong&gt;Estimado Señor {NombreDestinatario}&lt;/strong&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Por Encargo de &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; le informamos que se ha(n) generado la(s) siguiente(s) Órden(es) de Compra:&lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;strong&gt;Órdenes de Compra:&lt;/strong&gt;&lt;/p&gt; {ListaOC} &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Para Aceptar o Rechazar esta(s) Órden(es) de Compra, debe responder a este Correo, &lt;strong&gt;como Plazo Máximo dentro de 8 horas hábiles&lt;/strong&gt;, señalando claramente su desición. En caso de Rechazar la(s) OC debe explicar claramente las razones del rechazo.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;strong&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra,responda este correo indicado el nombre y correo electrónico del contacto&lt;/strong&gt;.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;a href=https://apps.agilice.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://apps.agilice.com/ clicktracking=off&gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Agilice y realizar enlínea la gestión completa de sus negocios con &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; a través de &lt;a href=https://apps.agilice.com/ clicktracking=off&gt;https://apps.agilice.com&lt;/a&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;&lt;strong&gt;NOTAS:&lt;/strong&gt; {Mensaje}&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;p&gt;Agilice S.A.&lt;/p&gt; &lt;p&gt;Servicio de Activación de Órdenes de Compra.&lt;/p&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (201000, 'Agilice','B2belectrafk@iconstruye.com', 'Nueva(s) Órden(es) de Compra de {EmpresaCompradora}', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;    body {     font-family: Arial, Helvetica, sans-serif;     font-size: small;     padding: 12px;    }      p {     text-align: justify;    }      p.parrafo {     text-indent: 24px;    }   &lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;&lt;strong&gt;Estimado Señor {NombreDestinatario}&lt;/strong&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Por Encargo de &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; le informamos que se ha(n) generado la(s) siguiente(s) Órden(es) de Compra:&lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;strong&gt;Órdenes de Compra:&lt;/strong&gt;&lt;/p&gt; {ListaOC} &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Para Aceptar o Rechazar esta(s) Órden(es) de Compra, debe responder a este Correo, &lt;strong&gt;como Plazo Máximo dentro de 8 horas hábiles&lt;/strong&gt;, señalando claramente su desición. En caso de Rechazar la(s) OC debe explicar claramente las razones del rechazo.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;strong&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra,responda este correo indicado el nombre y correo electrónico del contacto&lt;/strong&gt;.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;a href=https://apps.agilice.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://apps.agilice.com/ clicktracking=off&gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Agilice y realizar enlínea la gestión completa de sus negocios con &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; a través de &lt;a href=https://apps.agilice.com/ clicktracking=off&gt;https://apps.agilice.com&lt;/a&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;&lt;strong&gt;NOTAS:&lt;/strong&gt; {Mensaje}&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;p&gt;Agilice S.A.&lt;/p&gt; &lt;p&gt;Servicio de Activación de Órdenes de Compra.&lt;/p&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)',1000,2);</v>
       </c>
       <c r="T112" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (21000, 'Redmat','B2belectrafk@iconstruye.com', 'Nueva(s) Órden(es) de Compra de {EmpresaCompradora}', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;    body {     font-family: Arial, Helvetica, sans-serif;     font-size: small;     padding: 12px;    }      p {     text-align: justify;    }      p.parrafo {     text-indent: 24px;    }   &lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;&lt;strong&gt;Estimado Señor {NombreDestinatario}&lt;/strong&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Por Encargo de &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; le informamos que se ha(n) generado la(s) siguiente(s) Órden(es) de Compra:&lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;strong&gt;Órdenes de Compra:&lt;/strong&gt;&lt;/p&gt; {ListaOC} &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Para Aceptar o Rechazar esta(s) Órden(es) de Compra, debe responder a este Correo, &lt;strong&gt;como Plazo Máximo dentro de 8 horas hábiles&lt;/strong&gt;, señalando claramente su desición. En caso de Rechazar la(s) OC debe explicar claramente las razones del rechazo.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;strong&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra,responda este correo indicado el nombre y correo electrónico del contacto&lt;/strong&gt;.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Redmat y realizar enlínea la gestión completa de sus negocios con &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; a través de &lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;https://redmat.iconstruye.co&lt;/a&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;&lt;strong&gt;NOTAS:&lt;/strong&gt; {Mensaje}&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;p&gt;Redmat S.A.&lt;/p&gt; &lt;p&gt;Servicio de Activación de Órdenes de Compra.&lt;/p&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (301000, 'Redmat','B2belectrafk@iconstruye.com', 'Nueva(s) Órden(es) de Compra de {EmpresaCompradora}', '&lt;!DOCTYPE html&gt;&lt;html lang=es&gt; &lt;head&gt;&lt;meta charset=UTF-8&gt;&lt;style type=text/css&gt;    body {     font-family: Arial, Helvetica, sans-serif;     font-size: small;     padding: 12px;    }      p {     text-align: justify;    }      p.parrafo {     text-indent: 24px;    }   &lt;/style&gt;&lt;/head&gt; &lt;body&gt; &lt;p&gt;&lt;strong&gt;Estimado Señor {NombreDestinatario}&lt;/strong&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Por Encargo de &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; le informamos que se ha(n) generado la(s) siguiente(s) Órden(es) de Compra:&lt;/p&gt; &lt;br&gt; &lt;p&gt;&lt;strong&gt;Órdenes de Compra:&lt;/strong&gt;&lt;/p&gt; {ListaOC} &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;Para Aceptar o Rechazar esta(s) Órden(es) de Compra, debe responder a este Correo, &lt;strong&gt;como Plazo Máximo dentro de 8 horas hábiles&lt;/strong&gt;, señalando claramente su desición. En caso de Rechazar la(s) OC debe explicar claramente las razones del rechazo.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;strong&gt;Si usted no es el representante interno en su organización para gestionar esta Orden de Compra,responda este correo indicado el nombre y correo electrónico del contacto&lt;/strong&gt;.&lt;/p&gt; &lt;p class=parrafo&gt;&lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;Contáctenos&lt;/a&gt; para su incorporación como &lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;Proveedor Integrado&lt;/a&gt;, a la Comunidad de Redmat y realizar enlínea la gestión completa de sus negocios con &lt;strong&gt;{EmpresaCompradora}&lt;/strong&gt; a través de &lt;a href=https://redmat.iconstruye.com/ clicktracking=off&gt;https://redmat.iconstruye.co&lt;/a&gt;&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p class=parrafo&gt;&lt;strong&gt;NOTAS:&lt;/strong&gt; {Mensaje}&lt;/p&gt; &lt;br&gt;&lt;br&gt; &lt;p&gt;Atentamente,&lt;/p&gt; &lt;p&gt;Redmat S.A.&lt;/p&gt; &lt;p&gt;Servicio de Activación de Órdenes de Compra.&lt;/p&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Aviso de Nueva Orden de Compra a Proveedor No Integrado (PNI)',1000,3);</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6">
         <v>143</v>
       </c>
@@ -14559,15 +14570,15 @@
         <v>770</v>
       </c>
       <c r="S113" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20143, 'Agilice','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de LoCampino', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://locampino.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal LoCampino');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20143, 'Agilice','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de LoCampino', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://locampino.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal LoCampino',143,2);</v>
       </c>
       <c r="T113" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20143, 'Redmat','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de LoCampino', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://locampino.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal LoCampino');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30143, 'Redmat','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de LoCampino', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://locampino.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal LoCampino',143,3);</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="6">
         <v>144</v>
       </c>
@@ -14623,15 +14634,15 @@
         <v>778</v>
       </c>
       <c r="S114" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20144, 'Agilice','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de SalfaCorp', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://salfacorp.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal SalfaCorp');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20144, 'Agilice','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de SalfaCorp', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://salfacorp.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal SalfaCorp',144,2);</v>
       </c>
       <c r="T114" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20144, 'Redmat','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de SalfaCorp', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://salfacorp.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal SalfaCorp');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30144, 'Redmat','iconstruye@iconstruye.com', 'Recuperar contraseña - Portal de Pagos de SalfaCorp', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Recuperación de Contraseña&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Recuperación de &lt;strong&gt;Contraseña&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: justify; margin-bottom: 15px;"&gt;Junto con saludarte, recordamos que los datos de acceso a nuestro sistema son:&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;En caso de requerir información adicional, comunícate con nosotros al 2 486 1111 o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://salfacorp.iconstruye.com style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Usuario Recuperar Contraseña Portal SalfaCorp',144,3);</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6">
         <v>150</v>
       </c>
@@ -14687,15 +14698,15 @@
         <v>787</v>
       </c>
       <c r="S115" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20150, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Sigro', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Agilice&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Agilice&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Agilice, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://apps.agilice.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://sigro.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro portal Sigro');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20150, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Sigro', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Agilice&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Agilice&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Agilice, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://apps.agilice.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://sigro.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro portal Sigro',150,2);</v>
       </c>
       <c r="T115" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20150, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Sigro', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Redmat&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Redmat&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Redmat, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://sigro.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro portal Sigro');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30150, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Sigro', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Redmat&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Redmat&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Redmat, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://sigro.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro portal Sigro',150,3);</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
         <v>151</v>
       </c>
@@ -14751,15 +14762,15 @@
         <v>796</v>
       </c>
       <c r="S116" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20151, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Besalco', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Agilice&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Agilice&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Agilice, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://apps.agilice.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://besalco.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro portal Besalco');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20151, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Besalco', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Agilice&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Agilice&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Agilice, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://apps.agilice.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://besalco.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro portal Besalco',151,2);</v>
       </c>
       <c r="T116" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20151, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Besalco', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Redmat&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Redmat&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Redmat, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://besalco.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro portal Besalco');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30151, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Besalco', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Redmat&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Redmat&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Redmat, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://besalco.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro portal Besalco',151,3);</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
         <v>152</v>
       </c>
@@ -14815,15 +14826,15 @@
         <v>805</v>
       </c>
       <c r="S117" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20152, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Icafal', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Agilice&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Agilice&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Agilice, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://apps.agilice.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://icafal.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal Icafal');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20152, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Icafal', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Agilice&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Agilice&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Agilice, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://apps.agilice.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://icafal.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal Icafal',152,2);</v>
       </c>
       <c r="T117" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20152, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Icafal', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Redmat&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Redmat&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Redmat, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://icafal.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal Icafal');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30152, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de Icafal', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Redmat&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Redmat&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Redmat, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://icafal.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal Icafal',152,3);</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6">
         <v>153</v>
       </c>
@@ -14879,15 +14890,15 @@
         <v>813</v>
       </c>
       <c r="S118" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20153, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de LoCampino', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Agilice&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Agilice&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Agilice, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://apps.agilice.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://locampino.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal LoCampino');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20153, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de LoCampino', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Agilice&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Agilice&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Agilice, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://apps.agilice.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://locampino.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal LoCampino',153,2);</v>
       </c>
       <c r="T118" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20153, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de LoCampino', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Redmat&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Redmat&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Redmat, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://locampino.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal LoCampino');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30153, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de LoCampino', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Redmat&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Redmat&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Redmat, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://locampino.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal LoCampino',153,3);</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6">
         <v>154</v>
       </c>
@@ -14943,15 +14954,15 @@
         <v>821</v>
       </c>
       <c r="S119" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20154, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de SalfaCorp', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Agilice&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Agilice&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Agilice, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://apps.agilice.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://salfacorp.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal SalfaCorp');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20154, 'Agilice','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de SalfaCorp', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Agilice&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Agilice&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Agilice, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://apps.agilice.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://salfacorp.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Agilice | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal SalfaCorp',154,2);</v>
       </c>
       <c r="T119" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20154, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de SalfaCorp', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Redmat&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Redmat&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Redmat, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://salfacorp.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal SalfaCorp');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30154, 'Redmat','iconstruye@iconstruye.com', 'Bienvenido a Portal de Pagos de SalfaCorp', '&lt;!DOCTYPE html&gt;&lt;html lang=en&gt;&lt;head&gt;&lt;base href=http://diseno.iconstruye.cl/ic/desarrollando/portal-provedores/V5/email-avisos-portal-pago/aviso-nota-correccion.html&gt;&lt;meta http-equiv=Content-Type content="text/html; charset=UTF-8"&gt;&lt;meta name=viewport content="width=device-width, initial-scale=1"&gt;&lt;meta http-equiv=X-UA-Compatible content="IE=edge"&gt;&lt;title&gt;Bienvenido a Redmat&lt;/title&gt;&lt;style type=text/css&gt;/* Outlines the grids, remove when sending *//*table td { border: 1px solid cyan; }*//* CLIENT-SPECIFIC STYLES */body, table, td, a { -webkit-text-size-adjust: 100%; -ms-text-size-adjust: 100%; font-family: Helvetica, sans-serif; font-weight: 300; color: #333333; font-size: 14px;}table, td { mso-table-lspace: 0pt; mso-table-rspace: 0pt; }img { -ms-interpolation-mode: bicubic; }h1 {font-size: 1.2em;}.orange {display: none;}.container-orange {background-color: #ff7d28;width: 100%;}.container-green {background-color: #48a548;width: 100%;}.boxes {width: 48%;/*background-color: #efefef;*/padding: 20px;}.footer img {display: block;width: 35%;height: auto;}/* RESET STYLES */img { border: 0; outline: none; text-decoration: none; }table { border-collapse: collapse !important; }body { margin: 0 !important; padding: 0 !important; width: 100% !important; }/* iOS BLUE LINKS */a[x-apple-data-detectors] {color: inherit !important;text-decoration: none !important;font-size: inherit !important;font-family: inherit !important;font-weight: inherit !important;line-height: inherit !important;}/* ANDROID CENTER FIX */div[style*="margin: 16px 0;"] { margin: 0 !important; }/* MEDIA QUERIES */@media all and (max-width:639px) { .wrapper{ width:320px!important; padding: 0 !important; }.container{ width:300px!important;padding: 0 !important; }.mobile{ width:300px!important; display:block!important; padding: 0 !important; }.img{ width:100% !important; height:auto !important; }*[class="mobileOff"] { width: 0px !important; display: none !important; }*[class*="mobileOn"] { display: block !important; max-height:none !important; }}@media screen and (max-width:380px) {h1 {font-size: 1.4em;text-align: center;color: #666666;}h3 {font-size: 1.6em!important;}.wrapper { width:100%!important; padding: 0 !important;}.mobile {width: 100% !important; padding: 0 !important; }.mobile p {text-align: center!important;font-size: 1.3em !important; }.boton {font-size: 1.8em !important;padding: 30px !important;}.footer p {font-size: 0.9em !important;}.footer p a { font-size: 0.9em !important; }.footer img {display: block;width: 50%;height: auto;}.logo {width: 70% !important;}.orange {position: absolute;top: 0;background-color: #ff7d28;display: block!important;}.up {display: none!important;}.down {margin-top: 90px!important;}.container-img {width:100%!important;padding: 0 !important;}.container-orange {width:100%!important;padding: 0 !important;}.container-orange h3 {font-size: 1.6em !important;}.boxes {padding: 10px!important;border-bottom: 1px solid #dddddd;}}&lt;/style&gt;&lt;script type=text/javascript data-savepage-src=chrome-extension://aadgmnobpdmgmigaicncghmmoeflnamj/ng-inspector.js src&gt;&lt;/script&gt;&lt;link rel=icon href&gt;&lt;/head&gt;&lt;body style="margin:0; padding:0; background-color:#F2F2F2;"&gt;&lt;span style="display: block; width: 640px !important; max-width: 640px; height: 1px" class=mobileOff&gt;&lt;/span&gt;&lt;center&gt;&lt;table width=100% border=0 cellpadding=0 cellspacing=0 bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top bgcolor=#373B46 style=background-color:#373B46;&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td width=100% class=mobile align=center valign=middle style=padding:10px;&gt;&lt;img class=logo src=https://cl.iconstruye.com/landing-home-prov/assents/images/logo-1.png style="width: 120px;"&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container-orange&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=middle style=min-height:110px&gt;&lt;h3 style="font-size: 1.8em; font-weight: 200; color: #ffffff;"&gt;Bienvenido a &lt;strong&gt;Redmat&lt;/strong&gt;&lt;/h3&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#FFFFFF&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td align=center valign=top style="padding: 10px 0;"&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class=mobile align=left valign=top&gt;&lt;p style="font-size: 1.1em; margin-bottom: 25px;"&gt;Estimado (a): &lt;strong&gt;&lt;nombusuario&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Te damos la bienvenida al Portal de Proveedores de Redmat, la plataforma tecnológica que permite a constructoras y proveedores intercambiar información de los procesos de facturación y pago de facturas.&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 15px;"&gt;Hacemos envío de tus datos de acceso a nuestra plataforma:&lt;br&gt;&lt;br&gt;Usuario: &lt;strong&gt;&lt;idusuario&gt;&lt;/strong&gt;&lt;br&gt;Organización: &lt;strong&gt;&lt;nombempresa&gt;&lt;/strong&gt;&lt;br&gt;Clave: &lt;strong&gt;&lt;clave&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p style=" font-size: 1.1em; text-align: left; margin-bottom: 45px;"&gt;Para información adicional nos encuentras en:&lt;br&gt;Fono: &lt;fonocontacto&gt; o al correo &lt;a style="color: #ff7d28;" href=mailto:portalproveedores@iconstruye.com&gt;portalproveedores@iconstruye.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Atentamente,&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;a style="color: #ff7d28;" href=https://redmat.iconstruye.com&gt;www.iconstruye.com&lt;/a&gt; &lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=top&gt;&lt;a href=https://salfacorp.iconstruye.com/ style="background:#ff7d28; color:#fff; padding:10px 20px; text-decoration: none; border-radius:4px; margin: 10px 0;display:inline-block;font-size: 1.2em;font-weight: 400;line-height: 26px;"&gt;Ingresar al Portal de Pagos&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=20 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;table width=640 cellpadding=0 cellspacing=0 border=0 class=wrapper bgcolor=#F2F2F2&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td class=mobile align=center valign=middle style="padding:5px 10px;"&gt;&lt;img src=http://diseno.iconstruye.cl/mailing/newsletter/images/201802/201802-logo-ic-grey.png&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td align=center valign=top&gt;&lt;table width=600 cellpadding=0 cellspacing=0 border=0 class=container&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td class="mobile footer" align=center valign=top&gt;&lt;p style="line-height: 1.5em; font-size: 0.9em; text-align: center; color: #999999;"&gt;Correo enviado a través de Redmat | Todos los Derechos Reservados |&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td height=10 style="font-size:10px; line-height:10px;"&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt; &lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/center&gt;&lt;div id=extension-kmmojbkhfhninkelnlcnliacgncnnikf-installed&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;','Registro Portal SalfaCorp',154,3);</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
         <v>6508</v>
       </c>
@@ -15005,15 +15016,15 @@
         <v>828</v>
       </c>
       <c r="S120" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26508, 'Agilice','iconstruye@iconstruye.com', 'Líneas de Pedido de Material Modificada', '&lt;div style=width:600px&gt;&lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Estimado(a) &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludar, informamos que el pedido de material N° &lt;numpm&gt; solicitado por Ud. ha sido modificado. &lt;br&gt;&lt;br&gt;&lt;b&gt; N° pedido: &lt;/b&gt;&lt;numpm&gt;&lt;br&gt;&lt;b&gt; Nombre pedido: &lt;/b&gt;&lt;nompm&gt;&lt;br&gt;&lt;b&gt; Centro de gestión: &lt;/b&gt;&lt;nomborgc&gt;&lt;br&gt;&lt;b&gt; Fecha de creación: &lt;/b&gt;&lt;/b&gt;&lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;&lt;mensajealerta&gt;&lt;br&gt;&lt;tablalineas&gt;&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;&lt;/div&gt;','Se envia cuando se modifican las cantidades de las líneas de un pedido de material');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (206508, 'Agilice','iconstruye@iconstruye.com', 'Líneas de Pedido de Material Modificada', '&lt;div style=width:600px&gt;&lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Estimado(a) &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludar, informamos que el pedido de material N° &lt;numpm&gt; solicitado por Ud. ha sido modificado. &lt;br&gt;&lt;br&gt;&lt;b&gt; N° pedido: &lt;/b&gt;&lt;numpm&gt;&lt;br&gt;&lt;b&gt; Nombre pedido: &lt;/b&gt;&lt;nompm&gt;&lt;br&gt;&lt;b&gt; Centro de gestión: &lt;/b&gt;&lt;nomborgc&gt;&lt;br&gt;&lt;b&gt; Fecha de creación: &lt;/b&gt;&lt;/b&gt;&lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;&lt;mensajealerta&gt;&lt;br&gt;&lt;tablalineas&gt;&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Agilice&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://apps.agilice.com/img/logo-agilice.png img&gt;&lt;/div&gt;','Se envia cuando se modifican las cantidades de las líneas de un pedido de material',6508,2);</v>
       </c>
       <c r="T120" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (26508, 'Redmat','iconstruye@iconstruye.com', 'Líneas de Pedido de Material Modificada', '&lt;div style=width:600px&gt;&lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Estimado(a) &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludar, informamos que el pedido de material N° &lt;numpm&gt; solicitado por Ud. ha sido modificado. &lt;br&gt;&lt;br&gt;&lt;b&gt; N° pedido: &lt;/b&gt;&lt;numpm&gt;&lt;br&gt;&lt;b&gt; Nombre pedido: &lt;/b&gt;&lt;nompm&gt;&lt;br&gt;&lt;b&gt; Centro de gestión: &lt;/b&gt;&lt;nomborgc&gt;&lt;br&gt;&lt;b&gt; Fecha de creación: &lt;/b&gt;&lt;/b&gt;&lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;&lt;mensajealerta&gt;&lt;br&gt;&lt;tablalineas&gt;&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;&lt;/div&gt;','Se envia cuando se modifican las cantidades de las líneas de un pedido de material');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (306508, 'Redmat','iconstruye@iconstruye.com', 'Líneas de Pedido de Material Modificada', '&lt;div style=width:600px&gt;&lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Estimado(a) &lt;nombsolicitante&gt;: &lt;br&gt; Junto con saludar, informamos que el pedido de material N° &lt;numpm&gt; solicitado por Ud. ha sido modificado. &lt;br&gt;&lt;br&gt;&lt;b&gt; N° pedido: &lt;/b&gt;&lt;numpm&gt;&lt;br&gt;&lt;b&gt; Nombre pedido: &lt;/b&gt;&lt;nompm&gt;&lt;br&gt;&lt;b&gt; Centro de gestión: &lt;/b&gt;&lt;nomborgc&gt;&lt;br&gt;&lt;b&gt; Fecha de creación: &lt;/b&gt;&lt;/b&gt;&lt;fechacreacion&gt;&lt;br&gt;&lt;br&gt;&lt;mensajealerta&gt;&lt;br&gt;&lt;tablalineas&gt;&lt;br&gt;&lt;br&gt; Atentamente,&lt;br&gt;&lt;br&gt;Equipo Redmat&lt;br&gt;&lt;link&gt;&lt;br&gt;Mesa de Ayuda&lt;br&gt;486 11 11&lt;br&gt;&lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png img&gt;&lt;/div&gt;','Se envia cuando se modifican las cantidades de las líneas de un pedido de material',6508,3);</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="6">
         <v>161</v>
       </c>
@@ -15069,15 +15080,15 @@
         <v>836</v>
       </c>
       <c r="S121" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20161, 'Agilice','iconstruye@iconstruye.com', 'Recepción de Hormigón &lt;NumRecepcion&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Recepción de Hormigón N° &lt;numrecepcion&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt;&lt;br&gt;&lt;a href=https://apps.agilice.com&gt; https://apps.agilice.com &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una recepción de Hormigones');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20161, 'Agilice','iconstruye@iconstruye.com', 'Recepción de Hormigón &lt;NumRecepcion&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Recepción de Hormigón N° &lt;numrecepcion&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt;&lt;br&gt;&lt;a href=https://apps.agilice.com&gt; https://apps.agilice.com &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una recepción de Hormigones',161,2);</v>
       </c>
       <c r="T121" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20161, 'Redmat','iconstruye@iconstruye.com', 'Recepción de Hormigón &lt;NumRecepcion&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Recepción de Hormigón N° &lt;numrecepcion&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt;&lt;br&gt;&lt;a href=https://redmat.iconstruye.com&gt; https://redmat.iconstruye.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una recepción de Hormigones');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30161, 'Redmat','iconstruye@iconstruye.com', 'Recepción de Hormigón &lt;NumRecepcion&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Recepción de Hormigón N° &lt;numrecepcion&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt;&lt;br&gt;&lt;a href=https://redmat.iconstruye.com&gt; https://redmat.iconstruye.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una recepción de Hormigones',161,3);</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
         <v>162</v>
       </c>
@@ -15133,15 +15144,15 @@
         <v>843</v>
       </c>
       <c r="S122" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20162, 'Agilice','iconstruye@iconstruye.com', 'Recepción On Field &lt;NumRecepcion&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Recepción On Field N° &lt;numrecepcion&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt;&lt;br&gt;&lt;a href=https://apps.agilice.com&gt; https://apps.agilice.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una recepción On Field');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20162, 'Agilice','iconstruye@iconstruye.com', 'Recepción On Field &lt;NumRecepcion&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Recepción On Field N° &lt;numrecepcion&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt;&lt;br&gt;&lt;a href=https://apps.agilice.com&gt; https://apps.agilice.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una recepción On Field',162,2);</v>
       </c>
       <c r="T122" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20162, 'Redmat','iconstruye@iconstruye.com', 'Recepción On Field &lt;NumRecepcion&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Recepción On Field N° &lt;numrecepcion&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt;&lt;br&gt;&lt;a href=https://redmat.iconstruye.com&gt; https://redmat.iconstruye.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una recepción On Field');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30162, 'Redmat','iconstruye@iconstruye.com', 'Recepción On Field &lt;NumRecepcion&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Recepción On Field N° &lt;numrecepcion&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt;&lt;br&gt;&lt;a href=https://redmat.iconstruye.com&gt; https://redmat.iconstruye.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una recepción On Field',162,3);</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
         <v>163</v>
       </c>
@@ -15197,15 +15208,15 @@
         <v>850</v>
       </c>
       <c r="S123" s="9" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20163, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de Pedido de Material &lt;NumSolicitud&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Solicitud de Pedido de Material N° &lt;numsolicitud&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt;&lt;br&gt; &lt;a href=https://apps.agilice.com&gt;https://apps.agilice.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@apps.agilice.com&gt;comercial@apps.agilice.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una solicitud de Pedido de Materiales');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20163, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de Pedido de Material &lt;NumSolicitud&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Solicitud de Pedido de Material N° &lt;numsolicitud&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt;&lt;br&gt; &lt;a href=https://apps.agilice.com&gt;https://apps.agilice.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@apps.agilice.com&gt;comercial@apps.agilice.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una solicitud de Pedido de Materiales',163,2);</v>
       </c>
       <c r="T123" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20163, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de Pedido de Material &lt;NumSolicitud&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Solicitud de Pedido de Material N° &lt;numsolicitud&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt;&lt;br&gt; &lt;a href=https://redmat.iconstruye.com&gt;https://redmat.iconstruye.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una solicitud de Pedido de Materiales');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30163, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de Pedido de Material &lt;NumSolicitud&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Solicitud de Pedido de Material N° &lt;numsolicitud&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt;&lt;br&gt; &lt;a href=https://redmat.iconstruye.com&gt;https://redmat.iconstruye.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una solicitud de Pedido de Materiales',163,3);</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="10">
         <v>164</v>
       </c>
@@ -15261,12 +15272,12 @@
         <v>857</v>
       </c>
       <c r="S124" s="13" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20164, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de Consumo &lt;NumConsumo&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Solicitud de Consumo N° &lt;numconsumo&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt;&lt;br&gt;&lt;a&gt; www.apps.agilice.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@apps.agilice.com&gt;comercial@apps.agilice.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una solicitud de Consumo');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"20"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Agilice','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_A]]&amp;"', '"&amp;Table1[[#This Row],[A_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",2);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (20164, 'Agilice','iconstruye@iconstruye.com', 'Solicitud de Consumo &lt;NumConsumo&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Solicitud de Consumo N° &lt;numconsumo&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Agilice &lt;br&gt;&lt;br&gt;&lt;a&gt; www.apps.agilice.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@apps.agilice.com&gt;comercial@apps.agilice.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://apps.agilice.com/img/logo-agilice.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una solicitud de Consumo',164,2);</v>
       </c>
       <c r="T124" t="str">
-        <f>"INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (" &amp;  Table1[[#This Row],[IDMAIL]]+20000 &amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"');"</f>
-        <v>INSERT INTO MAIL (IDMAIL, MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION) VALUES (20164, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de Consumo &lt;NumConsumo&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Solicitud de Consumo N° &lt;numconsumo&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt;&lt;br&gt; &lt;a href=https://redmat.iconstruye.com&gt;redmat.iconstruye.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una solicitud de Consumo');</v>
+        <f>"INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES ("&amp;"30"&amp;Table1[[#This Row],[IDMAIL]]&amp; ", 'Redmat','" &amp; Table1[[#This Row],[MREMITENTEMAIL]]&amp;"', '" &amp; Table1[[#This Row],[MASUNTO_R]]&amp;"', '"&amp;Table1[[#This Row],[R_minified]]&amp;"','"&amp;Table1[[#This Row],[DESCRIPCION]]&amp;"',"&amp;Table1[[#This Row],[IDMAIL]]&amp;",3);"</f>
+        <v>INSERT INTO MAIL (IDMAIL,MREMITENTE, MREMITENTEMAIL, MASUNTO, MCUERPO1, DESCRIPCION, GRUPOMAIL, IDSITIO) VALUES (30164, 'Redmat','iconstruye@iconstruye.com', 'Solicitud de Consumo &lt;NumConsumo&gt; pendiente de atención', '&lt;div style=width:600px&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; &lt;b&gt;Estimado(a) &lt;nombreusuario&gt;:&lt;/b&gt; &lt;br&gt;&lt;br&gt; Te informamos que la Solicitud de Consumo N° &lt;numconsumo&gt;, del Centro de Gestión &lt;centrogestion&gt;, está pendiente de atención. &lt;/p&gt; &lt;br&gt; &lt;p style=font-family:Arial;font-size:12px;text-align:left&gt; Atentamente, &lt;br&gt;&lt;br&gt; Equipo Redmat &lt;br&gt;&lt;br&gt; &lt;a href=https://redmat.iconstruye.com&gt;redmat.iconstruye.com&lt;/a&gt; &lt;br&gt;&lt;br&gt; ¿Dudas? Escríbenos a &lt;a href=mailto:comercial@iconstruye.com&gt;comercial@iconstruye.com &lt;/a&gt; &lt;br&gt;&lt;br&gt; &lt;/p&gt; &lt;/div&gt; &lt;img src=https://redmat.iconstruye.com/img/logo-redmat.png&gt; &lt;/body&gt; &lt;/html&gt;','Se envía al crear una solicitud de Consumo',164,3);</v>
       </c>
     </row>
   </sheetData>
@@ -15276,4 +15287,28 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A66E27D6-2341-4C6D-BBF3-3243230A2869}">
+  <sheetPr codeName="Hoja2"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>861</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>